<commit_message>
se agrega fecha de calculo para el cat. Se formatean algunos valores numericos para el json del pdf
</commit_message>
<xml_diff>
--- a/Json_ofertas.xlsx
+++ b/Json_ofertas.xlsx
@@ -126,7 +126,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,12 +137,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -243,23 +237,23 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,7 +579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4">
         <v>673131</v>
       </c>
@@ -596,7 +590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="7">
         <v>738919</v>
       </c>
@@ -605,7 +599,7 @@
       </c>
       <c r="C3" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="7">
         <v>847334</v>
       </c>
@@ -614,7 +608,7 @@
       </c>
       <c r="C4" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="7">
         <v>915334</v>
       </c>
@@ -623,7 +617,7 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="7">
         <v>944006</v>
       </c>
@@ -632,7 +626,7 @@
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="7">
         <v>957527</v>
       </c>
@@ -641,7 +635,7 @@
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="7">
         <v>974191</v>
       </c>
@@ -650,7 +644,7 @@
       </c>
       <c r="C8" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="7">
         <v>1030366</v>
       </c>
@@ -659,7 +653,7 @@
       </c>
       <c r="C9" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="7">
         <v>2846689</v>
       </c>
@@ -668,7 +662,7 @@
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="7">
         <v>2860522</v>
       </c>
@@ -677,7 +671,7 @@
       </c>
       <c r="C11" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="7">
         <v>2945331</v>
       </c>
@@ -686,7 +680,7 @@
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="7">
         <v>2963137</v>
       </c>
@@ -695,7 +689,7 @@
       </c>
       <c r="C13" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="7">
         <v>2969347</v>
       </c>
@@ -704,7 +698,7 @@
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="7">
         <v>3023771</v>
       </c>
@@ -713,7 +707,7 @@
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="7">
         <v>3075427</v>
       </c>
@@ -722,7 +716,7 @@
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="7">
         <v>3078718</v>
       </c>
@@ -731,7 +725,7 @@
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="7">
         <v>3145143</v>
       </c>
@@ -740,7 +734,7 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="7">
         <v>3185555</v>
       </c>
@@ -749,7 +743,7 @@
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="7">
         <v>3222314</v>
       </c>
@@ -758,7 +752,7 @@
       </c>
       <c r="C20" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="7">
         <v>3231351</v>
       </c>
@@ -767,7 +761,7 @@
       </c>
       <c r="C21" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="7">
         <v>3266945</v>
       </c>
@@ -776,7 +770,7 @@
       </c>
       <c r="C22" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="7">
         <v>3283744</v>
       </c>
@@ -785,7 +779,7 @@
       </c>
       <c r="C23" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="7">
         <v>3395159</v>
       </c>

</xml_diff>

<commit_message>
- Se creo la clase de GenericUtilities - Se movio el metodo round de LoanSimulator a la clase GenericUtilities - Se agrego Json con valores formateados para el API de PDF
</commit_message>
<xml_diff>
--- a/Json_ofertas.xlsx
+++ b/Json_ofertas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>prospectus_id</t>
   </si>
@@ -40,7 +40,13 @@
     <t>{"Prospecto": 915334, "monto_maximo_cliente": 396656.0, "cuota_externa_total": 25526.0, "capacidad_maxima_pago": 390950.0, "bursolnum": 7262001, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 17032.558390112892, "monto_max": 396656.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 54.0, "plazo_min": 4, "tasa": 0.3813, "comision": 0.0, "proba": 0, "segmento": 26, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":7, "monto_otorgado":15300.0, "cuota":1116.0, "saldo":15358.0, "tasa_externa":-1.0, "tasa_kubo":0.0038, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0038, "fecha_inicio":"2017-06-23", "tipo_deuda":"R", "ahorro_cuota_mensual":2843.441609887108, "ahorro_total":153545.8469339038, "estatus_tasa":"Desbordamiento numérico", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":336000.0, "cuota":16556.0, "saldo":311616.0, "tasa_externa":0.5792, "tasa_kubo":0.0038, "numero_pagos_otorgado":144.0, "numero_pagos_restante":59.0, "frecuencia_externa":"S", "avance":0.0726, "fecha_inicio":"2023-02-20", "tipo_deuda":"I", "ahorro_cuota_mensual":2843.441609887108, "ahorro_total":153545.8469339038, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":22400.0, "cuota":1500, "saldo":22322.0, "tasa_externa":-1.0, "tasa_kubo":0.0038, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0035, "fecha_inicio":"2014-09-13", "tipo_deuda":"R", "ahorro_cuota_mensual":2843.441609887108, "ahorro_total":153545.8469339038, "estatus_tasa":"Falta Pago_periodico", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":15300.0, "cuota":704, "saldo":14035.0, "tasa_externa":-1.0, "tasa_kubo":0.0038, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0827, "fecha_inicio":"2017-06-23", "tipo_deuda":"R", "ahorro_cuota_mensual":2843.441609887108, "ahorro_total":153545.8469339038, "estatus_tasa":"Falta Pago_periodico", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":50000.0, "cuota":3282.0, "saldo":49566.0, "tasa_externa":0.6886, "tasa_kubo":0.0038, "numero_pagos_otorgado":36.0, "numero_pagos_restante":28.0, "frecuencia_externa":"M", "avance":0.0087, "fecha_inicio":"2023-07-04", "tipo_deuda":"I", "ahorro_cuota_mensual":2843.441609887108, "ahorro_total":153545.8469339038, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "GUBERNAMENTALES", "registro":5, "monto_otorgado":70670.0, "cuota":2356.0, "saldo":47524.0, "tasa_externa":0.0001, "tasa_kubo":0.0038, "numero_pagos_otorgado":30.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.3275, "fecha_inicio":"2023-05-04", "tipo_deuda":"I", "ahorro_cuota_mensual":2843.441609887108, "ahorro_total":153545.8469339038, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "GUBERNAMENTALES", "registro":6, "monto_otorgado":66472.0, "cuota":2216.0, "saldo":20676.0, "tasa_externa":0.0001, "tasa_kubo":0.0038, "numero_pagos_otorgado":30.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.689, "fecha_inicio":"2022-03-07", "tipo_deuda":"I", "ahorro_cuota_mensual":2843.441609887108, "ahorro_total":153545.8469339038, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
+    <t>Para deudas no consolidables, la tasa kubo viene como "tasa_kubo": 0.0038,</t>
+  </si>
+  <si>
     <t>{"Prospecto": 944006, "monto_maximo_cliente": 500000.0, "cuota_externa_total": 43825.0, "capacidad_maxima_pago": 816653.0, "bursolnum": 7261004, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 32175.26206082056, "monto_max": 500000.0, "cuota_min": 130.08822700780902, "monto_min": 5000, "plazo_max": 18.0, "plazo_min": 4, "tasa": 0.165, "comision": 0.0, "proba": 0, "segmento": 26, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.165], "comisiones": [0], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":4, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.0016, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2010-04-11", "tipo_deuda":"O", "ahorro_cuota_mensual":18733.73793917944, "ahorro_total":337207.2829052299, "estatus_tasa":"Falta Pago_periodico", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":2687140.0, "cuota":21291.0, "saldo":2121434.0, "tasa_externa":0.0738, "tasa_kubo":0.0016, "numero_pagos_otorgado":240.0, "numero_pagos_restante":163.0, "frecuencia_externa":"M", "avance":0.2105, "fecha_inicio":"2017-09-28", "tipo_deuda":"M", "ahorro_cuota_mensual":18733.73793917944, "ahorro_total":337207.2829052299, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":150000.0, "cuota":5533.0, "saldo":150756.0, "tasa_externa":0.1973, "tasa_kubo":0.0016, "numero_pagos_otorgado":36.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":-0.005, "fecha_inicio":"2023-12-20", "tipo_deuda":"I", "ahorro_cuota_mensual":18733.73793917944, "ahorro_total":337207.2829052299, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":20000.0, "cuota":499.0, "saldo":499.0, "tasa_externa":-1.0, "tasa_kubo":0.0016, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.975, "fecha_inicio":"2004-06-13", "tipo_deuda":"O", "ahorro_cuota_mensual":18733.73793917944, "ahorro_total":337207.2829052299, "estatus_tasa":"Desbordamiento numérico", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":322400.0, "cuota":1620.0, "saldo":4854.0, "tasa_externa":-1.0, "tasa_kubo":0.0016, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9849, "fecha_inicio":"1996-02-28", "tipo_deuda":"R", "ahorro_cuota_mensual":18733.73793917944, "ahorro_total":337207.2829052299, "estatus_tasa":"Desbordamiento numérico", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":694000.0, "cuota":10981, "saldo":89846.0, "tasa_externa":-1.0, "tasa_kubo":0.0016, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8705, "fecha_inicio":"2020-04-27", "tipo_deuda":"R", "ahorro_cuota_mensual":18733.73793917944, "ahorro_total":337207.2829052299, "estatus_tasa":"Falta Pago_periodico", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":60000.0, "cuota":4192.0, "saldo":3433.0, "tasa_externa":0.3081, "tasa_kubo":0.0016, "numero_pagos_otorgado":18.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.9428, "fecha_inicio":"2023-10-30", "tipo_deuda":"I", "ahorro_cuota_mensual":18733.73793917944, "ahorro_total":337207.2829052299, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":250163.0, "cuota":9116, "saldo":40761.0, "tasa_externa":-1.0, "tasa_kubo":0.0016, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8371, "fecha_inicio":"2009-04-29", "tipo_deuda":"R", "ahorro_cuota_mensual":18733.73793917944, "ahorro_total":337207.2829052299, "estatus_tasa":"Falta Pago_periodico", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":500000.0, "cuota":25000.0, "saldo":142230.0, "tasa_externa":-1.0, "tasa_kubo":0.0016, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7155, "fecha_inicio":"2013-11-01", "tipo_deuda":"R", "ahorro_cuota_mensual":18733.73793917944, "ahorro_total":337207.2829052299, "estatus_tasa":"Desbordamiento numérico", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":0.0, "cuota":0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.0016, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-1.0, "fecha_inicio":"2008-01-18", "tipo_deuda":"R", "ahorro_cuota_mensual":18733.73793917944, "ahorro_total":337207.2829052299, "estatus_tasa":"Falta Pago_periodico", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>Para deudas no consolidables, la tasa kubo viene como "tasa_kubo": 0.0016</t>
   </si>
   <si>
     <t>{"Prospecto": 957527, "monto_maximo_cliente": 360945.0, "cuota_externa_total": 35131.0, "capacidad_maxima_pago": 367456.0, "bursolnum": 7262364, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 21953.446212106446, "monto_max": 360945.0, "cuota_min": 299.79381766541826, "monto_min": 5000, "plazo_max": 54.0, "plazo_min": 4, "tasa": 0.5991, "comision": 0.0, "proba": 0, "segmento": 26, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":10800.0, "cuota":1800, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.006, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2012-07-16", "tipo_deuda":"R", "ahorro_cuota_mensual":739.5537878935538, "ahorro_total":39935.904546251906, "estatus_tasa":"Falta Pago_periodico", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":186600.0, "cuota":11788.0, "saldo":90098.0, "tasa_externa":0.7483, "tasa_kubo":0.006, "numero_pagos_otorgado":120.0, "numero_pagos_restante":17.0, "frecuencia_externa":"S", "avance":0.5172, "fecha_inicio":"2020-08-18", "tipo_deuda":"I", "ahorro_cuota_mensual":739.5537878935538, "ahorro_total":39935.904546251906, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":10000.0, "cuota":1110.0, "saldo":11978.0, "tasa_externa":-1.0, "tasa_kubo":0.006, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.1978, "fecha_inicio":"2013-10-01", "tipo_deuda":"R", "ahorro_cuota_mensual":739.5537878935538, "ahorro_total":39935.904546251906, "estatus_tasa":"Desbordamiento numérico", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":126300.0, "cuota":7995.0, "saldo":126264.0, "tasa_externa":-1.0, "tasa_kubo":0.006, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0003, "fecha_inicio":"2019-01-10", "tipo_deuda":"R", "ahorro_cuota_mensual":739.5537878935538, "ahorro_total":39935.904546251906, "estatus_tasa":"Desbordamiento numérico", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":224000.0, "cuota":14238.0, "saldo":214947.0, "tasa_externa":0.6876, "tasa_kubo":0.006, "numero_pagos_otorgado":40.0, "numero_pagos_restante":29.0, "frecuencia_externa":"M", "avance":0.0404, "fecha_inicio":"2023-04-12", "tipo_deuda":"I", "ahorro_cuota_mensual":739.5537878935538, "ahorro_total":39935.904546251906, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
@@ -565,7 +571,7 @@
   <cols>
     <col min="1" max="1" style="8" width="8.862142857142858" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="9" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="68.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -615,23 +621,27 @@
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="7">
         <v>944006</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="7">
         <v>957527</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -640,7 +650,7 @@
         <v>974191</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -649,7 +659,7 @@
         <v>1030366</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C9" s="6"/>
     </row>
@@ -658,7 +668,7 @@
         <v>2846689</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6"/>
     </row>
@@ -667,7 +677,7 @@
         <v>2860522</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6"/>
     </row>
@@ -676,7 +686,7 @@
         <v>2945331</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -685,7 +695,7 @@
         <v>2963137</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C13" s="6"/>
     </row>
@@ -694,7 +704,7 @@
         <v>2969347</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C14" s="6"/>
     </row>
@@ -703,7 +713,7 @@
         <v>3023771</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C15" s="6"/>
     </row>
@@ -712,7 +722,7 @@
         <v>3075427</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16" s="6"/>
     </row>
@@ -721,7 +731,7 @@
         <v>3078718</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C17" s="6"/>
     </row>
@@ -730,7 +740,7 @@
         <v>3145143</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C18" s="6"/>
     </row>
@@ -739,7 +749,7 @@
         <v>3185555</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" s="6"/>
     </row>
@@ -748,7 +758,7 @@
         <v>3222314</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C20" s="6"/>
     </row>
@@ -757,7 +767,7 @@
         <v>3231351</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C21" s="6"/>
     </row>
@@ -766,7 +776,7 @@
         <v>3266945</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C22" s="6"/>
     </row>
@@ -775,7 +785,7 @@
         <v>3283744</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C23" s="6"/>
     </row>
@@ -784,7 +794,7 @@
         <v>3395159</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C24" s="6"/>
     </row>
@@ -793,7 +803,7 @@
         <v>3398532</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C25" s="6"/>
     </row>
@@ -802,7 +812,7 @@
         <v>3429016</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C26" s="6"/>
     </row>
@@ -811,7 +821,7 @@
         <v>3491079</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C27" s="6"/>
     </row>
@@ -820,7 +830,7 @@
         <v>3550281</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C28" s="6"/>
     </row>
@@ -829,7 +839,7 @@
         <v>3563076</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C29" s="6"/>
     </row>
@@ -838,7 +848,7 @@
         <v>3565514</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C30" s="6"/>
     </row>
@@ -847,7 +857,7 @@
         <v>3672001</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C31" s="6"/>
     </row>
@@ -856,7 +866,7 @@
         <v>3688011</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C32" s="6"/>
     </row>

</xml_diff>

<commit_message>
revolver saving were hidden into json to pdf when they can not be selected
</commit_message>
<xml_diff>
--- a/Json_ofertas.xlsx
+++ b/Json_ofertas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>prospectus_id</t>
   </si>
@@ -76,10 +76,19 @@
     <t>{"Prospecto": 4606694, "monto_maximo_cliente": 102071.0, "cuota_externa_total": 19385.0, "capacidad_maxima_pago": 131688.0, "bursolnum": 7353978, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 6314.992394796616, "monto_max": 102071.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.7554, "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":82000.0, "cuota":4100.0, "saldo":68609.0, "tasa_externa":0.0124, "tasa_kubo":0.7554, "numero_pagos_otorgado":900.0, "numero_pagos_restante":877.0, "frecuencia_externa":"Z", "avance":0.1633, "fecha_inicio":"2022-05-03", "tipo_deuda":"R", "ahorro_cuota_mensual":-989.5401044568471, "ahorro_total":-58382.86616295398, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":8500.0, "cuota":425.0, "saldo":8432.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.008, "fecha_inicio":"2021-02-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-200.50105905610258, "ahorro_total":-11829.562484310052, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":18000.0, "cuota":900.0, "saldo":17864.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0076, "fecha_inicio":"2020-07-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-425.1839325163917, "ahorro_total":-25085.85201846711, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":8000.0, "cuota":1432.0, "saldo":7166.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1042, "fecha_inicio":"2023-11-02", "tipo_deuda":"R", "ahorro_cuota_mensual":900.4131179795979, "ahorro_total":53124.37396079628, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":347900.0, "cuota":12658.0, "saldo":225451.0, "tasa_externa":0.4005, "tasa_kubo":0.7554, "numero_pagos_otorgado":144.0, "numero_pagos_restante":35.0, "frecuencia_externa":"S", "avance":0.352, "fecha_inicio":"2021-02-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-13149.853231216566, "ahorro_total":-775841.3406417774, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":15000.0, "cuota":1738.0, "saldo":11240.0, "tasa_externa":0.8996, "tasa_kubo":0.7554, "numero_pagos_otorgado":28.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.2507, "fecha_inicio":"2023-07-26", "tipo_deuda":"I", "ahorro_cuota_mensual":625.2727839371989, "ahorro_total":36891.09425229474, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":9000.0, "cuota":1305.0, "saldo":9396.0, "tasa_externa":0.8999, "tasa_kubo":0.7554, "numero_pagos_otorgado":10.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":-0.044, "fecha_inicio":"2024-01-10", "tipo_deuda":"I", "ahorro_cuota_mensual":637.3636703623195, "ahorro_total":37604.45655137685, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
+    <t>Revolvente con tasa reportada ¿es correcto? Trae una tasa del "tasa_externa": 0.0124</t>
+  </si>
+  <si>
     <t>{"Prospecto": 4688988, "monto_maximo_cliente": 52860.0, "cuota_externa_total": 13586.0, "capacidad_maxima_pago": 55274.0, "bursolnum": 7352817, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 6126.168016794589, "monto_max": 52860.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 12.0, "plazo_min": 4, "tasa": 0.5668, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":8, "monto_otorgado":243530.0, "cuota":7430.0, "saldo":228721.0, "tasa_externa":0.2733, "tasa_kubo":0.5668, "numero_pagos_otorgado":60.0, "numero_pagos_restante":44.0, "frecuencia_externa":"M", "avance":0.0608, "fecha_inicio":"2022-11-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-20793.717312334207, "ahorro_total":-249524.6077480105, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":40000.0, "cuota":4728.0, "saldo":15835.0, "tasa_externa":0.7099, "tasa_kubo":0.5668, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6041, "fecha_inicio":"2023-09-05", "tipo_deuda":"I", "ahorro_cuota_mensual":92.23154234234698, "ahorro_total":1106.7785081081638, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":500.0, "cuota":1765.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-08-13", "tipo_deuda":"R", "ahorro_cuota_mensual":1765.0, "ahorro_total":21180.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":7000.0, "cuota":717.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-01-31", "tipo_deuda":"R", "ahorro_cuota_mensual":717.0, "ahorro_total":8604.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":114260.0, "cuota":5713.0, "saldo":21872.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8086, "fecha_inicio":"2019-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":3178.161807352795, "ahorro_total":38137.94168823354, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":25100.0, "cuota":2221.0, "saldo":9456.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6233, "fecha_inicio":"2020-08-19", "tipo_deuda":"R", "ahorro_cuota_mensual":1125.1043366097308, "ahorro_total":13501.252039316769, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":37000.0, "cuota":2805.0, "saldo":21532.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4181, "fecha_inicio":"2020-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":309.565839242885, "ahorro_total":3714.7900709146197, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":7000.0, "cuota":1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-09-23", "tipo_deuda":"R", "ahorro_cuota_mensual":1.0, "ahorro_total":12.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
+    <t>Revolvente con saldo cero</t>
+  </si>
+  <si>
     <t>{"Prospecto": 4699870, "monto_maximo_cliente": 5233.0, "cuota_externa_total": 5659.0, "capacidad_maxima_pago": 9574.0, "bursolnum": 7354566, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1063.747520887488, "monto_max": 5233.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 6.0, "plazo_min": 4, "tasa": 0.6193, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":400.0, "cuota":84.0, "saldo":158.0, "tasa_externa":0.8555, "tasa_kubo":0.6193, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.605, "fecha_inicio":"2022-10-20", "tipo_deuda":"I", "ahorro_cuota_mensual":2.689277975349654, "ahorro_total":16.135667852097924, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":12410.0, "cuota":3584.0, "saldo":12431.0, "tasa_externa":0.7338, "tasa_kubo":0.6193, "numero_pagos_otorgado":4.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0017, "fecha_inicio":"2024-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":1061.3348491852234, "ahorro_total":6368.009095111341, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":400.0, "cuota":101.0, "saldo":257.0, "tasa_externa":1.6226, "tasa_kubo":0.6193, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3575, "fecha_inicio":"2022-11-11", "tipo_deuda":"I", "ahorro_cuota_mensual":19.689277975349654, "ahorro_total":118.13566785209792, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":16500.0, "cuota":750.0, "saldo":82.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.995, "fecha_inicio":"2022-04-28", "tipo_deuda":"R", "ahorro_cuota_mensual":733.3313019849467, "ahorro_total":4399.98781190968, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":6000.0, "cuota":1057.0, "saldo":3951.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3415, "fecha_inicio":"2021-02-25", "tipo_deuda":"R", "ahorro_cuota_mensual":253.85334320151617, "ahorro_total":1523.120059209097, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":400.0, "cuota":83.0, "saldo":155.0, "tasa_externa":0.8084, "tasa_kubo":0.6193, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6125, "fecha_inicio":"2022-10-28", "tipo_deuda":"I", "ahorro_cuota_mensual":1.689277975349654, "ahorro_total":10.135667852097924, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>Creditos Revolventes con saldo cero</t>
   </si>
   <si>
     <t>{"Prospecto": 4742252, "monto_maximo_cliente": 5078.0, "cuota_externa_total": 1935.0, "capacidad_maxima_pago": 35143.0, "bursolnum": 7353080, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 275.58896455537393, "monto_max": 5078.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 23.0, "plazo_min": 4, "tasa": 0.7007, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":7699.0, "cuota":608.0, "saldo":5078.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3404, "fecha_inicio":"2019-07-08", "tipo_deuda":"R", "ahorro_cuota_mensual":166.19043565531155, "ahorro_total":3822.3800200721657, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":13000.0, "cuota":1327.0, "saldo":6402.0, "tasa_externa":0.8966, "tasa_kubo":0.7007, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5075, "fecha_inicio":"2023-01-20", "tipo_deuda":"I", "ahorro_cuota_mensual":195.93967379264473, "ahorro_total":4506.612497230829, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
@@ -504,7 +513,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="72.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="73.7192857142857" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="104.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -615,7 +624,9 @@
       <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
@@ -635,32 +646,38 @@
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3">
         <v>4688988</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3">
         <v>4699870</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3">
         <v>4742252</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4"/>
     </row>
@@ -669,7 +686,7 @@
         <v>4836047</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C17" s="4"/>
     </row>
@@ -678,7 +695,7 @@
         <v>4882834</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4"/>
     </row>
@@ -687,7 +704,7 @@
         <v>4915388</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4"/>
     </row>
@@ -696,7 +713,7 @@
         <v>5063684</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4"/>
     </row>
@@ -705,7 +722,7 @@
         <v>5137408</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4"/>
     </row>
@@ -714,7 +731,7 @@
         <v>5345402</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C22" s="4"/>
     </row>
@@ -723,7 +740,7 @@
         <v>5696494</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C23" s="4"/>
     </row>

</xml_diff>

<commit_message>
comments where added to json tests
</commit_message>
<xml_diff>
--- a/Json_ofertas.xlsx
+++ b/Json_ofertas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="148">
   <si>
     <t>prospectus_id</t>
   </si>
@@ -22,22 +22,25 @@
     <t>Json</t>
   </si>
   <si>
+    <t>Monto maximo igual a la deuda consolidable</t>
+  </si>
+  <si>
     <t>{"Prospecto": 28837, "monto_maximo_cliente": 160000.0, "cuota_externa_total": 26582.0, "capacidad_maxima_pago": 151418.0, "bursolnum": 7317484, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4795.847147179248, "monto_max": 160000.0, "cuota_min": 130.08822700780902, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.165, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.165], "comisiones": [0], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":12900.0, "cuota":808.0, "saldo":10588.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1792, "fecha_inicio":"2022-08-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-597.8502317941084, "ahorro_total":-5978.502317941084, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":15, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2019-02-24", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":13, "monto_otorgado":350000.0, "cuota":1011.0, "saldo":81278.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":40.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7678, "fecha_inicio":"2015-06-04", "tipo_deuda":"M", "ahorro_cuota_mensual":-1753.2323454138273, "ahorro_total":-70129.2938165531, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":12, "monto_otorgado":858.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-01-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":923.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-07-09", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":17000.0, "cuota":862.0, "saldo":15404.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.0939, "fecha_inicio":"2023-10-04", "tipo_deuda":"I", "ahorro_cuota_mensual":3.896736049547485, "ahorro_total":93.52166518913964, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":16, "monto_otorgado":20000.0, "cuota":1305.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2010-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":1305.0, "ahorro_total":-1305.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":259150.0, "cuota":7238.0, "saldo":231420.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":54.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.107, "fecha_inicio":"2023-04-18", "tipo_deuda":"I", "ahorro_cuota_mensual":43.21710984879246, "ahorro_total":2333.723931834793, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":30000.0, "cuota":3007.0, "saldo":28876.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0375, "fecha_inicio":"2022-04-20", "tipo_deuda":"R", "ahorro_cuota_mensual":31883.00000000014, "ahorro_total":-31883.00000000014, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":80000.0, "cuota":5160.0, "saldo":80762.0, "tasa_externa":0.7762, "tasa_kubo":0.165, "numero_pagos_otorgado":144.0, "numero_pagos_restante":68.0, "frecuencia_externa":"S", "avance":-0.0095, "fecha_inicio":"2023-12-04", "tipo_deuda":"I", "ahorro_cuota_mensual":3283.444156192121, "ahorro_total":236407.9792458327, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":39500.0, "cuota":4500.0, "saldo":77318.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.9574, "fecha_inicio":"2009-01-06", "tipo_deuda":"R", "ahorro_cuota_mensual":81818.00000000036, "ahorro_total":-81818.00000000036, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":69600.0, "cuota":2596.0, "saldo":39767.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.4286, "fecha_inicio":"2023-09-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-4989.05241340077, "ahorro_total":-49890.524134007705, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":80000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":43.0, "numero_pagos_restante":16.0, "frecuencia_externa":"S", "avance":1.0, "fecha_inicio":"2023-10-16", "tipo_deuda":"I", "ahorro_cuota_mensual":-4340.230522526159, "ahorro_total":-95485.0714955755, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":11900.0, "cuota":744.0, "saldo":9704.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1845, "fecha_inicio":"2022-07-14", "tipo_deuda":"I", "ahorro_cuota_mensual":-552.869593670534, "ahorro_total":-5528.69593670534, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":14, "monto_otorgado":80000.0, "cuota":5156.0, "saldo":80073.0, "tasa_externa":0.7756, "tasa_kubo":0.165, "numero_pagos_otorgado":144.0, "numero_pagos_restante":70.0, "frecuencia_externa":"S", "avance":-0.0009, "fecha_inicio":"2024-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":3279.444156192121, "ahorro_total":236119.9792458327, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 39500, "monto_maximo_cliente": 71900.0, "cuota_externa_total": 27925.0, "capacidad_maxima_pago": 81060.0, "bursolnum": 7317209, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2965.3458995878814, "monto_max": 71900.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.3337, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":137585.0, "cuota":4665.0, "saldo":82503.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":36.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.4003, "fecha_inicio":"2022-11-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-1850.9934737731373, "ahorro_total":-66635.76505583295, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":100000.0, "cuota":4632.0, "saldo":94959.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":36.0, "numero_pagos_restante":29.0, "frecuencia_externa":"M", "avance":0.0504, "fecha_inicio":"2023-09-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-103.97664990597605, "ahorro_total":-3743.1593966151377, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":65000.0, "cuota":3101.0, "saldo":65669.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":36.0, "numero_pagos_restante":32.0, "frecuencia_externa":"M", "avance":-0.0103, "fecha_inicio":"2023-12-04", "tipo_deuda":"I", "ahorro_cuota_mensual":22.615177561115615, "ahorro_total":814.1463922001622, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":71900.0, "cuota":4588.0, "saldo":72761.0, "tasa_externa":0.7567, "tasa_kubo":0.3337, "numero_pagos_otorgado":120.0, "numero_pagos_restante":57.0, "frecuencia_externa":"S", "avance":-0.012, "fecha_inicio":"2024-01-04", "tipo_deuda":"I", "ahorro_cuota_mensual":1863.1069267607159, "ahorro_total":111786.41560564295, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":15, "monto_otorgado":4500.0, "cuota":29.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":900.0, "numero_pagos_restante":767.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2013-03-08", "tipo_deuda":"R", "ahorro_cuota_mensual":29.0, "ahorro_total":26100.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":14, "monto_otorgado":20000.0, "cuota":1000.0, "saldo":2718.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8641, "fecha_inicio":"2019-08-11", "tipo_deuda":"R", "ahorro_cuota_mensual":3717.999999999993, "ahorro_total":-3717.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":500.0, "cuota":6336.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-08-03", "tipo_deuda":"R", "ahorro_cuota_mensual":6336.0, "ahorro_total":-6336.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":100000.0, "cuota":3589.0, "saldo":82549.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":48.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.1745, "fecha_inicio":"2022-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":-535.2641162557456, "ahorro_total":-25692.67758027579, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":102000.0, "cuota":344.0, "saldo":2161.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9788, "fecha_inicio":"2019-12-06", "tipo_deuda":"R", "ahorro_cuota_mensual":2504.9999999999945, "ahorro_total":-2504.9999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":30000.0, "cuota":1435.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-08-09", "tipo_deuda":"R", "ahorro_cuota_mensual":1435.0, "ahorro_total":-1435.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":37800.0, "cuota":3000.0, "saldo":6242.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8349, "fecha_inicio":"2021-03-09", "tipo_deuda":"R", "ahorro_cuota_mensual":9241.999999999985, "ahorro_total":-9241.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":45800.0, "cuota":2290.0, "saldo":5848.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8723, "fecha_inicio":"2023-08-25", "tipo_deuda":"R", "ahorro_cuota_mensual":8137.999999999985, "ahorro_total":-8137.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":20000.0, "cuota":96.0, "saldo":127.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9936, "fecha_inicio":"2022-11-01", "tipo_deuda":"R", "ahorro_cuota_mensual":222.99999999999966, "ahorro_total":-222.99999999999966, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":117200.0, "cuota":6776.0, "saldo":111852.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0456, "fecha_inicio":"2023-09-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-7122.1843719153785, "ahorro_total":-71221.84371915378, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":2000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-12-10", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
-    <t>ahorro_cuota_mensual -inf</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 240179, "monto_maximo_cliente": 28000.0, "cuota_externa_total": 7716.0, "capacidad_maxima_pago": 36100.0, "bursolnum": 7316960, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 912.2138553629048, "monto_max": 28000.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.6193, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":55000.0, "cuota":3654.0, "saldo":49283.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.1039, "fecha_inicio":"2023-03-24", "tipo_deuda":"I", "ahorro_cuota_mensual":1519.227833189288, "ahorro_total":54692.20199481437, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":16, "monto_otorgado":43736.0, "cuota":1136.0, "saldo":37772.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":154.0, "numero_pagos_restante":28.0, "frecuencia_externa":"W", "avance":0.1364, "fecha_inicio":"2023-05-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-499.6453448490415, "ahorro_total":-18986.52310426358, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":15, "monto_otorgado":43736.0, "cuota":1136.0, "saldo":36636.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":154.0, "numero_pagos_restante":27.0, "frecuencia_externa":"W", "avance":0.1623, "fecha_inicio":"2023-04-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-499.6453448490415, "ahorro_total":-18986.52310426358, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":8000.0, "cuota":-1.0, "saldo":637.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9204, "fecha_inicio":"2023-09-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":5600.0, "cuota":-1.0, "saldo":1090.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8054, "fecha_inicio":"2023-09-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":35000.0, "cuota":980.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-03-09", "tipo_deuda":"R", "ahorro_cuota_mensual":980.0, "ahorro_total":-980.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":6000.0, "cuota":300.0, "saldo":4674.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":23.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.221, "fecha_inicio":"2022-03-24", "tipo_deuda":"R", "ahorro_cuota_mensual":46.33658520444712, "ahorro_total":1065.7414597022837, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":12500.0, "cuota":625.0, "saldo":4046.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6763, "fecha_inicio":"2023-11-16", "tipo_deuda":"R", "ahorro_cuota_mensual":4670.999999999993, "ahorro_total":-4670.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":28000.0, "cuota":1389.0, "saldo":26826.0, "tasa_externa":0.4314, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.0419, "fecha_inicio":"2023-10-23", "tipo_deuda":"I", "ahorro_cuota_mensual":302.2068968963647, "ahorro_total":10879.44828826913, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":3000.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-03-24", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 380930, "monto_maximo_cliente": 41100.0, "cuota_externa_total": 9644.0, "capacidad_maxima_pago": 42113.0, "bursolnum": 7317848, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1921.2888041034741, "monto_max": 41100.0, "cuota_min": 232.85304854502846, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6722, "comision": 0.0444, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":12, "monto_otorgado":9000.0, "cuota":450.0, "saldo":2754.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.694, "fecha_inicio":"2022-05-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":1300.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-03-21", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":40000.0, "cuota":2856.0, "saldo":37674.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.0582, "fecha_inicio":"2023-06-27", "tipo_deuda":"I", "ahorro_cuota_mensual":657.6585748048092, "ahorro_total":23675.70869297313, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":9000.0, "cuota":450.0, "saldo":4919.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4534, "fecha_inicio":"2022-05-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":1, "monto_otorgado":41223.0, "cuota":2425.0, "saldo":40647.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":49.0, "numero_pagos_restante":44.0, "frecuencia_externa":"M", "avance":0.014, "fecha_inicio":"2023-11-03", "tipo_deuda":"I", "ahorro_cuota_mensual":400.892394629843, "ahorro_total":19643.727336862306, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":28000.0, "cuota":21042.0, "saldo":6100.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7821, "fecha_inicio":"2020-04-03", "tipo_deuda":"R", "ahorro_cuota_mensual":27141.99999999999, "ahorro_total":-27141.99999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":20000.0, "cuota":1666.0, "saldo":16133.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1934, "fecha_inicio":"2023-02-17", "tipo_deuda":"R", "ahorro_cuota_mensual":17798.999999999967, "ahorro_total":-17798.999999999967, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":41100.0, "cuota":2424.0, "saldo":41524.0, "tasa_externa":0.6929, "tasa_kubo":0.4428, "numero_pagos_otorgado":120.0, "numero_pagos_restante":57.0, "frecuencia_externa":"S", "avance":-0.0103, "fecha_inicio":"2024-01-09", "tipo_deuda":"I", "ahorro_cuota_mensual":509.94794095986595, "ahorro_total":30596.876457591956, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 405226, "monto_maximo_cliente": 205500.0, "cuota_externa_total": 239493.0, "capacidad_maxima_pago": 126007.0, "bursolnum": 7316530, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7183.5577919854995, "monto_max": 205500.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5292, "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":39, "monto_otorgado":495000.0, "cuota":31259.0, "saldo":228125.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":20.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5391, "fecha_inicio":"2021-01-20", "tipo_deuda":"O", "ahorro_cuota_mensual":16183.860777170179, "ahorro_total":323677.2155434036, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":21, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2019-06-07", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":18, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-07-06", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":17, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-11-19", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":16, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-05-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":350900.0, "cuota":16622.0, "saldo":206760.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":47.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.4108, "fecha_inicio":"2021-07-14", "tipo_deuda":"I", "ahorro_cuota_mensual":3063.1080061094963, "ahorro_total":143966.07628714634, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":138700.0, "cuota":6388.0, "saldo":107088.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":52.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.2279, "fecha_inicio":"2021-12-06", "tipo_deuda":"I", "ahorro_cuota_mensual":1275.0749096445152, "ahorro_total":66303.89530151479, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":13, "monto_otorgado":233160.0, "cuota":5691.0, "saldo":146279.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":60.0, "numero_pagos_restante":36.0, "frecuencia_externa":"M", "avance":0.3726, "fecha_inicio":"2022-03-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-2405.9989825443863, "ahorro_total":-144359.9389526632, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":226020.0, "cuota":4566.0, "saldo":134253.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":72.0, "numero_pagos_restante":34.0, "frecuencia_externa":"M", "avance":0.406, "fecha_inicio":"2021-01-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-2797.0599259490555, "ahorro_total":-201388.314668332, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-06-11", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":23, "monto_otorgado":300000.0, "cuota":1.0, "saldo":254513.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.1516, "fecha_inicio":"2023-07-03", "tipo_deuda":"O", "ahorro_cuota_mensual":-11340.308568610357, "ahorro_total":-408251.10846997285, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":300000.0, "cuota":1.0, "saldo":241667.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.1944, "fecha_inicio":"2023-07-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-13367.246693029854, "ahorro_total":-481220.88094907475, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":20, "monto_otorgado":45000.0, "cuota":2250.0, "saldo":24201.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4622, "fecha_inicio":"2020-12-09", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":22, "monto_otorgado":900000.0, "cuota":53621.0, "saldo":816040.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.0933, "fecha_inicio":"2023-09-15", "tipo_deuda":"O", "ahorro_cuota_mensual":6381.533609186947, "ahorro_total":153156.80662048672, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":59003.0, "cuota":722.0, "saldo":50966.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":144.0, "numero_pagos_restante":67.0, "frecuencia_externa":"S", "avance":0.1362, "fecha_inicio":"2023-10-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-1200.1423980655345, "ahorro_total":-86410.25266071848, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":132552.0, "cuota":3894.0, "saldo":108273.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":96.0, "numero_pagos_restante":36.0, "frecuencia_externa":"S", "avance":0.1832, "fecha_inicio":"2023-04-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-1176.214119532745, "ahorro_total":-56458.277737571756, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":205500.0, "cuota":7809.0, "saldo":76789.0, "tasa_externa":0.394, "tasa_kubo":0.2914, "numero_pagos_otorgado":60.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.6263, "fecha_inicio":"2020-03-04", "tipo_deuda":"I", "ahorro_cuota_mensual":672.5559662340393, "ahorro_total":40353.35797404236, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":155300.0, "cuota":8000.0, "saldo":40529.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.739, "fecha_inicio":"2012-03-20", "tipo_deuda":"R", "ahorro_cuota_mensual":48528.99999999988, "ahorro_total":-48528.99999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":135000.0, "cuota":6750.0, "saldo":91545.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3219, "fecha_inicio":"2016-02-24", "tipo_deuda":"R", "ahorro_cuota_mensual":98294.99999999975, "ahorro_total":-98294.99999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":14000.0, "cuota":1174.0, "saldo":11184.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2011, "fecha_inicio":"2023-11-02", "tipo_deuda":"R", "ahorro_cuota_mensual":12357.99999999997, "ahorro_total":-12357.99999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":106205.0, "cuota":9827.0, "saldo":170436.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":-0.6048, "fecha_inicio":"2023-06-29", "tipo_deuda":"I", "ahorro_cuota_mensual":3678.9343070973237, "ahorro_total":88294.42337033577, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":418548.0, "cuota":85856.0, "saldo":220008.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":78.0, "numero_pagos_restante":9.0, "frecuencia_externa":"W", "avance":0.4744, "fecha_inicio":"2023-05-10", "tipo_deuda":"I", "ahorro_cuota_mensual":58197.17535808449, "ahorro_total":1163943.5071616897, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":19, "monto_otorgado":136814.0, "cuota":6520.0, "saldo":106713.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":47.0, "numero_pagos_restante":37.0, "frecuencia_externa":"M", "avance":0.22, "fecha_inicio":"2023-06-15", "tipo_deuda":"I", "ahorro_cuota_mensual":1233.4618146134635, "ahorro_total":57972.70528683279, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 240179, "monto_maximo_cliente": 28000.0, "cuota_externa_total": 7716.0, "capacidad_maxima_pago": 36100.0, "bursolnum": 7316960, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 912.2138553629048, "monto_max": 28000.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.6193, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":55000.0, "cuota":3654.0, "saldo":49283.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.1039, "fecha_inicio":"2023-03-24", "tipo_deuda":"I", "ahorro_cuota_mensual":1519.227833189288, "ahorro_total":54692.20199481437, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":16, "monto_otorgado":43736.0, "cuota":1136.0, "saldo":37772.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":154.0, "numero_pagos_restante":28.0, "frecuencia_externa":"W", "avance":0.1364, "fecha_inicio":"2023-05-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-499.6453448490415, "ahorro_total":-18986.52310426358, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":15, "monto_otorgado":43736.0, "cuota":1136.0, "saldo":36636.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":154.0, "numero_pagos_restante":27.0, "frecuencia_externa":"W", "avance":0.1623, "fecha_inicio":"2023-04-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-499.6453448490415, "ahorro_total":-18986.52310426358, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":8000.0, "cuota":-1.0, "saldo":637.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9204, "fecha_inicio":"2023-09-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":5600.0, "cuota":-1.0, "saldo":1090.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8054, "fecha_inicio":"2023-09-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":35000.0, "cuota":980.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-03-09", "tipo_deuda":"R", "ahorro_cuota_mensual":980.0, "ahorro_total":-980.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":6000.0, "cuota":300.0, "saldo":4674.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":23.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.221, "fecha_inicio":"2022-03-24", "tipo_deuda":"R", "ahorro_cuota_mensual":46.33658520444712, "ahorro_total":1065.7414597022837, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":12500.0, "cuota":625.0, "saldo":4046.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6763, "fecha_inicio":"2023-11-16", "tipo_deuda":"R", "ahorro_cuota_mensual":4670.999999999993, "ahorro_total":-4670.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":28000.0, "cuota":1389.0, "saldo":26826.0, "tasa_externa":0.4314, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.0419, "fecha_inicio":"2023-10-23", "tipo_deuda":"I", "ahorro_cuota_mensual":302.2068968963647, "ahorro_total":10879.44828826913, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":3000.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-03-24", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 380930, "monto_maximo_cliente": 41100.0, "cuota_externa_total": 9644.0, "capacidad_maxima_pago": 42113.0, "bursolnum": 7317848, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1921.2888041034741, "monto_max": 41100.0, "cuota_min": 232.85304854502846, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6722, "comision": 0.0444, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":12, "monto_otorgado":9000.0, "cuota":450.0, "saldo":2754.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.694, "fecha_inicio":"2022-05-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":1300.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-03-21", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":40000.0, "cuota":2856.0, "saldo":37674.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.0582, "fecha_inicio":"2023-06-27", "tipo_deuda":"I", "ahorro_cuota_mensual":657.6585748048092, "ahorro_total":23675.70869297313, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":9000.0, "cuota":450.0, "saldo":4919.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4534, "fecha_inicio":"2022-05-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":1, "monto_otorgado":41223.0, "cuota":2425.0, "saldo":40647.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":49.0, "numero_pagos_restante":44.0, "frecuencia_externa":"M", "avance":0.014, "fecha_inicio":"2023-11-03", "tipo_deuda":"I", "ahorro_cuota_mensual":400.892394629843, "ahorro_total":19643.727336862306, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":28000.0, "cuota":21042.0, "saldo":6100.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7821, "fecha_inicio":"2020-04-03", "tipo_deuda":"R", "ahorro_cuota_mensual":27141.99999999999, "ahorro_total":-27141.99999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":20000.0, "cuota":1666.0, "saldo":16133.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1934, "fecha_inicio":"2023-02-17", "tipo_deuda":"R", "ahorro_cuota_mensual":17798.999999999967, "ahorro_total":-17798.999999999967, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":41100.0, "cuota":2424.0, "saldo":41524.0, "tasa_externa":0.6929, "tasa_kubo":0.4428, "numero_pagos_otorgado":120.0, "numero_pagos_restante":57.0, "frecuencia_externa":"S", "avance":-0.0103, "fecha_inicio":"2024-01-09", "tipo_deuda":"I", "ahorro_cuota_mensual":509.94794095986595, "ahorro_total":30596.876457591956, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>Deudas de servicios como consolidables</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 405226, "monto_maximo_cliente": 205500.0, "cuota_externa_total": 239493.0, "capacidad_maxima_pago": 126007.0, "bursolnum": 7316530, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7183.5577919854995, "monto_max": 205500.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5292, "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":39, "monto_otorgado":495000.0, "cuota":31259.0, "saldo":228125.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":20.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5391, "fecha_inicio":"2021-01-20", "tipo_deuda":"O", "ahorro_cuota_mensual":16183.860777170179, "ahorro_total":323677.2155434036, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":21, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2019-06-07", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":18, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-07-06", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":17, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-11-19", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":16, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-05-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":350900.0, "cuota":16622.0, "saldo":206760.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":47.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.4108, "fecha_inicio":"2021-07-14", "tipo_deuda":"I", "ahorro_cuota_mensual":3063.1080061094963, "ahorro_total":143966.07628714634, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":138700.0, "cuota":6388.0, "saldo":107088.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":52.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.2279, "fecha_inicio":"2021-12-06", "tipo_deuda":"I", "ahorro_cuota_mensual":1275.0749096445152, "ahorro_total":66303.89530151479, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":13, "monto_otorgado":233160.0, "cuota":5691.0, "saldo":146279.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":60.0, "numero_pagos_restante":36.0, "frecuencia_externa":"M", "avance":0.3726, "fecha_inicio":"2022-03-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-2405.9989825443863, "ahorro_total":-144359.9389526632, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":226020.0, "cuota":4566.0, "saldo":134253.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":72.0, "numero_pagos_restante":34.0, "frecuencia_externa":"M", "avance":0.406, "fecha_inicio":"2021-01-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-2797.0599259490555, "ahorro_total":-201388.314668332, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-06-11", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":23, "monto_otorgado":300000.0, "cuota":1.0, "saldo":254513.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.1516, "fecha_inicio":"2023-07-03", "tipo_deuda":"O", "ahorro_cuota_mensual":-11340.308568610357, "ahorro_total":-408251.10846997285, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":300000.0, "cuota":1.0, "saldo":241667.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.1944, "fecha_inicio":"2023-07-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-13367.246693029854, "ahorro_total":-481220.88094907475, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":20, "monto_otorgado":45000.0, "cuota":2250.0, "saldo":24201.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4622, "fecha_inicio":"2020-12-09", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":22, "monto_otorgado":900000.0, "cuota":53621.0, "saldo":816040.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.0933, "fecha_inicio":"2023-09-15", "tipo_deuda":"O", "ahorro_cuota_mensual":6381.533609186947, "ahorro_total":153156.80662048672, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":59003.0, "cuota":722.0, "saldo":50966.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":144.0, "numero_pagos_restante":67.0, "frecuencia_externa":"S", "avance":0.1362, "fecha_inicio":"2023-10-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-1200.1423980655345, "ahorro_total":-86410.25266071848, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":132552.0, "cuota":3894.0, "saldo":108273.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":96.0, "numero_pagos_restante":36.0, "frecuencia_externa":"S", "avance":0.1832, "fecha_inicio":"2023-04-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-1176.214119532745, "ahorro_total":-56458.277737571756, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":205500.0, "cuota":7809.0, "saldo":76789.0, "tasa_externa":0.394, "tasa_kubo":0.2914, "numero_pagos_otorgado":60.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.6263, "fecha_inicio":"2020-03-04", "tipo_deuda":"I", "ahorro_cuota_mensual":672.5559662340393, "ahorro_total":40353.35797404236, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":155300.0, "cuota":8000.0, "saldo":40529.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.739, "fecha_inicio":"2012-03-20", "tipo_deuda":"R", "ahorro_cuota_mensual":48528.99999999988, "ahorro_total":-48528.99999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":135000.0, "cuota":6750.0, "saldo":91545.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3219, "fecha_inicio":"2016-02-24", "tipo_deuda":"R", "ahorro_cuota_mensual":98294.99999999975, "ahorro_total":-98294.99999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":14000.0, "cuota":1174.0, "saldo":11184.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2011, "fecha_inicio":"2023-11-02", "tipo_deuda":"R", "ahorro_cuota_mensual":12357.99999999997, "ahorro_total":-12357.99999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":106205.0, "cuota":9827.0, "saldo":170436.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":-0.6048, "fecha_inicio":"2023-06-29", "tipo_deuda":"I", "ahorro_cuota_mensual":3678.9343070973237, "ahorro_total":88294.42337033577, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":418548.0, "cuota":85856.0, "saldo":220008.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":78.0, "numero_pagos_restante":9.0, "frecuencia_externa":"W", "avance":0.4744, "fecha_inicio":"2023-05-10", "tipo_deuda":"I", "ahorro_cuota_mensual":58197.17535808449, "ahorro_total":1163943.5071616897, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":19, "monto_otorgado":136814.0, "cuota":6520.0, "saldo":106713.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":47.0, "numero_pagos_restante":37.0, "frecuencia_externa":"M", "avance":0.22, "fecha_inicio":"2023-06-15", "tipo_deuda":"I", "ahorro_cuota_mensual":1233.4618146134635, "ahorro_total":57972.70528683279, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 458697, "monto_maximo_cliente": 175800.0, "cuota_externa_total": 60240.0, "capacidad_maxima_pago": 146606.0, "bursolnum": 7340616, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 11065.485474797928, "monto_max": 175800.0, "cuota_min": 278.44180193239873, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.5504, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":12000.0, "cuota":1367.0, "saldo":10020.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.165, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-9186.11744, "ahorro_total":-9186.11744, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":12000.0, "cuota":1367.0, "saldo":10020.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.165, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-9186.11744, "ahorro_total":-9186.11744, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":12000.0, "cuota":1367.0, "saldo":10020.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.165, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-9186.11744, "ahorro_total":-9186.11744, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":12000.0, "cuota":1367.0, "saldo":10020.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.165, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-9186.11744, "ahorro_total":-9186.11744, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":12000.0, "cuota":1367.0, "saldo":10020.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.165, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-9186.11744, "ahorro_total":-9186.11744, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":12000.0, "cuota":1367.0, "saldo":10020.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.165, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-9186.11744, "ahorro_total":-9186.11744, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":12000.0, "cuota":1367.0, "saldo":10020.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.165, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-9186.11744, "ahorro_total":-9186.11744, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":10000.0, "cuota":1521.0, "saldo":1521.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8479, "fecha_inicio":"2023-08-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-9011.053333333333, "ahorro_total":-9011.053333333333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":10000.0, "cuota":1521.0, "saldo":1521.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8479, "fecha_inicio":"2023-08-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-9011.053333333333, "ahorro_total":-9011.053333333333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":10000.0, "cuota":1521.0, "saldo":1521.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8479, "fecha_inicio":"2023-08-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-9011.053333333333, "ahorro_total":-9011.053333333333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":10000.0, "cuota":1521.0, "saldo":1521.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8479, "fecha_inicio":"2023-08-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-9011.053333333333, "ahorro_total":-9011.053333333333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":12000.0, "cuota":1367.0, "saldo":10020.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.165, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-9186.11744, "ahorro_total":-9186.11744, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":10000.0, "cuota":1521.0, "saldo":1521.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8479, "fecha_inicio":"2023-08-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-9011.053333333333, "ahorro_total":-9011.053333333333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":10000.0, "cuota":1521.0, "saldo":1521.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8479, "fecha_inicio":"2023-08-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-9011.053333333333, "ahorro_total":-9011.053333333333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":10000.0, "cuota":1521.0, "saldo":1521.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8479, "fecha_inicio":"2023-08-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-9011.053333333333, "ahorro_total":-9011.053333333333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":10000.0, "cuota":1521.0, "saldo":1521.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8479, "fecha_inicio":"2023-08-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-9011.053333333333, "ahorro_total":-9011.053333333333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":16, "monto_otorgado":79000.0, "cuota":8295.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":900.0, "numero_pagos_restante":826.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":8295.0, "ahorro_total":7465500.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":79000.0, "cuota":8295.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":900.0, "numero_pagos_restante":826.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":8295.0, "ahorro_total":7465500.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":79000.0, "cuota":8295.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":900.0, "numero_pagos_restante":826.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":8295.0, "ahorro_total":7465500.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":3500.0, "cuota":204.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-05-25", "tipo_deuda":"R", "ahorro_cuota_mensual":204.0, "ahorro_total":-204.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":3500.0, "cuota":204.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-05-25", "tipo_deuda":"R", "ahorro_cuota_mensual":204.0, "ahorro_total":-204.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":16000.0, "cuota":961.0, "saldo":14510.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0931, "fecha_inicio":"2022-01-08", "tipo_deuda":"R", "ahorro_cuota_mensual":15470.999999999989, "ahorro_total":-15470.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":16000.0, "cuota":961.0, "saldo":14510.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0931, "fecha_inicio":"2022-01-08", "tipo_deuda":"R", "ahorro_cuota_mensual":15470.999999999989, "ahorro_total":-15470.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":16000.0, "cuota":961.0, "saldo":14510.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0931, "fecha_inicio":"2022-01-08", "tipo_deuda":"R", "ahorro_cuota_mensual":15470.999999999989, "ahorro_total":-15470.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":16000.0, "cuota":961.0, "saldo":14510.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0931, "fecha_inicio":"2022-01-08", "tipo_deuda":"R", "ahorro_cuota_mensual":15470.999999999989, "ahorro_total":-15470.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":16000.0, "cuota":961.0, "saldo":14510.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0931, "fecha_inicio":"2022-01-08", "tipo_deuda":"R", "ahorro_cuota_mensual":15470.999999999989, "ahorro_total":-15470.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":16000.0, "cuota":961.0, "saldo":14510.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0931, "fecha_inicio":"2022-01-08", "tipo_deuda":"R", "ahorro_cuota_mensual":15470.999999999989, "ahorro_total":-15470.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":16000.0, "cuota":961.0, "saldo":14510.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0931, "fecha_inicio":"2022-01-08", "tipo_deuda":"R", "ahorro_cuota_mensual":15470.999999999989, "ahorro_total":-15470.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":16000.0, "cuota":961.0, "saldo":14510.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0931, "fecha_inicio":"2022-01-08", "tipo_deuda":"R", "ahorro_cuota_mensual":15470.999999999989, "ahorro_total":-15470.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":16, "monto_otorgado":79000.0, "cuota":8295.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":900.0, "numero_pagos_restante":826.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":8295.0, "ahorro_total":7465500.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":79000.0, "cuota":8295.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":900.0, "numero_pagos_restante":826.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":8295.0, "ahorro_total":7465500.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":79000.0, "cuota":8295.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":900.0, "numero_pagos_restante":826.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":8295.0, "ahorro_total":7465500.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":79000.0, "cuota":8295.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":900.0, "numero_pagos_restante":826.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":8295.0, "ahorro_total":7465500.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":79000.0, "cuota":8295.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":900.0, "numero_pagos_restante":826.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":8295.0, "ahorro_total":7465500.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":90000.0, "cuota":4849.0, "saldo":80026.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":48.0, "numero_pagos_restante":28.0, "frecuencia_externa":"M", "avance":0.1108, "fecha_inicio":"2022-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-373.21924255754857, "ahorro_total":-17914.52364276233, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":21000.0, "cuota":1772.0, "saldo":3367.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8397, "fecha_inicio":"2022-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-69.73504670700981, "ahorro_total":-1255.2308407261767, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":21000.0, "cuota":1772.0, "saldo":3367.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8397, "fecha_inicio":"2022-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-69.73504670700981, "ahorro_total":-1255.2308407261767, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":21000.0, "cuota":1772.0, "saldo":3367.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8397, "fecha_inicio":"2022-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-69.73504670700981, "ahorro_total":-1255.2308407261767, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":21000.0, "cuota":1772.0, "saldo":3367.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8397, "fecha_inicio":"2022-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-69.73504670700981, "ahorro_total":-1255.2308407261767, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":21000.0, "cuota":1772.0, "saldo":3367.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8397, "fecha_inicio":"2022-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-69.73504670700981, "ahorro_total":-1255.2308407261767, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":21000.0, "cuota":1772.0, "saldo":3367.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8397, "fecha_inicio":"2022-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-69.73504670700981, "ahorro_total":-1255.2308407261767, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":21000.0, "cuota":1772.0, "saldo":3367.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8397, "fecha_inicio":"2022-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-69.73504670700981, "ahorro_total":-1255.2308407261767, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":90000.0, "cuota":4849.0, "saldo":80026.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":48.0, "numero_pagos_restante":28.0, "frecuencia_externa":"M", "avance":0.1108, "fecha_inicio":"2022-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-373.21924255754857, "ahorro_total":-17914.52364276233, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":90000.0, "cuota":4849.0, "saldo":80026.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":48.0, "numero_pagos_restante":28.0, "frecuencia_externa":"M", "avance":0.1108, "fecha_inicio":"2022-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-373.21924255754857, "ahorro_total":-17914.52364276233, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":90000.0, "cuota":4849.0, "saldo":80026.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":48.0, "numero_pagos_restante":28.0, "frecuencia_externa":"M", "avance":0.1108, "fecha_inicio":"2022-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-373.21924255754857, "ahorro_total":-17914.52364276233, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":90000.0, "cuota":4849.0, "saldo":80026.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":48.0, "numero_pagos_restante":28.0, "frecuencia_externa":"M", "avance":0.1108, "fecha_inicio":"2022-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-373.21924255754857, "ahorro_total":-17914.52364276233, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":90000.0, "cuota":4849.0, "saldo":80026.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":48.0, "numero_pagos_restante":28.0, "frecuencia_externa":"M", "avance":0.1108, "fecha_inicio":"2022-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-373.21924255754857, "ahorro_total":-17914.52364276233, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":90000.0, "cuota":4849.0, "saldo":80026.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":48.0, "numero_pagos_restante":28.0, "frecuencia_externa":"M", "avance":0.1108, "fecha_inicio":"2022-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-373.21924255754857, "ahorro_total":-17914.52364276233, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":3500.0, "cuota":204.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-05-25", "tipo_deuda":"R", "ahorro_cuota_mensual":204.0, "ahorro_total":-204.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":90000.0, "cuota":4849.0, "saldo":80026.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":48.0, "numero_pagos_restante":28.0, "frecuencia_externa":"M", "avance":0.1108, "fecha_inicio":"2022-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-373.21924255754857, "ahorro_total":-17914.52364276233, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":17000.0, "cuota":1053.0, "saldo":16004.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":36.0, "numero_pagos_restante":25.0, "frecuencia_externa":"M", "avance":0.0586, "fecha_inicio":"2023-05-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-17.04125751743345, "ahorro_total":-613.4852706276042, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":17000.0, "cuota":1053.0, "saldo":16004.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":36.0, "numero_pagos_restante":25.0, "frecuencia_externa":"M", "avance":0.0586, "fecha_inicio":"2023-05-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-17.04125751743345, "ahorro_total":-613.4852706276042, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":17000.0, "cuota":1053.0, "saldo":16004.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":36.0, "numero_pagos_restante":25.0, "frecuencia_externa":"M", "avance":0.0586, "fecha_inicio":"2023-05-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-17.04125751743345, "ahorro_total":-613.4852706276042, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":17000.0, "cuota":1053.0, "saldo":16004.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":36.0, "numero_pagos_restante":25.0, "frecuencia_externa":"M", "avance":0.0586, "fecha_inicio":"2023-05-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-17.04125751743345, "ahorro_total":-613.4852706276042, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":191900.0, "cuota":4327.0, "saldo":8282.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9568, "fecha_inicio":"2018-03-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-6133.490877377719, "ahorro_total":-441611.34317119577, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":191900.0, "cuota":4327.0, "saldo":8282.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9568, "fecha_inicio":"2018-03-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-6133.490877377719, "ahorro_total":-441611.34317119577, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":191900.0, "cuota":4327.0, "saldo":8282.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9568, "fecha_inicio":"2018-03-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-6133.490877377719, "ahorro_total":-441611.34317119577, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":191900.0, "cuota":4327.0, "saldo":8282.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9568, "fecha_inicio":"2018-03-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-6133.490877377719, "ahorro_total":-441611.34317119577, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":191900.0, "cuota":4327.0, "saldo":8282.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9568, "fecha_inicio":"2018-03-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-6133.490877377719, "ahorro_total":-441611.34317119577, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":191900.0, "cuota":4327.0, "saldo":8282.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9568, "fecha_inicio":"2018-03-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-6133.490877377719, "ahorro_total":-441611.34317119577, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":191900.0, "cuota":4327.0, "saldo":8282.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9568, "fecha_inicio":"2018-03-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-6133.490877377719, "ahorro_total":-441611.34317119577, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":17000.0, "cuota":1053.0, "saldo":16004.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":36.0, "numero_pagos_restante":25.0, "frecuencia_externa":"M", "avance":0.0586, "fecha_inicio":"2023-05-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-17.04125751743345, "ahorro_total":-613.4852706276042, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":17000.0, "cuota":1053.0, "saldo":16004.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":36.0, "numero_pagos_restante":25.0, "frecuencia_externa":"M", "avance":0.0586, "fecha_inicio":"2023-05-03",</t>
@@ -91,7 +94,7 @@
     <t>{"Prospecto": 2090977, "monto_maximo_cliente": 58300.0, "cuota_externa_total": 12003.0, "capacidad_maxima_pago": 57593.86, "bursolnum": 7316152, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3618.98259942061, "monto_max": 58300.0, "cuota_min": 299.79381766541826, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.5991, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":30000.0, "cuota":2392.0, "saldo":16462.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":24.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.4513, "fecha_inicio":"2022-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":47.53026370028374, "ahorro_total":1140.7263288068098, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":5000.0, "cuota":218.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":900.0, "numero_pagos_restante":871.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-11-17", "tipo_deuda":"R", "ahorro_cuota_mensual":218.0, "ahorro_total":196200.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":47000.0, "cuota":2841.0, "saldo":16747.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6437, "fecha_inicio":"2021-08-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-293.9951506002203, "ahorro_total":-10583.825421607931, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":10800.0, "cuota":540.0, "saldo":10458.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0317, "fecha_inicio":"2023-07-06", "tipo_deuda":"R", "ahorro_cuota_mensual":10997.999999999989, "ahorro_total":-10997.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":58300.0, "cuota":6532.0, "saldo":54256.0, "tasa_externa":1.4595, "tasa_kubo":0.5991, "numero_pagos_otorgado":261.0, "numero_pagos_restante":55.0, "frecuencia_externa":"W", "avance":0.0694, "fecha_inicio":"2023-06-08", "tipo_deuda":"I", "ahorro_cuota_mensual":3066.438881547675, "ahorro_total":199318.5273005989, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":8000.0, "cuota":400.0, "saldo":3851.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5186, "fecha_inicio":"2019-06-24", "tipo_deuda":"R", "ahorro_cuota_mensual":4250.999999999996, "ahorro_total":-4250.999999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 2162754, "monto_maximo_cliente": 54000.0, "cuota_externa_total": 11791.0, "capacidad_maxima_pago": 64709.0, "bursolnum": 7317537, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5451.090349008467, "monto_max": 54000.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 16.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":2, "monto_otorgado":17200.0, "cuota":1589.0, "saldo":12415.0, "tasa_externa":0.7305, "tasa_kubo":0.6509, "numero_pagos_otorgado":18.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.2782, "fecha_inicio":"2023-06-11", "tipo_deuda":"I", "ahorro_cuota_mensual":-34.54721391740736, "ahorro_total":-621.8498505133325, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":36800.0, "cuota":4431.0, "saldo":21148.0, "tasa_externa":0.751, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4253, "fecha_inicio":"2022-08-17", "tipo_deuda":"I", "ahorro_cuota_mensual":-28.941040968760717, "ahorro_total":-347.2924916251286, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":8500.0, "cuota":425.0, "saldo":4988.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4132, "fecha_inicio":"2021-10-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":8563.0, "cuota":428.0, "saldo":2893.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6622, "fecha_inicio":"2014-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":1, "monto_otorgado":625.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-11-15", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":52527.0, "cuota":3401.0, "saldo":48417.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":40.0, "numero_pagos_restante":25.0, "frecuencia_externa":"M", "avance":0.0782, "fecha_inicio":"2023-01-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-219.31153671878928, "ahorro_total":-8772.461468751571, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":21020.0, "cuota":1736.0, "saldo":21248.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":24.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":-0.0108, "fecha_inicio":"2024-01-25", "tipo_deuda":"I", "ahorro_cuota_mensual":15.681535038260336, "ahorro_total":376.35684091824805, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":7, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2013-10-04", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+    <t>{"Prospecto": 2162754, "monto_maximo_cliente": 54000.0, "cuota_externa_total": 11791.0, "capacidad_maxima_pago": 64709.0, "bursolnum": 7317537, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5451.090349008467, "monto_max": 54000.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 16.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":2, "monto_otorgado":17200.0, "cuota":1589.0, "saldo":12415.0, "tasa_externa":0.7305, "tasa_kubo":0.6509, "numero_pagos_otorgado":18.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.2782, "fecha_inicio":"2023-06-11", "tipo_deuda":"I", "ahorro_cuota_mensual":-34.54721391740736, "ahorro_total":-621.8498505133325, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":36800.0, "cuota":4431.0, "saldo":21148.0, "tasa_externa":0.751, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4253, "fecha_inicio":"2022-08-17", "tipo_deuda":"I", "ahorro_cuota_mensual":-28.941040968760717, "ahorro_total":-347.2924916251286, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":8500.0, "cuota":425.0, "saldo":4988.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4132, "fecha_inicio":"2021-10-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":8563.0, "cuota":428.0, "saldo":2893.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6622, "fecha_inicio":"2014-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":1, "monto_otorgado":625.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-11-15", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":52527.0, "cuota":3401.0, "saldo":48417.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":40.0, "numero_pagos_restante":25.0, "frecuencia_externa":"M", "avance":0.0782, "fecha_inicio":"2023-01-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-219.31153671878928, "ahorro_total":-8772.461468751571, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":21020.0, "cuota":1736.0, "saldo":21248.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":24.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":-0.0108, "fecha_inicio":"2024-01-25", "tipo_deuda":"I", "ahorro_cuota_mensual":15.681535038260336, "ahorro_total":376.35684091824805, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":7, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2013-10-04", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 2298632, "monto_maximo_cliente": 102436.0, "cuota_externa_total": 27186.0, "capacidad_maxima_pago": 99249.0, "bursolnum": 7317447, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3713.0879129157443, "monto_max": 102436.0, "cuota_min": 163.04445621498797, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.3337, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2622, 0.2306, 0.2], "comisiones": [0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "HIPOTECAGOBIERNO", "registro":10, "monto_otorgado":1242826.0, "cuota":9082.0, "saldo":1055485.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":720.0, "numero_pagos_restante":256.0, "frecuencia_externa":"S", "avance":0.1507, "fecha_inicio":"2015-07-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-22422.513836329126, "ahorro_total":-8072104.981078485, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":9, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2015-11-04", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":1116.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2010-10-08", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "GUBERNAMENTALES", "registro":7, "monto_otorgado":2169.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"1989-08-14", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":100000.0, "cuota":5441.0, "saldo":89582.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":51.0, "numero_pagos_restante":29.0, "frecuencia_externa":"M", "avance":0.1042, "fecha_inicio":"2022-06-03", "tipo_deuda":"I", "ahorro_cuota_mensual":1925.5944447306283, "ahorro_total":98205.31668126205, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":4, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2024-01-12", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":7800.0, "cuota":5702.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2003-12-01", "tipo_deuda":"R", "ahorro_cuota_mensual":5702.0, "ahorro_total":-5702.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":54000.0, "cuota":3046.0, "saldo":46577.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1375, "fecha_inicio":"2020-03-21", "tipo_deuda":"R", "ahorro_cuota_mensual":49622.99999999976, "ahorro_total":-49622.99999999976, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":102436.0, "cuota":4407.0, "saldo":66155.0, "tasa_externa":0.3276, "tasa_kubo":0.2622, "numero_pagos_otorgado":37.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.3542, "fecha_inicio":"2022-07-05", "tipo_deuda":"I", "ahorro_cuota_mensual":107.77989184105809, "ahorro_total":3987.8559981191493, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":94365.0, "cuota":5210.0, "saldo":82966.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":48.0, "numero_pagos_restante":28.0, "frecuencia_externa":"M", "avance":0.1208, "fecha_inicio":"2022-08-17", "tipo_deuda":"I", "ahorro_cuota_mensual":1789.468732649711, "ahorro_total":85894.49916718612, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
@@ -109,19 +112,19 @@
     <t>{"Prospecto": 2687735, "monto_maximo_cliente": 90000.0, "cuota_externa_total": 15609.0, "capacidad_maxima_pago": 105064.0, "bursolnum": 7316666, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2757.042788185569, "monto_max": 90000.0, "cuota_min": 151.9292154681686, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6722, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2306, 0.2], "comisiones": [0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":90000.0, "cuota":3418.0, "saldo":86903.0, "tasa_externa":0.3937, "tasa_kubo":0.2306, "numero_pagos_otorgado":60.0, "numero_pagos_restante":49.0, "frecuencia_externa":"M", "avance":0.0344, "fecha_inicio":"2023-04-24", "tipo_deuda":"I", "ahorro_cuota_mensual":683.2741215729652, "ahorro_total":40996.44729437791, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":41990.0, "cuota":3500.0, "saldo":38435.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0847, "fecha_inicio":"2016-10-26", "tipo_deuda":"R", "ahorro_cuota_mensual":41934.99999999983, "ahorro_total":-41934.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":60000.0, "cuota":3665.0, "saldo":38258.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":36.0, "numero_pagos_restante":13.0, "frecuencia_externa":"M", "avance":0.3624, "fecha_inicio":"2022-04-22", "tipo_deuda":"I", "ahorro_cuota_mensual":1223.5401680305313, "ahorro_total":44047.446049099126, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":152600.0, "cuota":8526.0, "saldo":117442.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":48.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.2304, "fecha_inicio":"2022-01-27", "tipo_deuda":"I", "ahorro_cuota_mensual":3316.175786938158, "ahorro_total":159176.4377730316, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 2710338, "monto_maximo_cliente": 67158.0, "cuota_externa_total": 9897.0, "capacidad_maxima_pago": 73379.0, "bursolnum": 7317075, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4311.526817290196, "monto_max": 67158.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.5668, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "COOPERATIVA", "registro":48, "monto_otorgado":5000.0, "cuota":868.0, "saldo":378.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":26.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.9244, "fecha_inicio":"2012-07-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-132.23070171786173, "ahorro_total":-793.3842103071704, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":33, "monto_otorgado":999.0, "cuota":462.0, "saldo":462.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":929.0, "frecuencia_externa":"M", "avance":0.5375, "fecha_inicio":"2018-04-28", "tipo_deuda":"R", "ahorro_cuota_mensual":436.686712, "ahorro_total":436686.712, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-09-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":483.0, "cuota":175.0, "saldo":172.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6439, "fecha_inicio":"2023-06-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-3.9561450096482247, "ahorro_total":-11.868435028944674, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":21, "monto_otorgado":178.0, "cuota":67.0, "saldo":65.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6348, "fecha_inicio":"2023-06-12", "tipo_deuda":"I", "ahorro_cuota_mensual":1.0492881744981588, "ahorro_total":3.1478645234944764, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":12000.0, "cuota":600.0, "saldo":2596.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7837, "fecha_inicio":"2010-05-31", "tipo_deuda":"R", "ahorro_cuota_mensual":3196.0000000000005, "ahorro_total":-3196.0000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":5400.0, "cuota":270.0, "saldo":1401.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7406, "fecha_inicio":"2024-01-31", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":4000.0, "cuota":352.0, "saldo":3350.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":18.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.1625, "fecha_inicio":"2023-08-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-3.1095943541449174, "ahorro_total":-55.97269837460851, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":2600.0, "cuota":243.0, "saldo":731.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7188, "fecha_inicio":"2023-12-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":8100.0, "cuota":837.0, "saldo":2236.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.724, "fecha_inicio":"2023-09-04", "tipo_deuda":"R", "ahorro_cuota_mensual":3073.0000000000005, "ahorro_total":-3073.0000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":11000.0, "cuota":725.0, "saldo":5546.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4958, "fecha_inicio":"2022-12-27", "tipo_deuda":"R", "ahorro_cuota_mensual":6271.000000000001, "ahorro_total":-6271.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":2300.0, "cuota":550.0, "saldo":1448.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3704, "fecha_inicio":"2023-11-20", "tipo_deuda":"R", "ahorro_cuota_mensual":1998.0000000000002, "ahorro_total":-1998.0000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":19000.0, "cuota":950.0, "saldo":10157.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4654, "fecha_inicio":"2020-04-13", "tipo_deuda":"R", "ahorro_cuota_mensual":11107.000000000004, "ahorro_total":-11107.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":25000.0, "cuota":800.0, "saldo":3321.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8672, "fecha_inicio":"2020-10-12", "tipo_deuda":"R", "ahorro_cuota_mensual":4121.000000000001, "ahorro_total":-4121.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":67158.0, "cuota":5064.0, "saldo":48544.0, "tasa_externa":0.8371, "tasa_kubo":0.5668, "numero_pagos_otorgado":72.0, "numero_pagos_restante":20.0, "frecuencia_externa":"S", "avance":0.2772, "fecha_inicio":"2022-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":752.473182709804, "ahorro_total":27089.034577552942, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":2600.0, "cuota":338.0, "saldo":1688.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3508, "fecha_inicio":"2024-01-01", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 2710338, "monto_maximo_cliente": 67158.0, "cuota_externa_total": 9897.0, "capacidad_maxima_pago": 73379.0, "bursolnum": 7317075, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4311.526817290196, "monto_max": 67158.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.5668, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "COOPERATIVA", "registro":48, "monto_otorgado":5000.0, "cuota":868.0, "saldo":378.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":26.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.9244, "fecha_inicio":"2012-07-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-132.23070171786173, "ahorro_total":-793.3842103071704, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":33, "monto_otorgado":999.0, "cuota":462.0, "saldo":462.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":929.0, "frecuencia_externa":"M", "avance":0.5375, "fecha_inicio":"2018-04-28", "tipo_deuda":"R", "ahorro_cuota_mensual":436.686712, "ahorro_total":436686.712, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-09-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":483.0, "cuota":175.0, "saldo":172.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6439, "fecha_inicio":"2023-06-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-3.9561450096482247, "ahorro_total":-11.868435028944674, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":21, "monto_otorgado":178.0, "cuota":67.0, "saldo":65.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6348, "fecha_inicio":"2023-06-12", "tipo_deuda":"I", "ahorro_cuota_mensual":1.0492881744981588, "ahorro_total":3.1478645234944764, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":12000.0, "cuota":600.0, "saldo":2596.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7837, "fecha_inicio":"2010-05-31", "tipo_deuda":"R", "ahorro_cuota_mensual":3196.0000000000005, "ahorro_total":-3196.0000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":5400.0, "cuota":270.0, "saldo":1401.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7406, "fecha_inicio":"2024-01-31", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":4000.0, "cuota":352.0, "saldo":3350.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":18.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.1625, "fecha_inicio":"2023-08-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-3.1095943541449174, "ahorro_total":-55.97269837460851, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":2600.0, "cuota":243.0, "saldo":731.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7188, "fecha_inicio":"2023-12-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":8100.0, "cuota":837.0, "saldo":2236.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.724, "fecha_inicio":"2023-09-04", "tipo_deuda":"R", "ahorro_cuota_mensual":3073.0000000000005, "ahorro_total":-3073.0000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":11000.0, "cuota":725.0, "saldo":5546.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4958, "fecha_inicio":"2022-12-27", "tipo_deuda":"R", "ahorro_cuota_mensual":6271.000000000001, "ahorro_total":-6271.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":2300.0, "cuota":550.0, "saldo":1448.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3704, "fecha_inicio":"2023-11-20", "tipo_deuda":"R", "ahorro_cuota_mensual":1998.0000000000002, "ahorro_total":-1998.0000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":19000.0, "cuota":950.0, "saldo":10157.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4654, "fecha_inicio":"2020-04-13", "tipo_deuda":"R", "ahorro_cuota_mensual":11107.000000000004, "ahorro_total":-11107.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":25000.0, "cuota":800.0, "saldo":3321.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8672, "fecha_inicio":"2020-10-12", "tipo_deuda":"R", "ahorro_cuota_mensual":4121.000000000001, "ahorro_total":-4121.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":67158.0, "cuota":5064.0, "saldo":48544.0, "tasa_externa":0.8371, "tasa_kubo":0.5668, "numero_pagos_otorgado":72.0, "numero_pagos_restante":20.0, "frecuencia_externa":"S", "avance":0.2772, "fecha_inicio":"2022-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":752.473182709804, "ahorro_total":27089.034577552942, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":2600.0, "cuota":338.0, "saldo":1688.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3508, "fecha_inicio":"2024-01-01", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 2790904, "monto_maximo_cliente": 231000.0, "cuota_externa_total": 50312.0, "capacidad_maxima_pago": 227250.0, "bursolnum": 7316902, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 15778.821653385676, "monto_max": 231000.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.6722, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":229000.0, "cuota":12732.0, "saldo":177201.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":48.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.2262, "fecha_inicio":"2021-12-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-2910.208478897486, "ahorro_total":-139690.00698707934, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":94100.0, "cuota":1499.0, "saldo":3838.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9592, "fecha_inicio":"1996-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":5337.000000000005, "ahorro_total":-5337.000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":206000.0, "cuota":13274.0, "saldo":201548.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":120.0, "numero_pagos_restante":47.0, "frecuencia_externa":"S", "avance":0.0216, "fecha_inicio":"2023-03-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-425.23395633006476, "ahorro_total":-25514.037379803885, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":1, "monto_otorgado":46500.0, "cuota":2830.0, "saldo":46284.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0046, "fecha_inicio":"2019-08-01", "tipo_deuda":"R", "ahorro_cuota_mensual":49114.00000000006, "ahorro_total":-49114.00000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":231000.0, "cuota":21476.0, "saldo":230588.0, "tasa_externa":1.1158, "tasa_kubo":0.6722, "numero_pagos_otorgado":96.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0018, "fecha_inicio":"2019-07-17", "tipo_deuda":"I", "ahorro_cuota_mensual":5697.178346614324, "ahorro_total":273464.56063748756, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 2878373, "monto_maximo_cliente": 125000.0, "cuota_externa_total": 81336.0, "capacidad_maxima_pago": 101704.0, "bursolnum": 7374699, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4369.560700721107, "monto_max": 125000.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":19, "monto_otorgado":15000.0, "cuota":-1.0, "saldo":13698.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0868, "fecha_inicio":"2023-12-06", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":18, "monto_otorgado":2459.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-08-10", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":13, "monto_otorgado":261238.0, "cuota":8972.0, "saldo":264919.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":46.0, "frecuencia_externa":"M", "avance":-0.0141, "fecha_inicio":"2024-02-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-1020.5508189879838, "ahorro_total":-48986.43931142322, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":11, "monto_otorgado":68100.0, "cuota":49049.0, "saldo":19427.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7147, "fecha_inicio":"2017-02-21", "tipo_deuda":"R", "ahorro_cuota_mensual":68475.99999999994, "ahorro_total":-68475.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":166000.0, "cuota":11561.0, "saldo":165222.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":0.0047, "fecha_inicio":"2023-10-12", "tipo_deuda":"I", "ahorro_cuota_mensual":4163.90349652348, "ahorro_total":149900.52587484528, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":33, "monto_otorgado":1700.0, "cuota":586.0, "saldo":1138.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3306, "fecha_inicio":"2023-02-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-12.886730074731418, "ahorro_total":-38.66019022419425, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":32, "monto_otorgado":9900.0, "cuota":935.0, "saldo":6855.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3076, "fecha_inicio":"2022-10-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-48.733156271222015, "ahorro_total":-584.7978752546642, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":31, "monto_otorgado":6800.0, "cuota":6945.0, "saldo":6804.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0006, "fecha_inicio":"2023-02-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-46.5469333333167, "ahorro_total":-46.5469333333167, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":30, "monto_otorgado":5500.0, "cuota":675.0, "saldo":3784.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.312, "fecha_inicio":"2022-11-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-25.366658169637276, "ahorro_total":-228.29992352673548, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":20, "monto_otorgado":15000.0, "cuota":1910.0, "saldo":9214.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3857, "fecha_inicio":"2024-01-31", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":35100.0, "cuota":3235.0, "saldo":22032.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3723, "fecha_inicio":"2020-01-18", "tipo_deuda":"R", "ahorro_cuota_mensual":25266.999999999938, "ahorro_total":-25266.999999999938, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":100000.0, "cuota":6800.0, "saldo":79624.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":34.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.2038, "fecha_inicio":"2022-12-27", "tipo_deuda":"I", "ahorro_cuota_mensual":2190.6759204203354, "ahorro_total":74482.9812942914, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":63000.0, "cuota":3540.0, "saldo":58338.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.074, "fecha_inicio":"2017-11-15", "tipo_deuda":"R", "ahorro_cuota_mensual":61877.99999999984, "ahorro_total":-61877.99999999984, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":125000.0, "cuota":5006.0, "saldo":123369.0, "tasa_externa":0.3728, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":40.0, "frecuencia_externa":"M", "avance":0.013, "fecha_inicio":"2023-08-16", "tipo_deuda":"I", "ahorro_cuota_mensual":224.65558466418315, "ahorro_total":10783.468063880791, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":28000.0, "cuota":230.0, "saldo":22751.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1875, "fecha_inicio":"2018-12-21", "tipo_deuda":"R", "ahorro_cuota_mensual":22980.999999999935, "ahorro_total":-22980.999999999935, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":25000.0, "cuota":20454.0, "saldo":15822.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3671, "fecha_inicio":"2023-06-26", "tipo_deuda":"R", "ahorro_cuota_mensual":36275.999999999956, "ahorro_total":-36275.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":20000.0, "cuota":1003.0, "saldo":19424.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0288, "fecha_inicio":"2018-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":20426.999999999945, "ahorro_total":-20426.999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":63000.0, "cuota":5000.0, "saldo":57266.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.091, "fecha_inicio":"2017-03-15", "tipo_deuda":"R", "ahorro_cuota_mensual":62265.99999999985, "ahorro_total":-62265.99999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":20000.0, "cuota":1000.0, "saldo":10569.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4716, "fecha_inicio":"2023-10-27", "tipo_deuda":"R", "ahorro_cuota_mensual":11568.99999999997, "ahorro_total":-11568.99999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":55000.0, "cuota":3406.0, "saldo":53546.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0264, "fecha_inicio":"2022-12-09", "tipo_deuda":"R", "ahorro_cuota_mensual":56951.999999999854, "ahorro_total":-56951.999999999854, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":3000.0, "cuota":449.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2013-07-01", "tipo_deuda":"R", "ahorro_cuota_mensual":449.0, "ahorro_total":-449.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":14, "monto_otorgado":35100.0, "cuota":3730.0, "saldo":31369.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1063, "fecha_inicio":"2020-01-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":44000.0, "cuota":2200.0, "saldo":43387.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0139, "fecha_inicio":"2017-04-12", "tipo_deuda":"R", "ahorro_cuota_mensual":45586.999999999876, "ahorro_total":-45586.999999999876, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 2878373, "monto_maximo_cliente": 125000.0, "cuota_externa_total": 81336.0, "capacidad_maxima_pago": 101704.0, "bursolnum": 7374699, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4369.560700721107, "monto_max": 125000.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":19, "monto_otorgado":15000.0, "cuota":-1.0, "saldo":13698.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0868, "fecha_inicio":"2023-12-06", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":18, "monto_otorgado":2459.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-08-10", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":13, "monto_otorgado":261238.0, "cuota":8972.0, "saldo":264919.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":46.0, "frecuencia_externa":"M", "avance":-0.0141, "fecha_inicio":"2024-02-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-1020.5508189879838, "ahorro_total":-48986.43931142322, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":11, "monto_otorgado":68100.0, "cuota":49049.0, "saldo":19427.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7147, "fecha_inicio":"2017-02-21", "tipo_deuda":"R", "ahorro_cuota_mensual":68475.99999999994, "ahorro_total":-68475.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":166000.0, "cuota":11561.0, "saldo":165222.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":0.0047, "fecha_inicio":"2023-10-12", "tipo_deuda":"I", "ahorro_cuota_mensual":4163.90349652348, "ahorro_total":149900.52587484528, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":33, "monto_otorgado":1700.0, "cuota":586.0, "saldo":1138.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3306, "fecha_inicio":"2023-02-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-12.886730074731418, "ahorro_total":-38.66019022419425, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":32, "monto_otorgado":9900.0, "cuota":935.0, "saldo":6855.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3076, "fecha_inicio":"2022-10-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-48.733156271222015, "ahorro_total":-584.7978752546642, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":31, "monto_otorgado":6800.0, "cuota":6945.0, "saldo":6804.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0006, "fecha_inicio":"2023-02-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-46.5469333333167, "ahorro_total":-46.5469333333167, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":30, "monto_otorgado":5500.0, "cuota":675.0, "saldo":3784.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.312, "fecha_inicio":"2022-11-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-25.366658169637276, "ahorro_total":-228.29992352673548, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":20, "monto_otorgado":15000.0, "cuota":1910.0, "saldo":9214.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3857, "fecha_inicio":"2024-01-31", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":35100.0, "cuota":3235.0, "saldo":22032.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3723, "fecha_inicio":"2020-01-18", "tipo_deuda":"R", "ahorro_cuota_mensual":25266.999999999938, "ahorro_total":-25266.999999999938, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":100000.0, "cuota":6800.0, "saldo":79624.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":34.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.2038, "fecha_inicio":"2022-12-27", "tipo_deuda":"I", "ahorro_cuota_mensual":2190.6759204203354, "ahorro_total":74482.9812942914, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":63000.0, "cuota":3540.0, "saldo":58338.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.074, "fecha_inicio":"2017-11-15", "tipo_deuda":"R", "ahorro_cuota_mensual":61877.99999999984, "ahorro_total":-61877.99999999984, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":125000.0, "cuota":5006.0, "saldo":123369.0, "tasa_externa":0.3728, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":40.0, "frecuencia_externa":"M", "avance":0.013, "fecha_inicio":"2023-08-16", "tipo_deuda":"I", "ahorro_cuota_mensual":224.65558466418315, "ahorro_total":10783.468063880791, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":28000.0, "cuota":230.0, "saldo":22751.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1875, "fecha_inicio":"2018-12-21", "tipo_deuda":"R", "ahorro_cuota_mensual":22980.999999999935, "ahorro_total":-22980.999999999935, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":25000.0, "cuota":20454.0, "saldo":15822.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3671, "fecha_inicio":"2023-06-26", "tipo_deuda":"R", "ahorro_cuota_mensual":36275.999999999956, "ahorro_total":-36275.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":20000.0, "cuota":1003.0, "saldo":19424.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0288, "fecha_inicio":"2018-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":20426.999999999945, "ahorro_total":-20426.999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":63000.0, "cuota":5000.0, "saldo":57266.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.091, "fecha_inicio":"2017-03-15", "tipo_deuda":"R", "ahorro_cuota_mensual":62265.99999999985, "ahorro_total":-62265.99999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":20000.0, "cuota":1000.0, "saldo":10569.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4716, "fecha_inicio":"2023-10-27", "tipo_deuda":"R", "ahorro_cuota_mensual":11568.99999999997, "ahorro_total":-11568.99999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":55000.0, "cuota":3406.0, "saldo":53546.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0264, "fecha_inicio":"2022-12-09", "tipo_deuda":"R", "ahorro_cuota_mensual":56951.999999999854, "ahorro_total":-56951.999999999854, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":3000.0, "cuota":449.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2013-07-01", "tipo_deuda":"R", "ahorro_cuota_mensual":449.0, "ahorro_total":-449.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":14, "monto_otorgado":35100.0, "cuota":3730.0, "saldo":31369.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1063, "fecha_inicio":"2020-01-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":44000.0, "cuota":2200.0, "saldo":43387.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0139, "fecha_inicio":"2017-04-12", "tipo_deuda":"R", "ahorro_cuota_mensual":45586.999999999876, "ahorro_total":-45586.999999999876, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 2901882, "monto_maximo_cliente": 328500.0, "cuota_externa_total": 42978.0, "capacidad_maxima_pago": 330366.0, "bursolnum": 7316468, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 10187.569080969615, "monto_max": 328500.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 51.0, "plazo_min": 4, "tasa": 0.2, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0], "deudas_buro": [ {"entidad": "BANCO", "registro":16, "monto_otorgado":209000.0, "cuota":11732.0, "saldo":209130.0, "tasa_externa":0.6547, "tasa_kubo":0.2, "numero_pagos_otorgado":120.0, "numero_pagos_restante":57.0, "frecuencia_externa":"S", "avance":-0.0006, "fecha_inicio":"2024-01-05", "tipo_deuda":"I", "ahorro_cuota_mensual":5816.151024556162, "ahorro_total":348969.0614733697, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":50, "monto_otorgado":1000.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2009-05-09", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":17, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2011-03-19", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":79100.0, "cuota":4982.0, "saldo":43011.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":48.0, "numero_pagos_restante":10.0, "frecuencia_externa":"S", "avance":0.4562, "fecha_inicio":"2023-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":831.4131206856209, "ahorro_total":19953.914896454902, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1921.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-06-13", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2005-03-23", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":14, "monto_otorgado":37930.0, "cuota":2675.0, "saldo":27513.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":17.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2746, "fecha_inicio":"2020-07-18", "tipo_deuda":"I", "ahorro_cuota_mensual":35.809750045089004, "ahorro_total":608.7657507665131, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":15, "monto_otorgado":101600.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-07-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":42500.0, "cuota":231.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-09-17", "tipo_deuda":"R", "ahorro_cuota_mensual":231.0, "ahorro_total":-231.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":119500.0, "cuota":9010.0, "saldo":90105.0, "tasa_externa":0.837, "tasa_kubo":0.2, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.246, "fecha_inicio":"2011-04-06", "tipo_deuda":"I", "ahorro_cuota_mensual":4371.722292111271, "ahorro_total":157382.00251600574, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":211500.0, "cuota":10575.0, "saldo":68445.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6764, "fecha_inicio":"2017-04-12", "tipo_deuda":"R", "ahorro_cuota_mensual":79019.99999999985, "ahorro_total":-79019.99999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":110000.0, "cuota":177.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-06-23", "tipo_deuda":"R", "ahorro_cuota_mensual":177.0, "ahorro_total":-177.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":51500.0, "cuota":120.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-02-06", "tipo_deuda":"R", "ahorro_cuota_mensual":120.0, "ahorro_total":-120.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":1, "monto_otorgado":114510.0, "cuota":5726.0, "saldo":46021.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5981, "fecha_inicio":"2003-08-29", "tipo_deuda":"R", "ahorro_cuota_mensual":51746.999999999905, "ahorro_total":-51746.999999999905, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":95778.0, "cuota":5681.0, "saldo":64169.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":13.0, "frecuencia_externa":"M", "avance":0.33, "fecha_inicio":"2023-05-09", "tipo_deuda":"I", "ahorro_cuota_mensual":655.2742082557188, "ahorro_total":15726.580998137251, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 2937559, "monto_maximo_cliente": 85395.0, "cuota_externa_total": 36859.0, "capacidad_maxima_pago": 67665.0, "bursolnum": 7317560, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5991.637935690177, "monto_max": 85395.0, "cuota_min": 299.79381766541826, "monto_min": 5000, "plazo_max": 31.0, "plazo_min": 4, "tasa": 0.5991, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":8000.0, "cuota":6430.0, "saldo":6430.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1963, "fecha_inicio":"2021-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":12859.999999999993, "ahorro_total":-12859.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":18, "monto_otorgado":6543.0, "cuota":124.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-02-08", "tipo_deuda":"R", "ahorro_cuota_mensual":124.0, "ahorro_total":-124.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":20, "monto_otorgado":12000.0, "cuota":600.0, "saldo":8960.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2533, "fecha_inicio":"2020-12-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":21, "monto_otorgado":8400.0, "cuota":420.0, "saldo":6099.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2739, "fecha_inicio":"2023-11-29", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":22, "monto_otorgado":8100.0, "cuota":-1.0, "saldo":339.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9581, "fecha_inicio":"2023-12-02", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":23, "monto_otorgado":4100.0, "cuota":-1.0, "saldo":6066.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.4795, "fecha_inicio":"2024-01-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1075.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-11-17", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":38, "monto_otorgado":14040.0, "cuota":468.0, "saldo":14040.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":120.0, "numero_pagos_restante":22.0, "frecuencia_externa":"W", "avance":0.0, "fecha_inicio":"2023-07-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-529.3177334154271, "ahorro_total":-15879.532002462814, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":65, "monto_otorgado":8000.0, "cuota":2476.0, "saldo":7231.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0961, "fecha_inicio":"2021-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":19, "monto_otorgado":28500.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-07-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":13700.0, "cuota":1625.0, "saldo":13152.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":12.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.04, "fecha_inicio":"2023-12-19", "tipo_deuda":"I", "ahorro_cuota_mensual":9.549540641746717, "ahorro_total":114.5944877009606, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":24, "monto_otorgado":7354.0, "cuota":504.0, "saldo":4752.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3538, "fecha_inicio":"2024-01-29", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":8000.0, "cuota":1294.0, "saldo":4426.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4468, "fecha_inicio":"2023-05-03", "tipo_deuda":"R", "ahorro_cuota_mensual":5719.9999999999945, "ahorro_total":-5719.9999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":2300.0, "cuota":300.0, "saldo":986.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5713, "fecha_inicio":"2023-11-22", "tipo_deuda":"R", "ahorro_cuota_mensual":1285.999999999999, "ahorro_total":-1285.999999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":13600.0, "cuota":883.0, "saldo":479.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9648, "fecha_inicio":"2023-06-19", "tipo_deuda":"R", "ahorro_cuota_mensual":1361.9999999999995, "ahorro_total":-1361.9999999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":20000.0, "cuota":1922.0, "saldo":16204.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1898, "fecha_inicio":"2023-10-16", "tipo_deuda":"R", "ahorro_cuota_mensual":18125.999999999985, "ahorro_total":-18125.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":19900.0, "cuota":1352.0, "saldo":13332.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.3301, "fecha_inicio":"2022-05-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-9470.459608264802, "ahorro_total":-18940.919216529604, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":84800.0, "cuota":5944.0, "saldo":76307.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1002, "fecha_inicio":"2023-06-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-40173.81782818367, "ahorro_total":-80347.63565636735, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":33700.0, "cuota":2364.0, "saldo":31661.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0605, "fecha_inicio":"2023-09-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-15963.48184917205, "ahorro_total":-31926.9636983441, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":12000.0, "cuota":2390.0, "saldo":1962.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8365, "fecha_inicio":"2019-02-11", "tipo_deuda":"R", "ahorro_cuota_mensual":4351.999999999998, "ahorro_total":-4351.999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":22815.0, "cuota":1141.0, "saldo":22770.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.002, "fecha_inicio":"2021-02-02", "tipo_deuda":"R", "ahorro_cuota_mensual":23910.999999999975, "ahorro_total":-23910.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":16000.0, "cuota":1437.0, "saldo":1727.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8921, "fecha_inicio":"2020-02-04", "tipo_deuda":"R", "ahorro_cuota_mensual":3163.999999999998, "ahorro_total":-3163.999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":48476.0, "cuota":3650.0, "saldo":47164.0, "tasa_externa":0.8355, "tasa_kubo":0.5991, "numero_pagos_otorgado":72.0, "numero_pagos_restante":30.0, "frecuencia_externa":"S", "avance":0.0271, "fecha_inicio":"2023-10-18", "tipo_deuda":"I", "ahorro_cuota_mensual":416.5526612660369, "ahorro_total":14995.89580557733, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":36919.0, "cuota":3416.0, "saldo":33775.0, "tasa_externa":0.9449, "tasa_kubo":0.5991, "numero_pagos_otorgado":48.0, "numero_pagos_restante":19.0, "frecuencia_externa":"S", "avance":0.0852, "fecha_inicio":"2023-10-23", "tipo_deuda":"I", "ahorro_cuota_mensual":530.817393518359, "ahorro_total":12739.617444440617, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":4749.0, "cuota":3284.0, "saldo":1642.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.6542, "fecha_inicio":"2023-12-09", "tipo_deuda":"I", "ahorro_cuota_mensual":1514.2084581612366, "ahorro_total":4542.62537448371, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":15, "monto_otorgado":2000.0, "cuota":1302.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-01-17", "tipo_deuda":"R", "ahorro_cuota_mensual":1302.0, "ahorro_total":-1302.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+    <t>{"Prospecto": 2937559, "monto_maximo_cliente": 85395.0, "cuota_externa_total": 36859.0, "capacidad_maxima_pago": 67665.0, "bursolnum": 7317560, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5991.637935690177, "monto_max": 85395.0, "cuota_min": 299.79381766541826, "monto_min": 5000, "plazo_max": 31.0, "plazo_min": 4, "tasa": 0.5991, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":8000.0, "cuota":6430.0, "saldo":6430.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1963, "fecha_inicio":"2021-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":12859.999999999993, "ahorro_total":-12859.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":18, "monto_otorgado":6543.0, "cuota":124.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-02-08", "tipo_deuda":"R", "ahorro_cuota_mensual":124.0, "ahorro_total":-124.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":20, "monto_otorgado":12000.0, "cuota":600.0, "saldo":8960.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2533, "fecha_inicio":"2020-12-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":21, "monto_otorgado":8400.0, "cuota":420.0, "saldo":6099.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2739, "fecha_inicio":"2023-11-29", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":22, "monto_otorgado":8100.0, "cuota":-1.0, "saldo":339.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9581, "fecha_inicio":"2023-12-02", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":23, "monto_otorgado":4100.0, "cuota":-1.0, "saldo":6066.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.4795, "fecha_inicio":"2024-01-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1075.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-11-17", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":38, "monto_otorgado":14040.0, "cuota":468.0, "saldo":14040.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":120.0, "numero_pagos_restante":22.0, "frecuencia_externa":"W", "avance":0.0, "fecha_inicio":"2023-07-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-529.3177334154271, "ahorro_total":-15879.532002462814, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":65, "monto_otorgado":8000.0, "cuota":2476.0, "saldo":7231.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0961, "fecha_inicio":"2021-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":19, "monto_otorgado":28500.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-07-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":13700.0, "cuota":1625.0, "saldo":13152.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":12.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.04, "fecha_inicio":"2023-12-19", "tipo_deuda":"I", "ahorro_cuota_mensual":9.549540641746717, "ahorro_total":114.5944877009606, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":24, "monto_otorgado":7354.0, "cuota":504.0, "saldo":4752.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3538, "fecha_inicio":"2024-01-29", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":8000.0, "cuota":1294.0, "saldo":4426.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4468, "fecha_inicio":"2023-05-03", "tipo_deuda":"R", "ahorro_cuota_mensual":5719.9999999999945, "ahorro_total":-5719.9999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":2300.0, "cuota":300.0, "saldo":986.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5713, "fecha_inicio":"2023-11-22", "tipo_deuda":"R", "ahorro_cuota_mensual":1285.999999999999, "ahorro_total":-1285.999999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":13600.0, "cuota":883.0, "saldo":479.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9648, "fecha_inicio":"2023-06-19", "tipo_deuda":"R", "ahorro_cuota_mensual":1361.9999999999995, "ahorro_total":-1361.9999999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":20000.0, "cuota":1922.0, "saldo":16204.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1898, "fecha_inicio":"2023-10-16", "tipo_deuda":"R", "ahorro_cuota_mensual":18125.999999999985, "ahorro_total":-18125.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":19900.0, "cuota":1352.0, "saldo":13332.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.3301, "fecha_inicio":"2022-05-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-9470.459608264802, "ahorro_total":-18940.919216529604, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":84800.0, "cuota":5944.0, "saldo":76307.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1002, "fecha_inicio":"2023-06-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-40173.81782818367, "ahorro_total":-80347.63565636735, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":33700.0, "cuota":2364.0, "saldo":31661.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0605, "fecha_inicio":"2023-09-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-15963.48184917205, "ahorro_total":-31926.9636983441, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":12000.0, "cuota":2390.0, "saldo":1962.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8365, "fecha_inicio":"2019-02-11", "tipo_deuda":"R", "ahorro_cuota_mensual":4351.999999999998, "ahorro_total":-4351.999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":22815.0, "cuota":1141.0, "saldo":22770.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.002, "fecha_inicio":"2021-02-02", "tipo_deuda":"R", "ahorro_cuota_mensual":23910.999999999975, "ahorro_total":-23910.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":16000.0, "cuota":1437.0, "saldo":1727.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8921, "fecha_inicio":"2020-02-04", "tipo_deuda":"R", "ahorro_cuota_mensual":3163.999999999998, "ahorro_total":-3163.999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":48476.0, "cuota":3650.0, "saldo":47164.0, "tasa_externa":0.8355, "tasa_kubo":0.5991, "numero_pagos_otorgado":72.0, "numero_pagos_restante":30.0, "frecuencia_externa":"S", "avance":0.0271, "fecha_inicio":"2023-10-18", "tipo_deuda":"I", "ahorro_cuota_mensual":416.5526612660369, "ahorro_total":14995.89580557733, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":36919.0, "cuota":3416.0, "saldo":33775.0, "tasa_externa":0.9449, "tasa_kubo":0.5991, "numero_pagos_otorgado":48.0, "numero_pagos_restante":19.0, "frecuencia_externa":"S", "avance":0.0852, "fecha_inicio":"2023-10-23", "tipo_deuda":"I", "ahorro_cuota_mensual":530.817393518359, "ahorro_total":12739.617444440617, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":4749.0, "cuota":3284.0, "saldo":1642.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.6542, "fecha_inicio":"2023-12-09", "tipo_deuda":"I", "ahorro_cuota_mensual":1514.2084581612366, "ahorro_total":4542.62537448371, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":15, "monto_otorgado":2000.0, "cuota":1302.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-01-17", "tipo_deuda":"R", "ahorro_cuota_mensual":1302.0, "ahorro_total":-1302.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 3073017, "monto_maximo_cliente": 21000.0, "cuota_externa_total": 16679.0, "capacidad_maxima_pago": 23321.0, "bursolnum": 7317317, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1150.271580551952, "monto_max": 21000.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 28.0, "plazo_min": 4, "tasa": 0.3337, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":27000.0, "cuota":47.0, "saldo":932.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9655, "fecha_inicio":"2018-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":978.9999999999977, "ahorro_total":-978.9999999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":90000.0, "cuota":6011.0, "saldo":78841.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":36.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.124, "fecha_inicio":"2022-12-02", "tipo_deuda":"I", "ahorro_cuota_mensual":1748.6210150846218, "ahorro_total":62950.356543046386, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":21000.0, "cuota":1670.0, "saldo":8844.0, "tasa_externa":0.7274, "tasa_kubo":0.3337, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5789, "fecha_inicio":"2022-08-11", "tipo_deuda":"I", "ahorro_cuota_mensual":399.65367432061726, "ahorro_total":9591.688183694814, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2017-04-23", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":28100.0, "cuota":584.0, "saldo":20572.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2679, "fecha_inicio":"2016-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":21155.999999999945, "ahorro_total":-21155.999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":26000.0, "cuota":1300.0, "saldo":23446.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0982, "fecha_inicio":"2019-03-04", "tipo_deuda":"R", "ahorro_cuota_mensual":24745.999999999938, "ahorro_total":-24745.999999999938, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":3, "monto_otorgado":200000.0, "cuota":7741.0, "saldo":188085.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":60.0, "numero_pagos_restante":53.0, "frecuencia_externa":"M", "avance":0.0596, "fecha_inicio":"2023-09-19", "tipo_deuda":"I", "ahorro_cuota_mensual":161.32524829128215, "ahorro_total":9679.514897476929, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
@@ -145,7 +148,7 @@
     <t>{"Prospecto": 3473842, "monto_maximo_cliente": 5800.0, "cuota_externa_total": 2951.0, "capacidad_maxima_pago": 9849.0, "bursolnum": 7316387, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 628.0988813440744, "monto_max": 5800.0, "cuota_min": 232.85304854502846, "monto_min": 5000, "plazo_max": 12.0, "plazo_min": 4, "tasa": 0.4428, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":16, "monto_otorgado":13100.0, "cuota":655.0, "saldo":1329.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8985, "fecha_inicio":"2023-05-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-730.886515999998, "ahorro_total":-730.886515999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":12000.0, "cuota":1651.0, "saldo":7430.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3808, "fecha_inicio":"2023-09-11", "tipo_deuda":"I", "ahorro_cuota_mensual":16.397674972638697, "ahorro_total":147.57907475374827, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":15, "monto_otorgado":13100.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-03-21", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":17, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2017-05-28", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":4530.0, "cuota":524.0, "saldo":250.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9448, "fecha_inicio":"2013-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":773.9999999999995, "ahorro_total":-773.9999999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":5800.0, "cuota":1145.0, "saldo":4886.0, "tasa_externa":0.616, "tasa_kubo":0.4428, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1576, "fecha_inicio":"2024-01-22", "tipo_deuda":"I", "ahorro_cuota_mensual":28.460368362937515, "ahorro_total":170.7622101776251, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":2000.0, "cuota":3580.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-05-13", "tipo_deuda":"R", "ahorro_cuota_mensual":3580.0, "ahorro_total":-3580.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":4500.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-10-01", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":36000.0, "cuota":1450.0, "saldo":4228.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8826, "fecha_inicio":"2018-07-15", "tipo_deuda":"R", "ahorro_cuota_mensual":5677.999999999992, "ahorro_total":-5677.999999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 3549605, "monto_maximo_cliente": 163300.0, "cuota_externa_total": 55494.0, "capacidad_maxima_pago": 143773.0, "bursolnum": 7317920, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 8244.36739815244, "monto_max": 163300.0, "cuota_min": 244.39480798426723, "monto_min": 5000, "plazo_max": 52.0, "plazo_min": 4, "tasa": 0.4706, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":16, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2015-08-10", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":56000.0, "cuota":3904.0, "saldo":56000.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":24.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":21.760060625548704, "ahorro_total":522.2414550131689, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":13, "monto_otorgado":1436320.0, "cuota":12683.0, "saldo":1228340.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":360.0, "numero_pagos_restante":256.0, "frecuencia_externa":"M", "avance":0.1448, "fecha_inicio":"2015-07-24", "tipo_deuda":"M", "ahorro_cuota_mensual":-43195.83057950822, "ahorro_total":-15550499.00862296, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":10, "monto_otorgado":315700.0, "cuota":5410.0, "saldo":32456.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":60.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8972, "fecha_inicio":"2019-06-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-10021.088176126632, "ahorro_total":-601265.290567598, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":30000.0, "cuota":2095.0, "saldo":28849.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":24.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.0384, "fecha_inicio":"2023-11-23", "tipo_deuda":"I", "ahorro_cuota_mensual":15.228603906543867, "ahorro_total":365.4864937570528, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":7, "monto_otorgado":80000.0, "cuota":4000.0, "saldo":52724.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3409, "fecha_inicio":"2019-09-20", "tipo_deuda":"R", "ahorro_cuota_mensual":56724.00000000002, "ahorro_total":-56724.00000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-02-07", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":26, "monto_otorgado":23400.0, "cuota":1250.0, "saldo":10949.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5321, "fecha_inicio":"2004-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":17, "monto_otorgado":78000.0, "cuota":3900.0, "saldo":8885.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8861, "fecha_inicio":"2013-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":12785.000000000004, "ahorro_total":-12785.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":14, "monto_otorgado":97963.0, "cuota":4898.0, "saldo":54845.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4401, "fecha_inicio":"2002-11-01", "tipo_deuda":"R", "ahorro_cuota_mensual":59743.00000000002, "ahorro_total":-59743.00000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":100000.0, "cuota":5000.0, "saldo":70192.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":900.0, "numero_pagos_restante":830.0, "frecuencia_externa":"Z", "avance":0.2981, "fecha_inicio":"2018-06-21", "tipo_deuda":"R", "ahorro_cuota_mensual":1806.8723306666661, "ahorro_total":1626185.0975999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":96000.0, "cuota":5660.0, "saldo":82134.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1444, "fecha_inicio":"2023-11-07", "tipo_deuda":"R", "ahorro_cuota_mensual":87794.00000000004, "ahorro_total":-87794.00000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":258500.0, "cuota":12925.0, "saldo":51012.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8027, "fecha_inicio":"2013-10-01", "tipo_deuda":"R", "ahorro_cuota_mensual":63937.00000000002, "ahorro_total":-63937.00000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":102000.0, "cuota":800.0, "saldo":3291.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9677, "fecha_inicio":"2023-05-12", "tipo_deuda":"R", "ahorro_cuota_mensual":4091.0000000000014, "ahorro_total":-4091.0000000000014, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":254000.0, "cuota":4000.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-06-12", "tipo_deuda":"R", "ahorro_cuota_mensual":4000.0, "ahorro_total":-4000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":23400.0, "cuota":40.0, "saldo":53.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9977, "fecha_inicio":"2012-03-27", "tipo_deuda":"R", "ahorro_cuota_mensual":93.00000000000003, "ahorro_total":-93.00000000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":163300.0, "cuota":20572.0, "saldo":148413.0, "tasa_externa":1.6396, "tasa_kubo":0.4706, "numero_pagos_otorgado":208.0, "numero_pagos_restante":43.0, "frecuencia_externa":"W", "avance":0.0912, "fecha_inicio":"2023-07-04", "tipo_deuda":"I", "ahorro_cuota_mensual":12327.63260184756, "ahorro_total":641036.895296073, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":79430.0, "cuota":3972.0, "saldo":5365.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9325, "fecha_inicio":"2004-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":9337.000000000004, "ahorro_total":-9337.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 3549605, "monto_maximo_cliente": 163300.0, "cuota_externa_total": 55494.0, "capacidad_maxima_pago": 143773.0, "bursolnum": 7317920, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 8244.36739815244, "monto_max": 163300.0, "cuota_min": 244.39480798426723, "monto_min": 5000, "plazo_max": 52.0, "plazo_min": 4, "tasa": 0.4706, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":16, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2015-08-10", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":56000.0, "cuota":3904.0, "saldo":56000.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":24.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":21.760060625548704, "ahorro_total":522.2414550131689, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":13, "monto_otorgado":1436320.0, "cuota":12683.0, "saldo":1228340.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":360.0, "numero_pagos_restante":256.0, "frecuencia_externa":"M", "avance":0.1448, "fecha_inicio":"2015-07-24", "tipo_deuda":"M", "ahorro_cuota_mensual":-43195.83057950822, "ahorro_total":-15550499.00862296, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":10, "monto_otorgado":315700.0, "cuota":5410.0, "saldo":32456.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":60.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8972, "fecha_inicio":"2019-06-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-10021.088176126632, "ahorro_total":-601265.290567598, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":30000.0, "cuota":2095.0, "saldo":28849.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":24.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.0384, "fecha_inicio":"2023-11-23", "tipo_deuda":"I", "ahorro_cuota_mensual":15.228603906543867, "ahorro_total":365.4864937570528, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":7, "monto_otorgado":80000.0, "cuota":4000.0, "saldo":52724.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3409, "fecha_inicio":"2019-09-20", "tipo_deuda":"R", "ahorro_cuota_mensual":56724.00000000002, "ahorro_total":-56724.00000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-02-07", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":26, "monto_otorgado":23400.0, "cuota":1250.0, "saldo":10949.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5321, "fecha_inicio":"2004-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":17, "monto_otorgado":78000.0, "cuota":3900.0, "saldo":8885.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8861, "fecha_inicio":"2013-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":12785.000000000004, "ahorro_total":-12785.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":14, "monto_otorgado":97963.0, "cuota":4898.0, "saldo":54845.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4401, "fecha_inicio":"2002-11-01", "tipo_deuda":"R", "ahorro_cuota_mensual":59743.00000000002, "ahorro_total":-59743.00000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":100000.0, "cuota":5000.0, "saldo":70192.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":900.0, "numero_pagos_restante":830.0, "frecuencia_externa":"Z", "avance":0.2981, "fecha_inicio":"2018-06-21", "tipo_deuda":"R", "ahorro_cuota_mensual":1806.8723306666661, "ahorro_total":1626185.0975999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":96000.0, "cuota":5660.0, "saldo":82134.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1444, "fecha_inicio":"2023-11-07", "tipo_deuda":"R", "ahorro_cuota_mensual":87794.00000000004, "ahorro_total":-87794.00000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":258500.0, "cuota":12925.0, "saldo":51012.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8027, "fecha_inicio":"2013-10-01", "tipo_deuda":"R", "ahorro_cuota_mensual":63937.00000000002, "ahorro_total":-63937.00000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":102000.0, "cuota":800.0, "saldo":3291.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9677, "fecha_inicio":"2023-05-12", "tipo_deuda":"R", "ahorro_cuota_mensual":4091.0000000000014, "ahorro_total":-4091.0000000000014, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":254000.0, "cuota":4000.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-06-12", "tipo_deuda":"R", "ahorro_cuota_mensual":4000.0, "ahorro_total":-4000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":23400.0, "cuota":40.0, "saldo":53.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9977, "fecha_inicio":"2012-03-27", "tipo_deuda":"R", "ahorro_cuota_mensual":93.00000000000003, "ahorro_total":-93.00000000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":163300.0, "cuota":20572.0, "saldo":148413.0, "tasa_externa":1.6396, "tasa_kubo":0.4706, "numero_pagos_otorgado":208.0, "numero_pagos_restante":43.0, "frecuencia_externa":"W", "avance":0.0912, "fecha_inicio":"2023-07-04", "tipo_deuda":"I", "ahorro_cuota_mensual":12327.63260184756, "ahorro_total":641036.895296073, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":79430.0, "cuota":3972.0, "saldo":5365.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9325, "fecha_inicio":"2004-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":9337.000000000004, "ahorro_total":-9337.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 3553967, "monto_maximo_cliente": 18500.0, "cuota_externa_total": 6464.0, "capacidad_maxima_pago": 24836.0, "bursolnum": 7316324, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1420.8663578375517, "monto_max": 18500.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 26.0, "plazo_min": 4, "tasa": 0.6193, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":35500.0, "cuota":2277.0, "saldo":15899.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":36.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.5521, "fecha_inicio":"2021-10-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-147.13159246341274, "ahorro_total":-5296.737328682859, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":1, "monto_otorgado":15000.0, "cuota":1553.0, "saldo":14197.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":15.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.0535, "fecha_inicio":"2023-11-09", "tipo_deuda":"I", "ahorro_cuota_mensual":9.913850674547348, "ahorro_total":148.70776011821022, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":15800.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-05-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-16745.87753333335, "ahorro_total":-16745.87753333335, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":7000.0, "cuota":558.0, "saldo":6186.0, "tasa_externa":0.7306, "tasa_kubo":0.6193, "numero_pagos_otorgado":24.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.1163, "fecha_inicio":"2023-08-17", "tipo_deuda":"I", "ahorro_cuota_mensual":0.9391266801566189, "ahorro_total":22.539040323758854, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":11500.0, "cuota":1376.0, "saldo":10053.0, "tasa_externa":0.737, "tasa_kubo":0.6193, "numero_pagos_otorgado":12.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.1258, "fecha_inicio":"2023-11-23", "tipo_deuda":"I", "ahorro_cuota_mensual":5.32417194305026, "ahorro_total":63.89006331660312, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":9800.0, "cuota":700.0, "saldo":9232.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.058, "fecha_inicio":"2023-05-07", "tipo_deuda":"R", "ahorro_cuota_mensual":9932.000000000004, "ahorro_total":-9932.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
@@ -181,10 +184,10 @@
     <t>{"Prospecto": 3805773, "monto_maximo_cliente": 68000.0, "cuota_externa_total": 8123.0, "capacidad_maxima_pago": 82877.0, "bursolnum": 7315963, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2083.0989955179853, "monto_max": 68000.0, "cuota_min": 151.9292154681686, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2306, 0.2], "comisiones": [0.03845, 0.03845], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":2, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-05-30", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":52000.0, "cuota":3447.0, "saldo":9804.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":26.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8115, "fecha_inicio":"2022-02-04", "tipo_deuda":"I", "ahorro_cuota_mensual":790.1471643479604, "ahorro_total":20543.82627304697, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":68000.0, "cuota":2676.0, "saldo":56967.0, "tasa_externa":0.4147, "tasa_kubo":0.2306, "numero_pagos_otorgado":60.0, "numero_pagos_restante":40.0, "frecuencia_externa":"M", "avance":0.1622, "fecha_inicio":"2022-07-25", "tipo_deuda":"I", "ahorro_cuota_mensual":609.7626696329071, "ahorro_total":36585.76017797443, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":3000.0, "cuota":150.0, "saldo":1945.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3517, "fecha_inicio":"2023-05-29", "tipo_deuda":"R", "ahorro_cuota_mensual":2094.999999999992, "ahorro_total":-2094.999999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":117500.0, "cuota":5875.0, "saldo":84305.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2825, "fecha_inicio":"2016-06-01", "tipo_deuda":"R", "ahorro_cuota_mensual":90179.99999999965, "ahorro_total":-90179.99999999965, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":29000.0, "cuota":1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-05-24", "tipo_deuda":"R", "ahorro_cuota_mensual":1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 3868724, "monto_maximo_cliente": 73000.0, "cuota_externa_total": 31174.0, "capacidad_maxima_pago": 62214.0, "bursolnum": 7317173, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4235.800052296678, "monto_max": 73000.0, "cuota_min": 278.44180193239873, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.5504, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":28, "monto_otorgado":722.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-03-08", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":15, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2002-04-02", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":14, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2016-01-02", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-10-21", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":7, "monto_otorgado":363704.0, "cuota":5850.0, "saldo":482570.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":360.0, "numero_pagos_restante":211.0, "frecuencia_externa":"M", "avance":-0.3268, "fecha_inicio":"2011-10-26", "tipo_deuda":"M", "ahorro_cuota_mensual":-19825.297908418557, "ahorro_total":-7137107.247030681, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":50000.0, "cuota":3688.0, "saldo":42605.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":24.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.1479, "fecha_inicio":"2023-06-05", "tipo_deuda":"I", "ahorro_cuota_mensual":-49.354436781702134, "ahorro_total":-1184.5064827608512, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":3, "monto_otorgado":236321.0, "cuota":5997.0, "saldo":83697.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":60.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.6458, "fecha_inicio":"2020-05-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-7163.329014893279, "ahorro_total":-429799.7408935968, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-05-20", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":13, "monto_otorgado":13634.0, "cuota":682.0, "saldo":4256.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6878, "fecha_inicio":"2023-11-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":14700.0, "cuota":1110.0, "saldo":2222.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8488, "fecha_inicio":"2023-09-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":12000.0, "cuota":2835.0, "saldo":2835.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7638, "fecha_inicio":"2023-08-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":75700.0, "cuota":4660.0, "saldo":64968.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1418, "fecha_inicio":"2014-03-01", "tipo_deuda":"R", "ahorro_cuota_mensual":69627.99999999994, "ahorro_total":-69627.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":24100.0, "cuota":1205.0, "saldo":15500.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3568, "fecha_inicio":"2022-10-10", "tipo_deuda":"R", "ahorro_cuota_mensual":16704.999999999985, "ahorro_total":-16704.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":6200.0, "cuota":450.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-03-18", "tipo_deuda":"R", "ahorro_cuota_mensual":450.0, "ahorro_total":-450.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":73000.0, "cuota":5352.0, "saldo":69663.0, "tasa_externa":0.8602, "tasa_kubo":0.5504, "numero_pagos_otorgado":96.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0457, "fecha_inicio":"2017-09-12", "tipo_deuda":"I", "ahorro_cuota_mensual":1116.1999477033223, "ahorro_total":53577.59748975947, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-04-03", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3926429, "monto_maximo_cliente": 9200.0, "cuota_externa_total": 13483.0, "capacidad_maxima_pago": 4896.0, "bursolnum": 7316286, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 285.3139590408537, "monto_max": 9200.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 51.0, "plazo_min": 4, "tasa": 0.5292, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":19, "monto_otorgado":14302.0, "cuota":715.0, "saldo":2974.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7921, "fecha_inicio":"2023-12-01", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":20, "monto_otorgado":14303.0, "cuota":715.0, "saldo":5696.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6018, "fecha_inicio":"2024-01-15", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":21, "monto_otorgado":14320.0, "cuota":716.0, "saldo":1991.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.861, "fecha_inicio":"2024-01-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":1543.0, "cuota":918.0, "saldo":918.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4051, "fecha_inicio":"2019-01-19", "tipo_deuda":"O", "ahorro_cuota_mensual":1835.9999999999982, "ahorro_total":-1835.9999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":40000.0, "cuota":2848.0, "saldo":18988.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5253, "fecha_inicio":"2022-09-13", "tipo_deuda":"I", "ahorro_cuota_mensual":749.0938663391257, "ahorro_total":17978.252792139017, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":23600.0, "cuota":1813.0, "saldo":3445.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":21.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.854, "fecha_inicio":"2022-06-16", "tipo_deuda":"I", "ahorro_cuota_mensual":434.97967644236405, "ahorro_total":9134.573205289646, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":18, "monto_otorgado":14360.0, "cuota":718.0, "saldo":1166.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9188, "fecha_inicio":"2023-11-29", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":20000.0, "cuota":1425.0, "saldo":11286.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.4357, "fecha_inicio":"2022-11-16", "tipo_deuda":"I", "ahorro_cuota_mensual":375.54693316956286, "ahorro_total":9013.126396069509, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":14351.0, "cuota":718.0, "saldo":1736.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.879, "fecha_inicio":"2023-11-05", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":15, "monto_otorgado":14317.0, "cuota":716.0, "saldo":1134.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9208, "fecha_inicio":"2023-09-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":14, "monto_otorgado":11917.0, "cuota":596.0, "saldo":708.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9406, "fecha_inicio":"2023-09-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":13, "monto_otorgado":14400.0, "cuota":236.0, "saldo":236.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9836, "fecha_inicio":"2023-07-24", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":15000.0, "cuota":1428.0, "saldo":14927.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":27.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.0049, "fecha_inicio":"2023-09-15", "tipo_deuda":"R", "ahorro_cuota_mensual":713.147882840986, "ahorro_total":19254.99283670662, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":8000.0, "cuota":400.0, "saldo":7932.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0085, "fecha_inicio":"2021-03-08", "tipo_deuda":"R", "ahorro_cuota_mensual":8331.999999999985, "ahorro_total":-8331.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":8700.0, "cuota":435.0, "saldo":8649.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0059, "fecha_inicio":"2020-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":9083.999999999982, "ahorro_total":-9083.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":6500.0, "cuota":497.0, "saldo":4961.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2368, "fecha_inicio":"2021-01-11", "tipo_deuda":"R", "ahorro_cuota_mensual":5457.99999999999, "ahorro_total":-5457.99999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":9200.0, "cuota":368.0, "saldo":8268.0, "tasa_externa":0.426, "tasa_kubo":0.2, "numero_pagos_otorgado":120.0, "numero_pagos_restante":42.0, "frecuencia_externa":"S", "avance":0.1013, "fecha_inicio":"2022-10-03", "tipo_deuda":"I", "ahorro_cuota_mensual":107.58942309051048, "ahorro_total":6455.3653854306285, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":12400.0, "cuota":1007.0, "saldo":12223.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0143, "fecha_inicio":"2023-09-11", "tipo_deuda":"R", "ahorro_cuota_mensual":13229.999999999976, "ahorro_total":-13229.999999999976, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":16, "monto_otorgado":14384.0, "cuota":719.0, "saldo":2811.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8046, "fecha_inicio":"2023-10-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 3868724, "monto_maximo_cliente": 73000.0, "cuota_externa_total": 31174.0, "capacidad_maxima_pago": 62214.0, "bursolnum": 7317173, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4235.800052296678, "monto_max": 73000.0, "cuota_min": 278.44180193239873, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.5504, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":28, "monto_otorgado":722.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-03-08", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":15, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2002-04-02", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":14, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2016-01-02", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-10-21", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":7, "monto_otorgado":363704.0, "cuota":5850.0, "saldo":482570.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":360.0, "numero_pagos_restante":211.0, "frecuencia_externa":"M", "avance":-0.3268, "fecha_inicio":"2011-10-26", "tipo_deuda":"M", "ahorro_cuota_mensual":-19825.297908418557, "ahorro_total":-7137107.247030681, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":50000.0, "cuota":3688.0, "saldo":42605.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":24.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.1479, "fecha_inicio":"2023-06-05", "tipo_deuda":"I", "ahorro_cuota_mensual":-49.354436781702134, "ahorro_total":-1184.5064827608512, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":3, "monto_otorgado":236321.0, "cuota":5997.0, "saldo":83697.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":60.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.6458, "fecha_inicio":"2020-05-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-7163.329014893279, "ahorro_total":-429799.7408935968, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-05-20", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":13, "monto_otorgado":13634.0, "cuota":682.0, "saldo":4256.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6878, "fecha_inicio":"2023-11-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":14700.0, "cuota":1110.0, "saldo":2222.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8488, "fecha_inicio":"2023-09-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":12000.0, "cuota":2835.0, "saldo":2835.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7638, "fecha_inicio":"2023-08-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":75700.0, "cuota":4660.0, "saldo":64968.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1418, "fecha_inicio":"2014-03-01", "tipo_deuda":"R", "ahorro_cuota_mensual":69627.99999999994, "ahorro_total":-69627.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":24100.0, "cuota":1205.0, "saldo":15500.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3568, "fecha_inicio":"2022-10-10", "tipo_deuda":"R", "ahorro_cuota_mensual":16704.999999999985, "ahorro_total":-16704.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":6200.0, "cuota":450.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-03-18", "tipo_deuda":"R", "ahorro_cuota_mensual":450.0, "ahorro_total":-450.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":73000.0, "cuota":5352.0, "saldo":69663.0, "tasa_externa":0.8602, "tasa_kubo":0.5504, "numero_pagos_otorgado":96.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0457, "fecha_inicio":"2017-09-12", "tipo_deuda":"I", "ahorro_cuota_mensual":1116.1999477033223, "ahorro_total":53577.59748975947, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-04-03", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3926429, "monto_maximo_cliente": 9200.0, "cuota_externa_total": 13483.0, "capacidad_maxima_pago": 4896.0, "bursolnum": 7316286, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 285.3139590408537, "monto_max": 9200.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 51.0, "plazo_min": 4, "tasa": 0.5292, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":19, "monto_otorgado":14302.0, "cuota":715.0, "saldo":2974.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7921, "fecha_inicio":"2023-12-01", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":20, "monto_otorgado":14303.0, "cuota":715.0, "saldo":5696.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6018, "fecha_inicio":"2024-01-15", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":21, "monto_otorgado":14320.0, "cuota":716.0, "saldo":1991.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.861, "fecha_inicio":"2024-01-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":1543.0, "cuota":918.0, "saldo":918.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4051, "fecha_inicio":"2019-01-19", "tipo_deuda":"O", "ahorro_cuota_mensual":1835.9999999999982, "ahorro_total":-1835.9999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":40000.0, "cuota":2848.0, "saldo":18988.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5253, "fecha_inicio":"2022-09-13", "tipo_deuda":"I", "ahorro_cuota_mensual":749.0938663391257, "ahorro_total":17978.252792139017, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":23600.0, "cuota":1813.0, "saldo":3445.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":21.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.854, "fecha_inicio":"2022-06-16", "tipo_deuda":"I", "ahorro_cuota_mensual":434.97967644236405, "ahorro_total":9134.573205289646, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":18, "monto_otorgado":14360.0, "cuota":718.0, "saldo":1166.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9188, "fecha_inicio":"2023-11-29", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":20000.0, "cuota":1425.0, "saldo":11286.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.4357, "fecha_inicio":"2022-11-16", "tipo_deuda":"I", "ahorro_cuota_mensual":375.54693316956286, "ahorro_total":9013.126396069509, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":14351.0, "cuota":718.0, "saldo":1736.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.879, "fecha_inicio":"2023-11-05", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":15, "monto_otorgado":14317.0, "cuota":716.0, "saldo":1134.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9208, "fecha_inicio":"2023-09-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":14, "monto_otorgado":11917.0, "cuota":596.0, "saldo":708.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9406, "fecha_inicio":"2023-09-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":13, "monto_otorgado":14400.0, "cuota":236.0, "saldo":236.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9836, "fecha_inicio":"2023-07-24", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":15000.0, "cuota":1428.0, "saldo":14927.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":27.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.0049, "fecha_inicio":"2023-09-15", "tipo_deuda":"R", "ahorro_cuota_mensual":713.147882840986, "ahorro_total":19254.99283670662, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":8000.0, "cuota":400.0, "saldo":7932.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0085, "fecha_inicio":"2021-03-08", "tipo_deuda":"R", "ahorro_cuota_mensual":8331.999999999985, "ahorro_total":-8331.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":8700.0, "cuota":435.0, "saldo":8649.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0059, "fecha_inicio":"2020-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":9083.999999999982, "ahorro_total":-9083.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":6500.0, "cuota":497.0, "saldo":4961.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2368, "fecha_inicio":"2021-01-11", "tipo_deuda":"R", "ahorro_cuota_mensual":5457.99999999999, "ahorro_total":-5457.99999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":9200.0, "cuota":368.0, "saldo":8268.0, "tasa_externa":0.426, "tasa_kubo":0.2, "numero_pagos_otorgado":120.0, "numero_pagos_restante":42.0, "frecuencia_externa":"S", "avance":0.1013, "fecha_inicio":"2022-10-03", "tipo_deuda":"I", "ahorro_cuota_mensual":107.58942309051048, "ahorro_total":6455.3653854306285, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":12400.0, "cuota":1007.0, "saldo":12223.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0143, "fecha_inicio":"2023-09-11", "tipo_deuda":"R", "ahorro_cuota_mensual":13229.999999999976, "ahorro_total":-13229.999999999976, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":16, "monto_otorgado":14384.0, "cuota":719.0, "saldo":2811.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8046, "fecha_inicio":"2023-10-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 3941195, "monto_maximo_cliente": 17500.0, "cuota_externa_total": 9248.0, "capacidad_maxima_pago": 18752.0, "bursolnum": 7316202, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 570.1336596018155, "monto_max": 17500.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.5292, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":9880.0, "cuota":50.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-07-10", "tipo_deuda":"R", "ahorro_cuota_mensual":50.0, "ahorro_total":-50.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-10-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":50000.0, "cuota":2966.0, "saldo":17853.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":29.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6429, "fecha_inicio":"2022-03-24", "tipo_deuda":"I", "ahorro_cuota_mensual":697.4097295381043, "ahorro_total":20224.882156605025, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":1075.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2017-01-03", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":17500.0, "cuota":891.0, "saldo":17170.0, "tasa_externa":0.4536, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":0.0189, "fecha_inicio":"2024-01-08", "tipo_deuda":"I", "ahorro_cuota_mensual":211.75431056022796, "ahorro_total":7623.155180168207, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":84000.0, "cuota":4200.0, "saldo":23239.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7233, "fecha_inicio":"2015-06-24", "tipo_deuda":"R", "ahorro_cuota_mensual":27438.999999999956, "ahorro_total":-27438.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":27000.0, "cuota":1350.0, "saldo":3514.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8699, "fecha_inicio":"2017-07-11", "tipo_deuda":"R", "ahorro_cuota_mensual":4863.999999999993, "ahorro_total":-4863.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":16500.0, "cuota":1430.0, "saldo":17375.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.053, "fecha_inicio":"2021-09-10", "tipo_deuda":"R", "ahorro_cuota_mensual":18804.999999999967, "ahorro_total":-18804.999999999967, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
@@ -214,7 +217,7 @@
     <t>{"Prospecto": 4206571, "monto_maximo_cliente": 61616.0, "cuota_externa_total": 26246.0, "capacidad_maxima_pago": 58970.0, "bursolnum": 7316836, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2380.862607852828, "monto_max": 61616.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.6722, "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":210000.0, "cuota":14377.0, "saldo":174233.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.1703, "fecha_inicio":"2022-10-13", "tipo_deuda":"I", "ahorro_cuota_mensual":5019.227314879101, "ahorro_total":180692.18333564763, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":28000.0, "cuota":2384.0, "saldo":20121.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":21.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.2814, "fecha_inicio":"2023-04-27", "tipo_deuda":"I", "ahorro_cuota_mensual":599.4862096941742, "ahorro_total":12589.21040357766, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":22000.0, "cuota":1100.0, "saldo":1555.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9293, "fecha_inicio":"2018-10-06", "tipo_deuda":"R", "ahorro_cuota_mensual":2654.999999999996, "ahorro_total":-2654.999999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":21000.0, "cuota":1777.0, "saldo":18732.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.108, "fecha_inicio":"2024-01-16", "tipo_deuda":"R", "ahorro_cuota_mensual":20508.99999999995, "ahorro_total":-20508.99999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":48000.0, "cuota":2400.0, "saldo":17498.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6355, "fecha_inicio":"2018-05-04", "tipo_deuda":"R", "ahorro_cuota_mensual":19897.999999999953, "ahorro_total":-19897.999999999953, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":25200.0, "cuota":182.0, "saldo":20982.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1674, "fecha_inicio":"2019-03-22", "tipo_deuda":"R", "ahorro_cuota_mensual":21163.99999999994, "ahorro_total":-21163.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":23800.0, "cuota":1190.0, "saldo":16321.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3142, "fecha_inicio":"2018-09-22", "tipo_deuda":"R", "ahorro_cuota_mensual":17510.999999999956, "ahorro_total":-17510.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":48800.0, "cuota":2250.0, "saldo":45800.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0615, "fecha_inicio":"2023-06-02", "tipo_deuda":"R", "ahorro_cuota_mensual":48049.999999999876, "ahorro_total":-48049.999999999876, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":61616.0, "cuota":3053.0, "saldo":55098.0, "tasa_externa":0.4304, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":26.0, "frecuencia_externa":"M", "avance":0.1058, "fecha_inicio":"2023-06-09", "tipo_deuda":"I", "ahorro_cuota_mensual":307.34037254090845, "ahorro_total":11064.253411472704, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":23000.0, "cuota":1150.0, "saldo":15960.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":69.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.3061, "fecha_inicio":"2018-06-11", "tipo_deuda":"R", "ahorro_cuota_mensual":622.901501410678, "ahorro_total":42980.20359733678, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":14800.0, "cuota":1000.0, "saldo":10000.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3243, "fecha_inicio":"2020-10-19", "tipo_deuda":"R", "ahorro_cuota_mensual":10999.999999999973, "ahorro_total":-10999.999999999973, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":14000.0, "cuota":1508.0, "saldo":11490.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":52.0, "numero_pagos_restante":7.0, "frecuencia_externa":"W", "avance":0.1793, "fecha_inicio":"2023-10-06", "tipo_deuda":"I", "ahorro_cuota_mensual":206.95647902858582, "ahorro_total":2690.4342273716156, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 4231833, "monto_maximo_cliente": 35000.0, "cuota_externa_total": 15791.0, "capacidad_maxima_pago": 32133.66, "bursolnum": 7316042, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1385.4815374669631, "monto_max": 35000.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.3337, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":13500.0, "cuota":2152.0, "saldo":21520.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.5941, "fecha_inicio":"2024-01-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":13, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2014-01-07", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":26395.0, "cuota":1836.0, "saldo":7005.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7346, "fecha_inicio":"2022-11-10", "tipo_deuda":"I", "ahorro_cuota_mensual":85.70097278459752, "ahorro_total":1542.6175101227554, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":173000.0, "cuota":7322.0, "saldo":137084.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.2076, "fecha_inicio":"2023-02-10", "tipo_deuda":"I", "ahorro_cuota_mensual":607.1711843953963, "ahorro_total":21858.162638234266, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":13100.0, "cuota":164.0, "saldo":549.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9581, "fecha_inicio":"2018-11-08", "tipo_deuda":"R", "ahorro_cuota_mensual":712.999999999999, "ahorro_total":-712.999999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":14, "monto_otorgado":24000.0, "cuota":337.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-06-23", "tipo_deuda":"R", "ahorro_cuota_mensual":337.0, "ahorro_total":-337.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":25900.0, "cuota":1295.0, "saldo":18543.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2841, "fecha_inicio":"2019-06-10", "tipo_deuda":"R", "ahorro_cuota_mensual":19837.999999999964, "ahorro_total":-19837.999999999964, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":88000.0, "cuota":4350.0, "saldo":39772.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.548, "fecha_inicio":"2018-04-28", "tipo_deuda":"R", "ahorro_cuota_mensual":44121.99999999992, "ahorro_total":-44121.99999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":7200.0, "cuota":553.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-01-26", "tipo_deuda":"R", "ahorro_cuota_mensual":553.0, "ahorro_total":-553.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":35000.0, "cuota":1901.0, "saldo":967.0, "tasa_externa":0.2724, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9724, "fecha_inicio":"2022-02-24", "tipo_deuda":"I", "ahorro_cuota_mensual":64.45713304673473, "ahorro_total":1546.9711931216334, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":138800.0, "cuota":6940.0, "saldo":53995.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.611, "fecha_inicio":"2018-02-06", "tipo_deuda":"R", "ahorro_cuota_mensual":60934.9999999999, "ahorro_total":-60934.9999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":2550.0, "cuota":345.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-01-29", "tipo_deuda":"R", "ahorro_cuota_mensual":345.0, "ahorro_total":-345.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":500.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-02-24", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":17700.0, "cuota":885.0, "saldo":12840.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2746, "fecha_inicio":"2022-02-24", "tipo_deuda":"R", "ahorro_cuota_mensual":13724.999999999975, "ahorro_total":-13724.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":4550.0, "cuota":519.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-04-18", "tipo_deuda":"R", "ahorro_cuota_mensual":519.0, "ahorro_total":-519.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+    <t>{"Prospecto": 4231833, "monto_maximo_cliente": 35000.0, "cuota_externa_total": 15791.0, "capacidad_maxima_pago": 32133.66, "bursolnum": 7316042, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1385.4815374669631, "monto_max": 35000.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.3337, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":13500.0, "cuota":2152.0, "saldo":21520.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.5941, "fecha_inicio":"2024-01-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":13, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2014-01-07", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":26395.0, "cuota":1836.0, "saldo":7005.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7346, "fecha_inicio":"2022-11-10", "tipo_deuda":"I", "ahorro_cuota_mensual":85.70097278459752, "ahorro_total":1542.6175101227554, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":173000.0, "cuota":7322.0, "saldo":137084.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.2076, "fecha_inicio":"2023-02-10", "tipo_deuda":"I", "ahorro_cuota_mensual":607.1711843953963, "ahorro_total":21858.162638234266, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":13100.0, "cuota":164.0, "saldo":549.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9581, "fecha_inicio":"2018-11-08", "tipo_deuda":"R", "ahorro_cuota_mensual":712.999999999999, "ahorro_total":-712.999999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":14, "monto_otorgado":24000.0, "cuota":337.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-06-23", "tipo_deuda":"R", "ahorro_cuota_mensual":337.0, "ahorro_total":-337.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":25900.0, "cuota":1295.0, "saldo":18543.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2841, "fecha_inicio":"2019-06-10", "tipo_deuda":"R", "ahorro_cuota_mensual":19837.999999999964, "ahorro_total":-19837.999999999964, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":88000.0, "cuota":4350.0, "saldo":39772.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.548, "fecha_inicio":"2018-04-28", "tipo_deuda":"R", "ahorro_cuota_mensual":44121.99999999992, "ahorro_total":-44121.99999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":7200.0, "cuota":553.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-01-26", "tipo_deuda":"R", "ahorro_cuota_mensual":553.0, "ahorro_total":-553.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":35000.0, "cuota":1901.0, "saldo":967.0, "tasa_externa":0.2724, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9724, "fecha_inicio":"2022-02-24", "tipo_deuda":"I", "ahorro_cuota_mensual":64.45713304673473, "ahorro_total":1546.9711931216334, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":138800.0, "cuota":6940.0, "saldo":53995.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.611, "fecha_inicio":"2018-02-06", "tipo_deuda":"R", "ahorro_cuota_mensual":60934.9999999999, "ahorro_total":-60934.9999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":2550.0, "cuota":345.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-01-29", "tipo_deuda":"R", "ahorro_cuota_mensual":345.0, "ahorro_total":-345.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":500.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-02-24", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":17700.0, "cuota":885.0, "saldo":12840.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2746, "fecha_inicio":"2022-02-24", "tipo_deuda":"R", "ahorro_cuota_mensual":13724.999999999975, "ahorro_total":-13724.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":4550.0, "cuota":519.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-04-18", "tipo_deuda":"R", "ahorro_cuota_mensual":519.0, "ahorro_total":-519.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 4261012, "monto_maximo_cliente": 54022.0, "cuota_externa_total": 20198.0, "capacidad_maxima_pago": 45476.0, "bursolnum": 7315917, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2772.155536151241, "monto_max": 54022.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0433, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":16, "monto_otorgado":3500.0, "cuota":179.0, "saldo":1849.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4717, "fecha_inicio":"2016-06-04", "tipo_deuda":"R", "ahorro_cuota_mensual":2028.000000000004, "ahorro_total":-2028.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":35000.0, "cuota":3007.0, "saldo":5670.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":20.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.838, "fecha_inicio":"2022-07-12", "tipo_deuda":"I", "ahorro_cuota_mensual":502.75659598887705, "ahorro_total":10055.131919777541, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":47700.0, "cuota":3183.0, "saldo":42525.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":36.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.1085, "fecha_inicio":"2023-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":768.9179452645271, "ahorro_total":27681.04602952298, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":8500.0, "cuota":652.0, "saldo":8178.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":29.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.0379, "fecha_inicio":"2023-10-30", "tipo_deuda":"I", "ahorro_cuota_mensual":169.96146841460467, "ahorro_total":4928.882584023535, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":2, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-03-14", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-06-22", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":18, "monto_otorgado":17000.0, "cuota":213.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-11-30", "tipo_deuda":"R", "ahorro_cuota_mensual":213.0, "ahorro_total":-213.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":17, "monto_otorgado":10000.0, "cuota":500.0, "saldo":3264.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6736, "fecha_inicio":"2020-11-13", "tipo_deuda":"R", "ahorro_cuota_mensual":3764.0000000000073, "ahorro_total":-3764.0000000000073, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":15, "monto_otorgado":10791.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2010-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":13, "monto_otorgado":17000.0, "cuota":838.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":900.0, "numero_pagos_restante":847.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-10-28", "tipo_deuda":"R", "ahorro_cuota_mensual":838.0, "ahorro_total":754200.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":14, "monto_otorgado":24000.0, "cuota":1200.0, "saldo":22912.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0453, "fecha_inicio":"2018-11-15", "tipo_deuda":"R", "ahorro_cuota_mensual":24112.00000000005, "ahorro_total":-24112.00000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":12000.0, "cuota":604.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-01-13", "tipo_deuda":"R", "ahorro_cuota_mensual":604.0, "ahorro_total":-604.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":12600.0, "cuota":8073.0, "saldo":7695.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3893, "fecha_inicio":"2023-06-08", "tipo_deuda":"R", "ahorro_cuota_mensual":15768.000000000016, "ahorro_total":-15768.000000000016, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":54022.0, "cuota":3279.0, "saldo":44400.0, "tasa_externa":0.3963, "tasa_kubo":0.3813, "numero_pagos_otorgado":24.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1781, "fecha_inicio":"2023-07-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-151.11364784276975, "ahorro_total":-3626.727548226474, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":336.0, "cuota":40.0, "saldo":143.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5744, "fecha_inicio":"2023-05-31", "tipo_deuda":"I", "ahorro_cuota_mensual":4.847904926197529, "ahorro_total":58.17485911437035, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":327.0, "cuota":39.0, "saldo":108.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6697, "fecha_inicio":"2023-04-18", "tipo_deuda":"I", "ahorro_cuota_mensual":4.789478901388669, "ahorro_total":57.47374681666403, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":398.0, "cuota":82.0, "saldo":80.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.799, "fecha_inicio":"2023-08-17", "tipo_deuda":"I", "ahorro_cuota_mensual":6.851323509131163, "ahorro_total":41.10794105478698, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":191.0, "cuota":77.0, "saldo":74.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6126, "fecha_inicio":"2023-11-23", "tipo_deuda":"I", "ahorro_cuota_mensual":8.583339252222174, "ahorro_total":25.750017756666523, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
@@ -232,7 +235,7 @@
     <t>{"Prospecto": 4389079, "monto_maximo_cliente": 70000.0, "cuota_externa_total": 11667.0, "capacidad_maxima_pago": 78633.0, "bursolnum": 7316903, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3433.1575734085386, "monto_max": 70000.0, "cuota_min": 244.39480798426723, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5668, "comision": 0.0455, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":2174.0, "cuota":122.0, "saldo":490.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":8.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.7746, "fecha_inicio":"2023-10-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-14.741437083058429, "ahorro_total":-58.965748332233716, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":30000.0, "cuota":1810.0, "saldo":22052.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":36.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.2649, "fecha_inicio":"2022-08-26", "tipo_deuda":"I", "ahorro_cuota_mensual":100.68241140596501, "ahorro_total":3624.5668106147405, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":41924.0, "cuota":2647.0, "saldo":40031.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.0452, "fecha_inicio":"2023-07-17", "tipo_deuda":"I", "ahorro_cuota_mensual":258.2856471927894, "ahorro_total":9298.283298940418, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":2000.0, "cuota":267.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-07-18", "tipo_deuda":"R", "ahorro_cuota_mensual":267.0, "ahorro_total":-267.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-10-17", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":10000.0, "cuota":1132.0, "saldo":4124.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.5876, "fecha_inicio":"2023-06-01", "tipo_deuda":"I", "ahorro_cuota_mensual":32.25358358036624, "ahorro_total":387.0430029643949, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":71100.0, "cuota":3555.0, "saldo":14256.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7995, "fecha_inicio":"2017-11-22", "tipo_deuda":"R", "ahorro_cuota_mensual":17811.000000000007, "ahorro_total":-17811.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":70000.0, "cuota":3978.0, "saldo":62869.0, "tasa_externa":0.679, "tasa_kubo":0.4706, "numero_pagos_otorgado":146.0, "numero_pagos_restante":56.0, "frecuencia_externa":"S", "avance":0.1019, "fecha_inicio":"2022-10-31", "tipo_deuda":"I", "ahorro_cuota_mensual":664.8254846366553, "ahorro_total":48532.26037847584, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":14000.0, "cuota":1089.0, "saldo":4582.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6727, "fecha_inicio":"2022-07-18", "tipo_deuda":"R", "ahorro_cuota_mensual":5671.000000000002, "ahorro_total":-5671.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 4433343, "monto_maximo_cliente": 100000.0, "cuota_externa_total": 19438.0, "capacidad_maxima_pago": 95376.0, "bursolnum": 7317022, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 6567.032899983563, "monto_max": 100000.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 52.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":15, "monto_otorgado":811.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-11-08", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":14, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2013-03-20", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":30000.0, "cuota":2003.0, "saldo":24010.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":36.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.1997, "fecha_inicio":"2022-09-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-120.69378190660336, "ahorro_total":-4344.976148637721, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":15000.0, "cuota":1046.0, "saldo":14688.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":36.0, "numero_pagos_restante":26.0, "frecuencia_externa":"M", "avance":0.0208, "fecha_inicio":"2023-06-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-15.846890953301681, "ahorro_total":-570.4880743188605, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":44, "monto_otorgado":9720.0, "cuota":630.0, "saldo":630.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9352, "fecha_inicio":"2019-12-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-548.0061662558794, "ahorro_total":-6576.073995070553, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":13, "monto_otorgado":5061.0, "cuota":519.0, "saldo":5194.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0263, "fecha_inicio":"2023-12-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":5061.0, "cuota":432.0, "saldo":2592.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4878, "fecha_inicio":"2023-12-26", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":5062.0, "cuota":253.0, "saldo":327.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9354, "fecha_inicio":"2023-11-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":5100.0, "cuota":919.0, "saldo":2753.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4602, "fecha_inicio":"2023-11-08", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":10000.0, "cuota":1196.0, "saldo":8748.0, "tasa_externa":0.736, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1252, "fecha_inicio":"2020-06-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-15.940500263250215, "ahorro_total":-191.28600315900258, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":90000.0, "cuota":6236.0, "saldo":80757.0, "tasa_externa":0.8227, "tasa_kubo":0.6509, "numero_pagos_otorgado":112.0, "numero_pagos_restante":44.0, "frecuencia_externa":"S", "avance":0.1027, "fecha_inicio":"2023-03-29", "tipo_deuda":"I", "ahorro_cuota_mensual":381.09089912038144, "ahorro_total":21341.09035074136, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":2000.0, "cuota":524.0, "saldo":581.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7095, "fecha_inicio":"2019-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":1105.0000000000007, "ahorro_total":-1105.0000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":7400.0, "cuota":370.0, "saldo":4802.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3511, "fecha_inicio":"2022-05-16", "tipo_deuda":"R", "ahorro_cuota_mensual":5172.0000000000055, "ahorro_total":-5172.0000000000055, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":44200.0, "cuota":3016.0, "saldo":35838.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1892, "fecha_inicio":"2022-12-05", "tipo_deuda":"I", "ahorro_cuota_mensual":-21191.015201068985, "ahorro_total":-42382.03040213797, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":25000.0, "cuota":1732.0, "saldo":22910.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0836, "fecha_inicio":"2023-07-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-11959.75067933766, "ahorro_total":-23919.50135867532, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":17400.0, "cuota":1450.0, "saldo":7150.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5891, "fecha_inicio":"2023-06-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-658.7764704580554, "ahorro_total":-7905.317645496665, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 4433343, "monto_maximo_cliente": 100000.0, "cuota_externa_total": 19438.0, "capacidad_maxima_pago": 95376.0, "bursolnum": 7317022, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 6567.032899983563, "monto_max": 100000.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 52.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":15, "monto_otorgado":811.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-11-08", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":14, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2013-03-20", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":30000.0, "cuota":2003.0, "saldo":24010.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":36.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.1997, "fecha_inicio":"2022-09-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-120.69378190660336, "ahorro_total":-4344.976148637721, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":15000.0, "cuota":1046.0, "saldo":14688.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":36.0, "numero_pagos_restante":26.0, "frecuencia_externa":"M", "avance":0.0208, "fecha_inicio":"2023-06-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-15.846890953301681, "ahorro_total":-570.4880743188605, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":44, "monto_otorgado":9720.0, "cuota":630.0, "saldo":630.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9352, "fecha_inicio":"2019-12-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-548.0061662558794, "ahorro_total":-6576.073995070553, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":13, "monto_otorgado":5061.0, "cuota":519.0, "saldo":5194.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0263, "fecha_inicio":"2023-12-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":5061.0, "cuota":432.0, "saldo":2592.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4878, "fecha_inicio":"2023-12-26", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":5062.0, "cuota":253.0, "saldo":327.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9354, "fecha_inicio":"2023-11-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":5100.0, "cuota":919.0, "saldo":2753.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4602, "fecha_inicio":"2023-11-08", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":10000.0, "cuota":1196.0, "saldo":8748.0, "tasa_externa":0.736, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1252, "fecha_inicio":"2020-06-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-15.940500263250215, "ahorro_total":-191.28600315900258, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":90000.0, "cuota":6236.0, "saldo":80757.0, "tasa_externa":0.8227, "tasa_kubo":0.6509, "numero_pagos_otorgado":112.0, "numero_pagos_restante":44.0, "frecuencia_externa":"S", "avance":0.1027, "fecha_inicio":"2023-03-29", "tipo_deuda":"I", "ahorro_cuota_mensual":381.09089912038144, "ahorro_total":21341.09035074136, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":2000.0, "cuota":524.0, "saldo":581.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7095, "fecha_inicio":"2019-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":1105.0000000000007, "ahorro_total":-1105.0000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":7400.0, "cuota":370.0, "saldo":4802.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3511, "fecha_inicio":"2022-05-16", "tipo_deuda":"R", "ahorro_cuota_mensual":5172.0000000000055, "ahorro_total":-5172.0000000000055, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":44200.0, "cuota":3016.0, "saldo":35838.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1892, "fecha_inicio":"2022-12-05", "tipo_deuda":"I", "ahorro_cuota_mensual":-21191.015201068985, "ahorro_total":-42382.03040213797, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":25000.0, "cuota":1732.0, "saldo":22910.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0836, "fecha_inicio":"2023-07-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-11959.75067933766, "ahorro_total":-23919.50135867532, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":17400.0, "cuota":1450.0, "saldo":7150.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5891, "fecha_inicio":"2023-06-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-658.7764704580554, "ahorro_total":-7905.317645496665, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 4445474, "monto_maximo_cliente": 275400.0, "cuota_externa_total": 14552.0, "capacidad_maxima_pago": 282978.0, "bursolnum": 7316097, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7865.90822866068, "monto_max": 275400.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.7007, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":38311.0, "cuota":2494.0, "saldo":17125.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.553, "fecha_inicio":"2022-09-15", "tipo_deuda":"I", "ahorro_cuota_mensual":483.72017783295587, "ahorro_total":11609.28426799094, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":700.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-06-25", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":48300.0, "cuota":2576.0, "saldo":13481.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7209, "fecha_inicio":"2021-08-18", "tipo_deuda":"I", "ahorro_cuota_mensual":701.2818971462293, "ahorro_total":25246.148297264255, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":150000.0, "cuota":4101.0, "saldo":134521.0, "tasa_externa":0.2181, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":45.0, "frecuencia_externa":"M", "avance":0.1032, "fecha_inicio":"2023-01-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-144.82462352428502, "ahorro_total":-8689.477411457101, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":5000.0, "cuota":486.0, "saldo":1694.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":20.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6612, "fecha_inicio":"2022-09-15", "tipo_deuda":"I", "ahorro_cuota_mensual":182.18014049477893, "ahorro_total":3643.6028098955785, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":125400.0, "cuota":3430.0, "saldo":123799.0, "tasa_externa":0.2183, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":53.0, "frecuencia_externa":"M", "avance":0.0128, "fecha_inicio":"2023-09-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-119.50938526630262, "ahorro_total":-7170.563115978157, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":7500.0, "cuota":1.0, "saldo":6080.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1893, "fecha_inicio":"2006-07-31", "tipo_deuda":"R", "ahorro_cuota_mensual":6080.999999999988, "ahorro_total":-6080.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":5000.0, "cuota":339.0, "saldo":3969.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2062, "fecha_inicio":"1992-03-14", "tipo_deuda":"R", "ahorro_cuota_mensual":4307.999999999993, "ahorro_total":-4307.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":132100.0, "cuota":1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-05-02", "tipo_deuda":"R", "ahorro_cuota_mensual":1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":122200.0, "cuota":1465.0, "saldo":119578.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":52.0, "frecuencia_externa":"M", "avance":0.0215, "fecha_inicio":"2023-07-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-1993.9317932977842, "ahorro_total":-119635.90759786706, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
@@ -274,7 +277,7 @@
     <t>{"Prospecto": 4611310, "monto_maximo_cliente": 500000.0, "cuota_externa_total": 36961.0, "capacidad_maxima_pago": 514148.0, "bursolnum": 7316572, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 20721.45438704324, "monto_max": 500000.0, "cuota_min": 200.2991210698785, "monto_min": 5000, "plazo_max": 54.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0428, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":63000.0, "cuota":4923.0, "saldo":37119.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":24.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.4108, "fecha_inicio":"2022-11-22", "tipo_deuda":"I", "ahorro_cuota_mensual":1001.2811315986633, "ahorro_total":24030.747158367918, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":50000.0, "cuota":4042.0, "saldo":46237.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":24.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.0753, "fecha_inicio":"2023-08-10", "tipo_deuda":"I", "ahorro_cuota_mensual":929.5247076179867, "ahorro_total":22308.59298283168, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":203234.0, "cuota":4914.0, "saldo":168297.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":60.0, "numero_pagos_restante":44.0, "frecuencia_externa":"M", "avance":0.1719, "fecha_inicio":"2022-12-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-3227.518314303139, "ahorro_total":-193651.09885818834, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":1, "monto_otorgado":1283.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"1991-07-08", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":236500.0, "cuota":13694.0, "saldo":236500.0, "tasa_externa":0.343, "tasa_kubo":0.3617, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2022-10-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-1028.0081329669229, "ahorro_total":-24672.19519120615, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":40000.0, "cuota":1159.0, "saldo":38068.0, "tasa_externa":0.2469, "tasa_kubo":0.3617, "numero_pagos_otorgado":60.0, "numero_pagos_restante":49.0, "frecuencia_externa":"M", "avance":0.0483, "fecha_inicio":"2023-05-11", "tipo_deuda":"I", "ahorro_cuota_mensual":-443.3929685590281, "ahorro_total":-26603.578113541684, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":80000.0, "cuota":2540.0, "saldo":76437.0, "tasa_externa":0.2942, "tasa_kubo":0.3617, "numero_pagos_otorgado":60.0, "numero_pagos_restante":48.0, "frecuencia_externa":"M", "avance":0.0445, "fecha_inicio":"2023-04-14", "tipo_deuda":"I", "ahorro_cuota_mensual":-664.7859371180562, "ahorro_total":-39887.15622708337, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":80000.0, "cuota":2319.0, "saldo":76990.0, "tasa_externa":0.2472, "tasa_kubo":0.3617, "numero_pagos_otorgado":60.0, "numero_pagos_restante":50.0, "frecuencia_externa":"M", "avance":0.0376, "fecha_inicio":"2023-06-14", "tipo_deuda":"I", "ahorro_cuota_mensual":-885.7859371180562, "ahorro_total":-53147.15622708337, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":12620.0, "cuota":1166.0, "saldo":10644.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":12.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.1566, "fecha_inicio":"2023-12-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-139.69332329686017, "ahorro_total":-1676.319879562322, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":133100.0, "cuota":2000.0, "saldo":50990.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6169, "fecha_inicio":"2023-10-12", "tipo_deuda":"R", "ahorro_cuota_mensual":52989.999999999876, "ahorro_total":-52989.999999999876, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":70000.0, "cuota":2204.0, "saldo":65058.0, "tasa_externa":0.2898, "tasa_kubo":0.3617, "numero_pagos_otorgado":60.0, "numero_pagos_restante":46.0, "frecuencia_externa":"M", "avance":0.0706, "fecha_inicio":"2023-02-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-600.1876949782995, "ahorro_total":-36011.26169869797, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 4620988, "monto_maximo_cliente": 14700.0, "cuota_externa_total": 3041.0, "capacidad_maxima_pago": 21659.0, "bursolnum": 7317306, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 581.9022457361245, "monto_max": 14700.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":29000.0, "cuota":1935.0, "saldo":23980.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.1731, "fecha_inicio":"2022-11-24", "tipo_deuda":"I", "ahorro_cuota_mensual":809.3928574998065, "ahorro_total":29138.142869993033, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":3045.0, "cuota":-1.0, "saldo":327.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8926, "fecha_inicio":"2024-01-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":3745.0, "cuota":-1.0, "saldo":2520.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3271, "fecha_inicio":"2023-12-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":3274.0, "cuota":-1.0, "saldo":269.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9178, "fecha_inicio":"2023-11-23", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":3612.0, "cuota":-1.0, "saldo":109.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9698, "fecha_inicio":"2023-11-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":5000.0, "cuota":250.0, "saldo":2239.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5522, "fecha_inicio":"2022-01-20", "tipo_deuda":"R", "ahorro_cuota_mensual":2488.999999999996, "ahorro_total":-2488.999999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":5600.0, "cuota":6287.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-02-07", "tipo_deuda":"R", "ahorro_cuota_mensual":6287.0, "ahorro_total":-6287.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":1500.0, "cuota":142.0, "saldo":1411.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0593, "fecha_inicio":"2021-08-31", "tipo_deuda":"R", "ahorro_cuota_mensual":1552.9999999999973, "ahorro_total":-1552.9999999999973, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":14700.0, "cuota":909.0, "saldo":15159.0, "tasa_externa":0.4177, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":-0.0312, "fecha_inicio":"2023-12-08", "tipo_deuda":"I", "ahorro_cuota_mensual":137.65199587962866, "ahorro_total":3303.647901111088, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":7, "monto_otorgado":3950.0, "cuota":-1.0, "saldo":50.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9873, "fecha_inicio":"2023-10-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 4620988, "monto_maximo_cliente": 14700.0, "cuota_externa_total": 3041.0, "capacidad_maxima_pago": 21659.0, "bursolnum": 7317306, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 581.9022457361245, "monto_max": 14700.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":29000.0, "cuota":1935.0, "saldo":23980.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.1731, "fecha_inicio":"2022-11-24", "tipo_deuda":"I", "ahorro_cuota_mensual":809.3928574998065, "ahorro_total":29138.142869993033, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":3045.0, "cuota":-1.0, "saldo":327.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8926, "fecha_inicio":"2024-01-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":3745.0, "cuota":-1.0, "saldo":2520.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3271, "fecha_inicio":"2023-12-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":3274.0, "cuota":-1.0, "saldo":269.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9178, "fecha_inicio":"2023-11-23", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":3612.0, "cuota":-1.0, "saldo":109.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9698, "fecha_inicio":"2023-11-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":5000.0, "cuota":250.0, "saldo":2239.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5522, "fecha_inicio":"2022-01-20", "tipo_deuda":"R", "ahorro_cuota_mensual":2488.999999999996, "ahorro_total":-2488.999999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":5600.0, "cuota":6287.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-02-07", "tipo_deuda":"R", "ahorro_cuota_mensual":6287.0, "ahorro_total":-6287.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":1500.0, "cuota":142.0, "saldo":1411.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0593, "fecha_inicio":"2021-08-31", "tipo_deuda":"R", "ahorro_cuota_mensual":1552.9999999999973, "ahorro_total":-1552.9999999999973, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":14700.0, "cuota":909.0, "saldo":15159.0, "tasa_externa":0.4177, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":-0.0312, "fecha_inicio":"2023-12-08", "tipo_deuda":"I", "ahorro_cuota_mensual":137.65199587962866, "ahorro_total":3303.647901111088, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":7, "monto_otorgado":3950.0, "cuota":-1.0, "saldo":50.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9873, "fecha_inicio":"2023-10-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 4648381, "monto_maximo_cliente": 36000.0, "cuota_externa_total": 7631.0, "capacidad_maxima_pago": 38369.0, "bursolnum": 7317407, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1172.846385466592, "monto_max": 36000.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.6722, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":70000.0, "cuota":3500.0, "saldo":32430.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5367, "fecha_inicio":"2012-01-01", "tipo_deuda":"R", "ahorro_cuota_mensual":35929.99999999994, "ahorro_total":-35929.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":36000.0, "cuota":1722.0, "saldo":6487.0, "tasa_externa":0.4007, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8198, "fecha_inicio":"2021-06-29", "tipo_deuda":"I", "ahorro_cuota_mensual":324.6945817238975, "ahorro_total":11689.00494206031, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":9750.0, "cuota":488.0, "saldo":1180.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.879, "fecha_inicio":"2010-01-03", "tipo_deuda":"R", "ahorro_cuota_mensual":1667.9999999999977, "ahorro_total":-1667.9999999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":33000.0, "cuota":2256.0, "saldo":29552.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.1045, "fecha_inicio":"2023-01-05", "tipo_deuda":"I", "ahorro_cuota_mensual":975.1366999135728, "ahorro_total":35104.92119688862, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":5, "monto_otorgado":150988.0, "cuota":1043.0, "saldo":181845.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":360.0, "numero_pagos_restante":269.0, "frecuencia_externa":"M", "avance":-0.2044, "fecha_inicio":"2016-08-29", "tipo_deuda":"M", "ahorro_cuota_mensual":-2476.2394995790823, "ahorro_total":-891446.2198484696, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
@@ -292,7 +295,7 @@
     <t>{"Prospecto": 4682600, "monto_maximo_cliente": 130000.0, "cuota_externa_total": 25531.0, "capacidad_maxima_pago": 123841.0, "bursolnum": 7316245, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 9424.495741759796, "monto_max": 130000.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.6722, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":14, "monto_otorgado":55000.0, "cuota":2750.0, "saldo":19894.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6383, "fecha_inicio":"2019-06-05", "tipo_deuda":"R", "ahorro_cuota_mensual":22644.000000000022, "ahorro_total":-22644.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":12, "monto_otorgado":999.0, "cuota":374.0, "saldo":374.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":899.0, "frecuencia_externa":"M", "avance":0.6256, "fecha_inicio":"2015-11-13", "tipo_deuda":"R", "ahorro_cuota_mensual":349.6977293333333, "ahorro_total":349697.7293333333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":686.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-05-30", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":16800.0, "cuota":1552.0, "saldo":6533.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6111, "fecha_inicio":"2022-12-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-58.11245803984184, "ahorro_total":-1046.0242447171531, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":36800.0, "cuota":2980.0, "saldo":32041.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":25.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1293, "fecha_inicio":"2023-06-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-36.34167434656683, "ahorro_total":-908.5418586641708, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":13000.0, "cuota":650.0, "saldo":4973.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6175, "fecha_inicio":"2022-09-10", "tipo_deuda":"R", "ahorro_cuota_mensual":5623.000000000006, "ahorro_total":-5623.000000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":22700.0, "cuota":1135.0, "saldo":10867.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5213, "fecha_inicio":"2023-06-08", "tipo_deuda":"R", "ahorro_cuota_mensual":12002.000000000013, "ahorro_total":-12002.000000000013, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":-1.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-1.0, "fecha_inicio":"2019-05-11", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":74500.0, "cuota":3725.0, "saldo":36573.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5091, "fecha_inicio":"2018-11-08", "tipo_deuda":"R", "ahorro_cuota_mensual":40298.000000000044, "ahorro_total":-40298.000000000044, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":130000.0, "cuota":14620.0, "saldo":129566.0, "tasa_externa":1.3394, "tasa_kubo":0.6722, "numero_pagos_otorgado":72.0, "numero_pagos_restante":9.0, "frecuencia_externa":"S", "avance":0.0033, "fecha_inicio":"2022-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":5195.504258240204, "ahorro_total":187038.15329664733, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":38000.0, "cuota":1857.0, "saldo":14121.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6284, "fecha_inicio":"2018-12-11", "tipo_deuda":"R", "ahorro_cuota_mensual":15978.000000000018, "ahorro_total":-15978.000000000018, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":8780.0, "cuota":989.0, "saldo":6462.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.264, "fecha_inicio":"2022-05-06", "tipo_deuda":"R", "ahorro_cuota_mensual":7451.000000000007, "ahorro_total":-7451.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":11100.0, "cuota":672.0, "saldo":10153.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0853, "fecha_inicio":"2023-04-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-871.912730530313, "ahorro_total":-8719.12730530313, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":4100.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-12-11", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 4691173, "monto_maximo_cliente": 18000.0, "cuota_externa_total": 10602.0, "capacidad_maxima_pago": 27010.5, "bursolnum": 7317221, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 712.5333621258668, "monto_max": 18000.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.5391, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":2500.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2024-01-20", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":39000.0, "cuota":2233.0, "saldo":33234.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.1478, "fecha_inicio":"2023-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":719.2524635342222, "ahorro_total":25893.088687232, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":7150.0, "cuota":-1.0, "saldo":98.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9863, "fecha_inicio":"2021-04-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":10000.0, "cuota":1425.0, "saldo":10389.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0389, "fecha_inicio":"2024-01-05", "tipo_deuda":"I", "ahorro_cuota_mensual":203.7405547651083, "ahorro_total":1833.6649928859747, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":2557.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-05-11", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":51000.0, "cuota":2990.0, "saldo":21785.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5728, "fecha_inicio":"2021-03-16", "tipo_deuda":"R", "ahorro_cuota_mensual":24774.99999999996, "ahorro_total":-24774.99999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":7150.0, "cuota":97.0, "saldo":98.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9863, "fecha_inicio":"2021-04-16", "tipo_deuda":"R", "ahorro_cuota_mensual":194.9999999999998, "ahorro_total":-194.9999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":20000.0, "cuota":0.0, "saldo":149.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9926, "fecha_inicio":"2023-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":148.99999999999972, "ahorro_total":-148.99999999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":57350.0, "cuota":4559.0, "saldo":30880.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4616, "fecha_inicio":"2017-09-15", "tipo_deuda":"R", "ahorro_cuota_mensual":35438.99999999994, "ahorro_total":-35438.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":6500.0, "cuota":149.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-03-28", "tipo_deuda":"R", "ahorro_cuota_mensual":149.0, "ahorro_total":-149.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":21800.0, "cuota":1312.0, "saldo":17853.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1811, "fecha_inicio":"2022-07-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-1106.4607963202552, "ahorro_total":-11064.607963202552, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":39000.0, "cuota":1950.0, "saldo":3040.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9221, "fecha_inicio":"2022-09-30", "tipo_deuda":"R", "ahorro_cuota_mensual":4989.9999999999945, "ahorro_total":-4989.9999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":18000.0, "cuota":1096.0, "saldo":16159.0, "tasa_externa":0.3999, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.1023, "fecha_inicio":"2023-11-10", "tipo_deuda":"I", "ahorro_cuota_mensual":151.49223985260642, "ahorro_total":3635.813756462554, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":7, "monto_otorgado":18700.0, "cuota":1176.0, "saldo":18233.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.025, "fecha_inicio":"2023-11-07", "tipo_deuda":"I", "ahorro_cuota_mensual":450.17746328435794, "ahorro_total":16206.388678236886, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 4691173, "monto_maximo_cliente": 18000.0, "cuota_externa_total": 10602.0, "capacidad_maxima_pago": 27010.5, "bursolnum": 7317221, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 712.5333621258668, "monto_max": 18000.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.5391, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":2500.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2024-01-20", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":39000.0, "cuota":2233.0, "saldo":33234.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.1478, "fecha_inicio":"2023-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":719.2524635342222, "ahorro_total":25893.088687232, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":7150.0, "cuota":-1.0, "saldo":98.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9863, "fecha_inicio":"2021-04-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":10000.0, "cuota":1425.0, "saldo":10389.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0389, "fecha_inicio":"2024-01-05", "tipo_deuda":"I", "ahorro_cuota_mensual":203.7405547651083, "ahorro_total":1833.6649928859747, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":2557.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-05-11", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":51000.0, "cuota":2990.0, "saldo":21785.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5728, "fecha_inicio":"2021-03-16", "tipo_deuda":"R", "ahorro_cuota_mensual":24774.99999999996, "ahorro_total":-24774.99999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":7150.0, "cuota":97.0, "saldo":98.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9863, "fecha_inicio":"2021-04-16", "tipo_deuda":"R", "ahorro_cuota_mensual":194.9999999999998, "ahorro_total":-194.9999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":20000.0, "cuota":0.0, "saldo":149.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9926, "fecha_inicio":"2023-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":148.99999999999972, "ahorro_total":-148.99999999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":57350.0, "cuota":4559.0, "saldo":30880.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4616, "fecha_inicio":"2017-09-15", "tipo_deuda":"R", "ahorro_cuota_mensual":35438.99999999994, "ahorro_total":-35438.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":6500.0, "cuota":149.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-03-28", "tipo_deuda":"R", "ahorro_cuota_mensual":149.0, "ahorro_total":-149.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":21800.0, "cuota":1312.0, "saldo":17853.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1811, "fecha_inicio":"2022-07-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-1106.4607963202552, "ahorro_total":-11064.607963202552, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":39000.0, "cuota":1950.0, "saldo":3040.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9221, "fecha_inicio":"2022-09-30", "tipo_deuda":"R", "ahorro_cuota_mensual":4989.9999999999945, "ahorro_total":-4989.9999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":18000.0, "cuota":1096.0, "saldo":16159.0, "tasa_externa":0.3999, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.1023, "fecha_inicio":"2023-11-10", "tipo_deuda":"I", "ahorro_cuota_mensual":151.49223985260642, "ahorro_total":3635.813756462554, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":7, "monto_otorgado":18700.0, "cuota":1176.0, "saldo":18233.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.025, "fecha_inicio":"2023-11-07", "tipo_deuda":"I", "ahorro_cuota_mensual":450.17746328435794, "ahorro_total":16206.388678236886, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 4721165, "monto_maximo_cliente": 199100.0, "cuota_externa_total": 15160.0, "capacidad_maxima_pago": 201940.0, "bursolnum": 7317408, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 6959.836284108579, "monto_max": 199100.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6722, "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":14, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-07-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":33000.0, "cuota":2256.0, "saldo":28974.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.122, "fecha_inicio":"2023-01-17", "tipo_deuda":"I", "ahorro_cuota_mensual":785.492863766716, "ahorro_total":28277.743095601778, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":15, "monto_otorgado":30000.0, "cuota":1500.0, "saldo":4619.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.846, "fecha_inicio":"2022-02-26", "tipo_deuda":"R", "ahorro_cuota_mensual":6118.999999999987, "ahorro_total":-6118.999999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":36500.0, "cuota":1825.0, "saldo":15412.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5778, "fecha_inicio":"2021-10-29", "tipo_deuda":"R", "ahorro_cuota_mensual":17236.999999999956, "ahorro_total":-17236.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":55000.0, "cuota":9795.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-10-01", "tipo_deuda":"R", "ahorro_cuota_mensual":9795.0, "ahorro_total":-9795.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":10, "monto_otorgado":41900.0, "cuota":2095.0, "saldo":7533.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8202, "fecha_inicio":"2023-03-07", "tipo_deuda":"R", "ahorro_cuota_mensual":9627.999999999978, "ahorro_total":-9627.999999999978, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":174077.0, "cuota":4500.0, "saldo":58342.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6648, "fecha_inicio":"2021-08-19", "tipo_deuda":"R", "ahorro_cuota_mensual":62841.99999999984, "ahorro_total":-62841.99999999984, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":15000.0, "cuota":3572.0, "saldo":1255.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9163, "fecha_inicio":"2021-01-21", "tipo_deuda":"R", "ahorro_cuota_mensual":4826.999999999996, "ahorro_total":-4826.999999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":8900.0, "cuota":445.0, "saldo":4702.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4717, "fecha_inicio":"2021-10-08", "tipo_deuda":"R", "ahorro_cuota_mensual":5146.999999999987, "ahorro_total":-5146.999999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":41300.0, "cuota":4288.0, "saldo":32070.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2235, "fecha_inicio":"2021-04-26", "tipo_deuda":"R", "ahorro_cuota_mensual":36357.99999999991, "ahorro_total":-36357.99999999991, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":21900.0, "cuota":1768.0, "saldo":17566.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1979, "fecha_inicio":"2022-01-17", "tipo_deuda":"I", "ahorro_cuota_mensual":-775.4111452566885, "ahorro_total":-7754.111452566885, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":90000.0, "cuota":4500.0, "saldo":75272.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":900.0, "numero_pagos_restante":880.0, "frecuencia_externa":"Z", "avance":0.1636, "fecha_inicio":"2022-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":2379.6881226372584, "ahorro_total":2141719.3103735326, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":150000.0, "cuota":6202.0, "saldo":145872.0, "tasa_externa":0.3942, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":44.0, "frecuencia_externa":"M", "avance":0.0275, "fecha_inicio":"2023-12-18", "tipo_deuda":"I", "ahorro_cuota_mensual":464.38670159701996, "ahorro_total":22290.56167665696, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":49100.0, "cuota":1711.0, "saldo":45458.0, "tasa_externa":0.3446, "tasa_kubo":0.2914, "numero_pagos_otorgado":60.0, "numero_pagos_restante":48.0, "frecuencia_externa":"M", "avance":0.0742, "fecha_inicio":"2023-04-17", "tipo_deuda":"I", "ahorro_cuota_mensual":5.8934206427802565, "ahorro_total":353.6052385668154, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":50000.0, "cuota":0.0, "saldo":3168.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9366, "fecha_inicio":"2024-01-21", "tipo_deuda":"R", "ahorro_cuota_mensual":3167.9999999999914, "ahorro_total":-3167.9999999999914, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
@@ -304,7 +307,7 @@
     <t>{"Prospecto": 4733030, "monto_maximo_cliente": 27500.0, "cuota_externa_total": 6966.0, "capacidad_maxima_pago": 27164.0, "bursolnum": 7316674, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1993.6433299876494, "monto_max": 27500.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.6722, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":10700.0, "cuota":535.0, "saldo":8883.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1698, "fecha_inicio":"2022-09-02", "tipo_deuda":"R", "ahorro_cuota_mensual":9418.000000000011, "ahorro_total":-9418.000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":27500.0, "cuota":3120.0, "saldo":27363.0, "tasa_externa":1.3523, "tasa_kubo":0.6722, "numero_pagos_otorgado":72.0, "numero_pagos_restante":26.0, "frecuencia_externa":"S", "avance":0.005, "fecha_inicio":"2023-06-08", "tipo_deuda":"I", "ahorro_cuota_mensual":1126.3566700123506, "ahorro_total":40548.84012044462, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":22000.0, "cuota":1744.0, "saldo":5456.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.752, "fecha_inicio":"2021-12-24", "tipo_deuda":"R", "ahorro_cuota_mensual":7200.000000000006, "ahorro_total":-7200.000000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":15000.0, "cuota":1732.0, "saldo":11135.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":13.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2577, "fecha_inicio":"2023-08-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-12.030941924668241, "ahorro_total":-156.40224502068713, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 4766643, "monto_maximo_cliente": 52500.0, "cuota_externa_total": 22700.0, "capacidad_maxima_pago": 55411.0, "bursolnum": 7317472, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2339.4431712802248, "monto_max": 52500.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.2914, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":15000.0, "cuota":1026.0, "saldo":12942.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.1372, "fecha_inicio":"2023-01-27", "tipo_deuda":"I", "ahorro_cuota_mensual":357.58766534850724, "ahorro_total":12873.155952546262, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":8, "monto_otorgado":321816.0, "cuota":3814.0, "saldo":277712.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":360.0, "numero_pagos_restante":345.0, "frecuencia_externa":"M", "avance":0.137, "fecha_inicio":"2023-01-02", "tipo_deuda":"M", "ahorro_cuota_mensual":-4009.131741815442, "ahorro_total":-1443287.427053559, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":35000.0, "cuota":2498.0, "saldo":35402.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":-0.0115, "fecha_inicio":"2023-10-11", "tipo_deuda":"I", "ahorro_cuota_mensual":938.371219146517, "ahorro_total":33781.36388927461, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":170900.0, "cuota":4204.0, "saldo":137460.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":60.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.1957, "fecha_inicio":"2022-09-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-1730.8821672535405, "ahorro_total":-103852.93003521243, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":801.0, "cuota":327.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-12-23", "tipo_deuda":"O", "ahorro_cuota_mensual":327.0, "ahorro_total":-327.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":13500.0, "cuota":675.0, "saldo":5018.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6283, "fecha_inicio":"2021-08-20", "tipo_deuda":"R", "ahorro_cuota_mensual":5692.999999999986, "ahorro_total":-5692.999999999986, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":14000.0, "cuota":995.0, "saldo":8592.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3863, "fecha_inicio":"2021-08-20", "tipo_deuda":"R", "ahorro_cuota_mensual":9586.999999999976, "ahorro_total":-9586.999999999976, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":57231.0, "cuota":1408.0, "saldo":46033.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":60.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.1957, "fecha_inicio":"2022-09-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-579.4736179876381, "ahorro_total":-34768.41707925829, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":10000.0, "cuota":22.0, "saldo":9208.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0792, "fecha_inicio":"2022-01-21", "tipo_deuda":"R", "ahorro_cuota_mensual":9229.999999999975, "ahorro_total":-9229.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":52500.0, "cuota":5006.0, "saldo":50113.0, "tasa_externa":1.1139, "tasa_kubo":0.2914, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0455, "fecha_inicio":"2013-04-16", "tipo_deuda":"I", "ahorro_cuota_mensual":2666.5568287197752, "ahorro_total":95996.0458339119, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":8800.0, "cuota":3017.0, "saldo":9051.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0285, "fecha_inicio":"2023-12-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 4766643, "monto_maximo_cliente": 52500.0, "cuota_externa_total": 22700.0, "capacidad_maxima_pago": 55411.0, "bursolnum": 7317472, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2339.4431712802248, "monto_max": 52500.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.2914, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":15000.0, "cuota":1026.0, "saldo":12942.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.1372, "fecha_inicio":"2023-01-27", "tipo_deuda":"I", "ahorro_cuota_mensual":357.58766534850724, "ahorro_total":12873.155952546262, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":8, "monto_otorgado":321816.0, "cuota":3814.0, "saldo":277712.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":360.0, "numero_pagos_restante":345.0, "frecuencia_externa":"M", "avance":0.137, "fecha_inicio":"2023-01-02", "tipo_deuda":"M", "ahorro_cuota_mensual":-4009.131741815442, "ahorro_total":-1443287.427053559, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":35000.0, "cuota":2498.0, "saldo":35402.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":-0.0115, "fecha_inicio":"2023-10-11", "tipo_deuda":"I", "ahorro_cuota_mensual":938.371219146517, "ahorro_total":33781.36388927461, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":170900.0, "cuota":4204.0, "saldo":137460.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":60.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.1957, "fecha_inicio":"2022-09-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-1730.8821672535405, "ahorro_total":-103852.93003521243, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":801.0, "cuota":327.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-12-23", "tipo_deuda":"O", "ahorro_cuota_mensual":327.0, "ahorro_total":-327.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":13500.0, "cuota":675.0, "saldo":5018.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6283, "fecha_inicio":"2021-08-20", "tipo_deuda":"R", "ahorro_cuota_mensual":5692.999999999986, "ahorro_total":-5692.999999999986, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":14000.0, "cuota":995.0, "saldo":8592.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3863, "fecha_inicio":"2021-08-20", "tipo_deuda":"R", "ahorro_cuota_mensual":9586.999999999976, "ahorro_total":-9586.999999999976, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":57231.0, "cuota":1408.0, "saldo":46033.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":60.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.1957, "fecha_inicio":"2022-09-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-579.4736179876381, "ahorro_total":-34768.41707925829, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":10000.0, "cuota":22.0, "saldo":9208.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0792, "fecha_inicio":"2022-01-21", "tipo_deuda":"R", "ahorro_cuota_mensual":9229.999999999975, "ahorro_total":-9229.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":52500.0, "cuota":5006.0, "saldo":50113.0, "tasa_externa":1.1139, "tasa_kubo":0.2914, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0455, "fecha_inicio":"2013-04-16", "tipo_deuda":"I", "ahorro_cuota_mensual":2666.5568287197752, "ahorro_total":95996.0458339119, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":8800.0, "cuota":3017.0, "saldo":9051.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0285, "fecha_inicio":"2023-12-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 4767970, "monto_maximo_cliente": 50136.0, "cuota_externa_total": 8262.0, "capacidad_maxima_pago": 51439.0, "bursolnum": 7317400, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2442.556728911599, "monto_max": 50136.0, "cuota_min": 227.39637225020516, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.5991, "comision": 0.0439, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "HIPOTECAGOBIERNO", "registro":6, "monto_otorgado":181296.0, "cuota":1146.0, "saldo":103539.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":360.0, "numero_pagos_restante":276.0, "frecuencia_externa":"M", "avance":0.4289, "fecha_inicio":"2017-04-21", "tipo_deuda":"M", "ahorro_cuota_mensual":-3152.7685910880573, "ahorro_total":-1134996.6927917006, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":953.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-05-08", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":10, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2017-08-18", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":782.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2006-02-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":48000.0, "cuota":3008.0, "saldo":42106.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":36.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.1228, "fecha_inicio":"2023-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":415.79883213376934, "ahorro_total":14968.757956815696, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":50136.0, "cuota":2962.0, "saldo":50136.0, "tasa_externa":0.587, "tasa_kubo":0.4295, "numero_pagos_otorgado":36.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2023-09-28", "tipo_deuda":"I", "ahorro_cuota_mensual":254.445880163722, "ahorro_total":9160.051685893992, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":50000.0, "cuota":602.0, "saldo":43118.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":36.0, "numero_pagos_restante":26.0, "frecuencia_externa":"M", "avance":0.1376, "fecha_inicio":"2023-05-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-2098.209549860657, "ahorro_total":-75535.54379498365, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":5700.0, "cuota":544.0, "saldo":5449.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.044, "fecha_inicio":"2010-05-27", "tipo_deuda":"R", "ahorro_cuota_mensual":5992.999999999996, "ahorro_total":-5992.999999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":78600.0, "cuota":1198.0, "saldo":27905.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.645, "fecha_inicio":"2017-07-18", "tipo_deuda":"R", "ahorro_cuota_mensual":29102.999999999985, "ahorro_total":-29102.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":6000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-09-01", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
@@ -322,7 +325,7 @@
     <t>{"Prospecto": 4881018, "monto_maximo_cliente": 77000.0, "cuota_externa_total": 7115.0, "capacidad_maxima_pago": 79370.0, "bursolnum": 7317459, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2199.255387098302, "monto_max": 77000.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.2, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":36494.0, "cuota":1028.0, "saldo":27499.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":142.0, "numero_pagos_restante":26.0, "frecuencia_externa":"W", "avance":0.2465, "fecha_inicio":"2023-06-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-388.4795537380023, "ahorro_total":-13985.263934568084, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":2840.0, "cuota":80.0, "saldo":2140.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":142.0, "numero_pagos_restante":26.0, "frecuencia_externa":"W", "avance":0.2465, "fecha_inicio":"2023-06-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-30.23187188622586, "ahorro_total":-1088.347387904131, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":17000.0, "cuota":850.0, "saldo":2184.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8715, "fecha_inicio":"2023-08-28", "tipo_deuda":"R", "ahorro_cuota_mensual":3033.999999999996, "ahorro_total":-3033.999999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":4, "monto_otorgado":21200.0, "cuota":1462.0, "saldo":20945.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":48.0, "numero_pagos_restante":43.0, "frecuencia_externa":"M", "avance":0.012, "fecha_inicio":"2023-10-23", "tipo_deuda":"I", "ahorro_cuota_mensual":780.1836616007942, "ahorro_total":37448.81575683812, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":4000.0, "cuota":250.0, "saldo":1631.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5922, "fecha_inicio":"2021-12-21", "tipo_deuda":"R", "ahorro_cuota_mensual":1880.999999999997, "ahorro_total":-1880.999999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":77000.0, "cuota":2106.0, "saldo":77621.0, "tasa_externa":0.2183, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":57.0, "frecuencia_externa":"M", "avance":-0.0081, "fecha_inicio":"2024-01-17", "tipo_deuda":"I", "ahorro_cuota_mensual":-73.5233067424665, "ahorro_total":-4411.39840454799, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":22000.0, "cuota":1939.0, "saldo":19930.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":30.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.0941, "fecha_inicio":"2023-03-14", "tipo_deuda":"I", "ahorro_cuota_mensual":965.68327673236, "ahorro_total":28970.4983019708, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 4884745, "monto_maximo_cliente": 28112.0, "cuota_externa_total": 21663.0, "capacidad_maxima_pago": 25073.0, "bursolnum": 7317557, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1405.0673550598951, "monto_max": 28112.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.046, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":70000.0, "cuota":4826.0, "saldo":63945.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":36.0, "numero_pagos_restante":23.0, "frecuencia_externa":"M", "avance":0.0865, "fecha_inicio":"2023-03-17", "tipo_deuda":"I", "ahorro_cuota_mensual":780.0338822209287, "ahorro_total":28081.219759953434, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":30, "monto_otorgado":21609.0, "cuota":6455.0, "saldo":6455.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7013, "fecha_inicio":"2011-12-04", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":1650.0, "cuota":620.0, "saldo":1197.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2745, "fecha_inicio":"2020-10-29", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":35656.0, "cuota":1783.0, "saldo":32821.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0795, "fecha_inicio":"2016-08-03", "tipo_deuda":"R", "ahorro_cuota_mensual":34604.00000000007, "ahorro_total":-34604.00000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":3500.0, "cuota":25.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-03-08", "tipo_deuda":"R", "ahorro_cuota_mensual":25.0, "ahorro_total":-25.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":10, "monto_otorgado":35000.0, "cuota":500.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-01-26", "tipo_deuda":"R", "ahorro_cuota_mensual":500.0, "ahorro_total":-500.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":3900.0, "cuota":3128.0, "saldo":3128.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1979, "fecha_inicio":"2020-09-23", "tipo_deuda":"R", "ahorro_cuota_mensual":6256.000000000007, "ahorro_total":-6256.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":1650.0, "cuota":620.0, "saldo":1197.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2745, "fecha_inicio":"2020-10-29", "tipo_deuda":"R", "ahorro_cuota_mensual":1817.0000000000025, "ahorro_total":-1817.0000000000025, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":6400.0, "cuota":407.0, "saldo":3263.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4902, "fecha_inicio":"2021-12-23", "tipo_deuda":"R", "ahorro_cuota_mensual":3670.000000000007, "ahorro_total":-3670.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":2071.0, "cuota":959.0, "saldo":959.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5369, "fecha_inicio":"2018-08-27", "tipo_deuda":"O", "ahorro_cuota_mensual":1918.000000000002, "ahorro_total":-1918.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":3000.0, "cuota":264.0, "saldo":2633.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1223, "fecha_inicio":"2020-09-11", "tipo_deuda":"R", "ahorro_cuota_mensual":2897.0000000000055, "ahorro_total":-2897.0000000000055, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":47700.0, "cuota":621.0, "saldo":1569.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":49.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.9671, "fecha_inicio":"2020-02-06", "tipo_deuda":"R", "ahorro_cuota_mensual":539.1267691419298, "ahorro_total":26417.21168795456, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":28112.0, "cuota":1950.0, "saldo":22468.0, "tasa_externa":0.8298, "tasa_kubo":0.4818, "numero_pagos_otorgado":122.0, "numero_pagos_restante":37.0, "frecuencia_externa":"S", "avance":0.2008, "fecha_inicio":"2022-03-23", "tipo_deuda":"I", "ahorro_cuota_mensual":553.8207180282427, "ahorro_total":33783.063799722804, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":6600.0, "cuota":570.0, "saldo":6682.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0124, "fecha_inicio":"2008-02-01", "tipo_deuda":"R", "ahorro_cuota_mensual":7252.000000000014, "ahorro_total":-7252.000000000014, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 4884745, "monto_maximo_cliente": 28112.0, "cuota_externa_total": 21663.0, "capacidad_maxima_pago": 25073.0, "bursolnum": 7317557, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1405.0673550598951, "monto_max": 28112.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.046, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":70000.0, "cuota":4826.0, "saldo":63945.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":36.0, "numero_pagos_restante":23.0, "frecuencia_externa":"M", "avance":0.0865, "fecha_inicio":"2023-03-17", "tipo_deuda":"I", "ahorro_cuota_mensual":780.0338822209287, "ahorro_total":28081.219759953434, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":30, "monto_otorgado":21609.0, "cuota":6455.0, "saldo":6455.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7013, "fecha_inicio":"2011-12-04", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":1650.0, "cuota":620.0, "saldo":1197.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2745, "fecha_inicio":"2020-10-29", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":35656.0, "cuota":1783.0, "saldo":32821.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0795, "fecha_inicio":"2016-08-03", "tipo_deuda":"R", "ahorro_cuota_mensual":34604.00000000007, "ahorro_total":-34604.00000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":3500.0, "cuota":25.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-03-08", "tipo_deuda":"R", "ahorro_cuota_mensual":25.0, "ahorro_total":-25.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":10, "monto_otorgado":35000.0, "cuota":500.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-01-26", "tipo_deuda":"R", "ahorro_cuota_mensual":500.0, "ahorro_total":-500.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":3900.0, "cuota":3128.0, "saldo":3128.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1979, "fecha_inicio":"2020-09-23", "tipo_deuda":"R", "ahorro_cuota_mensual":6256.000000000007, "ahorro_total":-6256.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":1650.0, "cuota":620.0, "saldo":1197.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2745, "fecha_inicio":"2020-10-29", "tipo_deuda":"R", "ahorro_cuota_mensual":1817.0000000000025, "ahorro_total":-1817.0000000000025, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":6400.0, "cuota":407.0, "saldo":3263.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4902, "fecha_inicio":"2021-12-23", "tipo_deuda":"R", "ahorro_cuota_mensual":3670.000000000007, "ahorro_total":-3670.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":2071.0, "cuota":959.0, "saldo":959.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5369, "fecha_inicio":"2018-08-27", "tipo_deuda":"O", "ahorro_cuota_mensual":1918.000000000002, "ahorro_total":-1918.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":3000.0, "cuota":264.0, "saldo":2633.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1223, "fecha_inicio":"2020-09-11", "tipo_deuda":"R", "ahorro_cuota_mensual":2897.0000000000055, "ahorro_total":-2897.0000000000055, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":47700.0, "cuota":621.0, "saldo":1569.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":49.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.9671, "fecha_inicio":"2020-02-06", "tipo_deuda":"R", "ahorro_cuota_mensual":539.1267691419298, "ahorro_total":26417.21168795456, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":28112.0, "cuota":1950.0, "saldo":22468.0, "tasa_externa":0.8298, "tasa_kubo":0.4818, "numero_pagos_otorgado":122.0, "numero_pagos_restante":37.0, "frecuencia_externa":"S", "avance":0.2008, "fecha_inicio":"2022-03-23", "tipo_deuda":"I", "ahorro_cuota_mensual":553.8207180282427, "ahorro_total":33783.063799722804, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":6600.0, "cuota":570.0, "saldo":6682.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0124, "fecha_inicio":"2008-02-01", "tipo_deuda":"R", "ahorro_cuota_mensual":7252.000000000014, "ahorro_total":-7252.000000000014, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 4907839, "monto_maximo_cliente": 40600.0, "cuota_externa_total": 3248.0, "capacidad_maxima_pago": 47352.0, "bursolnum": 7317596, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1568.7974207807197, "monto_max": 40600.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.6193, "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":17000.0, "cuota":1142.0, "saldo":15096.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.112, "fecha_inicio":"2023-03-31", "tipo_deuda":"I", "ahorro_cuota_mensual":384.4660207283083, "ahorro_total":13840.776746219099, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":6630.0, "cuota":3653.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":3653.0, "ahorro_total":-3653.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":3240.0, "cuota":154.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-03-17", "tipo_deuda":"R", "ahorro_cuota_mensual":154.0, "ahorro_total":-154.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":1, "monto_otorgado":40600.0, "cuota":2106.0, "saldo":37036.0, "tasa_externa":0.4678, "tasa_kubo":0.2914, "numero_pagos_otorgado":71.0, "numero_pagos_restante":27.0, "frecuencia_externa":"S", "avance":0.0878, "fecha_inicio":"2023-07-20", "tipo_deuda":"I", "ahorro_cuota_mensual":296.83061420995955, "ahorro_total":10685.902111558544, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
@@ -358,7 +361,7 @@
     <t>{"Prospecto": 5104626, "monto_maximo_cliente": 41200.0, "cuota_externa_total": 4256.0, "capacidad_maxima_pago": 51444.0, "bursolnum": 7317766, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2292.1517075495476, "monto_max": 41200.0, "cuota_min": 232.85304854502846, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0444, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":9300.0, "cuota":648.0, "saldo":8930.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":36.0, "numero_pagos_restante":26.0, "frecuencia_externa":"M", "avance":0.0398, "fecha_inicio":"2023-06-14", "tipo_deuda":"I", "ahorro_cuota_mensual":136.88561864211812, "ahorro_total":4927.882271116252, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":1548.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-12-26", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":20000.0, "cuota":1000.0, "saldo":5872.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7064, "fecha_inicio":"2023-04-28", "tipo_deuda":"R", "ahorro_cuota_mensual":6871.999999999989, "ahorro_total":-6871.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":17200.0, "cuota":860.0, "saldo":7939.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5384, "fecha_inicio":"2022-03-14", "tipo_deuda":"R", "ahorro_cuota_mensual":8798.999999999985, "ahorro_total":-8798.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":41200.0, "cuota":2816.0, "saldo":5281.0, "tasa_externa":0.5362, "tasa_kubo":0.4428, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8718, "fecha_inicio":"2022-03-28", "tipo_deuda":"I", "ahorro_cuota_mensual":35.69190208118107, "ahorro_total":856.6056499483457, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":19340.0, "cuota":967.0, "saldo":9309.0, "tasa_externa":-1.0, "tasa_kubo":0.4428, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5187, "fecha_inicio":"2022-11-02", "tipo_deuda":"R", "ahorro_cuota_mensual":10275.999999999982, "ahorro_total":-10275.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 5109565, "monto_maximo_cliente": 96000.0, "cuota_externa_total": 12391.0, "capacidad_maxima_pago": 98586.0, "bursolnum": 7317411, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4012.674951101334, "monto_max": 96000.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.8317, "comision": 0.0433, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":10900.0, "cuota":545.0, "saldo":5974.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":4.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4519, "fecha_inicio":"2023-09-07", "tipo_deuda":"R", "ahorro_cuota_mensual":-1088.61205199581, "ahorro_total":-4354.44820798324, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":15100.0, "cuota":1132.0, "saldo":14547.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0366, "fecha_inicio":"2023-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-700.697585391687, "ahorro_total":-7006.97585391687, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":96000.0, "cuota":4881.0, "saldo":79736.0, "tasa_externa":0.5423, "tasa_kubo":0.3813, "numero_pagos_otorgado":48.0, "numero_pagos_restante":29.0, "frecuencia_externa":"M", "avance":0.1694, "fecha_inicio":"2022-09-20", "tipo_deuda":"I", "ahorro_cuota_mensual":586.870796141563, "ahorro_total":28169.798214795024, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":7100.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2024-01-02", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":25600.0, "cuota":1280.0, "saldo":7078.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7235, "fecha_inicio":"2023-10-05", "tipo_deuda":"R", "ahorro_cuota_mensual":8358.000000000015, "ahorro_total":-8358.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":3600.0, "cuota":284.0, "saldo":537.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8508, "fecha_inicio":"2023-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":821.0000000000011, "ahorro_total":-821.0000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":7, "monto_otorgado":45000.0, "cuota":1250.0, "saldo":9167.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7963, "fecha_inicio":"2021-07-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-1027.435900693842, "ahorro_total":-36987.69242497832, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":4835.0, "cuota":667.0, "saldo":1330.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7249, "fecha_inicio":"2023-10-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":4835.0, "cuota":270.0, "saldo":806.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8333, "fecha_inicio":"2023-11-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":19000.0, "cuota":950.0, "saldo":2988.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8427, "fecha_inicio":"2021-04-08", "tipo_deuda":"R", "ahorro_cuota_mensual":3938.0000000000064, "ahorro_total":-3938.0000000000064, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":19, "monto_otorgado":25700.0, "cuota":1285.0, "saldo":20428.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2051, "fecha_inicio":"2022-03-04", "tipo_deuda":"R", "ahorro_cuota_mensual":21713.000000000044, "ahorro_total":-21713.000000000044, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":20, "monto_otorgado":22600.0, "cuota":1390.0, "saldo":20166.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1077, "fecha_inicio":"2020-03-13", "tipo_deuda":"R", "ahorro_cuota_mensual":21556.000000000044, "ahorro_total":-21556.000000000044, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":15000.0, "cuota":1427.0, "saldo":13499.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":24.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.1001, "fecha_inicio":"2023-06-14", "tipo_deuda":"I", "ahorro_cuota_mensual":474.5786768790206, "ahorro_total":11389.888245096494, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":637.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-02-28", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+    <t>{"Prospecto": 5109565, "monto_maximo_cliente": 96000.0, "cuota_externa_total": 12391.0, "capacidad_maxima_pago": 98586.0, "bursolnum": 7317411, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4012.674951101334, "monto_max": 96000.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.8317, "comision": 0.0433, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":10900.0, "cuota":545.0, "saldo":5974.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":4.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4519, "fecha_inicio":"2023-09-07", "tipo_deuda":"R", "ahorro_cuota_mensual":-1088.61205199581, "ahorro_total":-4354.44820798324, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":15100.0, "cuota":1132.0, "saldo":14547.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0366, "fecha_inicio":"2023-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-700.697585391687, "ahorro_total":-7006.97585391687, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":96000.0, "cuota":4881.0, "saldo":79736.0, "tasa_externa":0.5423, "tasa_kubo":0.3813, "numero_pagos_otorgado":48.0, "numero_pagos_restante":29.0, "frecuencia_externa":"M", "avance":0.1694, "fecha_inicio":"2022-09-20", "tipo_deuda":"I", "ahorro_cuota_mensual":586.870796141563, "ahorro_total":28169.798214795024, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":7100.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2024-01-02", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":25600.0, "cuota":1280.0, "saldo":7078.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7235, "fecha_inicio":"2023-10-05", "tipo_deuda":"R", "ahorro_cuota_mensual":8358.000000000015, "ahorro_total":-8358.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":3600.0, "cuota":284.0, "saldo":537.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8508, "fecha_inicio":"2023-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":821.0000000000011, "ahorro_total":-821.0000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":7, "monto_otorgado":45000.0, "cuota":1250.0, "saldo":9167.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7963, "fecha_inicio":"2021-07-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-1027.435900693842, "ahorro_total":-36987.69242497832, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":4835.0, "cuota":667.0, "saldo":1330.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7249, "fecha_inicio":"2023-10-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":4835.0, "cuota":270.0, "saldo":806.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8333, "fecha_inicio":"2023-11-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":19000.0, "cuota":950.0, "saldo":2988.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8427, "fecha_inicio":"2021-04-08", "tipo_deuda":"R", "ahorro_cuota_mensual":3938.0000000000064, "ahorro_total":-3938.0000000000064, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":19, "monto_otorgado":25700.0, "cuota":1285.0, "saldo":20428.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2051, "fecha_inicio":"2022-03-04", "tipo_deuda":"R", "ahorro_cuota_mensual":21713.000000000044, "ahorro_total":-21713.000000000044, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":20, "monto_otorgado":22600.0, "cuota":1390.0, "saldo":20166.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1077, "fecha_inicio":"2020-03-13", "tipo_deuda":"R", "ahorro_cuota_mensual":21556.000000000044, "ahorro_total":-21556.000000000044, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":15000.0, "cuota":1427.0, "saldo":13499.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":24.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.1001, "fecha_inicio":"2023-06-14", "tipo_deuda":"I", "ahorro_cuota_mensual":474.5786768790206, "ahorro_total":11389.888245096494, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":637.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-02-28", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 5115747, "monto_maximo_cliente": 116986.0, "cuota_externa_total": 13701.0, "capacidad_maxima_pago": 117511.0, "bursolnum": 7317829, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 8281.414692337528, "monto_max": 116986.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-12-15", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":70000.0, "cuota":4877.0, "saldo":66197.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.0543, "fecha_inicio":"2023-06-23", "tipo_deuda":"I", "ahorro_cuota_mensual":-78.28549111540815, "ahorro_total":-2818.2776801546934, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":1, "monto_otorgado":116986.0, "cuota":8824.0, "saldo":102206.0, "tasa_externa":0.8374, "tasa_kubo":0.6509, "numero_pagos_otorgado":72.0, "numero_pagos_restante":25.0, "frecuencia_externa":"S", "avance":0.1263, "fecha_inicio":"2023-05-15", "tipo_deuda":"I", "ahorro_cuota_mensual":542.5853076624717, "ahorro_total":19533.07107584898, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":9000.0, "cuota":393.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-01-24", "tipo_deuda":"R", "ahorro_cuota_mensual":393.0, "ahorro_total":-393.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
@@ -367,7 +370,7 @@
     <t>{"Prospecto": 5133040, "monto_maximo_cliente": 52400.0, "cuota_externa_total": 18019.0, "capacidad_maxima_pago": 44081.0, "bursolnum": 7317356, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3111.4575367866714, "monto_max": 52400.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.5668, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":50000.0, "cuota":3716.0, "saldo":48136.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0373, "fecha_inicio":"2023-08-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-2910.729558772964, "ahorro_total":-29107.29558772964, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":52400.0, "cuota":4194.0, "saldo":52994.0, "tasa_externa":0.9653, "tasa_kubo":0.5668, "numero_pagos_otorgado":122.0, "numero_pagos_restante":57.0, "frecuencia_externa":"S", "avance":-0.0113, "fecha_inicio":"2023-12-14", "tipo_deuda":"I", "ahorro_cuota_mensual":1207.6233127982796, "ahorro_total":73665.02208069505, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":13200.0, "cuota":5712.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-07-14", "tipo_deuda":"R", "ahorro_cuota_mensual":5712.0, "ahorro_total":-5712.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":10000.0, "cuota":500.0, "saldo":9053.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0947, "fecha_inicio":"2023-03-03", "tipo_deuda":"R", "ahorro_cuota_mensual":9553.000000000002, "ahorro_total":-9553.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":12100.0, "cuota":1098.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-05-29", "tipo_deuda":"R", "ahorro_cuota_mensual":1098.0, "ahorro_total":-1098.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":9, "monto_otorgado":17800.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2024-01-02", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":4, "monto_otorgado":674890.0, "cuota":6405.0, "saldo":671220.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":360.0, "numero_pagos_restante":352.0, "frecuencia_externa":"M", "avance":0.0054, "fecha_inicio":"2023-08-21", "tipo_deuda":"M", "ahorro_cuota_mensual":-30371.59144815558, "ahorro_total":-10933772.92133601, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":30000.0, "cuota":2248.0, "saldo":26668.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":24.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1111, "fecha_inicio":"2023-07-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-28.548900861652783, "ahorro_total":-685.1736206796668, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COOPERATIVA", "registro":6, "monto_otorgado":60000.0, "cuota":1250.0, "saldo":19472.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":48.0, "numero_pagos_restante":39.0, "frecuencia_externa":"M", "avance":0.6755, "fecha_inicio":"2023-06-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-2312.73763754199, "ahorro_total":-111011.40660201552, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 5158482, "monto_maximo_cliente": 100638.0, "cuota_externa_total": 67664.0, "capacidad_maxima_pago": 82275.0, "bursolnum": 7317410, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4150.576921317457, "monto_max": 100638.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.4818, "comision": 0.0423, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":17, "monto_otorgado":117700.0, "cuota":6210.0, "saldo":73230.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3778, "fecha_inicio":"2006-01-27", "tipo_deuda":"R", "ahorro_cuota_mensual":79439.99999999981, "ahorro_total":-79439.99999999981, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":19, "monto_otorgado":9917.0, "cuota":820.0, "saldo":1640.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8346, "fecha_inicio":"2023-09-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":18, "monto_otorgado":9966.0, "cuota":2311.0, "saldo":2311.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7681, "fecha_inicio":"2023-08-04", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":20, "monto_otorgado":9953.0, "cuota":1619.0, "saldo":4855.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5122, "fecha_inicio":"2023-10-02", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":96000.0, "cuota":7907.0, "saldo":80978.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":24.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1565, "fecha_inicio":"2023-06-30", "tipo_deuda":"I", "ahorro_cuota_mensual":2099.702511179965, "ahorro_total":50392.86026831916, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":22, "monto_otorgado":64000.0, "cuota":1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2004-01-24", "tipo_deuda":"R", "ahorro_cuota_mensual":1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":23, "monto_otorgado":39100.0, "cuota":2144.0, "saldo":20140.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4849, "fecha_inicio":"2003-12-27", "tipo_deuda":"R", "ahorro_cuota_mensual":22283.99999999995, "ahorro_total":-22283.99999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-02-05", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":95000.0, "cuota":8000.0, "saldo":76841.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1911, "fecha_inicio":"2007-03-02", "tipo_deuda":"R", "ahorro_cuota_mensual":84840.99999999981, "ahorro_total":-84840.99999999981, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":21, "monto_otorgado":9974.0, "cuota":689.0, "saldo":2758.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7235, "fecha_inicio":"2023-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":15, "monto_otorgado":44600.0, "cuota":3476.0, "saldo":38335.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1405, "fecha_inicio":"2018-05-30", "tipo_deuda":"R", "ahorro_cuota_mensual":41810.999999999905, "ahorro_total":-41810.999999999905, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":260100.0, "cuota":13005.0, "saldo":123543.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.525, "fecha_inicio":"2007-05-10", "tipo_deuda":"R", "ahorro_cuota_mensual":136547.99999999968, "ahorro_total":-136547.99999999968, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":109000.0, "cuota":6938.0, "saldo":109521.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0048, "fecha_inicio":"2004-01-29", "tipo_deuda":"R", "ahorro_cuota_mensual":116458.99999999972, "ahorro_total":-116458.99999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":100638.0, "cuota":4742.0, "saldo":69480.0, "tasa_externa":0.4002, "tasa_kubo":0.3337, "numero_pagos_otorgado":37.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.3096, "fecha_inicio":"2022-10-26", "tipo_deuda":"I", "ahorro_cuota_mensual":44.53254235675013, "ahorro_total":1647.7040671997547, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":25000.0, "cuota":1250.0, "saldo":2461.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9016, "fecha_inicio":"2022-08-04", "tipo_deuda":"R", "ahorro_cuota_mensual":3710.9999999999936, "ahorro_total":-3710.9999999999936, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":143100.0, "cuota":9300.0, "saldo":113621.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.206, "fecha_inicio":"2004-04-01", "tipo_deuda":"R", "ahorro_cuota_mensual":122920.99999999971, "ahorro_total":-122920.99999999971, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":42000.0, "cuota":2620.0, "saldo":40222.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0423, "fecha_inicio":"2023-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":42841.9999999999, "ahorro_total":-42841.9999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":117500.0, "cuota":10682.0, "saldo":89885.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.235, "fecha_inicio":"2013-08-05", "tipo_deuda":"R", "ahorro_cuota_mensual":100566.99999999978, "ahorro_total":-100566.99999999978, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":180000.0, "cuota":9000.0, "saldo":89736.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5015, "fecha_inicio":"2004-09-13", "tipo_deuda":"R", "ahorro_cuota_mensual":98735.99999999978, "ahorro_total":-98735.99999999978, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":70000.0, "cuota":3500.0, "saldo":51681.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2617, "fecha_inicio":"2023-06-29", "tipo_deuda":"R", "ahorro_cuota_mensual":55180.999999999876, "ahorro_total":-55180.999999999876, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":98000.0, "cuota":5390.0, "saldo":76502.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2194, "fecha_inicio":"2022-10-26", "tipo_deuda":"R", "ahorro_cuota_mensual":81891.99999999981, "ahorro_total":-81891.99999999981, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":14, "monto_otorgado":31500.0, "cuota":1575.0, "saldo":11540.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6337, "fecha_inicio":"2006-10-01", "tipo_deuda":"R", "ahorro_cuota_mensual":13114.99999999997, "ahorro_total":-13114.99999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 5158482, "monto_maximo_cliente": 100638.0, "cuota_externa_total": 67664.0, "capacidad_maxima_pago": 82275.0, "bursolnum": 7317410, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4150.576921317457, "monto_max": 100638.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.4818, "comision": 0.0423, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":17, "monto_otorgado":117700.0, "cuota":6210.0, "saldo":73230.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3778, "fecha_inicio":"2006-01-27", "tipo_deuda":"R", "ahorro_cuota_mensual":79439.99999999981, "ahorro_total":-79439.99999999981, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":19, "monto_otorgado":9917.0, "cuota":820.0, "saldo":1640.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8346, "fecha_inicio":"2023-09-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":18, "monto_otorgado":9966.0, "cuota":2311.0, "saldo":2311.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7681, "fecha_inicio":"2023-08-04", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":20, "monto_otorgado":9953.0, "cuota":1619.0, "saldo":4855.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5122, "fecha_inicio":"2023-10-02", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":96000.0, "cuota":7907.0, "saldo":80978.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":24.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1565, "fecha_inicio":"2023-06-30", "tipo_deuda":"I", "ahorro_cuota_mensual":2099.702511179965, "ahorro_total":50392.86026831916, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":22, "monto_otorgado":64000.0, "cuota":1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2004-01-24", "tipo_deuda":"R", "ahorro_cuota_mensual":1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":23, "monto_otorgado":39100.0, "cuota":2144.0, "saldo":20140.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4849, "fecha_inicio":"2003-12-27", "tipo_deuda":"R", "ahorro_cuota_mensual":22283.99999999995, "ahorro_total":-22283.99999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-02-05", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":95000.0, "cuota":8000.0, "saldo":76841.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1911, "fecha_inicio":"2007-03-02", "tipo_deuda":"R", "ahorro_cuota_mensual":84840.99999999981, "ahorro_total":-84840.99999999981, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":21, "monto_otorgado":9974.0, "cuota":689.0, "saldo":2758.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7235, "fecha_inicio":"2023-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":15, "monto_otorgado":44600.0, "cuota":3476.0, "saldo":38335.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1405, "fecha_inicio":"2018-05-30", "tipo_deuda":"R", "ahorro_cuota_mensual":41810.999999999905, "ahorro_total":-41810.999999999905, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":260100.0, "cuota":13005.0, "saldo":123543.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.525, "fecha_inicio":"2007-05-10", "tipo_deuda":"R", "ahorro_cuota_mensual":136547.99999999968, "ahorro_total":-136547.99999999968, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":109000.0, "cuota":6938.0, "saldo":109521.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0048, "fecha_inicio":"2004-01-29", "tipo_deuda":"R", "ahorro_cuota_mensual":116458.99999999972, "ahorro_total":-116458.99999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":100638.0, "cuota":4742.0, "saldo":69480.0, "tasa_externa":0.4002, "tasa_kubo":0.3337, "numero_pagos_otorgado":37.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.3096, "fecha_inicio":"2022-10-26", "tipo_deuda":"I", "ahorro_cuota_mensual":44.53254235675013, "ahorro_total":1647.7040671997547, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":25000.0, "cuota":1250.0, "saldo":2461.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9016, "fecha_inicio":"2022-08-04", "tipo_deuda":"R", "ahorro_cuota_mensual":3710.9999999999936, "ahorro_total":-3710.9999999999936, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":143100.0, "cuota":9300.0, "saldo":113621.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.206, "fecha_inicio":"2004-04-01", "tipo_deuda":"R", "ahorro_cuota_mensual":122920.99999999971, "ahorro_total":-122920.99999999971, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":42000.0, "cuota":2620.0, "saldo":40222.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0423, "fecha_inicio":"2023-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":42841.9999999999, "ahorro_total":-42841.9999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":117500.0, "cuota":10682.0, "saldo":89885.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.235, "fecha_inicio":"2013-08-05", "tipo_deuda":"R", "ahorro_cuota_mensual":100566.99999999978, "ahorro_total":-100566.99999999978, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":180000.0, "cuota":9000.0, "saldo":89736.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5015, "fecha_inicio":"2004-09-13", "tipo_deuda":"R", "ahorro_cuota_mensual":98735.99999999978, "ahorro_total":-98735.99999999978, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":70000.0, "cuota":3500.0, "saldo":51681.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2617, "fecha_inicio":"2023-06-29", "tipo_deuda":"R", "ahorro_cuota_mensual":55180.999999999876, "ahorro_total":-55180.999999999876, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":98000.0, "cuota":5390.0, "saldo":76502.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2194, "fecha_inicio":"2022-10-26", "tipo_deuda":"R", "ahorro_cuota_mensual":81891.99999999981, "ahorro_total":-81891.99999999981, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":14, "monto_otorgado":31500.0, "cuota":1575.0, "saldo":11540.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6337, "fecha_inicio":"2006-10-01", "tipo_deuda":"R", "ahorro_cuota_mensual":13114.99999999997, "ahorro_total":-13114.99999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 5177117, "monto_maximo_cliente": 15000.0, "cuota_externa_total": 6484.0, "capacidad_maxima_pago": 23516.0, "bursolnum": 7317655, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 428.4263741100588, "monto_max": 15000.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5391, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":35000.0, "cuota":2207.0, "saldo":33267.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":33.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.0495, "fecha_inicio":"2023-07-06", "tipo_deuda":"I", "ahorro_cuota_mensual":762.4429513834762, "ahorro_total":25160.617395654714, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":49000.0, "cuota":2450.0, "saldo":22834.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.534, "fecha_inicio":"2020-03-16", "tipo_deuda":"R", "ahorro_cuota_mensual":25283.999999999956, "ahorro_total":-25283.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":21349.0, "cuota":1404.0, "saldo":12926.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3945, "fecha_inicio":"2019-07-08", "tipo_deuda":"R", "ahorro_cuota_mensual":14329.999999999976, "ahorro_total":-14329.999999999976, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":21000.0, "cuota":3353.0, "saldo":17928.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1463, "fecha_inicio":"2022-03-01", "tipo_deuda":"R", "ahorro_cuota_mensual":21280.999999999964, "ahorro_total":-21280.999999999964, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":15000.0, "cuota":557.0, "saldo":4952.0, "tasa_externa":0.3806, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.6699, "fecha_inicio":"2019-11-14", "tipo_deuda":"I", "ahorro_cuota_mensual":132.41753764757152, "ahorro_total":7945.052258854292, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
@@ -382,13 +385,13 @@
     <t>{"Prospecto": 5215233, "monto_maximo_cliente": 12000.0, "cuota_externa_total": 7485.0, "capacidad_maxima_pago": 39515.0, "bursolnum": 7317135, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 342.74109928804705, "monto_max": 12000.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5991, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":2, "monto_otorgado":12000.0, "cuota":768.0, "saldo":9855.0, "tasa_externa":0.7592, "tasa_kubo":0.2, "numero_pagos_otorgado":120.0, "numero_pagos_restante":51.0, "frecuencia_externa":"S", "avance":0.1787, "fecha_inicio":"2023-07-13", "tipo_deuda":"I", "ahorro_cuota_mensual":428.33403011805717, "ahorro_total":25700.04180708343, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":83100.0, "cuota":2187.0, "saldo":186.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9978, "fecha_inicio":"2022-06-02", "tipo_deuda":"R", "ahorro_cuota_mensual":2372.9999999999995, "ahorro_total":-2372.9999999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":1921.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-06-08", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":69000.0, "cuota":4530.0, "saldo":55857.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.1905, "fecha_inicio":"2023-07-19", "tipo_deuda":"I", "ahorro_cuota_mensual":1851.8312816374705, "ahorro_total":66665.92613894894, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 5252137, "monto_maximo_cliente": 85000.0, "cuota_externa_total": 7250.0, "capacidad_maxima_pago": 90750.0, "bursolnum": 7317545, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3621.5346005800234, "monto_max": 85000.0, "cuota_min": 200.2991210698785, "monto_min": 5000, "plazo_max": 50.0, "plazo_min": 4, "tasa": 0.7007, "comision": 0.0428, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":16000.0, "cuota":800.0, "saldo":952.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9405, "fecha_inicio":"2021-05-05", "tipo_deuda":"R", "ahorro_cuota_mensual":1751.9999999999977, "ahorro_total":-1751.9999999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":18000.0, "cuota":1520.0, "saldo":16984.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":24.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.0564, "fecha_inicio":"2023-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":399.50889474247515, "ahorro_total":9588.213473819404, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":12, "monto_otorgado":22000.0, "cuota":1100.0, "saldo":11609.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4723, "fecha_inicio":"2018-04-03", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":100.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-01-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":11, "monto_otorgado":18000.0, "cuota":900.0, "saldo":4795.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7336, "fecha_inicio":"2023-01-12", "tipo_deuda":"R", "ahorro_cuota_mensual":5694.999999999989, "ahorro_total":-5694.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":35000.0, "cuota":2075.0, "saldo":7748.0, "tasa_externa":0.4, "tasa_kubo":0.3617, "numero_pagos_otorgado":25.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7786, "fecha_inicio":"2022-05-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-47.769301171188545, "ahorro_total":-1194.2325292797136, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":15600.0, "cuota":560.0, "saldo":14466.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0727, "fecha_inicio":"2020-01-13", "tipo_deuda":"R", "ahorro_cuota_mensual":15025.999999999967, "ahorro_total":-15025.999999999967, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":5944.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8811, "fecha_inicio":"2022-05-12", "tipo_deuda":"R", "ahorro_cuota_mensual":8443.999999999985, "ahorro_total":-8443.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":50000.0, "cuota":2061.0, "saldo":47726.0, "tasa_externa":0.3921, "tasa_kubo":0.3617, "numero_pagos_otorgado":48.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.0455, "fecha_inicio":"2023-09-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-102.96654858722286, "ahorro_total":-4942.394332186697, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":40000.0, "cuota":1.0, "saldo":13716.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6571, "fecha_inicio":"2022-09-28", "tipo_deuda":"R", "ahorro_cuota_mensual":13716.999999999969, "ahorro_total":-13716.999999999969, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":6300.0, "cuota":149.0, "saldo":5402.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1425, "fecha_inicio":"2018-12-10", "tipo_deuda":"R", "ahorro_cuota_mensual":5550.999999999988, "ahorro_total":-5550.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":26000.0, "cuota":1300.0, "saldo":7140.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7254, "fecha_inicio":"2022-10-17", "tipo_deuda":"R", "ahorro_cuota_mensual":8439.999999999984, "ahorro_total":-8439.999999999984, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 5252137, "monto_maximo_cliente": 85000.0, "cuota_externa_total": 7250.0, "capacidad_maxima_pago": 90750.0, "bursolnum": 7317545, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3621.5346005800234, "monto_max": 85000.0, "cuota_min": 200.2991210698785, "monto_min": 5000, "plazo_max": 50.0, "plazo_min": 4, "tasa": 0.7007, "comision": 0.0428, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":16000.0, "cuota":800.0, "saldo":952.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9405, "fecha_inicio":"2021-05-05", "tipo_deuda":"R", "ahorro_cuota_mensual":1751.9999999999977, "ahorro_total":-1751.9999999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":18000.0, "cuota":1520.0, "saldo":16984.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":24.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.0564, "fecha_inicio":"2023-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":399.50889474247515, "ahorro_total":9588.213473819404, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":12, "monto_otorgado":22000.0, "cuota":1100.0, "saldo":11609.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4723, "fecha_inicio":"2018-04-03", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":100.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-01-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":11, "monto_otorgado":18000.0, "cuota":900.0, "saldo":4795.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7336, "fecha_inicio":"2023-01-12", "tipo_deuda":"R", "ahorro_cuota_mensual":5694.999999999989, "ahorro_total":-5694.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":35000.0, "cuota":2075.0, "saldo":7748.0, "tasa_externa":0.4, "tasa_kubo":0.3617, "numero_pagos_otorgado":25.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7786, "fecha_inicio":"2022-05-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-47.769301171188545, "ahorro_total":-1194.2325292797136, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":15600.0, "cuota":560.0, "saldo":14466.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0727, "fecha_inicio":"2020-01-13", "tipo_deuda":"R", "ahorro_cuota_mensual":15025.999999999967, "ahorro_total":-15025.999999999967, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":5944.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8811, "fecha_inicio":"2022-05-12", "tipo_deuda":"R", "ahorro_cuota_mensual":8443.999999999985, "ahorro_total":-8443.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":50000.0, "cuota":2061.0, "saldo":47726.0, "tasa_externa":0.3921, "tasa_kubo":0.3617, "numero_pagos_otorgado":48.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.0455, "fecha_inicio":"2023-09-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-102.96654858722286, "ahorro_total":-4942.394332186697, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":40000.0, "cuota":1.0, "saldo":13716.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6571, "fecha_inicio":"2022-09-28", "tipo_deuda":"R", "ahorro_cuota_mensual":13716.999999999969, "ahorro_total":-13716.999999999969, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":6300.0, "cuota":149.0, "saldo":5402.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1425, "fecha_inicio":"2018-12-10", "tipo_deuda":"R", "ahorro_cuota_mensual":5550.999999999988, "ahorro_total":-5550.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":26000.0, "cuota":1300.0, "saldo":7140.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7254, "fecha_inicio":"2022-10-17", "tipo_deuda":"R", "ahorro_cuota_mensual":8439.999999999984, "ahorro_total":-8439.999999999984, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 5267958, "monto_maximo_cliente": 130000.0, "cuota_externa_total": 9618.0, "capacidad_maxima_pago": 129922.0, "bursolnum": 7317186, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 6497.536858202417, "monto_max": 130000.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.7554, "comision": 0.046, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":130000.0, "cuota":7310.0, "saldo":115003.0, "tasa_externa":0.6577, "tasa_kubo":0.4818, "numero_pagos_otorgado":122.0, "numero_pagos_restante":48.0, "frecuencia_externa":"S", "avance":0.1154, "fecha_inicio":"2023-03-03", "tipo_deuda":"I", "ahorro_cuota_mensual":853.5647888329377, "ahorro_total":52067.4521188092, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":47000.0, "cuota":2526.0, "saldo":7603.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8382, "fecha_inicio":"2023-05-27", "tipo_deuda":"R", "ahorro_cuota_mensual":10129.000000000015, "ahorro_total":-10129.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":23400.0, "cuota":1170.0, "saldo":5053.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7841, "fecha_inicio":"2021-03-31", "tipo_deuda":"R", "ahorro_cuota_mensual":6223.00000000001, "ahorro_total":-6223.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":20000.0, "cuota":2015.0, "saldo":17416.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":18.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.1292, "fecha_inicio":"2023-08-09", "tipo_deuda":"I", "ahorro_cuota_mensual":349.5670874171169, "ahorro_total":6292.207573508104, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 5283904, "monto_maximo_cliente": 372000.0, "cuota_externa_total": 32149.0, "capacidad_maxima_pago": 396351.0, "bursolnum": 7317657, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 13206.842106659838, "monto_max": 372000.0, "cuota_min": 163.04445621498797, "monto_min": 5000, "plazo_max": 50.0, "plazo_min": 4, "tasa": 0.2622, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2622, 0.2306, 0.2], "comisiones": [0, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":45000.0, "cuota":2988.0, "saldo":42605.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":30.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.0532, "fecha_inicio":"2023-08-11", "tipo_deuda":"I", "ahorro_cuota_mensual":828.0751421092141, "ahorro_total":24842.254263276423, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":13, "monto_otorgado":7744.0, "cuota":558.0, "saldo":4464.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4236, "fecha_inicio":"2023-11-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":3844.0, "cuota":266.0, "saldo":1592.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5858, "fecha_inicio":"2023-10-27", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":3836.0, "cuota":808.0, "saldo":3236.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1564, "fecha_inicio":"2023-09-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":65000.0, "cuota":2214.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":312.0, "numero_pagos_restante":217.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-05-02", "tipo_deuda":"R", "ahorro_cuota_mensual":2214.0, "ahorro_total":690768.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":88100.0, "cuota":5000.0, "saldo":78690.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1068, "fecha_inicio":"2018-11-22", "tipo_deuda":"R", "ahorro_cuota_mensual":83689.99999999959, "ahorro_total":-83689.99999999959, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":21600.0, "cuota":1469.0, "saldo":35086.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.6244, "fecha_inicio":"2013-08-28", "tipo_deuda":"R", "ahorro_cuota_mensual":36554.99999999981, "ahorro_total":-36554.99999999981, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":60200.0, "cuota":1320.0, "saldo":33746.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4394, "fecha_inicio":"2022-06-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-6244.83771967064, "ahorro_total":-56203.53947703576, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":8000.0, "cuota":113.0, "saldo":3371.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5786, "fecha_inicio":"2023-11-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-8089.767999999969, "ahorro_total":-8089.767999999969, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":372000.0, "cuota":13739.0, "saldo":353868.0, "tasa_externa":0.3775, "tasa_kubo":0.2622, "numero_pagos_otorgado":60.0, "numero_pagos_restante":26.0, "frecuencia_externa":"M", "avance":0.0487, "fecha_inicio":"2021-05-27", "tipo_deuda":"I", "ahorro_cuota_mensual":1608.4924576048925, "ahorro_total":96509.54745629354, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":66000.0, "cuota":4530.0, "saldo":56880.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1382, "fecha_inicio":"2023-02-10", "tipo_deuda":"R", "ahorro_cuota_mensual":61409.9999999997, "ahorro_total":-61409.9999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":27000.0, "cuota":700.0, "saldo":20440.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.243, "fecha_inicio":"2023-08-07", "tipo_deuda":"R", "ahorro_cuota_mensual":21139.99999999989, "ahorro_total":-21139.99999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":300700.0, "cuota":6358.0, "saldo":158943.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4714, "fecha_inicio":"2022-04-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-31428.49007151099, "ahorro_total":-282856.41064359894, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 5283904, "monto_maximo_cliente": 372000.0, "cuota_externa_total": 32149.0, "capacidad_maxima_pago": 396351.0, "bursolnum": 7317657, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 13206.842106659838, "monto_max": 372000.0, "cuota_min": 163.04445621498797, "monto_min": 5000, "plazo_max": 50.0, "plazo_min": 4, "tasa": 0.2622, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2622, 0.2306, 0.2], "comisiones": [0, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":45000.0, "cuota":2988.0, "saldo":42605.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":30.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.0532, "fecha_inicio":"2023-08-11", "tipo_deuda":"I", "ahorro_cuota_mensual":828.0751421092141, "ahorro_total":24842.254263276423, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":13, "monto_otorgado":7744.0, "cuota":558.0, "saldo":4464.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4236, "fecha_inicio":"2023-11-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":3844.0, "cuota":266.0, "saldo":1592.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5858, "fecha_inicio":"2023-10-27", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":3836.0, "cuota":808.0, "saldo":3236.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1564, "fecha_inicio":"2023-09-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":65000.0, "cuota":2214.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":312.0, "numero_pagos_restante":217.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-05-02", "tipo_deuda":"R", "ahorro_cuota_mensual":2214.0, "ahorro_total":690768.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":88100.0, "cuota":5000.0, "saldo":78690.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1068, "fecha_inicio":"2018-11-22", "tipo_deuda":"R", "ahorro_cuota_mensual":83689.99999999959, "ahorro_total":-83689.99999999959, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":21600.0, "cuota":1469.0, "saldo":35086.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.6244, "fecha_inicio":"2013-08-28", "tipo_deuda":"R", "ahorro_cuota_mensual":36554.99999999981, "ahorro_total":-36554.99999999981, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":60200.0, "cuota":1320.0, "saldo":33746.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4394, "fecha_inicio":"2022-06-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-6244.83771967064, "ahorro_total":-56203.53947703576, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":8000.0, "cuota":113.0, "saldo":3371.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5786, "fecha_inicio":"2023-11-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-8089.767999999969, "ahorro_total":-8089.767999999969, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":372000.0, "cuota":13739.0, "saldo":353868.0, "tasa_externa":0.3775, "tasa_kubo":0.2622, "numero_pagos_otorgado":60.0, "numero_pagos_restante":26.0, "frecuencia_externa":"M", "avance":0.0487, "fecha_inicio":"2021-05-27", "tipo_deuda":"I", "ahorro_cuota_mensual":1608.4924576048925, "ahorro_total":96509.54745629354, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":66000.0, "cuota":4530.0, "saldo":56880.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1382, "fecha_inicio":"2023-02-10", "tipo_deuda":"R", "ahorro_cuota_mensual":61409.9999999997, "ahorro_total":-61409.9999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":27000.0, "cuota":700.0, "saldo":20440.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.243, "fecha_inicio":"2023-08-07", "tipo_deuda":"R", "ahorro_cuota_mensual":21139.99999999989, "ahorro_total":-21139.99999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":300700.0, "cuota":6358.0, "saldo":158943.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4714, "fecha_inicio":"2022-04-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-31428.49007151099, "ahorro_total":-282856.41064359894, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 5286466, "monto_maximo_cliente": 39000.0, "cuota_externa_total": 4741.0, "capacidad_maxima_pago": 55206.0, "bursolnum": 7317498, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1363.3029386249852, "monto_max": 39000.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6193, "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":30000.0, "cuota":2357.0, "saldo":27394.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.0869, "fecha_inicio":"2023-08-14", "tipo_deuda":"I", "ahorro_cuota_mensual":620.3400424925353, "ahorro_total":14888.161019820847, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":461.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-11-12", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":25000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2024-01-11", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":25000.0, "cuota":0.0, "saldo":4126.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.835, "fecha_inicio":"2023-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":4125.999999999988, "ahorro_total":-4125.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":39000.0, "cuota":1984.0, "saldo":26248.0, "tasa_externa":0.5452, "tasa_kubo":0.2914, "numero_pagos_otorgado":96.0, "numero_pagos_restante":30.0, "frecuencia_externa":"S", "avance":0.327, "fecha_inicio":"2022-10-07", "tipo_deuda":"I", "ahorro_cuota_mensual":492.2205424152253, "ahorro_total":23626.586035930814, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":15800.0, "cuota":790.0, "saldo":9468.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4008, "fecha_inicio":"2018-05-13", "tipo_deuda":"R", "ahorro_cuota_mensual":10257.999999999975, "ahorro_total":-10257.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":19500.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-08-19", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
@@ -409,13 +412,13 @@
     <t>{"Prospecto": 5383814, "monto_maximo_cliente": 15084.0, "cuota_externa_total": 8260.0, "capacidad_maxima_pago": 22272.0, "bursolnum": 7316743, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1193.2774856689198, "monto_max": 15084.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 26.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "HIPOTECAGOBIERNO", "registro":5, "monto_otorgado":342176.0, "cuota":3227.0, "saldo":315822.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":360.0, "numero_pagos_restante":263.0, "frecuencia_externa":"M", "avance":0.077, "fecha_inicio":"2016-02-25", "tipo_deuda":"M", "ahorro_cuota_mensual":-16644.62551972764, "ahorro_total":-5992065.187101951, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":8, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2017-10-27", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":976.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-08-08", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":4, "monto_otorgado":350.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-04-06", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":4000.0, "cuota":275.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":264.0, "numero_pagos_restante":144.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2014-03-27", "tipo_deuda":"R", "ahorro_cuota_mensual":275.0, "ahorro_total":72600.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":5000.0, "cuota":250.0, "saldo":299.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9402, "fecha_inicio":"2021-07-27", "tipo_deuda":"R", "ahorro_cuota_mensual":549.0000000000005, "ahorro_total":-549.0000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":10000.0, "cuota":500.0, "saldo":972.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9028, "fecha_inicio":"2023-02-03", "tipo_deuda":"R", "ahorro_cuota_mensual":1472.0000000000011, "ahorro_total":-1472.0000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":15000.0, "cuota":3676.0, "saldo":13187.0, "tasa_externa":3.1879, "tasa_kubo":0.6509, "numero_pagos_otorgado":104.0, "numero_pagos_restante":20.0, "frecuencia_externa":"W", "avance":0.1209, "fecha_inicio":"2023-09-26", "tipo_deuda":"I", "ahorro_cuota_mensual":2489.3676554605013, "ahorro_total":64723.559041973036, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":10000.0, "cuota":1202.0, "saldo":7672.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2328, "fecha_inicio":"2023-09-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-9.940500263250215, "ahorro_total":-119.28600315900258, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 5417924, "monto_maximo_cliente": 52400.0, "cuota_externa_total": 14612.0, "capacidad_maxima_pago": 51548.0, "bursolnum": 7317734, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3926.51033237947, "monto_max": 52400.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 30.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":50000.0, "cuota":4038.0, "saldo":46182.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.0764, "fecha_inicio":"2023-09-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-54.09910790137883, "ahorro_total":-1298.378589633092, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":11, "monto_otorgado":6000.0, "cuota":300.0, "saldo":3775.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3708, "fecha_inicio":"2018-11-19", "tipo_deuda":"R", "ahorro_cuota_mensual":4075.0000000000045, "ahorro_total":-4075.0000000000045, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":6590.0, "cuota":330.0, "saldo":1818.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7241, "fecha_inicio":"2024-01-24", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":6585.0, "cuota":329.0, "saldo":1552.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7643, "fecha_inicio":"2024-01-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":6585.0, "cuota":329.0, "saldo":1746.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7349, "fecha_inicio":"2024-01-01", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":5400.0, "cuota":1150.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-06-25", "tipo_deuda":"R", "ahorro_cuota_mensual":1150.0, "ahorro_total":-1150.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":6, "monto_otorgado":6585.0, "cuota":1261.0, "saldo":8823.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.3399, "fecha_inicio":"2023-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":10000.0, "cuota":1467.0, "saldo":8108.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1892, "fecha_inicio":"2022-10-12", "tipo_deuda":"R", "ahorro_cuota_mensual":9575.000000000011, "ahorro_total":-9575.000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":52400.0, "cuota":6060.0, "saldo":48482.0, "tasa_externa":1.3555, "tasa_kubo":0.6509, "numero_pagos_otorgado":61.0, "numero_pagos_restante":24.0, "frecuencia_externa":"S", "avance":0.0748, "fecha_inicio":"2023-10-09", "tipo_deuda":"I", "ahorro_cuota_mensual":2133.48966762053, "ahorro_total":64004.69002861589, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":8800.0, "cuota":390.0, "saldo":3379.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.616, "fecha_inicio":"2020-12-09", "tipo_deuda":"R", "ahorro_cuota_mensual":3769.0000000000036, "ahorro_total":-3769.0000000000036, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":7, "monto_otorgado":6585.0, "cuota":856.0, "saldo":4280.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.35, "fecha_inicio":"2023-12-20", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 5417924, "monto_maximo_cliente": 52400.0, "cuota_externa_total": 14612.0, "capacidad_maxima_pago": 51548.0, "bursolnum": 7317734, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3926.51033237947, "monto_max": 52400.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 30.0, "plazo_min": 4, "tasa": 0.6509, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":50000.0, "cuota":4038.0, "saldo":46182.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.0764, "fecha_inicio":"2023-09-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-54.09910790137883, "ahorro_total":-1298.378589633092, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":11, "monto_otorgado":6000.0, "cuota":300.0, "saldo":3775.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3708, "fecha_inicio":"2018-11-19", "tipo_deuda":"R", "ahorro_cuota_mensual":4075.0000000000045, "ahorro_total":-4075.0000000000045, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":6590.0, "cuota":330.0, "saldo":1818.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7241, "fecha_inicio":"2024-01-24", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":6585.0, "cuota":329.0, "saldo":1552.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7643, "fecha_inicio":"2024-01-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":6585.0, "cuota":329.0, "saldo":1746.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7349, "fecha_inicio":"2024-01-01", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":5400.0, "cuota":1150.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-06-25", "tipo_deuda":"R", "ahorro_cuota_mensual":1150.0, "ahorro_total":-1150.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":6, "monto_otorgado":6585.0, "cuota":1261.0, "saldo":8823.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.3399, "fecha_inicio":"2023-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":10000.0, "cuota":1467.0, "saldo":8108.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1892, "fecha_inicio":"2022-10-12", "tipo_deuda":"R", "ahorro_cuota_mensual":9575.000000000011, "ahorro_total":-9575.000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":52400.0, "cuota":6060.0, "saldo":48482.0, "tasa_externa":1.3555, "tasa_kubo":0.6509, "numero_pagos_otorgado":61.0, "numero_pagos_restante":24.0, "frecuencia_externa":"S", "avance":0.0748, "fecha_inicio":"2023-10-09", "tipo_deuda":"I", "ahorro_cuota_mensual":2133.48966762053, "ahorro_total":64004.69002861589, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":8800.0, "cuota":390.0, "saldo":3379.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.616, "fecha_inicio":"2020-12-09", "tipo_deuda":"R", "ahorro_cuota_mensual":3769.0000000000036, "ahorro_total":-3769.0000000000036, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":7, "monto_otorgado":6585.0, "cuota":856.0, "saldo":4280.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.35, "fecha_inicio":"2023-12-20", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 5446631, "monto_maximo_cliente": 500000.0, "cuota_externa_total": 67944.0, "capacidad_maxima_pago": 572056.0, "bursolnum": 7317746, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 19125.377661343267, "monto_max": 500000.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.2914, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":13, "monto_otorgado":119200.0, "cuota":5960.0, "saldo":63954.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4635, "fecha_inicio":"2022-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":69913.99999999983, "ahorro_total":-69913.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":4920.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-10-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":4920.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-10-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":4920.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-10-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":4920.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-10-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":4920.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-10-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":4920.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-10-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":4920.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-10-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":130000.0, "cuota":6500.0, "saldo":64593.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5031, "fecha_inicio":"2016-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":71092.99999999983, "ahorro_total":-71092.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":130000.0, "cuota":6500.0, "saldo":64593.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5031, "fecha_inicio":"2016-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":71092.99999999983, "ahorro_total":-71092.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":130000.0, "cuota":6500.0, "saldo":64593.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5031, "fecha_inicio":"2016-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":71092.99999999983, "ahorro_total":-71092.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":130000.0, "cuota":6500.0, "saldo":64593.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5031, "fecha_inicio":"2016-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":71092.99999999983, "ahorro_total":-71092.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":130000.0, "cuota":6500.0, "saldo":64593.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5031, "fecha_inicio":"2016-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":71092.99999999983, "ahorro_total":-71092.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":13, "monto_otorgado":119200.0, "cuota":5960.0, "saldo":63954.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4635, "fecha_inicio":"2022-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":69913.99999999983, "ahorro_total":-69913.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":4920.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-10-25", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":13, "monto_otorgado":119200.0, "cuota":5960.0, "saldo":63954.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4635, "fecha_inicio":"2022-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":69913.99999999983, "ahorro_total":-69913.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":29400.0, "cuota":112.0, "saldo":99.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9966, "fecha_inicio":"2023-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":210.99999999999972, "ahorro_total":-210.99999999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":119200.0, "cuota":5960.0, "saldo":63954.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4635, "fecha_inicio":"2022-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":69913.99999999983, "ahorro_total":-69913.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":29400.0, "cuota":112.0, "saldo":99.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9966, "fecha_inicio":"2023-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":210.99999999999972, "ahorro_total":-210.99999999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":29400.0, "cuota":112.0, "saldo":99.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9966, "fecha_inicio":"2023-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":210.99999999999972, "ahorro_total":-210.99999999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":29400.0, "cuota":112.0, "saldo":99.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9966, "fecha_inicio":"2023-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":210.99999999999972, "ahorro_total":-210.99999999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":29400.0, "cuota":112.0, "saldo":99.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9966, "fecha_inicio":"2023-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":210.99999999999972, "ahorro_total":-210.99999999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":6582.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8684, "fecha_inicio":"2022-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":9081.999999999982, "ahorro_total":-9081.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":6582.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8684, "fecha_inicio":"2022-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":9081.999999999982, "ahorro_total":-9081.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":6582.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8684, "fecha_inicio":"2022-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":9081.999999999982, "ahorro_total":-9081.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":6582.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8684, "fecha_inicio":"2022-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":9081.999999999982, "ahorro_total":-9081.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":6582.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8684, "fecha_inicio":"2022-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":9081.999999999982, "ahorro_total":-9081.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":6582.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8684, "fecha_inicio":"2022-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":9081.999999999982, "ahorro_total":-9081.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":6582.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8684, "fecha_inicio":"2022-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":9081.999999999982, "ahorro_total":-9081.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":6582.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8684, "fecha_inicio":"2022-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":9081.999999999982, "ahorro_total":-9081.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":119200.0, "cuota":5960.0, "saldo":63954.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4635, "fecha_inicio":"2022-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":69913.99999999983, "ahorro_total":-69913.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":119200.0, "cuota":5960.0, "saldo":63954.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4635, "fecha_inicio":"2022-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":69913.99999999983, "ahorro_total":-69913.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":119200.0, "cuota":5960.0, "saldo":63954.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4635, "fecha_inicio":"2022-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":69913.99999999983, "ahorro_total":-69913.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":119200.0, "cuota":5960.0, "saldo":63954.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4635, "fecha_inicio":"2022-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":69913.99999999983, "ahorro_total":-69913.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":130000.0, "cuota":6500.0, "saldo":64593.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5031, "fecha_inicio":"2016-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":71092.99999999983, "ahorro_total":-71092.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":103500.0, "cuota":5175.0, "saldo":40310.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6105, "fecha_inicio":"2022-02-12", "tipo_deuda":"R", "ahorro_cuota_mensual":45484.99999999989, "ahorro_total":-45484.99999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":130000.0, "cuota":6500.0, "saldo":64593.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5031, "fecha_inicio":"2016-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":71092.99999999983, "ahorro_total":-71092.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":16, "monto_otorgado":1700.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":16, "monto_otorgado":1700.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":16, "monto_otorgado":1700.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":16, "monto_otorgado":1700.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":16, "monto_otorgado":1700.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":29, "monto_otorgado":9999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":16, "monto_otorgado":1700.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":29, "monto_otorgado":9999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":29, "monto_otorgado":9999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":29, "monto_otorgado":9999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":29, "monto_otorgado":9999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":29, "monto_otorgado":9999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":29, "monto_otorgado":9999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":29400.0, "cuota":112.0, "saldo":99.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9966, "fecha_inicio":"2023-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":210.99999999999972, "ahorro_total":-210.99999999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":29, "monto_otorgado":9999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":16, "monto_otorgado":1700.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":16, "monto_otorgado":1700.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-08-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":15, "monto_otorgado":86018.0, "cuota":0.0, "saldo":134165.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.5597, "fecha_inicio":"2021-03-30", "tipo_deuda":"O", "ahorro_cuota_mensual":134164.99999999962, "ahorro_total":-134164.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":100000.0, "cuota":8083.0, "saldo":97398.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.026, "fecha_inicio":"2023-10-10", "tipo_deuda":"I", "ahorro_cuota_mensual":2294.1334749751168, "ahorro_total":55059.2033994028, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":100000.0, "cuota":8083.0, "saldo":97398.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.026, "fecha_inicio":"2023-10-10", "tipo_deuda":"I", "ahorro_cuota_mensual":2294.1334749751168, "ahorro_total":55059.2033994028, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":100000.0, "cuota":8083.0, "saldo":97398.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.026, "fecha_inicio":"2023-10-10", "tipo_deuda":"I", "ahorro_cuota_mensual":2294.1334749751168, "ahorro_total":55059.2033994028, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":100000.0, "cuota":8083.0, "saldo":97398.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.026, "fecha_inicio":"2023-10-10", "tipo_deuda":"I", "ahorro_cuota_mensual":2294.1334749751168, "ahorro_total":55059.2033994028, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":100000.0, "cuota":8083.0, "saldo":97398.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.026, "fecha_inicio":"2023-10-10", "tipo_deuda":"I", "ahorro_cuota_mensual":2294.1334749751168, "ahorro_total":55059.2033994028, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":100000.0, "cuota":8083.0, "saldo":97398.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.026, "fecha_inicio":"2023-10-10", "tipo_deuda":"I", "ahorro_cuota_mensual":2294.1334749751168, "ahorro_total":55059.2033994028, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":100000.0, "cuota":8083.0, "saldo":97398.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.026, "fecha_inicio":"2023-10-10", "tipo_deuda":"I", "ahorro_cuota_mensual":2294.1334749751168, "ahorro_total":55059.2033994028, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":100000.0, "cuota":8083.0, "saldo":97398.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.026, "fecha_inicio":"2023-10-10", "tipo_deuda":"I", "ahorro_cuota_mensual":2294.1334749751168, "ahorro_total":55059.2033994028, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":15, "monto_otorgado":86018.0, "cuota":0.0, "saldo":134165.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.5597, "fecha_inicio":"2021-03-30", "tipo_deuda":"O", "ahorro_cuota_mensual":134164.99999999962, "ahorro_total":-134164.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":15, "monto_otorgado":86018.0, "cuota":0.0, "saldo":134165.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.5597, "fecha_inicio":"2021-03-30", "tipo_deuda":"O", "ahorro_cuota_mensual":134164.99999999962, "ahorro_total":-134164.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":15, "monto_otorgado":86018.0, "cuota":0.0, "saldo":134165.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.5597, "fecha_inicio":"2021-03-30", "tipo_deuda":"O", "ahorro_cuota_mensual":134164.99999999962, "ahorro_total":-134164.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":15, "monto_otorgado":86018.0, "cuota":0.0, "saldo":134165.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.5597, "fecha_inicio":"2021-03-30", "tipo_deuda":"O", "ahorro_cuota_mensual":134164.99999999962, "ahorro_total":-134164.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":15, "monto_otorgado":86018.0, "cuota":0.0, "saldo":134165.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.5597, "fecha_inicio":"2021-03-30", "tipo_deuda":"O", "ahorro_cuota_mensual":134164.99999999962, "ahorro_total":-134164.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":15, "monto_otorgado":86018.0, "cuota":0.0, "saldo":134165.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.5597, "fecha_inicio":"2021-03-30", "tipo_deuda":"O", "ahorro_cuota_mensual":134164.99999999962, "ahorro_total":-134164.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":15, "monto_otorgado":86018.0, "cuota":0.0, "saldo":134165.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.5597, "fecha_inicio":"2021-03-30", "tipo_deuda":"O", "ahorro_cuota_mensual":134164.99999999962, "ahorro_total":-134164.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":130000.0, "cuota":6500.0, "saldo":64593.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5031, "fecha_inicio":"2016-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":71092.99999999983, "ahorro_total":-71092.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":29400.0, "cuota":112.0, "saldo":99.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_</t>
   </si>
   <si>
-    <t>{"Prospecto": 5476222, "monto_maximo_cliente": 60000.0, "cuota_externa_total": 23965.0, "capacidad_maxima_pago": 57935.0, "bursolnum": 7316956, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3696.1110273840345, "monto_max": 60000.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 22.0, "plazo_min": 4, "tasa": 0.2914, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":1365.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-02-01", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":14, "monto_otorgado":8500.0, "cuota":425.0, "saldo":826.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9028, "fecha_inicio":"2023-09-04", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-05-01", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":5000.0, "cuota":599.0, "saldo":4170.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.166, "fecha_inicio":"2023-10-16", "tipo_deuda":"I", "ahorro_cuota_mensual":102.16507259029186, "ahorro_total":1225.9808710835023, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":8986.0, "cuota":449.0, "saldo":658.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9268, "fecha_inicio":"2023-12-12", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":16, "monto_otorgado":10252.0, "cuota":513.0, "saldo":2250.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7805, "fecha_inicio":"2023-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":20000.0, "cuota":1202.0, "saldo":8584.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5708, "fecha_inicio":"2023-11-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-662.5658076752466, "ahorro_total":-3312.829038376233, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":15, "monto_otorgado":10300.0, "cuota":515.0, "saldo":702.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9318, "fecha_inicio":"2023-09-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":18200.0, "cuota":12044.0, "saldo":4727.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7403, "fecha_inicio":"2023-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":16770.999999999985, "ahorro_total":-16770.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":1750.0, "cuota":1838.0, "saldo":919.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.4749, "fecha_inicio":"2023-12-31", "tipo_deuda":"I", "ahorro_cuota_mensual":1221.4989543348352, "ahorro_total":3664.4968630045055, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":8932.0, "cuota":1350.0, "saldo":885.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9009, "fecha_inicio":"2018-07-13", "tipo_deuda":"R", "ahorro_cuota_mensual":2234.9999999999973, "ahorro_total":-2234.9999999999973, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":7000.0, "cuota":904.0, "saldo":6312.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0983, "fecha_inicio":"2022-01-11", "tipo_deuda":"R", "ahorro_cuota_mensual":7215.999999999983, "ahorro_total":-7215.999999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":14000.0, "cuota":1184.0, "saldo":13800.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0143, "fecha_inicio":"2021-07-09", "tipo_deuda":"R", "ahorro_cuota_mensual":14983.999999999962, "ahorro_total":-14983.999999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":17000.0, "cuota":1973.0, "saldo":16906.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0055, "fecha_inicio":"2023-11-27", "tipo_deuda":"R", "ahorro_cuota_mensual":18878.999999999953, "ahorro_total":-18878.999999999953, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":60000.0, "cuota":4212.0, "saldo":58005.0, "tasa_externa":0.4945, "tasa_kubo":0.2914, "numero_pagos_otorgado":43.0, "numero_pagos_restante":12.0, "frecuencia_externa":"S", "avance":0.0332, "fecha_inicio":"2023-06-16", "tipo_deuda":"I", "ahorro_cuota_mensual":515.8889726159655, "ahorro_total":11349.557397551242, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+    <t>{"Prospecto": 5476222, "monto_maximo_cliente": 60000.0, "cuota_externa_total": 23965.0, "capacidad_maxima_pago": 57935.0, "bursolnum": 7316956, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3696.1110273840345, "monto_max": 60000.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 22.0, "plazo_min": 4, "tasa": 0.2914, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":1365.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-02-01", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":14, "monto_otorgado":8500.0, "cuota":425.0, "saldo":826.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9028, "fecha_inicio":"2023-09-04", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-05-01", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":5000.0, "cuota":599.0, "saldo":4170.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.166, "fecha_inicio":"2023-10-16", "tipo_deuda":"I", "ahorro_cuota_mensual":102.16507259029186, "ahorro_total":1225.9808710835023, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":8986.0, "cuota":449.0, "saldo":658.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9268, "fecha_inicio":"2023-12-12", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":16, "monto_otorgado":10252.0, "cuota":513.0, "saldo":2250.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7805, "fecha_inicio":"2023-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":20000.0, "cuota":1202.0, "saldo":8584.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5708, "fecha_inicio":"2023-11-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-662.5658076752466, "ahorro_total":-3312.829038376233, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":15, "monto_otorgado":10300.0, "cuota":515.0, "saldo":702.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9318, "fecha_inicio":"2023-09-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":18200.0, "cuota":12044.0, "saldo":4727.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7403, "fecha_inicio":"2023-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":16770.999999999985, "ahorro_total":-16770.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":1750.0, "cuota":1838.0, "saldo":919.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.4749, "fecha_inicio":"2023-12-31", "tipo_deuda":"I", "ahorro_cuota_mensual":1221.4989543348352, "ahorro_total":3664.4968630045055, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":8932.0, "cuota":1350.0, "saldo":885.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9009, "fecha_inicio":"2018-07-13", "tipo_deuda":"R", "ahorro_cuota_mensual":2234.9999999999973, "ahorro_total":-2234.9999999999973, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":7000.0, "cuota":904.0, "saldo":6312.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0983, "fecha_inicio":"2022-01-11", "tipo_deuda":"R", "ahorro_cuota_mensual":7215.999999999983, "ahorro_total":-7215.999999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":14000.0, "cuota":1184.0, "saldo":13800.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0143, "fecha_inicio":"2021-07-09", "tipo_deuda":"R", "ahorro_cuota_mensual":14983.999999999962, "ahorro_total":-14983.999999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":17000.0, "cuota":1973.0, "saldo":16906.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0055, "fecha_inicio":"2023-11-27", "tipo_deuda":"R", "ahorro_cuota_mensual":18878.999999999953, "ahorro_total":-18878.999999999953, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":60000.0, "cuota":4212.0, "saldo":58005.0, "tasa_externa":0.4945, "tasa_kubo":0.2914, "numero_pagos_otorgado":43.0, "numero_pagos_restante":12.0, "frecuencia_externa":"S", "avance":0.0332, "fecha_inicio":"2023-06-16", "tipo_deuda":"I", "ahorro_cuota_mensual":515.8889726159655, "ahorro_total":11349.557397551242, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 5484371, "monto_maximo_cliente": 76088.0, "cuota_externa_total": 15093.0, "capacidad_maxima_pago": 73348.18, "bursolnum": 7317669, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5477.424358859572, "monto_max": 76088.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 37.0, "plazo_min": 4, "tasa": 0.6722, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":2, "monto_otorgado":76088.0, "cuota":6932.0, "saldo":63899.0, "tasa_externa":1.0614, "tasa_kubo":0.6722, "numero_pagos_otorgado":74.0, "numero_pagos_restante":26.0, "frecuencia_externa":"S", "avance":0.1602, "fecha_inicio":"2023-05-05", "tipo_deuda":"I", "ahorro_cuota_mensual":1454.5756411404282, "ahorro_total":53819.29872219584, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":113000.0, "cuota":2248.0, "saldo":9633.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9148, "fecha_inicio":"2015-06-02", "tipo_deuda":"R", "ahorro_cuota_mensual":11881.000000000011, "ahorro_total":-11881.000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":95000.0, "cuota":4750.0, "saldo":23364.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7541, "fecha_inicio":"2023-06-21", "tipo_deuda":"R", "ahorro_cuota_mensual":28114.00000000003, "ahorro_total":-28114.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":17000.0, "cuota":1970.0, "saldo":13293.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2181, "fecha_inicio":"2023-06-02", "tipo_deuda":"R", "ahorro_cuota_mensual":15263.000000000015, "ahorro_total":-15263.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":66300.0, "cuota":3315.0, "saldo":20751.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.687, "fecha_inicio":"2022-10-18", "tipo_deuda":"R", "ahorro_cuota_mensual":24066.000000000025, "ahorro_total":-24066.000000000025, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":24600.0, "cuota":1230.0, "saldo":5465.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7778, "fecha_inicio":"2019-09-20", "tipo_deuda":"R", "ahorro_cuota_mensual":6695.000000000006, "ahorro_total":-6695.000000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":39600.0, "cuota":1.0, "saldo":439.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9889, "fecha_inicio":"2011-10-04", "tipo_deuda":"R", "ahorro_cuota_mensual":440.0000000000005, "ahorro_total":-440.0000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-09-19", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":40000.0, "cuota":3865.0, "saldo":36534.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":18.0, "numero_pagos_restante":13.0, "frecuencia_externa":"M", "avance":0.0866, "fecha_inicio":"2023-10-25", "tipo_deuda":"I", "ahorro_cuota_mensual":31.398909428947718, "ahorro_total":565.1803697210589, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
@@ -430,10 +433,10 @@
     <t>{"Prospecto": 5544466, "monto_maximo_cliente": 500000.0, "cuota_externa_total": 133564.0, "capacidad_maxima_pago": 727247.0, "bursolnum": 7317838, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 20239.78127720747, "monto_max": 500000.0, "cuota_min": 200.2991210698785, "monto_min": 5000, "plazo_max": 58.0, "plazo_min": 4, "tasa": 0.3617, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":600000.0, "cuota":28080.0, "saldo":464773.0, "tasa_externa":0.5256, "tasa_kubo":0.3617, "numero_pagos_otorgado":120.0, "numero_pagos_restante":40.0, "frecuencia_externa":"S", "avance":0.2254, "fecha_inicio":"2022-08-09", "tipo_deuda":"I", "ahorro_cuota_mensual":4044.1054716145736, "ahorro_total":242646.32829687442, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":250000.0, "cuota":12500.0, "saldo":182160.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":76.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.2714, "fecha_inicio":"2017-09-28", "tipo_deuda":"R", "ahorro_cuota_mensual":5626.40440515134, "ahorro_total":427606.73479150183, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":441000.0, "cuota":22050.0, "saldo":32203.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.927, "fecha_inicio":"2014-07-20", "tipo_deuda":"R", "ahorro_cuota_mensual":54252.99999999993, "ahorro_total":-54252.99999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":577500.0, "cuota":28875.0, "saldo":640887.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.1098, "fecha_inicio":"2014-06-06", "tipo_deuda":"R", "ahorro_cuota_mensual":669761.9999999985, "ahorro_total":-669761.9999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":376598.0, "cuota":12626.0, "saldo":158758.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":36.0, "numero_pagos_restante":12.0, "frecuencia_externa":"M", "avance":0.5784, "fecha_inicio":"2022-03-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-5924.801625948363, "ahorro_total":-213292.85853414107, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":140000.0, "cuota":7000.0, "saldo":108694.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2236, "fecha_inicio":"2021-04-10", "tipo_deuda":"R", "ahorro_cuota_mensual":115693.99999999975, "ahorro_total":-115693.99999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":2, "monto_otorgado":286400.0, "cuota":19851.0, "saldo":271861.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0508, "fecha_inicio":"2006-07-10", "tipo_deuda":"R", "ahorro_cuota_mensual":291711.99999999936, "ahorro_total":-291711.99999999936, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":4, "monto_otorgado":870517.0, "cuota":18734.0, "saldo":392494.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":48.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.5491, "fecha_inicio":"2022-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-18941.393359530077, "ahorro_total":-909186.8812574437, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-09-29", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":44919.0, "cuota":2557.0, "saldo":43610.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":28.0, "numero_pagos_restante":23.0, "frecuencia_externa":"M", "avance":0.0291, "fecha_inicio":"2023-11-16", "tipo_deuda":"I", "ahorro_cuota_mensual":15.54241772362684, "ahorro_total":435.18769626155154, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":60181.0, "cuota":4740.0, "saldo":59153.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":24.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.0171, "fecha_inicio":"2023-11-16", "tipo_deuda":"I", "ahorro_cuota_mensual":993.7624885831606, "ahorro_total":23850.299725995854, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":10, "monto_otorgado":54500.0, "cuota":2418.0, "saldo":38594.0, "tasa_externa":0.3392, "tasa_kubo":0.3617, "numero_pagos_otorgado":36.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.2919, "fecha_inicio":"2023-02-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-266.60981899581475, "ahorro_total":-9597.953483849331, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
-    <t>{"Prospecto": 5547392, "monto_maximo_cliente": 500000.0, "cuota_externa_total": 46459.0, "capacidad_maxima_pago": 517877.0, "bursolnum": 7317891, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 17987.656733921576, "monto_max": 500000.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 55.0, "plazo_min": 4, "tasa": 0.3337, "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":7, "monto_otorgado":15000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-11-03", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":58500.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2014-01-14", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":100000.0, "cuota":8622.0, "saldo":99776.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.0022, "fecha_inicio":"2023-11-13", "tipo_deuda":"I", "ahorro_cuota_mensual":2833.1334749751168, "ahorro_total":67995.2033994028, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":6000.0, "cuota":1244.0, "saldo":4614.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.231, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":5857.999999999987, "ahorro_total":-5857.999999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":77011.0, "cuota":4494.0, "saldo":70275.0, "tasa_externa":0.3517, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.0875, "fecha_inicio":"2023-09-05", "tipo_deuda":"I", "ahorro_cuota_mensual":35.93600041308764, "ahorro_total":862.4640099141034, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":386000.0, "cuota":19300.0, "saldo":285213.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2611, "fecha_inicio":"2007-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":304512.9999999992, "ahorro_total":-304512.9999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":225500.0, "cuota":11275.0, "saldo":86785.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6151, "fecha_inicio":"2008-06-12", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":415000.0, "cuota":15404.0, "saldo":375261.0, "tasa_externa":0.3234, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":38.0, "frecuencia_externa":"M", "avance":0.0958, "fecha_inicio":"2023-06-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-470.06345891491037, "ahorro_total":-22563.046027915698, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5550621, "monto_maximo_cliente": 149997.0, "cuota_externa_total": 12974.0, "capacidad_maxima_pago": 157966.0, "bursolnum": 7317367, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 10649.214805333773, "monto_max": 149997.0, "cuota_min": 345.4415646244417, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.821, "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":3, "monto_otorgado":149997.0, "cuota":11328.0, "saldo":146954.0, "tasa_externa":0.8388, "tasa_kubo":0.7007, "numero_pagos_otorgado":72.0, "numero_pagos_restante":32.0, "frecuencia_externa":"S", "avance":0.0203, "fecha_inicio":"2023-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":108.02772949290011, "ahorro_total":3888.998261744404, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":19500.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-11-23", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":29000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2004-07-31", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":600.0, "cuota":400.0, "saldo":400.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3333, "fecha_inicio":"2023-12-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-inf, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":74, "monto_otorgado":0.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2005-03-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":5300.0, "cuota":706.0, "saldo":4902.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.0751, "fecha_inicio":"2023-11-14", "tipo_deuda":"I", "ahorro_cuota_mensual":46.75379753824268, "ahorro_total":561.0455704589122, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":1036.0, "cuota":540.0, "saldo":540.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4788, "fecha_inicio":"2018-03-18", "tipo_deuda":"O", "ahorro_cuota_mensual":1079.9999999999995, "ahorro_total":-1079.9999999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+    <t>{"Prospecto": 5547392, "monto_maximo_cliente": 500000.0, "cuota_externa_total": 46459.0, "capacidad_maxima_pago": 517877.0, "bursolnum": 7317891, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 17987.656733921576, "monto_max": 500000.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 55.0, "plazo_min": 4, "tasa": 0.3337, "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":7, "monto_otorgado":15000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-11-03", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":58500.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2014-01-14", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":100000.0, "cuota":8622.0, "saldo":99776.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.0022, "fecha_inicio":"2023-11-13", "tipo_deuda":"I", "ahorro_cuota_mensual":2833.1334749751168, "ahorro_total":67995.2033994028, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":6000.0, "cuota":1244.0, "saldo":4614.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.231, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":5857.999999999987, "ahorro_total":-5857.999999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":77011.0, "cuota":4494.0, "saldo":70275.0, "tasa_externa":0.3517, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.0875, "fecha_inicio":"2023-09-05", "tipo_deuda":"I", "ahorro_cuota_mensual":35.93600041308764, "ahorro_total":862.4640099141034, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":386000.0, "cuota":19300.0, "saldo":285213.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2611, "fecha_inicio":"2007-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":304512.9999999992, "ahorro_total":-304512.9999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":225500.0, "cuota":11275.0, "saldo":86785.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6151, "fecha_inicio":"2008-06-12", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":415000.0, "cuota":15404.0, "saldo":375261.0, "tasa_externa":0.3234, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":38.0, "frecuencia_externa":"M", "avance":0.0958, "fecha_inicio":"2023-06-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-470.06345891491037, "ahorro_total":-22563.046027915698, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5550621, "monto_maximo_cliente": 149997.0, "cuota_externa_total": 12974.0, "capacidad_maxima_pago": 157966.0, "bursolnum": 7317367, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 10649.214805333773, "monto_max": 149997.0, "cuota_min": 345.4415646244417, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.821, "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "BANCO", "registro":3, "monto_otorgado":149997.0, "cuota":11328.0, "saldo":146954.0, "tasa_externa":0.8388, "tasa_kubo":0.7007, "numero_pagos_otorgado":72.0, "numero_pagos_restante":32.0, "frecuencia_externa":"S", "avance":0.0203, "fecha_inicio":"2023-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":108.02772949290011, "ahorro_total":3888.998261744404, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":19500.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-11-23", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":29000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2004-07-31", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":600.0, "cuota":400.0, "saldo":400.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3333, "fecha_inicio":"2023-12-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":74, "monto_otorgado":0.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2005-03-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":5300.0, "cuota":706.0, "saldo":4902.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.0751, "fecha_inicio":"2023-11-14", "tipo_deuda":"I", "ahorro_cuota_mensual":46.75379753824268, "ahorro_total":561.0455704589122, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":1036.0, "cuota":540.0, "saldo":540.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4788, "fecha_inicio":"2018-03-18", "tipo_deuda":"O", "ahorro_cuota_mensual":1079.9999999999995, "ahorro_total":-1079.9999999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
   <si>
     <t>{"Prospecto": 5555834, "monto_maximo_cliente": 216000.0, "cuota_externa_total": 37484.0, "capacidad_maxima_pago": 233771.0, "bursolnum": 7317878, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 8262.16314970029, "monto_max": 216000.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.2914, "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":1000.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2010-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":6, "monto_otorgado":957301.0, "cuota":8990.0, "saldo":610774.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":360.0, "numero_pagos_restante":246.0, "frecuencia_externa":"M", "avance":0.362, "fecha_inicio":"2014-10-16", "tipo_deuda":"M", "ahorro_cuota_mensual":-8215.469934592616, "ahorro_total":-2957569.1764533417, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":5, "monto_otorgado":357520.0, "cuota":6182.0, "saldo":202251.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":60.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.4343, "fecha_inicio":"2021-07-19", "tipo_deuda":"I", "ahorro_cuota_mensual":-6233.676257673995, "ahorro_total":-374020.57546043966, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":1, "monto_otorgado":216000.0, "cuota":16136.0, "saldo":192094.0, "tasa_externa":0.8799, "tasa_kubo":0.2914, "numero_pagos_otorgado":97.0, "numero_pagos_restante":38.0, "frecuencia_externa":"S", "avance":0.1107, "fecha_inicio":"2023-05-23", "tipo_deuda":"I", "ahorro_cuota_mensual":7873.836850299709, "ahorro_total":377944.168814386, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":2, "monto_otorgado":360.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-06-29", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":97900.0, "cuota":4895.0, "saldo":43175.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.559, "fecha_inicio":"2021-09-29", "tipo_deuda":"R", "ahorro_cuota_mensual":48069.99999999988, "ahorro_total":-48069.99999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":60000.0, "cuota":4952.0, "saldo":59469.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.0089, "fecha_inicio":"2023-11-14", "tipo_deuda":"I", "ahorro_cuota_mensual":1478.6800849850706, "ahorro_total":35488.322039641695, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
@@ -442,7 +445,13 @@
     <t>{"Prospecto": 5556081, "monto_maximo_cliente": 316003.0, "cuota_externa_total": 23712.0, "capacidad_maxima_pago": 338169.0, "bursolnum": 7317231, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 9025.601299860062, "monto_max": 316003.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.2914, "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":2, "monto_otorgado":1221.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-01-17", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":10, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2002-03-23", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":15000.0, "cuota":1711.0, "saldo":13415.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.1057, "fecha_inicio":"2023-11-14", "tipo_deuda":"I", "ahorro_cuota_mensual":298.40695334541124, "ahorro_total":3580.883440144935, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":11, "monto_otorgado":811.0, "cuota":1023.0, "saldo":1023.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.2614, "fecha_inicio":"2009-12-14", "tipo_deuda":"O", "ahorro_cuota_mensual":2045.9999999999982, "ahorro_total":-2045.9999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":1, "monto_otorgado":237792.0, "cuota":8219.0, "saldo":78079.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.6717, "fecha_inicio":"2021-12-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-1010.6680561864159, "ahorro_total":-36384.05002271097, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":59400.0, "cuota":2970.0, "saldo":6481.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8909, "fecha_inicio":"2023-11-22", "tipo_deuda":"R", "ahorro_cuota_mensual":9450.999999999987, "ahorro_total":-9450.999999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":34676.0, "cuota":1159.0, "saldo":17008.0, "tasa_externa":0.2252, "tasa_kubo":0.2, "numero_pagos_otorgado":44.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.5095, "fecha_inicio":"2022-05-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-18.409014537201756, "ahorro_total":-809.9966396368773, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":44627.0, "cuota":1355.0, "saldo":33019.0, "tasa_externa":0.1847, "tasa_kubo":0.2, "numero_pagos_otorgado":46.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":0.2601, "fecha_inicio":"2023-03-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-118.4225517298596, "ahorro_total":-5447.437379573542, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":57000.0, "cuota":200.0, "saldo":54663.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.041, "fecha_inicio":"2016-10-11", "tipo_deuda":"R", "ahorro_cuota_mensual":54862.99999999989, "ahorro_total":-54862.99999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":236700.0, "cuota":7681.0, "saldo":196294.0, "tasa_externa":0.3058, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":39.0, "frecuencia_externa":"M", "avance":0.1707, "fecha_inicio":"2022-06-29", "tipo_deuda":"I", "ahorro_cuota_mensual":981.0887440786782, "ahorro_total":58865.32464472069, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":62969.0, "cuota":1821.0, "saldo":15507.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":45.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.7537, "fecha_inicio":"2021-04-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-286.8510756114638, "ahorro_total":-12908.29840251587, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
   </si>
   <si>
+    <t>monto maximo muy ajustado a las deudas consolidables</t>
+  </si>
+  <si>
     <t>{"Prospecto": 5587133, "monto_maximo_cliente": 120000.0, "cuota_externa_total": 14277.0, "capacidad_maxima_pago": 149878.0, "bursolnum": 7317592, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5997.726330648386, "monto_max": 120000.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.7554, "comision": 0.046, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":4, "monto_otorgado":871.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-01-25", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":30000.0, "cuota":2027.0, "saldo":21420.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":36.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.286, "fecha_inicio":"2022-07-12", "tipo_deuda":"I", "ahorro_cuota_mensual":293.0145209518266, "ahorro_total":10548.52275426576, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":3030.0, "cuota":1451.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-04-28", "tipo_deuda":"R", "ahorro_cuota_mensual":1451.0, "ahorro_total":-1451.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":10200.0, "cuota":4148.0, "saldo":3423.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6644, "fecha_inicio":"2023-07-23", "tipo_deuda":"R", "ahorro_cuota_mensual":7571.000000000007, "ahorro_total":-7571.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":500.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-09-15", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":21000.0, "cuota":720.0, "saldo":580.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9724, "fecha_inicio":"2022-04-11", "tipo_deuda":"R", "ahorro_cuota_mensual":1300.0000000000011, "ahorro_total":-1300.0000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":120000.0, "cuota":6950.0, "saldo":87879.0, "tasa_externa":0.6482, "tasa_kubo":0.4818, "numero_pagos_otorgado":96.0, "numero_pagos_restante":14.0, "frecuencia_externa":"S", "avance":0.2677, "fecha_inicio":"2021-06-15", "tipo_deuda":"I", "ahorro_cuota_mensual":652.8720397873758, "ahorro_total":31337.85790979404, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":10000.0, "cuota":500.0, "saldo":2163.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7837, "fecha_inicio":"2023-03-24", "tipo_deuda":"R", "ahorro_cuota_mensual":2663.0000000000045, "ahorro_total":-2663.0000000000045, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":12000.0, "cuota":1700.0, "saldo":3197.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7336, "fecha_inicio":"2022-10-26", "tipo_deuda":"R", "ahorro_cuota_mensual":4897.000000000006, "ahorro_total":-4897.000000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":15000.0, "cuota":750.0, "saldo":7114.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5257, "fecha_inicio":"2023-03-15", "tipo_deuda":"R", "ahorro_cuota_mensual":7864.0000000000155, "ahorro_total":-7864.0000000000155, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":30000.0, "cuota":3860.0, "saldo":26831.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":12.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.1056, "fecha_inicio":"2023-11-27", "tipo_deuda":"I", "ahorro_cuota_mensual":540.3240688517226, "ahorro_total":6483.888826220671, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":3000.0, "cuota":3200.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-04-24", "tipo_deuda":"R", "ahorro_cuota_mensual":3200.0, "ahorro_total":-3200.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>todo bien</t>
   </si>
   <si>
     <t>{"Prospecto": 5610632, "monto_maximo_cliente": 500000.0, "cuota_externa_total": 39729.0, "capacidad_maxima_pago": 639036.88, "bursolnum": 7317550, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 20132.49706217271, "monto_max": 500000.0, "cuota_min": 200.2991210698785, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5668, "comision": 0.0428, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":100000.0, "cuota":11651.0, "saldo":97858.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":12.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.0214, "fecha_inicio":"2023-12-05", "tipo_deuda":"I", "ahorro_cuota_mensual":1304.7771529567344, "ahorro_total":15657.325835480813, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FONDOS Y FIDEIC", "registro":3, "monto_otorgado":261262.0, "cuota":13063.0, "saldo":77481.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":40.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.7034, "fecha_inicio":"2015-03-19", "tipo_deuda":"R", "ahorro_cuota_mensual":9436.782392573523, "ahorro_total":377471.2957029409, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":1, "monto_otorgado":506576.0, "cuota":21226.0, "saldo":506576.0, "tasa_externa":0.4529, "tasa_kubo":0.3617, "numero_pagos_otorgado":60.0, "numero_pagos_restante":53.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2023-09-11", "tipo_deuda":"I", "ahorro_cuota_mensual":932.654488981043, "ahorro_total":55959.26933886258, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":18000.0, "cuota":1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2013-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
@@ -473,7 +482,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -848,11 +857,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="34.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="55.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -860,196 +869,196 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="3">
-        <v>28837</v>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="3">
-        <v>39500</v>
-      </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="3">
-        <v>380930</v>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="3">
-        <v>405226</v>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3">
         <v>458697</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3">
         <v>458697</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3">
         <v>458697</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3">
         <v>458697</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="3">
-        <v>557483</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="3">
-        <v>659364</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="3">
-        <v>829025</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="3">
-        <v>847726</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="3">
-        <v>920002</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="3">
-        <v>976655</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="3">
-        <v>1177743</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3">
         <v>1302408</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="3">
         <v>1448462</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="3">
         <v>1496214</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="3">
         <v>1550610</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="3">
         <v>1630602</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="3">
         <v>1784380</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="3">
         <v>1848246</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="3">
         <v>2009039</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
@@ -1057,7 +1066,7 @@
         <v>2090977</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
@@ -1065,7 +1074,7 @@
         <v>2162754</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
@@ -1073,7 +1082,7 @@
         <v>2298632</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
@@ -1081,7 +1090,7 @@
         <v>2311104</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
@@ -1089,7 +1098,7 @@
         <v>2372071</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
@@ -1097,7 +1106,7 @@
         <v>2612016</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
@@ -1105,7 +1114,7 @@
         <v>2687735</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
@@ -1113,7 +1122,7 @@
         <v>2710338</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
@@ -1121,7 +1130,7 @@
         <v>2790904</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
@@ -1129,7 +1138,7 @@
         <v>2878373</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
@@ -1137,7 +1146,7 @@
         <v>2901882</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
@@ -1145,7 +1154,7 @@
         <v>2937559</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
@@ -1153,7 +1162,7 @@
         <v>3073017</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
@@ -1161,7 +1170,7 @@
         <v>3159500</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
@@ -1169,7 +1178,7 @@
         <v>3284861</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
@@ -1177,7 +1186,7 @@
         <v>3312894</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
@@ -1185,7 +1194,7 @@
         <v>3341344</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
@@ -1193,7 +1202,7 @@
         <v>3463619</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
@@ -1201,7 +1210,7 @@
         <v>3473842</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
@@ -1209,7 +1218,7 @@
         <v>3549605</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
@@ -1217,7 +1226,7 @@
         <v>3553967</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
@@ -1225,7 +1234,7 @@
         <v>3567378</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
@@ -1233,7 +1242,7 @@
         <v>3589493</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
@@ -1241,7 +1250,7 @@
         <v>3632363</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
@@ -1249,7 +1258,7 @@
         <v>3728149</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
@@ -1257,7 +1266,7 @@
         <v>3730883</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
@@ -1265,7 +1274,7 @@
         <v>3741894</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
@@ -1273,7 +1282,7 @@
         <v>3748714</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
@@ -1281,7 +1290,7 @@
         <v>3786062</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
@@ -1289,7 +1298,7 @@
         <v>3800116</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
@@ -1297,7 +1306,7 @@
         <v>3805773</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
@@ -1305,7 +1314,7 @@
         <v>3868724</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
@@ -1313,7 +1322,7 @@
         <v>3926429</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
@@ -1321,7 +1330,7 @@
         <v>3941195</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
@@ -1329,7 +1338,7 @@
         <v>3987119</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
@@ -1337,7 +1346,7 @@
         <v>4007295</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
@@ -1345,7 +1354,7 @@
         <v>4018492</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
@@ -1353,7 +1362,7 @@
         <v>4039644</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
@@ -1361,7 +1370,7 @@
         <v>4134401</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
@@ -1369,7 +1378,7 @@
         <v>4143061</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
@@ -1377,7 +1386,7 @@
         <v>4170086</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25">
@@ -1385,7 +1394,7 @@
         <v>4206571</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25">
@@ -1393,7 +1402,7 @@
         <v>4231833</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25">
@@ -1401,7 +1410,7 @@
         <v>4261012</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="17.25">
@@ -1409,7 +1418,7 @@
         <v>4287160</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25">
@@ -1417,7 +1426,7 @@
         <v>4302613</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="17.25">
@@ -1425,7 +1434,7 @@
         <v>4356609</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="17.25">
@@ -1433,7 +1442,7 @@
         <v>4389079</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="17.25">
@@ -1441,7 +1450,7 @@
         <v>4433343</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25">
@@ -1449,7 +1458,7 @@
         <v>4445474</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="17.25">
@@ -1457,7 +1466,7 @@
         <v>4450135</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25">
@@ -1465,7 +1474,7 @@
         <v>4482737</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25">
@@ -1473,7 +1482,7 @@
         <v>4495647</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="17.25">
@@ -1481,7 +1490,7 @@
         <v>4551959</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25">
@@ -1489,7 +1498,7 @@
         <v>4557823</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="17.25">
@@ -1497,7 +1506,7 @@
         <v>4569317</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="17.25">
@@ -1505,7 +1514,7 @@
         <v>4569546</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="17.25">
@@ -1513,7 +1522,7 @@
         <v>4572013</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="17.25">
@@ -1521,7 +1530,7 @@
         <v>4584137</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="17.25">
@@ -1529,7 +1538,7 @@
         <v>4596838</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="17.25">
@@ -1537,7 +1546,7 @@
         <v>4609687</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="17.25">
@@ -1545,7 +1554,7 @@
         <v>4611310</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="17.25">
@@ -1553,7 +1562,7 @@
         <v>4620988</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="17.25">
@@ -1561,7 +1570,7 @@
         <v>4648381</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="17.25">
@@ -1569,7 +1578,7 @@
         <v>4651445</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="17.25">
@@ -1577,7 +1586,7 @@
         <v>4672618</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="17.25">
@@ -1585,7 +1594,7 @@
         <v>4682530</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="17.25">
@@ -1593,7 +1602,7 @@
         <v>4682600</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="17.25">
@@ -1601,7 +1610,7 @@
         <v>4691173</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="17.25">
@@ -1609,7 +1618,7 @@
         <v>4721165</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25">
@@ -1617,7 +1626,7 @@
         <v>4726077</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
@@ -1625,7 +1634,7 @@
         <v>4733030</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="17.25">
@@ -1633,7 +1642,7 @@
         <v>4766643</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="17.25">
@@ -1641,7 +1650,7 @@
         <v>4767970</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="17.25">
@@ -1649,7 +1658,7 @@
         <v>4803033</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="17.25">
@@ -1657,7 +1666,7 @@
         <v>4803129</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="17.25">
@@ -1665,7 +1674,7 @@
         <v>4831217</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="17.25">
@@ -1673,7 +1682,7 @@
         <v>4881018</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="17.25">
@@ -1681,7 +1690,7 @@
         <v>4884745</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="17.25">
@@ -1689,7 +1698,7 @@
         <v>4907839</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25">
@@ -1697,7 +1706,7 @@
         <v>4916169</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="17.25">
@@ -1705,7 +1714,7 @@
         <v>4928823</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="17.25">
@@ -1713,7 +1722,7 @@
         <v>4935313</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="17.25">
@@ -1721,7 +1730,7 @@
         <v>4940454</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25">
@@ -1729,7 +1738,7 @@
         <v>4982051</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25">
@@ -1737,7 +1746,7 @@
         <v>5002691</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="17.25">
@@ -1745,7 +1754,7 @@
         <v>5037305</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="17.25">
@@ -1753,7 +1762,7 @@
         <v>5096951</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="17.25">
@@ -1761,7 +1770,7 @@
         <v>5097565</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="17.25">
@@ -1769,7 +1778,7 @@
         <v>5104626</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="17.25">
@@ -1777,7 +1786,7 @@
         <v>5109565</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="17.25">
@@ -1785,7 +1794,7 @@
         <v>5115747</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="17.25">
@@ -1793,7 +1802,7 @@
         <v>5133040</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="17.25">
@@ -1801,7 +1810,7 @@
         <v>5158482</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="17.25">
@@ -1809,7 +1818,7 @@
         <v>5177117</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="17.25">
@@ -1817,7 +1826,7 @@
         <v>5205463</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="17.25">
@@ -1825,7 +1834,7 @@
         <v>5206962</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="17.25">
@@ -1833,7 +1842,7 @@
         <v>5215233</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="17.25">
@@ -1841,7 +1850,7 @@
         <v>5252137</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="17.25">
@@ -1849,7 +1858,7 @@
         <v>5267958</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="17.25">
@@ -1857,7 +1866,7 @@
         <v>5283904</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="17.25">
@@ -1865,7 +1874,7 @@
         <v>5286466</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="17.25">
@@ -1873,7 +1882,7 @@
         <v>5286748</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="17.25">
@@ -1881,7 +1890,7 @@
         <v>5310347</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="17.25">
@@ -1889,159 +1898,159 @@
         <v>5327026</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="17.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="19.5">
       <c r="A131" s="3">
         <v>5361027</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="17.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="19.5">
       <c r="A132" s="3">
         <v>5383814</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="17.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="19.5">
       <c r="A133" s="3">
         <v>5417924</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="17.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="19.5">
       <c r="A134" s="3">
         <v>5446631</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="17.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="19.5">
       <c r="A135" s="3">
         <v>5446631</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="17.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="19.5">
       <c r="A136" s="3">
         <v>5446631</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="17.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="19.5">
       <c r="A137" s="3">
         <v>5446631</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="17.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="19.5">
       <c r="A138" s="3">
         <v>5476222</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="17.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="19.5">
       <c r="A139" s="3">
         <v>5484371</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="17.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="19.5">
       <c r="A140" s="3">
         <v>5511694</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="17.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="19.5">
       <c r="A141" s="3">
         <v>5532709</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="17.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="19.5">
       <c r="A142" s="3">
         <v>5544466</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="17.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="19.5">
       <c r="A143" s="3">
         <v>5547392</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="17.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="19.5">
       <c r="A144" s="3">
         <v>5550621</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="17.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="19.5">
       <c r="A145" s="3">
         <v>5555834</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="17.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="19.5">
       <c r="A146" s="3">
         <v>5556081</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="17.25">
-      <c r="A147" s="3">
-        <v>5587133</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="19.5">
+      <c r="A147" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="17.25">
-      <c r="A148" s="3">
-        <v>5610632</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5">
+      <c r="A148" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="B148" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5">
+      <c r="A149" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="17.25">
-      <c r="A149" s="3">
-        <v>5660133</v>
-      </c>
       <c r="B149" s="4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega funcionalidad para simular frecuencias y plazo y Se corrige error que no permitia actualizar offerRate mediante la funcion setOfferRate
</commit_message>
<xml_diff>
--- a/Json_ofertas.xlsx
+++ b/Json_ofertas.xlsx
@@ -621,7 +621,7 @@
     <col min="2" max="2" style="6" width="82.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>24059</v>
       </c>
@@ -637,7 +637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>189189</v>
       </c>
@@ -645,7 +645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>230009</v>
       </c>
@@ -653,7 +653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>301784</v>
       </c>
@@ -661,7 +661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>653012</v>
       </c>
@@ -669,7 +669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>820117</v>
       </c>
@@ -677,7 +677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>985053</v>
       </c>
@@ -685,7 +685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>1360950</v>
       </c>
@@ -693,7 +693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>1585349</v>
       </c>
@@ -701,7 +701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>1669798</v>
       </c>
@@ -709,7 +709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
         <v>1764064</v>
       </c>
@@ -717,7 +717,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3">
         <v>1823294</v>
       </c>
@@ -725,7 +725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3">
         <v>2352204</v>
       </c>
@@ -733,7 +733,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3">
         <v>2371630</v>
       </c>
@@ -741,7 +741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3">
         <v>2417292</v>
       </c>
@@ -749,7 +749,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3">
         <v>2433653</v>
       </c>

</xml_diff>

<commit_message>
Se actualiza la formula para la ponderación de tasas y como la tasas de cada deuda se obtiene para la ponderacion. Se mejora la forma de calcular los plazos maximos y minimos de CatSimulation
</commit_message>
<xml_diff>
--- a/Json_ofertas.xlsx
+++ b/Json_ofertas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
   <si>
     <t>prospectus_id</t>
   </si>
@@ -22,202 +22,202 @@
     <t>Json</t>
   </si>
   <si>
-    <t>{"Prospecto": 24059, "monto_maximo_cliente": 962287.0, "cuota_externa_total": 41450.0, "capacidad_maxima_pago": 524380.0, "bursolnum": 6149272, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 19056.680029461608, "monto_max": 962287.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6265, "kubo_score": "D3", "comision": 0.0423, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":90000.0, "cuota":6131.0, "saldo":36957.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5894, "fecha_inicio":"2007-09-19", "tipo_deuda":"R", "ahorro_cuota_mensual":43087.999999999905, "ahorro_total":-43087.999999999905, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":2, "monto_otorgado":259758.0, "cuota":0.0, "saldo":316127.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.217, "fecha_inicio":"2021-03-19", "tipo_deuda":"O", "ahorro_cuota_mensual":316126.9999999992, "ahorro_total":-316126.9999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":3, "monto_otorgado":25000.0, "cuota":13291.0, "saldo":6666.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7334, "fecha_inicio":"2022-04-23", "tipo_deuda":"R", "ahorro_cuota_mensual":19956.99999999998, "ahorro_total":-19956.99999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":500000.0, "cuota":20063.0, "saldo":410362.0, "tasa_externa":0.3741, "tasa_kubo":0.3337, "numero_pagos_otorgado":48.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.1793, "fecha_inicio":"2022-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-558.320581278731, "ahorro_total":-26799.387901379087, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":188100.0, "cuota":116.0, "saldo":83383.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5567, "fecha_inicio":"2020-02-11", "tipo_deuda":"R", "ahorro_cuota_mensual":83498.9999999998, "ahorro_total":-83498.9999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":418000.0, "cuota":1.0, "saldo":11913.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9715, "fecha_inicio":"2023-03-09", "tipo_deuda":"R", "ahorro_cuota_mensual":11913.999999999969, "ahorro_total":-11913.999999999969, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":21000.0, "cuota":1050.0, "saldo":7241.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6552, "fecha_inicio":"2013-12-23", "tipo_deuda":"R", "ahorro_cuota_mensual":8290.999999999982, "ahorro_total":-8290.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":200000.0, "cuota":15001.0, "saldo":31618.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":25.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8419, "fecha_inicio":"2021-04-20", "tipo_deuda":"I", "ahorro_cuota_mensual":3224.5802279166437, "ahorro_total":80614.50569791609, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":380000.0, "cuota":39530.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":900.0, "numero_pagos_restante":802.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-02-12", "tipo_deuda":"R", "ahorro_cuota_mensual":39530.0, "ahorro_total":35577000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 189189, "monto_maximo_cliente": 528488.0, "cuota_externa_total": 32607.0, "capacidad_maxima_pago": 220250.0, "bursolnum": 7438900, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 12456.883028022743, "monto_max": 528488.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 50.0, "plazo_min": 4, "tasa": 0.5991, "kubo_score": "D1", "comision": 0.046, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":78000.0, "cuota":4897.0, "saldo":59756.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.2339, "fecha_inicio":"2022-10-27", "tipo_deuda":"I", "ahorro_cuota_mensual":388.6377544747493, "ahorro_total":13990.959161090974, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":1921.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-02-10", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":4, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-10-18", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":15000.0, "cuota":8126.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2015-09-19", "tipo_deuda":"R", "ahorro_cuota_mensual":8126.0, "ahorro_total":-8126.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":80000.0, "cuota":4428.0, "saldo":79840.0, "tasa_externa":0.6591, "tasa_kubo":0.4818, "numero_pagos_otorgado":144.0, "numero_pagos_restante":68.0, "frecuencia_externa":"S", "avance":0.002, "fecha_inicio":"2023-12-04", "tipo_deuda":"I", "ahorro_cuota_mensual":556.0318719877932, "ahorro_total":40034.29478312111, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":50.0, "cuota":53.0, "saldo":51.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.02, "fecha_inicio":"2024-02-17", "tipo_deuda":"I", "ahorro_cuota_mensual":0.6712999999998885, "ahorro_total":0.6712999999998885, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":80000.0, "cuota":4456.0, "saldo":73348.0, "tasa_externa":0.2063, "tasa_kubo":0.4818, "numero_pagos_otorgado":43.0, "numero_pagos_restante":18.0, "frecuencia_externa":"S", "avance":0.0831, "fecha_inicio":"2023-12-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-1433.2382484712107, "ahorro_total":-31531.241466366635, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":80000.0, "cuota":4456.0, "saldo":73348.0, "tasa_externa":0.2063, "tasa_kubo":0.4818, "numero_pagos_otorgado":43.0, "numero_pagos_restante":18.0, "frecuencia_externa":"S", "avance":0.0831, "fecha_inicio":"2023-12-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-1433.2382484712107, "ahorro_total":-31531.241466366635, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":80000.0, "cuota":4428.0, "saldo":79188.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":43.0, "numero_pagos_restante":19.0, "frecuencia_externa":"S", "avance":0.0101, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-1461.2382484712107, "ahorro_total":-32147.241466366635, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":80000.0, "cuota":4428.0, "saldo":79188.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":43.0, "numero_pagos_restante":19.0, "frecuencia_externa":"S", "avance":0.0101, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-1461.2382484712107, "ahorro_total":-32147.241466366635, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":80000.0, "cuota":4428.0, "saldo":79188.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":43.0, "numero_pagos_restante":19.0, "frecuencia_externa":"S", "avance":0.0101, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-1461.2382484712107, "ahorro_total":-32147.241466366635, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":82620.0, "cuota":4131.0, "saldo":46157.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4413, "fecha_inicio":"2019-09-19", "tipo_deuda":"R", "ahorro_cuota_mensual":50288.000000000095, "ahorro_total":-50288.000000000095, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":22000.0, "cuota":5000.0, "saldo":2281.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8963, "fecha_inicio":"2017-04-20", "tipo_deuda":"R", "ahorro_cuota_mensual":7281.000000000005, "ahorro_total":-7281.000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 230009, "monto_maximo_cliente": 135880.0, "cuota_externa_total": 32967.0, "capacidad_maxima_pago": 17133.0, "bursolnum": 7438906, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1286.01193274051, "monto_max": 135880.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 22.0, "plazo_min": 4, "tasa": 0.6509, "kubo_score": "D3", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":45370.0, "cuota":3031.0, "saldo":36745.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.1901, "fecha_inicio":"2022-10-05", "tipo_deuda":"I", "ahorro_cuota_mensual":-180.73289617008595, "ahorro_total":-6506.384262123094, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":12, "monto_otorgado":10000.0, "cuota":1071.0, "saldo":1071.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.8929, "fecha_inicio":"2023-10-31", "tipo_deuda":"O", "ahorro_cuota_mensual":2142.0000000000014, "ahorro_total":-2142.0000000000014, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":1921.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-06-24", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":31, "monto_otorgado":24000.0, "cuota":-1.0, "saldo":17889.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2546, "fecha_inicio":"2021-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":19, "monto_otorgado":1300.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-12-10", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":18, "monto_otorgado":14500.0, "cuota":789.0, "saldo":14198.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0208, "fecha_inicio":"2021-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":8000.0, "cuota":1027.0, "saldo":7847.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0191, "fecha_inicio":"2021-09-21", "tipo_deuda":"R", "ahorro_cuota_mensual":8874.000000000011, "ahorro_total":-8874.000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":16, "monto_otorgado":15100.0, "cuota":1806.0, "saldo":13206.0, "tasa_externa":0.7361, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1254, "fecha_inicio":"2021-10-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-24.030155397507997, "ahorro_total":-288.36186477009596, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":15, "monto_otorgado":30000.0, "cuota":3311.0, "saldo":30069.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0023, "fecha_inicio":"2022-07-25", "tipo_deuda":"R", "ahorro_cuota_mensual":33380.00000000004, "ahorro_total":-33380.00000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":11900.0, "cuota":660.0, "saldo":7377.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3801, "fecha_inicio":"2021-12-11", "tipo_deuda":"R", "ahorro_cuota_mensual":8037.000000000009, "ahorro_total":-8037.000000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":4299.0, "cuota":674.0, "saldo":1272.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7041, "fecha_inicio":"2023-07-27", "tipo_deuda":"I", "ahorro_cuota_mensual":33.89399478476162, "ahorro_total":305.04595306285455, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":2528.0, "cuota":520.0, "saldo":2212.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.125, "fecha_inicio":"2024-01-25", "tipo_deuda":"I", "ahorro_cuota_mensual":1.1727414266006235, "ahorro_total":7.036448559603741, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":1735.0, "cuota":1903.0, "saldo":1875.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0807, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":58.83322166666426, "ahorro_total":58.83322166666426, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":10000.0, "cuota":2660.0, "saldo":2660.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.734, "fecha_inicio":"2023-05-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-7969.2033333333475, "ahorro_total":-7969.2033333333475, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":10000.0, "cuota":2165.0, "saldo":3239.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6761, "fecha_inicio":"2022-04-04", "tipo_deuda":"R", "ahorro_cuota_mensual":5404.000000000004, "ahorro_total":-5404.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":2200.0, "cuota":110.0, "saldo":507.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7695, "fecha_inicio":"2023-08-20", "tipo_deuda":"R", "ahorro_cuota_mensual":5.94722306300892, "ahorro_total":35.68333837805352, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":5100.0, "cuota":795.0, "saldo":6445.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.2637, "fecha_inicio":"2021-08-14", "tipo_deuda":"R", "ahorro_cuota_mensual":7240.000000000008, "ahorro_total":-7240.000000000008, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":19800.0, "cuota":14647.0, "saldo":14647.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2603, "fecha_inicio":"2021-05-24", "tipo_deuda":"R", "ahorro_cuota_mensual":29294.000000000015, "ahorro_total":-29294.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 301784, "monto_maximo_cliente": 619161.0, "cuota_externa_total": 74716.0, "capacidad_maxima_pago": 470623.0, "bursolnum": 7438918, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 12311.431656976296, "monto_max": 619161.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "kubo_scores": ['K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":169900.0, "cuota":4015.0, "saldo":82194.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.5162, "fecha_inicio":"2021-03-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-794.1040235785067, "ahorro_total":-47646.2414147104, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":9, "monto_otorgado":674577.0, "cuota":15783.0, "saldo":642060.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":48.0, "numero_pagos_restante":40.0, "frecuencia_externa":"M", "avance":0.0482, "fecha_inicio":"2023-08-05", "tipo_deuda":"I", "ahorro_cuota_mensual":-5912.170759826469, "ahorro_total":-283784.1964716705, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":100000.0, "cuota":9134.0, "saldo":77867.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":18.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.2213, "fecha_inicio":"2023-08-25", "tipo_deuda":"I", "ahorro_cuota_mensual":2502.8235377328947, "ahorro_total":45050.82367919211, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":171263.0, "cuota":2055.0, "saldo":118095.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":110.0, "numero_pagos_restante":68.0, "frecuencia_externa":"M", "avance":0.3104, "fecha_inicio":"2020-10-21", "tipo_deuda":"M", "ahorro_cuota_mensual":-544.4705958174745, "ahorro_total":-59891.7655399222, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":19, "monto_otorgado":10000.0, "cuota":548.0, "saldo":548.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.9452, "fecha_inicio":"2010-01-27", "tipo_deuda":"O", "ahorro_cuota_mensual":1095.9999999999989, "ahorro_total":-1095.9999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":17, "monto_otorgado":1100.0, "cuota":249.0, "saldo":249.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7736, "fecha_inicio":"2020-09-11", "tipo_deuda":"O", "ahorro_cuota_mensual":497.99999999999955, "ahorro_total":-497.99999999999955, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":18, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2010-02-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":20, "monto_otorgado":10000.0, "cuota":866.0, "saldo":866.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.9134, "fecha_inicio":"2010-01-15", "tipo_deuda":"O", "ahorro_cuota_mensual":1731.9999999999984, "ahorro_total":-1731.9999999999984, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":8000.0, "cuota":11525.0, "saldo":11525.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.4406, "fecha_inicio":"2024-02-23", "tipo_deuda":"I", "ahorro_cuota_mensual":3370.333333333373, "ahorro_total":3370.333333333373, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":16, "monto_otorgado":522372.0, "cuota":6620.0, "saldo":360204.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":110.0, "numero_pagos_restante":68.0, "frecuencia_externa":"M", "avance":0.3104, "fecha_inicio":"2020-10-21", "tipo_deuda":"M", "ahorro_cuota_mensual":-1308.698983833673, "ahorro_total":-143956.88822170405, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":24, "monto_otorgado":11500.0, "cuota":1194.0, "saldo":11039.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0401, "fecha_inicio":"2024-01-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-10058.420666666612, "ahorro_total":-10058.420666666612, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":23, "monto_otorgado":6500.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-11-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":450.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-12-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":151670.0, "cuota":0.0, "saldo":48373.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.6811, "fecha_inicio":"2018-08-27", "tipo_deuda":"O", "ahorro_cuota_mensual":48372.999999999905, "ahorro_total":-48372.999999999905, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":254509.0, "cuota":7819.0, "saldo":210620.0, "tasa_externa":0.2769, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":40.0, "frecuencia_externa":"M", "avance":0.1724, "fecha_inicio":"2022-08-09", "tipo_deuda":"I", "ahorro_cuota_mensual":614.9961392763853, "ahorro_total":36899.76835658312, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":6000.0, "cuota":5181.0, "saldo":1724.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7127, "fecha_inicio":"2023-08-16", "tipo_deuda":"R", "ahorro_cuota_mensual":6904.999999999996, "ahorro_total":-6904.999999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":450.0, "cuota":415.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-12-18", "tipo_deuda":"R", "ahorro_cuota_mensual":415.0, "ahorro_total":-415.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":176537.0, "cuota":5403.0, "saldo":144020.0, "tasa_externa":0.2789, "tasa_kubo":0.2, "numero_pagos_otorgado":61.0, "numero_pagos_restante":40.0, "frecuencia_externa":"M", "avance":0.1842, "fecha_inicio":"2022-07-04", "tipo_deuda":"I", "ahorro_cuota_mensual":449.6318975041986, "ahorro_total":27427.545747756114, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":6000.0, "cuota":423.0, "saldo":4224.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.296, "fecha_inicio":"2020-11-10", "tipo_deuda":"R", "ahorro_cuota_mensual":4646.999999999992, "ahorro_total":-4646.999999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":41900.0, "cuota":2384.0, "saldo":31312.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2527, "fecha_inicio":"2020-11-02", "tipo_deuda":"R", "ahorro_cuota_mensual":33695.99999999994, "ahorro_total":-33695.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":100000.0, "cuota":6310.0, "saldo":77387.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2261, "fecha_inicio":"2021-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":83696.99999999985, "ahorro_total":-83696.99999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":7000.0, "cuota":350.0, "saldo":814.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8837, "fecha_inicio":"2021-07-08", "tipo_deuda":"R", "ahorro_cuota_mensual":1163.9999999999984, "ahorro_total":-1163.9999999999984, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":6500.0, "cuota":325.0, "saldo":5242.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1935, "fecha_inicio":"2024-01-08", "tipo_deuda":"R", "ahorro_cuota_mensual":5566.99999999999, "ahorro_total":-5566.99999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 653012, "monto_maximo_cliente": 1813329.0, "cuota_externa_total": 183771.0, "capacidad_maxima_pago": 1042229.0, "bursolnum": 7438957, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 14987.022334935153, "monto_max": 1813329.0, "cuota_min": 130.08822700780902, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.165, "kubo_score": "A1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.165], "comisiones": [0], "kubo_scores": ['A1'], "deudas_buro": [ {"entidad": "BANCO", "registro":4, "monto_otorgado":8522400.0, "cuota":79258.0, "saldo":8305944.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":240.0, "numero_pagos_restante":223.0, "frecuencia_externa":"M", "avance":0.0254, "fecha_inicio":"2022-11-30", "tipo_deuda":"M", "ahorro_cuota_mensual":-56260.152267569385, "ahorro_total":-13502436.544216651, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":288650.0, "cuota":9416.0, "saldo":44832.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":48.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8447, "fecha_inicio":"2020-07-07", "tipo_deuda":"I", "ahorro_cuota_mensual":763.9920060419372, "ahorro_total":36671.616290012986, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":143000.0, "cuota":4308.0, "saldo":112712.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":48.0, "numero_pagos_restante":32.0, "frecuencia_externa":"M", "avance":0.2118, "fecha_inicio":"2022-12-15", "tipo_deuda":"I", "ahorro_cuota_mensual":21.711612208547194, "ahorro_total":1042.1573860102653, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":150000.0, "cuota":5535.0, "saldo":121797.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":36.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.188, "fecha_inicio":"2023-05-02", "tipo_deuda":"I", "ahorro_cuota_mensual":25.97367264170225, "ahorro_total":935.052215101281, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-08-23", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":242500.0, "cuota":11940.0, "saldo":141785.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":43.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.4153, "fecha_inicio":"2020-10-16", "tipo_deuda":"I", "ahorro_cuota_mensual":-1216.3237714074185, "ahorro_total":-26759.122970963206, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":234500.0, "cuota":798.0, "saldo":1364.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9942, "fecha_inicio":"2018-04-16", "tipo_deuda":"R", "ahorro_cuota_mensual":2162.0000000000064, "ahorro_total":-2162.0000000000064, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":13, "monto_otorgado":798.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-07-18", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":10, "monto_otorgado":257900.0, "cuota":1099.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-07-12", "tipo_deuda":"R", "ahorro_cuota_mensual":1099.0, "ahorro_total":-1099.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":9, "monto_otorgado":83500.0, "cuota":4175.0, "saldo":19376.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.768, "fecha_inicio":"2017-06-02", "tipo_deuda":"R", "ahorro_cuota_mensual":23551.00000000009, "ahorro_total":-23551.00000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":173000.0, "cuota":3039.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-05-22", "tipo_deuda":"R", "ahorro_cuota_mensual":3039.0, "ahorro_total":-3039.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":500000.0, "cuota":27056.0, "saldo":466374.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":43.0, "numero_pagos_restante":10.0, "frecuencia_externa":"S", "avance":0.0673, "fecha_inicio":"2023-04-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-70.44076578849126, "ahorro_total":-1549.6968473468078, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":900000.0, "cuota":40703.0, "saldo":823395.0, "tasa_externa":0.4562, "tasa_kubo":0.165, "numero_pagos_otorgado":48.0, "numero_pagos_restante":39.0, "frecuencia_externa":"M", "avance":0.0851, "fecha_inicio":"2023-07-12", "tipo_deuda":"I", "ahorro_cuota_mensual":13726.35979711673, "ahorro_total":658865.270261603, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":185000.0, "cuota":9250.0, "saldo":60938.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6706, "fecha_inicio":"2018-07-31", "tipo_deuda":"R", "ahorro_cuota_mensual":70188.00000000029, "ahorro_total":-70188.00000000029, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":312635.0, "cuota":0.0, "saldo":222709.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.2876, "fecha_inicio":"2019-07-31", "tipo_deuda":"O", "ahorro_cuota_mensual":222709.0000000011, "ahorro_total":-222709.0000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":15, "monto_otorgado":172500.0, "cuota":8625.0, "saldo":108942.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3685, "fecha_inicio":"2014-03-13", "tipo_deuda":"R", "ahorro_cuota_mensual":117567.00000000052, "ahorro_total":-117567.00000000052, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 820117, "monto_maximo_cliente": 667576.0, "cuota_externa_total": 87443.0, "capacidad_maxima_pago": 56917.0, "bursolnum": 7438981, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5328.82868046942, "monto_max": 667576.0, "cuota_min": 227.39637225020516, "monto_min": 5000, "plazo_max": 24.0, "plazo_min": 4, "tasa": 0.4295, "kubo_score": "B1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":24, "monto_otorgado":41000.0, "cuota":2587.0, "saldo":34444.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1599, "fecha_inicio":"2023-05-04", "tipo_deuda":"R", "ahorro_cuota_mensual":37030.99999999998, "ahorro_total":-37030.99999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "GOBIERNO", "registro":30, "monto_otorgado":1.0, "cuota":-1.0, "saldo":1.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0, "fecha_inicio":"2014-10-01", "tipo_deuda":"R", "ahorro_cuota_mensual":-5.551115123125783e-16, "ahorro_total":5.551115123125783e-16, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":135796.0, "cuota":1758.0, "saldo":117416.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":120.0, "numero_pagos_restante":46.0, "frecuencia_externa":"S", "avance":0.1354, "fecha_inicio":"2023-02-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-4417.903553217772, "ahorro_total":-265074.21319306636, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":23, "monto_otorgado":19522.0, "cuota":3217.0, "saldo":9053.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":7.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5363, "fecha_inicio":"2023-10-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-53.82695757631336, "ahorro_total":-376.78870303419353, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":787641.0, "cuota":9310.0, "saldo":557181.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":120.0, "numero_pagos_restante":43.0, "frecuencia_externa":"S", "avance":0.2926, "fecha_inicio":"2022-11-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-26511.34120710477, "ahorro_total":-1590680.4724262862, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":22, "monto_otorgado":55617.0, "cuota":3980.0, "saldo":48884.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":21.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1211, "fecha_inicio":"2023-10-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-40.01721536074774, "ahorro_total":-840.3615225757026, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":29, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"1950-01-01", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":632433.0, "cuota":8848.0, "saldo":544965.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":120.0, "numero_pagos_restante":44.0, "frecuencia_externa":"S", "avance":0.1383, "fecha_inicio":"2022-12-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-19914.5939782628, "ahorro_total":-1194875.638695768, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MIC CREDITO PERS", "registro":21, "monto_otorgado":281000.0, "cuota":25168.0, "saldo":390182.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":36.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":-0.3885, "fecha_inicio":"2023-10-31", "tipo_deuda":"I", "ahorro_cuota_mensual":9992.822329783108, "ahorro_total":359741.6038721919, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":19, "monto_otorgado":15480.0, "cuota":1215.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-07-21", "tipo_deuda":"R", "ahorro_cuota_mensual":1215.0, "ahorro_total":-1215.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":18, "monto_otorgado":107100.0, "cuota":11000.0, "saldo":91427.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1463, "fecha_inicio":"2023-03-13", "tipo_deuda":"R", "ahorro_cuota_mensual":102426.99999999994, "ahorro_total":-102426.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":10000.0, "cuota":9045.0, "saldo":9045.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0955, "fecha_inicio":"2023-06-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-1370.1833333333343, "ahorro_total":-1370.1833333333343, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":16, "monto_otorgado":123830.0, "cuota":11859.0, "saldo":49227.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6025, "fecha_inicio":"2015-01-02", "tipo_deuda":"R", "ahorro_cuota_mensual":61085.99999999997, "ahorro_total":-61085.99999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":15, "monto_otorgado":80000.0, "cuota":5956.0, "saldo":76845.0, "tasa_externa":0.5727, "tasa_kubo":0.4295, "numero_pagos_otorgado":43.0, "numero_pagos_restante":11.0, "frecuencia_externa":"S", "avance":0.0394, "fecha_inicio":"2023-05-05", "tipo_deuda":"I", "ahorro_cuota_mensual":339.4593671993298, "ahorro_total":7468.106078385255, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":14, "monto_otorgado":107200.0, "cuota":5715.0, "saldo":84126.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2152, "fecha_inicio":"2021-06-28", "tipo_deuda":"R", "ahorro_cuota_mensual":89840.99999999994, "ahorro_total":-89840.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":71600.0, "cuota":146.0, "saldo":13409.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8127, "fecha_inicio":"2020-11-26", "tipo_deuda":"R", "ahorro_cuota_mensual":13554.999999999993, "ahorro_total":-13554.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":12, "monto_otorgado":109991.0, "cuota":0.0, "saldo":23942.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7823, "fecha_inicio":"2022-09-30", "tipo_deuda":"O", "ahorro_cuota_mensual":23941.999999999985, "ahorro_total":-23941.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":20, "monto_otorgado":9270.0, "cuota":340.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-04-26", "tipo_deuda":"R", "ahorro_cuota_mensual":340.0, "ahorro_total":-340.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 985053, "monto_maximo_cliente": 134184.0, "cuota_externa_total": 18240.0, "capacidad_maxima_pago": 83520.0, "bursolnum": 6636993, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5293.744643303981, "monto_max": 134184.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.6755, "kubo_score": "D5", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":64, "monto_otorgado":100.0, "cuota":104.0, "saldo":104.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.04, "fecha_inicio":"2023-04-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.479066666666668, "ahorro_total":-1.479066666666668, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-03-01", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":19000.0, "cuota":1796.0, "saldo":16658.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1233, "fecha_inicio":"2023-03-21", "tipo_deuda":"I", "ahorro_cuota_mensual":109.2294268178116, "ahorro_total":1966.1296827206088, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-01-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":65, "monto_otorgado":500.0, "cuota":518.0, "saldo":518.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.036, "fecha_inicio":"2023-04-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-9.395333333333383, "ahorro_total":-9.395333333333383, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":63, "monto_otorgado":299.0, "cuota":60.0, "saldo":292.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0234, "fecha_inicio":"2023-03-30", "tipo_deuda":"I", "ahorro_cuota_mensual":0.18620403727186385, "ahorro_total":1.1172242236311831, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":70000.0, "cuota":6788.0, "saldo":44302.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.3671, "fecha_inicio":"2022-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":61, "monto_otorgado":417.0, "cuota":155.0, "saldo":306.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2662, "fecha_inicio":"2023-03-22", "tipo_deuda":"I", "ahorro_cuota_mensual":0.4974897121670381, "ahorro_total":1.4924691365011142, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":17000.0, "cuota":1616.0, "saldo":14155.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1674, "fecha_inicio":"2023-05-29", "tipo_deuda":"R", "ahorro_cuota_mensual":15771.000000000004, "ahorro_total":-15771.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":62, "monto_otorgado":512.0, "cuota":188.0, "saldo":371.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2754, "fecha_inicio":"2023-03-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.7009239025670695, "ahorro_total":-5.1027717077012085, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":60400.0, "cuota":3020.0, "saldo":35020.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4202, "fecha_inicio":"2019-12-17", "tipo_deuda":"R", "ahorro_cuota_mensual":38040.00000000001, "ahorro_total":-38040.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":80000.0, "cuota":5900.0, "saldo":79434.0, "tasa_externa":0.56, "tasa_kubo":0.5668, "numero_pagos_otorgado":43.0, "numero_pagos_restante":12.0, "frecuencia_externa":"S", "avance":0.0071, "fecha_inicio":"2023-06-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-445.85407781089634, "ahorro_total":-9808.78971183972, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":19700.0, "cuota":985.0, "saldo":3181.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8385, "fecha_inicio":"2022-12-29", "tipo_deuda":"R", "ahorro_cuota_mensual":4166.000000000001, "ahorro_total":-4166.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 1360950, "monto_maximo_cliente": 70378.0, "cuota_externa_total": 33180.0, "capacidad_maxima_pago": 17920.0, "bursolnum": 7439045, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2842.5496999139004, "monto_max": 70378.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 15.0, "plazo_min": 4, "tasa": 0.4818, "kubo_score": "B5", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":53000.0, "cuota":3724.0, "saldo":22085.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5833, "fecha_inicio":"2022-09-19", "tipo_deuda":"I", "ahorro_cuota_mensual":10.032892732850996, "ahorro_total":240.7894255884239, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":36000.0, "cuota":2628.0, "saldo":25338.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":24.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.2962, "fecha_inicio":"2023-03-09", "tipo_deuda":"I", "ahorro_cuota_mensual":105.30536110155936, "ahorro_total":2527.3286664374245, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-09-19", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":871.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-01-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-01-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":871.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-01-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-11-24", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":12863.0, "cuota":4248.0, "saldo":2872.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":13.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.7767, "fecha_inicio":"2023-12-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-445.11245256584425, "ahorro_total":-1335.3373576975328, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":30200.0, "cuota":3374.0, "saldo":13928.0, "tasa_externa":0.5872, "tasa_kubo":0.4818, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5388, "fecha_inicio":"2021-07-26", "tipo_deuda":"I", "ahorro_cuota_mensual":32.19289597740044, "ahorro_total":386.3147517288053, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":24100.0, "cuota":1640.0, "saldo":23315.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0326, "fecha_inicio":"2022-05-12", "tipo_deuda":"R", "ahorro_cuota_mensual":24955.00000000005, "ahorro_total":-24955.00000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":4000.0, "cuota":17566.0, "saldo":17566.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-3.3915, "fecha_inicio":"2023-10-31", "tipo_deuda":"I", "ahorro_cuota_mensual":13379.70399999999, "ahorro_total":13379.70399999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 1585349, "monto_maximo_cliente": 209409.0, "cuota_externa_total": 21707.0, "capacidad_maxima_pago": 57635.0, "bursolnum": 7439082, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1739.1926046159667, "monto_max": 209409.0, "cuota_min": 151.9292154681686, "monto_min": 5000, "plazo_max": 58.0, "plazo_min": 4, "tasa": 0.4428, "kubo_score": "B2", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2306, 0.2], "comisiones": [0.03845, 0.03845], "kubo_scores": ['K2', 'K1'], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":9, "monto_otorgado":730.0, "cuota":730.0, "saldo":730.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2005-07-20", "tipo_deuda":"O", "ahorro_cuota_mensual":1459.9999999999968, "ahorro_total":-1459.9999999999968, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":22300.0, "cuota":1821.0, "saldo":11086.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5029, "fecha_inicio":"2023-03-07", "tipo_deuda":"I", "ahorro_cuota_mensual":303.4093495857137, "ahorro_total":5461.368292542847, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":67700.0, "cuota":5570.0, "saldo":45023.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":18.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.335, "fecha_inicio":"2023-06-13", "tipo_deuda":"I", "ahorro_cuota_mensual":962.7853348409326, "ahorro_total":17330.13602713679, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-03-09", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":7000.0, "cuota":838.0, "saldo":5448.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2217, "fecha_inicio":"2022-10-01", "tipo_deuda":"I", "ahorro_cuota_mensual":166.73313373753047, "ahorro_total":2000.7976048503656, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":14700.0, "cuota":1756.0, "saldo":12505.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1493, "fecha_inicio":"2022-11-02", "tipo_deuda":"I", "ahorro_cuota_mensual":346.33958084881397, "ahorro_total":4156.074970185768, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":31, "monto_otorgado":100.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-07-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":6000.0, "cuota":1055.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-12-05", "tipo_deuda":"R", "ahorro_cuota_mensual":1055.0, "ahorro_total":-1055.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":30000.0, "cuota":4540.0, "saldo":21572.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2809, "fecha_inicio":"2023-12-24", "tipo_deuda":"I", "ahorro_cuota_mensual":824.2306660563095, "ahorro_total":7418.075994506786, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":56300.0, "cuota":2332.0, "saldo":49172.0, "tasa_externa":0.3893, "tasa_kubo":0.2306, "numero_pagos_otorgado":47.0, "numero_pagos_restante":36.0, "frecuencia_externa":"M", "avance":0.1266, "fecha_inicio":"2023-06-01", "tipo_deuda":"I", "ahorro_cuota_mensual":386.8475546279644, "ahorro_total":18181.835067514327, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":11500.0, "cuota":812.0, "saldo":2921.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.746, "fecha_inicio":"2019-07-16", "tipo_deuda":"I", "ahorro_cuota_mensual":-483.6514684575052, "ahorro_total":-4836.514684575051, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":95000.0, "cuota":4750.0, "saldo":89707.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0557, "fecha_inicio":"2022-04-20", "tipo_deuda":"R", "ahorro_cuota_mensual":94456.99999999962, "ahorro_total":-94456.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":16700.0, "cuota":1125.0, "saldo":202.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9879, "fecha_inicio":"2018-02-21", "tipo_deuda":"R", "ahorro_cuota_mensual":1326.999999999999, "ahorro_total":-1326.999999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 1669798, "monto_maximo_cliente": 149281.0, "cuota_externa_total": 22802.0, "capacidad_maxima_pago": 49020.0, "bursolnum": 6320398, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1866.531573393356, "monto_max": 149281.0, "cuota_min": 130.08822700780902, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.165, "kubo_score": "A1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.165], "comisiones": [0], "kubo_scores": ['A1'], "deudas_buro": [ {"entidad": "HIPOTECAGOBIERNO", "registro":27, "monto_otorgado":1129549.0, "cuota":11548.0, "saldo":1140349.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":360.0, "numero_pagos_restante":334.0, "frecuencia_externa":"M", "avance":-0.0096, "fecha_inicio":"2022-02-14", "tipo_deuda":"M", "ahorro_cuota_mensual":-6701.832391336702, "ahorro_total":-2412659.660881213, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":39914.0, "cuota":2304.0, "saldo":37601.0, "tasa_externa":0.4359, "tasa_kubo":0.165, "numero_pagos_otorgado":104.0, "numero_pagos_restante":13.0, "frecuencia_externa":"W", "avance":0.0579, "fecha_inicio":"2023-03-25", "tipo_deuda":"I", "ahorro_cuota_mensual":416.55557235886386, "ahorro_total":10830.44488133046, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":26, "monto_otorgado":400.0, "cuota":81.0, "saldo":397.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0075, "fecha_inicio":"2023-04-16", "tipo_deuda":"I", "ahorro_cuota_mensual":10.56259744570842, "ahorro_total":63.37558467425052, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":25, "monto_otorgado":6000.0, "cuota":1234.0, "saldo":6022.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0037, "fecha_inicio":"2023-04-11", "tipo_deuda":"I", "ahorro_cuota_mensual":177.4389616856265, "ahorro_total":1064.633770113759, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":24, "monto_otorgado":392.0, "cuota":147.0, "saldo":291.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2577, "fecha_inicio":"2023-04-06", "tipo_deuda":"I", "ahorro_cuota_mensual":12.143081178895471, "ahorro_total":36.429243536686414, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":23, "monto_otorgado":549.0, "cuota":209.0, "saldo":412.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2495, "fecha_inicio":"2023-03-31", "tipo_deuda":"I", "ahorro_cuota_mensual":20.13150910003472, "ahorro_total":60.39452730010416, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":22, "monto_otorgado":286.0, "cuota":109.0, "saldo":216.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2448, "fecha_inicio":"2023-03-27", "tipo_deuda":"I", "ahorro_cuota_mensual":10.609492900928842, "ahorro_total":31.828478702786526, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":21, "monto_otorgado":1125.0, "cuota":416.0, "saldo":416.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6302, "fecha_inicio":"2023-03-13", "tipo_deuda":"I", "ahorro_cuota_mensual":28.974403893513795, "ahorro_total":86.92321168054139, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":20, "monto_otorgado":394.0, "cuota":80.0, "saldo":314.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.203, "fecha_inicio":"2023-03-11", "tipo_deuda":"I", "ahorro_cuota_mensual":10.61915848402279, "ahorro_total":63.71495090413674, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":388.0, "cuota":79.0, "saldo":310.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.201, "fecha_inicio":"2023-03-09", "tipo_deuda":"I", "ahorro_cuota_mensual":10.675719522337175, "ahorro_total":64.05431713402305, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":18, "monto_otorgado":300.0, "cuota":112.0, "saldo":112.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6267, "fecha_inicio":"2023-03-10", "tipo_deuda":"I", "ahorro_cuota_mensual":8.79317437160367, "ahorro_total":26.379523114811008, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":375.0, "cuota":78.0, "saldo":78.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.792, "fecha_inicio":"2022-12-19", "tipo_deuda":"I", "ahorro_cuota_mensual":11.964935105351657, "ahorro_total":71.78961063210994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":16, "monto_otorgado":344.0, "cuota":71.0, "saldo":277.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1948, "fecha_inicio":"2023-03-05", "tipo_deuda":"I", "ahorro_cuota_mensual":10.423833803309243, "ahorro_total":62.54300281985546, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":29400.0, "cuota":1470.0, "saldo":16303.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4455, "fecha_inicio":"2021-09-23", "tipo_deuda":"R", "ahorro_cuota_mensual":17773.00000000008, "ahorro_total":-17773.00000000008, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":15000.0, "cuota":750.0, "saldo":6143.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5905, "fecha_inicio":"2022-12-09", "tipo_deuda":"R", "ahorro_cuota_mensual":6893.00000000003, "ahorro_total":-6893.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":50822.0, "cuota":2405.0, "saldo":45008.0, "tasa_externa":0.3918, "tasa_kubo":0.165, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.1144, "fecha_inicio":"2022-10-17", "tipo_deuda":"I", "ahorro_cuota_mensual":538.468426606644, "ahorro_total":19384.863357839185, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":47600.0, "cuota":2380.0, "saldo":33691.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2922, "fecha_inicio":"2021-03-08", "tipo_deuda":"R", "ahorro_cuota_mensual":36071.00000000016, "ahorro_total":-36071.00000000016, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":17950.0, "cuota":-1.0, "saldo":14235.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.207, "fecha_inicio":"2020-05-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":299.0, "cuota":47.0, "saldo":47.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8428, "fecha_inicio":"2022-09-04", "tipo_deuda":"I", "ahorro_cuota_mensual":11.072423867181918, "ahorro_total":99.65181480463727, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":3000.0, "cuota":401.0, "saldo":1952.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3493, "fecha_inicio":"2022-09-28", "tipo_deuda":"I", "ahorro_cuota_mensual":124.32977798344541, "ahorro_total":1491.957335801345, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":17950.0, "cuota":2955.0, "saldo":14235.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.207, "fecha_inicio":"2020-05-11", "tipo_deuda":"R", "ahorro_cuota_mensual":17190.00000000007, "ahorro_total":-17190.00000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 1764064, "monto_maximo_cliente": 365624.0, "cuota_externa_total": 52270.0, "capacidad_maxima_pago": 63301.0, "bursolnum": 7439111, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1892.072695856917, "monto_max": 365624.0, "cuota_min": 130.08822700780902, "monto_min": 5000, "plazo_max": 37.0, "plazo_min": 4, "tasa": 0.165, "kubo_score": "A1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.165], "comisiones": [0], "kubo_scores": ['A1'], "deudas_buro": [ {"entidad": "AUTOMOTRIZ", "registro":3, "monto_otorgado":417995.0, "cuota":13068.0, "saldo":313638.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":36.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.2497, "fecha_inicio":"2023-04-16", "tipo_deuda":"I", "ahorro_cuota_mensual":-2283.6363980275437, "ahorro_total":-82210.91032899157, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":13, "monto_otorgado":100000.0, "cuota":8572.0, "saldo":63537.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":24.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.3646, "fecha_inicio":"2022-12-06", "tipo_deuda":"I", "ahorro_cuota_mensual":3524.3337414679263, "ahorro_total":84584.00979523023, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":9, "monto_otorgado":801020.0, "cuota":16577.0, "saldo":779049.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":72.0, "numero_pagos_restante":67.0, "frecuencia_externa":"M", "avance":0.0274, "fecha_inicio":"2023-12-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-2212.484525087337, "ahorro_total":-159298.88580628825, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2005-06-18", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":49169.0, "cuota":2334.0, "saldo":33288.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":32.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.323, "fecha_inicio":"2022-12-09", "tipo_deuda":"I", "ahorro_cuota_mensual":360.1716700839577, "ahorro_total":11525.493442686646, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-05-14", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-11-15", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":17, "monto_otorgado":41800.0, "cuota":2090.0, "saldo":43716.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0458, "fecha_inicio":"2016-03-11", "tipo_deuda":"R", "ahorro_cuota_mensual":45806.00000000021, "ahorro_total":-45806.00000000021, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":5, "monto_otorgado":30202.0, "cuota":0.0, "saldo":4150.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.8626, "fecha_inicio":"2016-04-06", "tipo_deuda":"O", "ahorro_cuota_mensual":4150.00000000002, "ahorro_total":-4150.00000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":15, "monto_otorgado":52571.0, "cuota":2395.0, "saldo":30301.0, "tasa_externa":0.3606, "tasa_kubo":0.165, "numero_pagos_otorgado":36.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.4236, "fecha_inicio":"2022-06-20", "tipo_deuda":"I", "ahorro_cuota_mensual":464.23317962964643, "ahorro_total":16712.394466667272, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":12800.0, "cuota":823.0, "saldo":10120.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2094, "fecha_inicio":"2020-09-23", "tipo_deuda":"R", "ahorro_cuota_mensual":10943.00000000005, "ahorro_total":-10943.00000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":109800.0, "cuota":905.0, "saldo":104474.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0485, "fecha_inicio":"2018-12-11", "tipo_deuda":"R", "ahorro_cuota_mensual":105379.0000000005, "ahorro_total":-105379.0000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":76000.0, "cuota":5796.0, "saldo":63719.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1616, "fecha_inicio":"2022-06-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-2486.528497391646, "ahorro_total":-24865.28497391646, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":2, "monto_otorgado":51000.0, "cuota":4500.0, "saldo":35510.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3037, "fecha_inicio":"2018-02-02", "tipo_deuda":"R", "ahorro_cuota_mensual":40010.000000000175, "ahorro_total":-40010.000000000175, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":40000.0, "cuota":2000.0, "saldo":7788.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8053, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":9788.000000000036, "ahorro_total":-9788.000000000036, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":16, "monto_otorgado":36900.0, "cuota":1904.0, "saldo":31295.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1519, "fecha_inicio":"2019-06-13", "tipo_deuda":"R", "ahorro_cuota_mensual":33199.000000000146, "ahorro_total":-33199.000000000146, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 1823294, "monto_maximo_cliente": 486133.0, "cuota_externa_total": 27020.0, "capacidad_maxima_pago": 417980.0, "bursolnum": 7439123, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 14506.941526394074, "monto_max": 486133.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":9, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2016-01-14", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1493.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-01-20", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":128100.0, "cuota":7315.0, "saldo":76840.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":12.0, "frecuencia_externa":"M", "avance":0.4002, "fecha_inicio":"2022-04-05", "tipo_deuda":"I", "ahorro_cuota_mensual":1606.7586620762522, "ahorro_total":57843.31183474508, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":59000.0, "cuota":2950.0, "saldo":25046.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5755, "fecha_inicio":"2015-01-05", "tipo_deuda":"R", "ahorro_cuota_mensual":27995.99999999993, "ahorro_total":-27995.99999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":415000.0, "cuota":15286.0, "saldo":375484.0, "tasa_externa":0.3185, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":39.0, "frecuencia_externa":"M", "avance":0.0952, "fecha_inicio":"2023-07-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-588.0634589149104, "ahorro_total":-28227.046027915698, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":131100.0, "cuota":1000.0, "saldo":24391.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.814, "fecha_inicio":"2018-03-26", "tipo_deuda":"R", "ahorro_cuota_mensual":25390.999999999935, "ahorro_total":-25390.999999999935, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":30000.0, "cuota":400.0, "saldo":990.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.967, "fecha_inicio":"2013-07-01", "tipo_deuda":"R", "ahorro_cuota_mensual":1389.9999999999973, "ahorro_total":-1389.9999999999973, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":15100.0, "cuota":522.0, "saldo":96.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9936, "fecha_inicio":"2021-12-21", "tipo_deuda":"R", "ahorro_cuota_mensual":617.9999999999998, "ahorro_total":-617.9999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":28792.0, "cuota":1769.0, "saldo":20610.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2842, "fecha_inicio":"2016-04-05", "tipo_deuda":"R", "ahorro_cuota_mensual":22378.999999999945, "ahorro_total":-22378.999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 2352204, "monto_maximo_cliente": 867997.0, "cuota_externa_total": 24592.0, "capacidad_maxima_pago": 586213.0, "bursolnum": 7439208, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 14280.87913700196, "monto_max": 867997.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.2914, "kubo_score": "A2", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "kubo_scores": ['K1'], "deudas_buro": [ {"entidad": "CIA Q' OTORGA", "registro":8, "monto_otorgado":356776.0, "cuota":0.0, "saldo":169286.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.5255, "fecha_inicio":"2013-08-03", "tipo_deuda":"O", "ahorro_cuota_mensual":169285.99999999968, "ahorro_total":-169285.99999999968, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":42675.0, "cuota":1878.0, "saldo":20079.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":38.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.5295, "fecha_inicio":"2022-01-26", "tipo_deuda":"I", "ahorro_cuota_mensual":282.0340888185283, "ahorro_total":10717.295375104075, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":50200.0, "cuota":2943.0, "saldo":18390.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6337, "fecha_inicio":"2022-09-29", "tipo_deuda":"I", "ahorro_cuota_mensual":308.87280225560244, "ahorro_total":7412.9472541344585, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":28, "monto_otorgado":9999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2006-10-07", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":39000.0, "cuota":2540.0, "saldo":28885.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2594, "fecha_inicio":"2005-09-01", "tipo_deuda":"R", "ahorro_cuota_mensual":31424.999999999945, "ahorro_total":-31424.999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":12000.0, "cuota":2500.0, "saldo":10830.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0975, "fecha_inicio":"2017-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":13329.99999999998, "ahorro_total":-13329.99999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":5, "monto_otorgado":35000.0, "cuota":2471.0, "saldo":30995.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1144, "fecha_inicio":"2006-09-14", "tipo_deuda":"R", "ahorro_cuota_mensual":33465.99999999994, "ahorro_total":-33465.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":9000.0, "cuota":450.0, "saldo":5746.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3616, "fecha_inicio":"2005-07-24", "tipo_deuda":"R", "ahorro_cuota_mensual":6195.999999999988, "ahorro_total":-6195.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":5000.0, "cuota":253.0, "saldo":2501.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4998, "fecha_inicio":"2012-04-09", "tipo_deuda":"R", "ahorro_cuota_mensual":2753.9999999999955, "ahorro_total":-2753.9999999999955, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":2, "monto_otorgado":213238.0, "cuota":0.0, "saldo":60363.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7169, "fecha_inicio":"2012-12-07", "tipo_deuda":"O", "ahorro_cuota_mensual":60362.99999999988, "ahorro_total":-60362.99999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":12000.0, "cuota":-1.0, "saldo":9391.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2174, "fecha_inicio":"2017-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":550000.0, "cuota":14085.0, "saldo":540423.0, "tasa_externa":0.2313, "tasa_kubo":0.2, "numero_pagos_otorgado":72.0, "numero_pagos_restante":69.0, "frecuencia_externa":"M", "avance":0.0174, "fecha_inicio":"2024-01-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-128.82499086995813, "ahorro_total":-9275.399342636985, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 2371630, "monto_maximo_cliente": 139935.0, "cuota_externa_total": 27210.0, "capacidad_maxima_pago": 59999.0, "bursolnum": 7439210, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2088.9021652901893, "monto_max": 139935.0, "cuota_min": 163.04445621498797, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.4818, "kubo_score": "B5", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2622, 0.2306, 0.2], "comisiones": [0.03845, 0.03845, 0.03845], "kubo_scores": ['K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "FONDOS Y FIDEIC", "registro":16, "monto_otorgado":235954.0, "cuota":11798.0, "saldo":51714.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":40.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.7808, "fecha_inicio":"2015-08-26", "tipo_deuda":"R", "ahorro_cuota_mensual":9725.886891565617, "ahorro_total":389035.4756626247, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":13, "monto_otorgado":1298.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-04-12", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":21000.0, "cuota":1222.0, "saldo":13279.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":36.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.3677, "fecha_inicio":"2022-07-27", "tipo_deuda":"I", "ahorro_cuota_mensual":325.73450352235034, "ahorro_total":11726.442126804612, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":49000.0, "cuota":3445.0, "saldo":27469.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":24.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.4394, "fecha_inicio":"2022-12-16", "tipo_deuda":"I", "ahorro_cuota_mensual":694.7884722352364, "ahorro_total":16674.923333645675, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":1800.0, "cuota":1575.0, "saldo":1575.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.125, "fecha_inicio":"2023-03-20", "tipo_deuda":"O", "ahorro_cuota_mensual":3149.999999999992, "ahorro_total":-3149.999999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":26, "monto_otorgado":4700.0, "cuota":1709.0, "saldo":3124.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3353, "fecha_inicio":"2023-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":62.253326361783365, "ahorro_total":186.7599790853501, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":22, "monto_otorgado":20000.0, "cuota":1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2013-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "OTRAS FINANCIERA", "registro":18, "monto_otorgado":0.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-1.0, "fecha_inicio":"2020-02-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":18232.0, "cuota":1.0, "saldo":1.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9999, "fecha_inicio":"2021-08-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-777.1291681800243, "ahorro_total":-27976.650054480873, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":14, "monto_otorgado":3000.0, "cuota":364.0, "saldo":2830.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0567, "fecha_inicio":"2022-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":3193.9999999999854, "ahorro_total":-3193.9999999999854, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":779.0, "cuota":290.0, "saldo":516.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3376, "fecha_inicio":"2024-02-18", "tipo_deuda":"I", "ahorro_cuota_mensual":17.06049813528284, "ahorro_total":51.181494405848525, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":797.0, "cuota":301.0, "saldo":536.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3275, "fecha_inicio":"2024-02-11", "tipo_deuda":"I", "ahorro_cuota_mensual":21.753808746881134, "ahorro_total":65.2614262406434, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":3000.0, "cuota":1236.0, "saldo":1099.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6337, "fecha_inicio":"2024-01-06", "tipo_deuda":"I", "ahorro_cuota_mensual":184.88510193305342, "ahorro_total":554.6553057991603, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":3000.0, "cuota":755.0, "saldo":2278.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2407, "fecha_inicio":"2023-12-24", "tipo_deuda":"I", "ahorro_cuota_mensual":209.71967113557582, "ahorro_total":1258.318026813455, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":57000.0, "cuota":2667.0, "saldo":42813.0, "tasa_externa":0.3825, "tasa_kubo":0.2622, "numero_pagos_otorgado":36.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.2489, "fecha_inicio":"2023-04-04", "tipo_deuda":"I", "ahorro_cuota_mensual":234.2793667035221, "ahorro_total":8434.057201326796, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":45500.0, "cuota":3240.0, "saldo":44206.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0284, "fecha_inicio":"2019-07-03", "tipo_deuda":"R", "ahorro_cuota_mensual":47445.99999999977, "ahorro_total":-47445.99999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":100000.0, "cuota":5391.0, "saldo":5391.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9461, "fecha_inicio":"2022-08-03", "tipo_deuda":"O", "ahorro_cuota_mensual":5029.9673278195405, "ahorro_total":95569.37922857127, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 2417292, "monto_maximo_cliente": 180701.0, "cuota_externa_total": 25756.0, "capacidad_maxima_pago": 98866.0, "bursolnum": 7439212, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2560.7719869453163, "monto_max": 180701.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":3, "monto_otorgado":275295.0, "cuota":7607.0, "saldo":270472.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":44.0, "frecuencia_externa":"M", "avance":0.0175, "fecha_inicio":"2023-12-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-2923.2416865589894, "ahorro_total":-140315.6009548315, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":66376.0, "cuota":3504.0, "saldo":49592.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":45.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.2529, "fecha_inicio":"2022-03-03", "tipo_deuda":"I", "ahorro_cuota_mensual":883.5556335192136, "ahorro_total":39760.003508364614, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":20000.0, "cuota":398.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-02-22", "tipo_deuda":"O", "ahorro_cuota_mensual":398.0, "ahorro_total":-398.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-04-02", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":4000.0, "cuota":5762.0, "saldo":5762.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.4405, "fecha_inicio":"2024-03-02", "tipo_deuda":"I", "ahorro_cuota_mensual":1649.3253333333432, "ahorro_total":1649.3253333333432, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":66272.0, "cuota":3085.0, "saldo":19180.0, "tasa_externa":0.3782, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7106, "fecha_inicio":"2021-09-27", "tipo_deuda":"I", "ahorro_cuota_mensual":131.86518386508487, "ahorro_total":4747.146619143055, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":84000.0, "cuota":5399.0, "saldo":75288.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1037, "fecha_inicio":"2023-01-19", "tipo_deuda":"R", "ahorro_cuota_mensual":80686.9999999998, "ahorro_total":-80686.9999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":38000.0, "cuota":1900.0, "saldo":35141.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0752, "fecha_inicio":"2019-09-12", "tipo_deuda":"R", "ahorro_cuota_mensual":37040.999999999905, "ahorro_total":-37040.999999999905, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-1.0, "fecha_inicio":"2024-02-01", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 2433653, "monto_maximo_cliente": 21803.0, "cuota_externa_total": 3187.0, "capacidad_maxima_pago": 19013.0, "bursolnum": 7439215, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 894.9272142949885, "monto_max": 21803.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 23.0, "plazo_min": 4, "tasa": 0.5668, "kubo_score": "C5", "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":4000.0, "cuota":50.0, "saldo":118.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9705, "fecha_inicio":"2023-10-07", "tipo_deuda":"R", "ahorro_cuota_mensual":167.99999999999966, "ahorro_total":-167.99999999999966, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":15000.0, "cuota":1426.0, "saldo":1426.0, "tasa_externa":0.2539, "tasa_kubo":0.2914, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9049, "fecha_inicio":"2023-03-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-64.5047822291242, "ahorro_total":-774.0573867494904, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":11000.0, "cuota":550.0, "saldo":2147.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8048, "fecha_inicio":"2024-01-30", "tipo_deuda":"R", "ahorro_cuota_mensual":2696.999999999994, "ahorro_total":-2696.999999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":7500.0, "cuota":375.0, "saldo":4538.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3949, "fecha_inicio":"2021-03-29", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":12000.0, "cuota":1419.0, "saldo":8251.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3124, "fecha_inicio":"2023-09-08", "tipo_deuda":"I", "ahorro_cuota_mensual":226.59617421670055, "ahorro_total":2719.1540906004066, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2020-07-23", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 2696976, "monto_maximo_cliente": 284982.0, "cuota_externa_total": 29232.0, "capacidad_maxima_pago": 29868.0, "bursolnum": 7439250, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1169.5751965916932, "monto_max": 284982.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 22.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":11, "monto_otorgado":14100.0, "cuota":1687.0, "saldo":11368.0, "tasa_externa":0.7368, "tasa_kubo":0.6193, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1938, "fecha_inicio":"2021-08-20", "tipo_deuda":"I", "ahorro_cuota_mensual":6.432245599739872, "ahorro_total":77.18694719687846, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":40000.0, "cuota":3209.0, "saldo":39670.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":24.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.0082, "fecha_inicio":"2024-01-23", "tipo_deuda":"I", "ahorro_cuota_mensual":25.795009600895355, "ahorro_total":619.0802304214885, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":10000.0, "cuota":539.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-08-21", "tipo_deuda":"R", "ahorro_cuota_mensual":539.0, "ahorro_total":-539.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":19500.0, "cuota":2764.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-01-23", "tipo_deuda":"R", "ahorro_cuota_mensual":2764.0, "ahorro_total":-2764.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":16000.0, "cuota":800.0, "saldo":8600.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4625, "fecha_inicio":"2022-03-09", "tipo_deuda":"R", "ahorro_cuota_mensual":9400.000000000002, "ahorro_total":-9400.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":23819.0, "cuota":1509.0, "saldo":9068.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6193, "fecha_inicio":"2023-03-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-688.6219230784272, "ahorro_total":-12395.19461541169, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":15000.0, "cuota":2055.0, "saldo":13840.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0773, "fecha_inicio":"2023-07-13", "tipo_deuda":"R", "ahorro_cuota_mensual":15895.000000000002, "ahorro_total":-15895.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":7000.0, "cuota":350.0, "saldo":442.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9369, "fecha_inicio":"2021-01-26", "tipo_deuda":"R", "ahorro_cuota_mensual":792.0000000000001, "ahorro_total":-792.0000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":180000.0, "cuota":17380.0, "saldo":150265.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1652, "fecha_inicio":"2023-06-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":39740.0, "cuota":1987.0, "saldo":30677.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2281, "fecha_inicio":"2021-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":32664.000000000007, "ahorro_total":-32664.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":2, "monto_otorgado":8600.0, "cuota":-1.0, "saldo":11718.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.3626, "fecha_inicio":"2024-01-19", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":2800.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-11-01", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":17200.0, "cuota":1786.0, "saldo":1786.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8962, "fecha_inicio":"2023-05-15", "tipo_deuda":"R", "ahorro_cuota_mensual":3572.0, "ahorro_total":-3572.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 2769844, "monto_maximo_cliente": 97559.0, "cuota_externa_total": 6547.0, "capacidad_maxima_pago": 76494.0, "bursolnum": 7439258, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1922.6238430723963, "monto_max": 97559.0, "cuota_min": 163.04445621498797, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.6722, "kubo_score": "D4", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2622, 0.2306, 0.2], "comisiones": [0.03845, 0.03845, 0.03845], "kubo_scores": ['K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":13, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2015-07-02", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":17400.0, "cuota":1706.0, "saldo":3135.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8198, "fecha_inicio":"2022-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":490.12123283039523, "ahorro_total":8822.182190947115, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-12-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":3000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-08-08", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":1163.0, "cuota":432.0, "saldo":418.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6406, "fecha_inicio":"2023-12-23", "tipo_deuda":"I", "ahorro_cuota_mensual":24.517791182713722, "ahorro_total":73.55337354814117, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":528.0, "cuota":202.0, "saldo":551.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0436, "fecha_inicio":"2024-02-08", "tipo_deuda":"I", "ahorro_cuota_mensual":17.00377794021739, "ahorro_total":51.01133382065217, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":32346.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-10-05", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":12500.0, "cuota":1.0, "saldo":5891.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5287, "fecha_inicio":"2023-04-11", "tipo_deuda":"R", "ahorro_cuota_mensual":5891.999999999969, "ahorro_total":-5891.999999999969, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":35500.0, "cuota":1775.0, "saldo":19879.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.44, "fecha_inicio":"2017-10-21", "tipo_deuda":"R", "ahorro_cuota_mensual":21653.999999999898, "ahorro_total":-21653.999999999898, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":16500.0, "cuota":825.0, "saldo":14557.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1178, "fecha_inicio":"2021-10-14", "tipo_deuda":"R", "ahorro_cuota_mensual":15381.999999999924, "ahorro_total":-15381.999999999924, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":53041.0, "cuota":2474.0, "saldo":48879.0, "tasa_externa":0.3919, "tasa_kubo":0.2622, "numero_pagos_otorgado":37.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":0.0785, "fecha_inicio":"2023-09-26", "tipo_deuda":"I", "ahorro_cuota_mensual":247.87897070504096, "ahorro_total":9171.521916086516, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":2500.0, "cuota":554.0, "saldo":2281.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0876, "fecha_inicio":"2024-01-09", "tipo_deuda":"I", "ahorro_cuota_mensual":99.59972594631319, "ahorro_total":597.5983556778791, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 2776466, "monto_maximo_cliente": 125700.0, "cuota_externa_total": 12413.0, "capacidad_maxima_pago": 73180.0, "bursolnum": 7439259, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1867.7676205702126, "monto_max": 125700.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5668, "kubo_score": "C5", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "kubo_scores": ['K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":8, "monto_otorgado":18500.0, "cuota":925.0, "saldo":12510.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3238, "fecha_inicio":"2022-05-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":35000.0, "cuota":2270.0, "saldo":35094.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":-0.0027, "fecha_inicio":"2024-01-22", "tipo_deuda":"I", "ahorro_cuota_mensual":911.5086211204559, "ahorro_total":32814.310360336414, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":4000.0, "cuota":200.0, "saldo":1480.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.63, "fecha_inicio":"2019-02-19", "tipo_deuda":"R", "ahorro_cuota_mensual":1679.999999999997, "ahorro_total":-1679.999999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":1300.0, "cuota":157.0, "saldo":797.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3869, "fecha_inicio":"2023-08-12", "tipo_deuda":"I", "ahorro_cuota_mensual":34.57526928993565, "ahorro_total":414.90323147922777, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "HIPOTECAGOBIERNO", "registro":10, "monto_otorgado":376362.0, "cuota":3755.0, "saldo":296059.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":360.0, "numero_pagos_restante":280.0, "frecuencia_externa":"M", "avance":0.2134, "fecha_inicio":"2017-08-30", "tipo_deuda":"M", "ahorro_cuota_mensual":-1974.6187797623443, "ahorro_total":-710862.760714444, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":15700.0, "cuota":2010.0, "saldo":1531.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9025, "fecha_inicio":"2023-12-27", "tipo_deuda":"R", "ahorro_cuota_mensual":3540.9999999999973, "ahorro_total":-3540.9999999999973, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":13200.0, "cuota":660.0, "saldo":5189.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6069, "fecha_inicio":"2022-03-07", "tipo_deuda":"R", "ahorro_cuota_mensual":5848.99999999999, "ahorro_total":-5848.99999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":65394.0, "cuota":2469.0, "saldo":55756.0, "tasa_externa":0.3903, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":40.0, "frecuencia_externa":"M", "avance":0.1474, "fecha_inicio":"2022-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":617.9902971283527, "ahorro_total":37079.41782770117, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":35970.0, "cuota":910.0, "saldo":34093.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":144.0, "numero_pagos_restante":59.0, "frecuencia_externa":"S", "avance":0.0522, "fecha_inicio":"2023-03-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-19.58415440289525, "ahorro_total":-1410.059117008458, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":2326.0, "cuota":282.0, "saldo":1624.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3018, "fecha_inicio":"2023-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":62.95390489876178, "ahorro_total":755.4468587851413, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 2871236, "monto_maximo_cliente": 346145.0, "cuota_externa_total": 34673.0, "capacidad_maxima_pago": 47657.0, "bursolnum": 7439278, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2039.827189219965, "monto_max": 346145.0, "cuota_min": 163.04445621498797, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5486, "kubo_score": "C3", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2622, 0.2306, 0.2], "comisiones": [0.03845, 0.03845, 0.03845], "kubo_scores": ['K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "HIPOTECARIA", "registro":47, "monto_otorgado":296539.0, "cuota":2219.0, "saldo":183061.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":360.0, "numero_pagos_restante":52.0, "frecuencia_externa":"M", "avance":0.3827, "fecha_inicio":"1998-08-18", "tipo_deuda":"M", "ahorro_cuota_mensual":-2421.4306052434104, "ahorro_total":-871715.0178876277, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":18, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":947.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-11-20", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":17, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":870.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-06-08", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":16, "monto_otorgado":73000.0, "cuota":3894.0, "saldo":3894.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9467, "fecha_inicio":"2021-03-24", "tipo_deuda":"I", "ahorro_cuota_mensual":778.4104170062656, "ahorro_total":28022.77501222556, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":78000.0, "cuota":4420.0, "saldo":74251.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":48.0, "numero_pagos_restante":38.0, "frecuencia_externa":"M", "avance":0.0481, "fecha_inicio":"2023-06-30", "tipo_deuda":"I", "ahorro_cuota_mensual":1592.6653011887615, "ahorro_total":76447.93445706056, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":14, "monto_otorgado":12958.0, "cuota":12709.0, "saldo":12709.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.0192, "fecha_inicio":"2024-02-22", "tipo_deuda":"O", "ahorro_cuota_mensual":25417.999999999935, "ahorro_total":-25417.999999999935, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":1075.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-09-23", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":19, "monto_otorgado":46000.0, "cuota":61.0, "saldo":231.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.995, "fecha_inicio":"2018-12-15", "tipo_deuda":"R", "ahorro_cuota_mensual":291.9999999999988, "ahorro_total":-291.9999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":5800.0, "cuota":370.0, "saldo":2256.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.611, "fecha_inicio":"2022-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":2625.999999999988, "ahorro_total":-2625.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":5500.0, "cuota":400.0, "saldo":1835.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6664, "fecha_inicio":"2022-09-27", "tipo_deuda":"R", "ahorro_cuota_mensual":2234.99999999999, "ahorro_total":-2234.99999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":62100.0, "cuota":2591.0, "saldo":47872.0, "tasa_externa":0.4003, "tasa_kubo":0.2622, "numero_pagos_otorgado":48.0, "numero_pagos_restante":29.0, "frecuencia_externa":"M", "avance":0.2291, "fecha_inicio":"2022-09-12", "tipo_deuda":"I", "ahorro_cuota_mensual":340.006605177206, "ahorro_total":16320.317048505887, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":3080.0, "cuota":80.0, "saldo":3000.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":154.0, "numero_pagos_restante":36.0, "frecuencia_externa":"W", "avance":0.026, "fecha_inicio":"2024-02-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-47.20467958546689, "ahorro_total":-1793.7778242477418, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":13000.0, "cuota":14.0, "saldo":7392.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4314, "fecha_inicio":"2019-10-11", "tipo_deuda":"R", "ahorro_cuota_mensual":7405.999999999962, "ahorro_total":-7405.999999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":15900.0, "cuota":795.0, "saldo":11123.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3004, "fecha_inicio":"2021-06-17", "tipo_deuda":"R", "ahorro_cuota_mensual":11917.999999999942, "ahorro_total":-11917.999999999942, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":43648.0, "cuota":1364.0, "saldo":27280.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":128.0, "numero_pagos_restante":20.0, "frecuencia_externa":"W", "avance":0.375, "fecha_inicio":"2023-04-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-643.4296133572952, "ahorro_total":-20589.747627433448, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":50600.0, "cuota":2530.0, "saldo":3416.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9325, "fecha_inicio":"2022-09-12", "tipo_deuda":"R", "ahorro_cuota_mensual":5945.999999999982, "ahorro_total":-5945.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":3080.0, "cuota":80.0, "saldo":2120.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":154.0, "numero_pagos_restante":26.0, "frecuencia_externa":"W", "avance":0.3117, "fecha_inicio":"2023-04-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-47.20467958546689, "ahorro_total":-1793.7778242477418, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":17024.0, "cuota":532.0, "saldo":11438.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":128.0, "numero_pagos_restante":22.0, "frecuencia_externa":"W", "avance":0.3281, "fecha_inicio":"2023-06-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-250.95641811296252, "ahorro_total":-8030.605379614801, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":57596.0, "cuota":1496.0, "saldo":56100.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":154.0, "numero_pagos_restante":36.0, "frecuencia_externa":"W", "avance":0.026, "fecha_inicio":"2024-02-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-882.7275082482306, "ahorro_total":-33543.64531343276, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":133364.0, "cuota":3464.0, "saldo":91519.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":154.0, "numero_pagos_restante":26.0, "frecuencia_externa":"W", "avance":0.3138, "fecha_inicio":"2023-04-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-2043.9626260507166, "ahorro_total":-77670.57978992723, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3002968, "monto_maximo_cliente": 85285.0, "cuota_externa_total": 7616.0, "capacidad_maxima_pago": 48952.0, "bursolnum": 7439315, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1760.5518677534276, "monto_max": 85285.0, "cuota_min": 151.9292154681686, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.5668, "kubo_score": "C5", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2306, 0.2], "comisiones": [0.03845, 0.03845], "kubo_scores": ['K2', 'K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":2, "monto_otorgado":15000.0, "cuota":1195.0, "saldo":14741.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0173, "fecha_inicio":"2018-12-14", "tipo_deuda":"R", "ahorro_cuota_mensual":15935.999999999936, "ahorro_total":-15935.999999999936, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":21000.0, "cuota":1788.0, "saldo":18976.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0964, "fecha_inicio":"2010-12-16", "tipo_deuda":"R", "ahorro_cuota_mensual":20763.99999999992, "ahorro_total":-20763.99999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":51568.0, "cuota":2337.0, "saldo":23798.0, "tasa_externa":0.3687, "tasa_kubo":0.2306, "numero_pagos_otorgado":37.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.5385, "fecha_inicio":"2022-02-01", "tipo_deuda":"I", "ahorro_cuota_mensual":275.7460416311369, "ahorro_total":10202.603540352065, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":1, "monto_otorgado":844.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-08-30", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":39000.0, "cuota":2296.0, "saldo":4308.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8895, "fecha_inicio":"2021-04-26", "tipo_deuda":"I", "ahorro_cuota_mensual":709.0511092198451, "ahorro_total":25525.839931914423, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3052806, "monto_maximo_cliente": 205933.0, "cuota_externa_total": 27981.0, "capacidad_maxima_pago": 80257.0, "bursolnum": 7439333, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4238.020125483156, "monto_max": 205933.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 44.0, "plazo_min": 4, "tasa": 0.4818, "kubo_score": "B5", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":19500.0, "cuota":1245.0, "saldo":4334.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7777, "fecha_inicio":"2012-03-10", "tipo_deuda":"R", "ahorro_cuota_mensual":5579.000000000009, "ahorro_total":-5579.000000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":17628.0, "cuota":3093.0, "saldo":17317.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0176, "fecha_inicio":"2020-03-17", "tipo_deuda":"R", "ahorro_cuota_mensual":20410.000000000036, "ahorro_total":-20410.000000000036, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":180000.0, "cuota":13090.0, "saldo":117229.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":24.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.3487, "fecha_inicio":"2023-02-20", "tipo_deuda":"I", "ahorro_cuota_mensual":476.52680550779587, "ahorro_total":11436.6433321871, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":78717.0, "cuota":4740.0, "saldo":7088.0, "tasa_externa":0.6091, "tasa_kubo":0.4818, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.91, "fecha_inicio":"2021-05-13", "tipo_deuda":"I", "ahorro_cuota_mensual":190.195501525498, "ahorro_total":6847.038054917928, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":40000.0, "cuota":3307.0, "saldo":39597.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0101, "fecha_inicio":"2022-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":42904.00000000009, "ahorro_total":-42904.00000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":21000.0, "cuota":2506.0, "saldo":10739.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4886, "fecha_inicio":"2011-08-03", "tipo_deuda":"R", "ahorro_cuota_mensual":13245.000000000022, "ahorro_total":-13245.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":61000.0, "cuota":3000.0, "saldo":55229.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0946, "fecha_inicio":"2018-04-17", "tipo_deuda":"R", "ahorro_cuota_mensual":58229.00000000012, "ahorro_total":-58229.00000000012, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3190170, "monto_maximo_cliente": 341101.0, "cuota_externa_total": 34548.0, "capacidad_maxima_pago": 137552.0, "bursolnum": 7439387, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7745.528415344514, "monto_max": 341101.0, "cuota_min": 269.2747621622814, "monto_min": 5000, "plazo_max": 52.0, "plazo_min": 4, "tasa": 0.5292, "kubo_score": "C1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":2448.0, "cuota":354.0, "saldo":1541.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3705, "fecha_inicio":"2023-10-25", "tipo_deuda":"I", "ahorro_cuota_mensual":7.81552043079472, "ahorro_total":70.33968387715248, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":26, "monto_otorgado":63000.0, "cuota":3322.0, "saldo":12002.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8095, "fecha_inicio":"2021-06-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-542.0784543044992, "ahorro_total":-19514.824354961973, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":49, "monto_otorgado":5500.0, "cuota":1160.0, "saldo":2194.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6011, "fecha_inicio":"2022-10-04", "tipo_deuda":"I", "ahorro_cuota_mensual":72.39469715204609, "ahorro_total":434.36818291227655, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":32, "monto_otorgado":25000.0, "cuota":2460.0, "saldo":7024.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.719, "fecha_inicio":"2023-03-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-379.05480487324303, "ahorro_total":-4548.657658478916, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":28, "monto_otorgado":10000.0, "cuota":500.0, "saldo":6711.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3289, "fecha_inicio":"2022-06-13", "tipo_deuda":"R", "ahorro_cuota_mensual":7211.000000000003, "ahorro_total":-7211.000000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":25, "monto_otorgado":12700.0, "cuota":748.0, "saldo":7992.0, "tasa_externa":0.6918, "tasa_kubo":0.5292, "numero_pagos_otorgado":120.0, "numero_pagos_restante":28.0, "frecuencia_externa":"S", "avance":0.3707, "fecha_inicio":"2021-08-06", "tipo_deuda":"I", "ahorro_cuota_mensual":64.04210410780524, "ahorro_total":3842.5262464683146, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":24, "monto_otorgado":127400.0, "cuota":7512.0, "saldo":97201.0, "tasa_externa":0.6927, "tasa_kubo":0.5292, "numero_pagos_otorgado":120.0, "numero_pagos_restante":36.0, "frecuencia_externa":"S", "avance":0.237, "fecha_inicio":"2022-04-28", "tipo_deuda":"I", "ahorro_cuota_mensual":650.8790601050705, "ahorro_total":39052.743606304226, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":23, "monto_otorgado":15000.0, "cuota":7771.0, "saldo":7771.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4819, "fecha_inicio":"2022-04-07", "tipo_deuda":"R", "ahorro_cuota_mensual":15542.000000000004, "ahorro_total":-15542.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":21, "monto_otorgado":76300.0, "cuota":3815.0, "saldo":32496.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5741, "fecha_inicio":"2023-10-05", "tipo_deuda":"R", "ahorro_cuota_mensual":36311.000000000015, "ahorro_total":-36311.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":20, "monto_otorgado":1115.0, "cuota":226.0, "saldo":221.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8018, "fecha_inicio":"2023-09-17", "tipo_deuda":"I", "ahorro_cuota_mensual":5.512743149914826, "ahorro_total":33.076458899488955, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":19, "monto_otorgado":1376.0, "cuota":275.0, "saldo":269.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8045, "fecha_inicio":"2023-09-24", "tipo_deuda":"I", "ahorro_cuota_mensual":2.900927869311886, "ahorro_total":17.405567215871315, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":1048.0, "cuota":214.0, "saldo":407.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6116, "fecha_inicio":"2023-10-13", "tipo_deuda":"I", "ahorro_cuota_mensual":6.761753202789862, "ahorro_total":40.57051921673917, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":1199.0, "cuota":255.0, "saldo":693.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.422, "fecha_inicio":"2023-11-16", "tipo_deuda":"I", "ahorro_cuota_mensual":17.902043979146043, "ahorro_total":107.41226387487626, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":27, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2018-06-29", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":873.0, "cuota":184.0, "saldo":643.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2635, "fecha_inicio":"2023-12-20", "tipo_deuda":"I", "ahorro_cuota_mensual":11.367376475224773, "ahorro_total":68.20425885134864, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":70000.0, "cuota":3876.0, "saldo":138580.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":43.0, "numero_pagos_restante":19.0, "frecuencia_externa":"S", "avance":-0.9797, "fecha_inicio":"2024-02-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-1498.1250205302822, "ahorro_total":-32958.75045166621, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":30000.0, "cuota":1660.0, "saldo":57336.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":43.0, "numero_pagos_restante":14.0, "frecuencia_externa":"S", "avance":-0.9112, "fecha_inicio":"2023-08-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-643.1964373701207, "ahorro_total":-14150.321622142656, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":10000.0, "cuota":540.0, "saldo":18528.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":43.0, "numero_pagos_restante":11.0, "frecuencia_externa":"S", "avance":-0.8528, "fecha_inicio":"2023-05-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-227.73214579004014, "ahorro_total":-5010.107207380883, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":759.0, "cuota":161.0, "saldo":437.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4242, "fecha_inicio":"2023-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":10.910468206982358, "ahorro_total":65.46280924189415, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":337.0, "cuota":127.0, "saldo":345.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0237, "fecha_inicio":"2024-02-20", "tipo_deuda":"I", "ahorro_cuota_mensual":2.982566567907469, "ahorro_total":8.947699703722407, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":3000.0, "cuota":296.0, "saldo":348.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":23.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.884, "fecha_inicio":"2022-05-11", "tipo_deuda":"R", "ahorro_cuota_mensual":269.91853997678163, "ahorro_total":6208.126419465978, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":227.0, "cuota":89.0, "saldo":168.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2599, "fecha_inicio":"2024-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":5.463034453753707, "ahorro_total":16.38910336126112, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":825.0, "cuota":325.0, "saldo":883.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0703, "fecha_inicio":"2024-02-02", "tipo_deuda":"I", "ahorro_cuota_mensual":21.39649085615332, "ahorro_total":64.18947256845996, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":362.0, "cuota":143.0, "saldo":268.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2597, "fecha_inicio":"2024-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":9.78246023021515, "ahorro_total":29.34738069064545, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":910.0, "cuota":359.0, "saldo":976.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0725, "fecha_inicio":"2024-02-01", "tipo_deuda":"I", "ahorro_cuota_mensual":24.11612930799936, "ahorro_total":72.34838792399808, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":735.0, "cuota":145.0, "saldo":737.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0027, "fecha_inicio":"2024-02-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-0.3436177442265773, "ahorro_total":-2.061706465359464, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":961.0, "cuota":381.0, "saldo":715.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.256, "fecha_inicio":"2024-01-01", "tipo_deuda":"I", "ahorro_cuota_mensual":27.347912379107015, "ahorro_total":82.04373713732105, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3332202, "monto_maximo_cliente": 325284.0, "cuota_externa_total": 28182.0, "capacidad_maxima_pago": 219949.0, "bursolnum": 7439443, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7932.571742423747, "monto_max": 325284.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0423, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":91000.0, "cuota":5815.0, "saldo":85364.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":33.0, "numero_pagos_restante":23.0, "frecuencia_externa":"M", "avance":0.0619, "fecha_inicio":"2023-07-03", "tipo_deuda":"I", "ahorro_cuota_mensual":1293.7409739580107, "ahorro_total":42693.452140614354, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":50000.0, "cuota":3094.0, "saldo":46214.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.0757, "fecha_inicio":"2023-07-26", "tipo_deuda":"I", "ahorro_cuota_mensual":726.011675047012, "ahorro_total":26136.42030169243, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":40000.0, "cuota":2543.0, "saldo":38950.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":36.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.0262, "fecha_inicio":"2023-11-27", "tipo_deuda":"I", "ahorro_cuota_mensual":648.6093400376094, "ahorro_total":23349.93624135394, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2005-10-13", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":52210.0, "cuota":2610.0, "saldo":17874.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6577, "fecha_inicio":"2012-01-25", "tipo_deuda":"R", "ahorro_cuota_mensual":20483.999999999953, "ahorro_total":-20483.999999999953, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":62046.0, "cuota":3636.0, "saldo":46892.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":71.0, "numero_pagos_restante":27.0, "frecuencia_externa":"S", "avance":0.2442, "fecha_inicio":"2023-08-01", "tipo_deuda":"I", "ahorro_cuota_mensual":697.515927799338, "ahorro_total":25110.573400776168, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":204000.0, "cuota":8641.0, "saldo":192245.0, "tasa_externa":0.4106, "tasa_kubo":0.3337, "numero_pagos_otorgado":48.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.0576, "fecha_inicio":"2023-10-12", "tipo_deuda":"I", "ahorro_cuota_mensual":227.5012028382771, "ahorro_total":10920.0577362373, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":41364.0, "cuota":2424.0, "saldo":33009.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":71.0, "numero_pagos_restante":29.0, "frecuencia_externa":"S", "avance":0.202, "fecha_inicio":"2023-09-12", "tipo_deuda":"I", "ahorro_cuota_mensual":465.01061853289207, "ahorro_total":16740.382267184115, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3334267, "monto_maximo_cliente": 238332.0, "cuota_externa_total": 16380.0, "capacidad_maxima_pago": 57628.0, "bursolnum": 7439444, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1465.8962563439925, "monto_max": 238332.0, "cuota_min": 163.04445621498797, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.5391, "kubo_score": "C2", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2622, 0.2306, 0.2], "comisiones": [0.03845, 0.03845, 0.03845], "kubo_scores": ['K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":1318.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-04-29", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":875.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-04-29", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":70000.0, "cuota":3772.0, "saldo":20039.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7137, "fecha_inicio":"2021-08-13", "tipo_deuda":"I", "ahorro_cuota_mensual":784.448345074501, "ahorro_total":28240.140422682038, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":3, "monto_otorgado":136635.0, "cuota":4427.0, "saldo":94057.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":48.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.3116, "fecha_inicio":"2022-07-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-525.729186821457, "ahorro_total":-25235.000967429936, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":1, "monto_otorgado":12990.0, "cuota":650.0, "saldo":9351.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":312.0, "numero_pagos_restante":218.0, "frecuencia_externa":"Z", "avance":0.2801, "fecha_inicio":"2016-06-14", "tipo_deuda":"R", "ahorro_cuota_mensual":412.89331168751505, "ahorro_total":128822.71324650469, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":12, "monto_otorgado":90995.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"S", "avance":1.0, "fecha_inicio":"2018-09-18", "tipo_deuda":"I", "ahorro_cuota_mensual":90994.99999999952, "ahorro_total":-90994.99999999952, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":40000.0, "cuota":2006.0, "saldo":36491.0, "tasa_externa":0.4406, "tasa_kubo":0.2622, "numero_pagos_otorgado":36.0, "numero_pagos_restante":29.0, "frecuencia_externa":"M", "avance":0.0877, "fecha_inicio":"2023-09-29", "tipo_deuda":"I", "ahorro_cuota_mensual":298.82762575685774, "ahorro_total":10757.794527246879, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":11673.0, "cuota":1000.0, "saldo":6369.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4544, "fecha_inicio":"2010-04-26", "tipo_deuda":"R", "ahorro_cuota_mensual":7368.999999999967, "ahorro_total":-7368.999999999967, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":104500.0, "cuota":5225.0, "saldo":21645.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7929, "fecha_inicio":"2012-01-01", "tipo_deuda":"R", "ahorro_cuota_mensual":26869.999999999887, "ahorro_total":-26869.999999999887, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":77400.0, "cuota":968.0, "saldo":2236.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9711, "fecha_inicio":"2023-07-31", "tipo_deuda":"R", "ahorro_cuota_mensual":3203.999999999988, "ahorro_total":-3203.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":84000.0, "cuota":4200.0, "saldo":22087.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7371, "fecha_inicio":"2012-08-01", "tipo_deuda":"R", "ahorro_cuota_mensual":26286.999999999887, "ahorro_total":-26286.999999999887, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":55000.0, "cuota":1907.0, "saldo":19481.0, "tasa_externa":-1.0, "tasa_kubo":0.2622, "numero_pagos_otorgado":36.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.6458, "fecha_inicio":"2022-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-440.3620145843206, "ahorro_total":-15853.032525035542, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3590341, "monto_maximo_cliente": 369159.0, "cuota_externa_total": 24466.0, "capacidad_maxima_pago": 95534.0, "bursolnum": 6203346, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 6310.318696733804, "monto_max": 369159.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 38.0, "plazo_min": 4, "tasa": 0.5951, "kubo_score": "D2", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":1816.0, "cuota":908.0, "saldo":1135.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":8.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.375, "fecha_inicio":"2023-03-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-75.28817492743553, "ahorro_total":-150.57634985487107, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":761.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-08-09", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":21011.0, "cuota":1352.0, "saldo":20237.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":36.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.0368, "fecha_inicio":"2022-08-31", "tipo_deuda":"I", "ahorro_cuota_mensual":3.099050625624386, "ahorro_total":111.5658225224779, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":104, "monto_otorgado":11000.0, "cuota":620.0, "saldo":311.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.9717, "fecha_inicio":"2018-10-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-654.8363258558547, "ahorro_total":-7858.035910270257, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":19500.0, "cuota":975.0, "saldo":19436.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0033, "fecha_inicio":"2023-01-13", "tipo_deuda":"R", "ahorro_cuota_mensual":20411.000000000007, "ahorro_total":-20411.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":55000.0, "cuota":4185.0, "saldo":55513.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":24.0, "numero_pagos_restante":12.0, "frecuencia_externa":"M", "avance":-0.0093, "fecha_inicio":"2023-04-24", "tipo_deuda":"I", "ahorro_cuota_mensual":11.327015086970277, "ahorro_total":271.84836208728666, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":19900.0, "cuota":995.0, "saldo":19246.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0329, "fecha_inicio":"2019-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":20241.000000000004, "ahorro_total":-20241.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":70000.0, "cuota":8748.0, "saldo":39263.0, "tasa_externa":1.4207, "tasa_kubo":0.5668, "numero_pagos_otorgado":48.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.4391, "fecha_inicio":"2022-03-08", "tipo_deuda":"I", "ahorro_cuota_mensual":3436.0525646561437, "ahorro_total":82465.26155174745, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":196497.0, "cuota":4093.0, "saldo":151466.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":37.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.2292, "fecha_inicio":"2022-05-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-8410.522715927074, "ahorro_total":-311189.3404893018, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":30000.0, "cuota":2212.0, "saldo":30399.0, "tasa_externa":0.8921, "tasa_kubo":0.5668, "numero_pagos_otorgado":144.0, "numero_pagos_restante":59.0, "frecuencia_externa":"S", "avance":-0.0133, "fecha_inicio":"2023-03-28", "tipo_deuda":"I", "ahorro_cuota_mensual":532.1983858143121, "ahorro_total":38318.28377863047, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":21164.0, "cuota":1628.0, "saldo":10435.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":52.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.5069, "fecha_inicio":"2022-11-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-690.4767827836872, "ahorro_total":-8976.198176187934, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3636540, "monto_maximo_cliente": 86445.0, "cuota_externa_total": 8027.0, "capacidad_maxima_pago": 31573.0, "bursolnum": 7439538, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3124.003761660951, "monto_max": 86445.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 16.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":909.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-09-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":39000.0, "cuota":2452.0, "saldo":18740.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":36.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.5195, "fecha_inicio":"2021-12-23", "tipo_deuda":"I", "ahorro_cuota_mensual":-211.13048186121387, "ahorro_total":-7600.697347003699, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":7000.0, "cuota":416.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-12-12", "tipo_deuda":"R", "ahorro_cuota_mensual":416.0, "ahorro_total":-416.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":31600.0, "cuota":3749.0, "saldo":27454.0, "tasa_externa":0.7181, "tasa_kubo":0.6193, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1312, "fecha_inicio":"2022-05-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-17.378797095618665, "ahorro_total":-208.54556514742399, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":18200.0, "cuota":910.0, "saldo":10884.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.402, "fecha_inicio":"2020-12-24", "tipo_deuda":"R", "ahorro_cuota_mensual":11794.000000000002, "ahorro_total":-11794.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":3000.0, "cuota":1232.0, "saldo":3728.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.2427, "fecha_inicio":"2021-12-08", "tipo_deuda":"R", "ahorro_cuota_mensual":4960.000000000001, "ahorro_total":-4960.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":43100.0, "cuota":1200.0, "saldo":40233.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0665, "fecha_inicio":"2021-08-27", "tipo_deuda":"R", "ahorro_cuota_mensual":41433.00000000001, "ahorro_total":-41433.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":4000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-07-04", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":4800.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-05-18", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3651682, "monto_maximo_cliente": 104739.0, "cuota_externa_total": 17674.0, "capacidad_maxima_pago": 47326.0, "bursolnum": 7439543, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1142.4703309601568, "monto_max": 104739.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5292, "kubo_score": "C1", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "kubo_scores": ['K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":17, "monto_otorgado":148333.0, "cuota":4252.0, "saldo":78550.0, "tasa_externa":0.2415, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4704, "fecha_inicio":"2011-09-27", "tipo_deuda":"I", "ahorro_cuota_mensual":53.36064079181506, "ahorro_total":3201.6384475089035, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":18, "monto_otorgado":120253.0, "cuota":3247.0, "saldo":80979.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":48.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3266, "fecha_inicio":"2013-06-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-620.4745349773443, "ahorro_total":-29782.777678912527, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":741.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-04-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":15000.0, "cuota":1007.0, "saldo":8460.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":27.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.436, "fecha_inicio":"2022-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":288.65192219567166, "ahorro_total":7793.601899283135, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":44700.0, "cuota":3504.0, "saldo":26222.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.4134, "fecha_inicio":"2021-11-16", "tipo_deuda":"I", "ahorro_cuota_mensual":-19496.218487949758, "ahorro_total":-38992.436975899516, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":20000.0, "cuota":1644.0, "saldo":9437.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.5282, "fecha_inicio":"2021-06-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-8646.9254979641, "ahorro_total":-17293.8509959282, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":24700.0, "cuota":988.0, "saldo":1642.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":100.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.9335, "fecha_inicio":"2022-06-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-267.2648987126802, "ahorro_total":-6681.622467817005, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":40000.0, "cuota":1068.0, "saldo":21158.0, "tasa_externa":0.2065, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.471, "fecha_inicio":"2021-04-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-64.21989960647602, "ahorro_total":-3853.193976388561, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":24000.0, "cuota":1200.0, "saldo":7793.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6753, "fecha_inicio":"2012-05-01", "tipo_deuda":"R", "ahorro_cuota_mensual":8992.999999999985, "ahorro_total":-8992.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":2000.0, "cuota":80.0, "saldo":140.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":100.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.93, "fecha_inicio":"2022-06-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-21.640882486856697, "ahorro_total":-541.0220621714175, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":30000.0, "cuota":1472.0, "saldo":23551.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.215, "fecha_inicio":"2023-09-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-102.17960024565582, "ahorro_total":-2452.3104058957397, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":246.0, "cuota":12.0, "saldo":3.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":82.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.9878, "fecha_inicio":"2022-06-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-2.947937087656877, "ahorro_total":-58.95874175313754, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3787395, "monto_maximo_cliente": 96578.0, "cuota_externa_total": 26867.0, "capacidad_maxima_pago": 60460.0, "bursolnum": 7439593, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2836.744033099388, "monto_max": 96578.0, "cuota_min": 200.2991210698785, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.4818, "kubo_score": "B5", "comision": 0.0428, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1061.0, "cuota":786.0, "saldo":786.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2592, "fecha_inicio":"2021-06-19", "tipo_deuda":"O", "ahorro_cuota_mensual":1571.9999999999982, "ahorro_total":-1571.9999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":1125.0, "cuota":716.0, "saldo":716.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3636, "fecha_inicio":"2018-07-17", "tipo_deuda":"O", "ahorro_cuota_mensual":1431.9999999999982, "ahorro_total":-1431.9999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":10, "monto_otorgado":974491.0, "cuota":9055.0, "saldo":986134.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":360.0, "numero_pagos_restante":354.0, "frecuencia_externa":"M", "avance":-0.0119, "fecha_inicio":"2023-10-26", "tipo_deuda":"M", "ahorro_cuota_mensual":-25424.663911575328, "ahorro_total":-9152879.008167118, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":706.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-06-06", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":60000.0, "cuota":3186.0, "saldo":43275.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.2788, "fecha_inicio":"2022-10-28", "tipo_deuda":"I", "ahorro_cuota_mensual":230.4662543165341, "ahorro_total":8296.785155395228, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":24900.0, "cuota":350.0, "saldo":1138.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9543, "fecha_inicio":"2017-06-06", "tipo_deuda":"R", "ahorro_cuota_mensual":1487.9999999999975, "ahorro_total":-1487.9999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":32, "monto_otorgado":999.0, "cuota":999.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-03-10", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":1, "monto_otorgado":24000.0, "cuota":1200.0, "saldo":5440.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7733, "fecha_inicio":"2018-09-28", "tipo_deuda":"R", "ahorro_cuota_mensual":6639.999999999987, "ahorro_total":-6639.999999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "AUTOMOTRIZ", "registro":5, "monto_otorgado":555820.0, "cuota":7456.0, "saldo":427425.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":60.0, "numero_pagos_restante":43.0, "frecuencia_externa":"M", "avance":0.231, "fecha_inicio":"2022-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-14810.051494611977, "ahorro_total":-888603.0896767186, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":65000.0, "cuota":3376.0, "saldo":37761.0, "tasa_externa":0.4747, "tasa_kubo":0.3617, "numero_pagos_otorgado":72.0, "numero_pagos_restante":26.0, "frecuencia_externa":"S", "avance":0.4191, "fecha_inicio":"2023-06-16", "tipo_deuda":"I", "ahorro_cuota_mensual":174.17177550957877, "ahorro_total":6270.183918344836, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":25000.0, "cuota":676.0, "saldo":11957.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":43.0, "numero_pagos_restante":17.0, "frecuencia_externa":"S", "avance":0.5217, "fecha_inicio":"2023-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-971.726599369646, "ahorro_total":-21377.985186132213, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3901833, "monto_maximo_cliente": 17200.0, "cuota_externa_total": 4349.0, "capacidad_maxima_pago": 24851.0, "bursolnum": 7439635, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1536.5203379078412, "monto_max": 17200.0, "cuota_min": 244.39480798426723, "monto_min": 5000, "plazo_max": 16.0, "plazo_min": 4, "tasa": 0.4706, "kubo_score": "B4", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":19500.0, "cuota":285.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-05-03", "tipo_deuda":"R", "ahorro_cuota_mensual":285.0, "ahorro_total":-285.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":17200.0, "cuota":2057.0, "saldo":9911.0, "tasa_externa":0.7359, "tasa_kubo":0.4706, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4238, "fecha_inicio":"2023-08-19", "tipo_deuda":"I", "ahorro_cuota_mensual":165.4361637582299, "ahorro_total":1985.2339650987587, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":40000.0, "cuota":2292.0, "saldo":31436.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":36.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.2141, "fecha_inicio":"2022-11-04", "tipo_deuda":"I", "ahorro_cuota_mensual":12.909881874620169, "ahorro_total":464.7557474863261, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":4, "monto_otorgado":811.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-05-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":2524.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-07-24", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":934.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-10-08", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 3965394, "monto_maximo_cliente": 64186.0, "cuota_externa_total": 7548.0, "capacidad_maxima_pago": 37144.0, "bursolnum": 7439652, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1042.5301204147484, "monto_max": 64186.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.5391, "kubo_score": "C2", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "kubo_scores": ['K1'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-01-06", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":20000.0, "cuota":2293.0, "saldo":16403.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.1798, "fecha_inicio":"2023-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":409.5426044605483, "ahorro_total":4914.51125352658, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":3000.0, "cuota":150.0, "saldo":236.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9213, "fecha_inicio":"2019-06-14", "tipo_deuda":"R", "ahorro_cuota_mensual":385.99999999999955, "ahorro_total":-385.99999999999955, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":39000.0, "cuota":1950.0, "saldo":18446.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.527, "fecha_inicio":"2021-03-17", "tipo_deuda":"R", "ahorro_cuota_mensual":20395.999999999964, "ahorro_total":-20395.999999999964, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":32000.0, "cuota":1589.0, "saldo":22789.0, "tasa_externa":0.4322, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.2878, "fecha_inicio":"2023-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":346.9507393101312, "ahorro_total":12490.226615164724, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":22100.0, "cuota":1105.0, "saldo":11654.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4727, "fecha_inicio":"2021-07-19", "tipo_deuda":"R", "ahorro_cuota_mensual":12758.999999999978, "ahorro_total":-12758.999999999978, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":1850.0, "cuota":1896.0, "saldo":1896.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0249, "fecha_inicio":"2024-03-25", "tipo_deuda":"I", "ahorro_cuota_mensual":10.233333333342443, "ahorro_total":10.233333333342443, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4100476, "monto_maximo_cliente": 453540.0, "cuota_externa_total": 32891.0, "capacidad_maxima_pago": 85385.0, "bursolnum": 7439697, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5225.90843441975, "monto_max": 453540.0, "cuota_min": 370.5085944866793, "monto_min": 5000, "plazo_max": 21.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":80000.0, "cuota":8168.0, "saldo":77105.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":15.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.0362, "fecha_inicio":"2023-11-28", "tipo_deuda":"O", "ahorro_cuota_mensual":-460.0154006330904, "ahorro_total":-6900.231009496356, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":7, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"1991-07-06", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":52600.0, "cuota":5540.0, "saldo":38823.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":18.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.2619, "fecha_inicio":"2023-06-14", "tipo_deuda":"I", "ahorro_cuota_mensual":196.28970415784534, "ahorro_total":3533.214674841216, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "OTRAS FINANCIERA", "registro":10, "monto_otorgado":42000.0, "cuota":-1.0, "saldo":40611.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0331, "fecha_inicio":"2024-01-25", "tipo_deuda":"R", "ahorro_cuota_mensual":40610.00000000001, "ahorro_total":-40610.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "OTRAS FINANCIERA", "registro":9, "monto_otorgado":60000.0, "cuota":-1.0, "saldo":33819.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4364, "fecha_inicio":"2023-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":33818.0, "ahorro_total":-33818.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":16500.0, "cuota":825.0, "saldo":15672.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0502, "fecha_inicio":"2022-01-21", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":100000.0, "cuota":5000.0, "saldo":14740.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8526, "fecha_inicio":"2023-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":19740.0, "ahorro_total":-19740.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":285200.0, "cuota":14260.0, "saldo":204522.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2829, "fecha_inicio":"2021-09-14", "tipo_deuda":"R", "ahorro_cuota_mensual":218782.00000000003, "ahorro_total":-218782.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":31300.0, "cuota":1565.0, "saldo":11795.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6232, "fecha_inicio":"2022-06-13", "tipo_deuda":"R", "ahorro_cuota_mensual":13360.000000000002, "ahorro_total":-13360.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":55276.0, "cuota":5800.0, "saldo":26016.0, "tasa_externa":0.5792, "tasa_kubo":0.7554, "numero_pagos_otorgado":13.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5293, "fecha_inicio":"2023-07-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-927.5612441832855, "ahorro_total":-12058.29617438271, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4161166, "monto_maximo_cliente": 191829.0, "cuota_externa_total": 12031.0, "capacidad_maxima_pago": 70552.0, "bursolnum": 7437950, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2702.237228177656, "monto_max": 191829.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5486, "kubo_score": "C3", "comision": 0.0423, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":30000.0, "cuota":1885.0, "saldo":20583.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":36.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.3139, "fecha_inicio":"2022-06-09", "tipo_deuda":"I", "ahorro_cuota_mensual":464.2070050282073, "ahorro_total":16711.452181015462, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":12, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2009-11-03", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-01-06", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":16, "monto_otorgado":24339.0, "cuota":4793.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2009-12-03", "tipo_deuda":"R", "ahorro_cuota_mensual":4793.0, "ahorro_total":-4793.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":16000.0, "cuota":1620.0, "saldo":17517.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0948, "fecha_inicio":"2022-05-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":3000.0, "cuota":445.0, "saldo":3325.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.1083, "fecha_inicio":"2023-02-09", "tipo_deuda":"R", "ahorro_cuota_mensual":3769.999999999992, "ahorro_total":-3769.999999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":70900.0, "cuota":3340.0, "saldo":56696.0, "tasa_externa":0.4856, "tasa_kubo":0.3337, "numero_pagos_otorgado":48.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":0.2003, "fecha_inicio":"2022-10-27", "tipo_deuda":"I", "ahorro_cuota_mensual":415.89674157467607, "ahorro_total":19963.04359558445, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":7000.0, "cuota":583.0, "saldo":6137.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1233, "fecha_inicio":"2008-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":6719.9999999999845, "ahorro_total":-6719.9999999999845, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":2560.0, "cuota":80.0, "saldo":920.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":128.0, "numero_pagos_restante":12.0, "frecuencia_externa":"W", "avance":0.6406, "fecha_inicio":"2022-08-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-49.44727545633333, "ahorro_total":-1582.3128146026665, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":1280.0, "cuota":40.0, "saldo":1270.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":128.0, "numero_pagos_restante":31.0, "frecuencia_externa":"W", "avance":0.0078, "fecha_inicio":"2024-03-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-24.723637728166665, "ahorro_total":-791.1564073013333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":12416.0, "cuota":388.0, "saldo":12319.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":128.0, "numero_pagos_restante":31.0, "frecuencia_externa":"W", "avance":0.0078, "fecha_inicio":"2024-03-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-239.81928596321666, "ahorro_total":-7674.217150822933, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":17500.0, "cuota":875.0, "saldo":17099.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0229, "fecha_inicio":"2024-02-06", "tipo_deuda":"R", "ahorro_cuota_mensual":17973.999999999956, "ahorro_total":-17973.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":16500.0, "cuota":825.0, "saldo":12226.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.259, "fecha_inicio":"2022-08-31", "tipo_deuda":"R", "ahorro_cuota_mensual":13050.999999999969, "ahorro_total":-13050.999999999969, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":10310.0, "cuota":899.0, "saldo":8792.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1472, "fecha_inicio":"2009-05-25", "tipo_deuda":"R", "ahorro_cuota_mensual":9690.999999999978, "ahorro_total":-9690.999999999978, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":39577.0, "cuota":2688.0, "saldo":38175.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":96.0, "numero_pagos_restante":39.0, "frecuencia_externa":"S", "avance":0.0354, "fecha_inicio":"2023-07-06", "tipo_deuda":"I", "ahorro_cuota_mensual":1055.7399907094634, "ahorro_total":50675.51955405425, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4177829, "monto_maximo_cliente": 55510.0, "cuota_externa_total": 18053.0, "capacidad_maxima_pago": 31947.0, "bursolnum": 7437953, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 825.4611706380136, "monto_max": 55510.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "kubo_scores": ['K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":27, "monto_otorgado":1050.0, "cuota":389.0, "saldo":1084.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0324, "fecha_inicio":"2023-02-09", "tipo_deuda":"I", "ahorro_cuota_mensual":25.380289495900342, "ahorro_total":76.14086848770103, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":28, "monto_otorgado":1293.0, "cuota":476.0, "saldo":1304.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0085, "fecha_inicio":"2023-02-24", "tipo_deuda":"I", "ahorro_cuota_mensual":28.22829935066585, "ahorro_total":84.68489805199755, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":26, "monto_otorgado":693.0, "cuota":257.0, "saldo":715.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0317, "fecha_inicio":"2023-02-09", "tipo_deuda":"I", "ahorro_cuota_mensual":17.010991067294185, "ahorro_total":51.032973201882555, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":15000.0, "cuota":1930.0, "saldo":12949.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.1367, "fecha_inicio":"2023-11-07", "tipo_deuda":"I", "ahorro_cuota_mensual":517.4069533454112, "ahorro_total":6208.883440144935, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":31600.0, "cuota":2446.0, "saldo":29239.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":23.0, "frecuencia_externa":"M", "avance":0.0747, "fecha_inicio":"2023-03-14", "tipo_deuda":"I", "ahorro_cuota_mensual":1219.4763550687546, "ahorro_total":43901.14878247517, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":50000.0, "cuota":5117.0, "saldo":49370.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":18.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.0126, "fecha_inicio":"2024-01-22", "tipo_deuda":"I", "ahorro_cuota_mensual":1801.4117688664473, "ahorro_total":32425.411839596054, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":22300.0, "cuota":1222.0, "saldo":17425.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2186, "fecha_inicio":"2022-07-15", "tipo_deuda":"R", "ahorro_cuota_mensual":18646.999999999964, "ahorro_total":-18646.999999999964, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":9000.0, "cuota":1544.0, "saldo":6309.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.299, "fecha_inicio":"2021-11-11", "tipo_deuda":"R", "ahorro_cuota_mensual":7852.999999999988, "ahorro_total":-7852.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":1099.0, "cuota":433.0, "saldo":801.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2712, "fecha_inicio":"2024-01-09", "tipo_deuda":"I", "ahorro_cuota_mensual":52.411369672375656, "ahorro_total":157.23410901712697, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":2076.0, "cuota":802.0, "saldo":2152.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0366, "fecha_inicio":"2024-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":83.0718866604658, "ahorro_total":249.21565998139738, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":419.0, "cuota":164.0, "saldo":303.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2768, "fecha_inicio":"2024-01-12", "tipo_deuda":"I", "ahorro_cuota_mensual":18.898420284554504, "ahorro_total":56.69526085366351, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":1132.0, "cuota":447.0, "saldo":829.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2677, "fecha_inicio":"2024-01-07", "tipo_deuda":"I", "ahorro_cuota_mensual":54.98332162796112, "ahorro_total":164.94996488388335, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":4014.0, "cuota":1570.0, "saldo":2913.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2743, "fecha_inicio":"2024-01-11", "tipo_deuda":"I", "ahorro_cuota_mensual":179.933792415756, "ahorro_total":539.801377247268, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":20000.0, "cuota":1256.0, "saldo":18985.0, "tasa_externa":0.3521, "tasa_kubo":0.2, "numero_pagos_otorgado":43.0, "numero_pagos_restante":15.0, "frecuencia_externa":"S", "avance":0.0507, "fecha_inicio":"2023-10-02", "tipo_deuda":"I", "ahorro_cuota_mensual":131.28152222031963, "ahorro_total":2888.193488847032, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4268611, "monto_maximo_cliente": 325496.0, "cuota_externa_total": 17804.0, "capacidad_maxima_pago": 141736.0, "bursolnum": 7438040, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4121.472630249849, "monto_max": 325496.0, "cuota_min": 151.9292154681686, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2306, 0.2], "comisiones": [0.03845, 0.03845], "kubo_scores": ['K2', 'K1'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":17, "monto_otorgado":100.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":70000.0, "cuota":4509.0, "saldo":50084.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":36.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.2845, "fecha_inicio":"2022-07-15", "tipo_deuda":"I", "ahorro_cuota_mensual":1660.6301960356195, "ahorro_total":59782.6870572823, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":42500.0, "cuota":2860.0, "saldo":40917.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0372, "fecha_inicio":"2017-09-22", "tipo_deuda":"R", "ahorro_cuota_mensual":43776.99999999983, "ahorro_total":-43776.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":86040.0, "cuota":2346.0, "saldo":80891.0, "tasa_externa":0.3146, "tasa_kubo":0.2306, "numero_pagos_otorgado":116.0, "numero_pagos_restante":85.0, "frecuencia_externa":"M", "avance":0.0598, "fecha_inicio":"2021-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":266.911106677685, "ahorro_total":30961.688374611458, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":48500.0, "cuota":2533.0, "saldo":37819.0, "tasa_externa":0.4757, "tasa_kubo":0.2306, "numero_pagos_otorgado":36.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.2202, "fecha_inicio":"2023-02-27", "tipo_deuda":"I", "ahorro_cuota_mensual":559.4866358246793, "ahorro_total":20141.518889688454, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":89900.0, "cuota":1500.0, "saldo":40105.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5539, "fecha_inicio":"2020-07-21", "tipo_deuda":"R", "ahorro_cuota_mensual":41604.99999999983, "ahorro_total":-41604.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":102000.0, "cuota":5556.0, "saldo":105693.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0362, "fecha_inicio":"2022-08-05", "tipo_deuda":"R", "ahorro_cuota_mensual":111248.99999999956, "ahorro_total":-111248.99999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":38000.0, "cuota":2089.0, "saldo":4241.0, "tasa_externa":-1.0, "tasa_kubo":0.2306, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8884, "fecha_inicio":"2022-01-03", "tipo_deuda":"R", "ahorro_cuota_mensual":6329.999999999983, "ahorro_total":-6329.999999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4302913, "monto_maximo_cliente": 199726.0, "cuota_externa_total": 23809.0, "capacidad_maxima_pago": 24898.0, "bursolnum": 7438070, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 223.28918533632032, "monto_max": 199726.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 51.0, "plazo_min": 4, "tasa": 0.8317, "kubo_score": "E3", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "kubo_scores": ['K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":100000.0, "cuota":8657.0, "saldo":99114.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":0.0089, "fecha_inicio":"2024-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":4775.59606034416, "ahorro_total":171921.45817238977, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":9, "monto_otorgado":36900.0, "cuota":1072.0, "saldo":34860.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0553, "fecha_inicio":"2023-05-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-36541.39999999982, "ahorro_total":-36541.39999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":1302381.0, "cuota":13825.0, "saldo":1174319.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":180.0, "numero_pagos_restante":144.0, "frecuencia_externa":"M", "avance":0.0983, "fecha_inicio":"2021-04-30", "tipo_deuda":"M", "ahorro_cuota_mensual":-9625.342161700813, "ahorro_total":-1732561.5891061465, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":2, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-07-26", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":12, "monto_otorgado":23000.0, "cuota":2853.0, "saldo":500.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9783, "fecha_inicio":"2017-04-18", "tipo_deuda":"R", "ahorro_cuota_mensual":3352.999999999999, "ahorro_total":-3352.999999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":21000.0, "cuota":2000.0, "saldo":10162.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5161, "fecha_inicio":"2019-01-26", "tipo_deuda":"R", "ahorro_cuota_mensual":12161.99999999998, "ahorro_total":-12161.99999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":82800.0, "cuota":85597.0, "saldo":79982.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.034, "fecha_inicio":"2018-12-27", "tipo_deuda":"R", "ahorro_cuota_mensual":165578.99999999983, "ahorro_total":-165578.99999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":27000.0, "cuota":2000.0, "saldo":18517.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3142, "fecha_inicio":"2020-02-22", "tipo_deuda":"R", "ahorro_cuota_mensual":20516.999999999964, "ahorro_total":-20516.999999999964, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":30000.0, "cuota":146.0, "saldo":13651.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.545, "fecha_inicio":"2022-12-13", "tipo_deuda":"R", "ahorro_cuota_mensual":13796.999999999975, "ahorro_total":-13796.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":7200.0, "cuota":255.0, "saldo":6559.0, "tasa_externa":0.3537, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":46.0, "frecuencia_externa":"M", "avance":0.089, "fecha_inicio":"2023-02-14", "tipo_deuda":"I", "ahorro_cuota_mensual":51.2004180708343, "ahorro_total":3072.025084250058, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":135500.0, "cuota":5100.0, "saldo":69714.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4855, "fecha_inicio":"2022-04-20", "tipo_deuda":"R", "ahorro_cuota_mensual":74813.99999999987, "ahorro_total":-74813.99999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4323421, "monto_maximo_cliente": 503880.0, "cuota_externa_total": 90443.0, "capacidad_maxima_pago": 203056.0, "bursolnum": 7438089, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4898.836400896599, "monto_max": 503880.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 55.0, "plazo_min": 4, "tasa": 0.5991, "kubo_score": "D1", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "kubo_scores": ['K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":9, "monto_otorgado":210000.0, "cuota":5419.0, "saldo":184781.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1201, "fecha_inicio":"2023-07-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-20227.44834993273, "ahorro_total":-182047.03514939456, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "OTRAS FINANCIERA", "registro":15, "monto_otorgado":317011.0, "cuota":0.0, "saldo":65449.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7935, "fecha_inicio":"2021-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":317010.9999999994, "ahorro_total":-317010.9999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":14, "monto_otorgado":1138.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-10-14", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":13, "monto_otorgado":350000.0, "cuota":20217.0, "saldo":131219.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":48.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":0.6251, "fecha_inicio":"2023-01-20", "tipo_deuda":"I", "ahorro_cuota_mensual":8960.598186805562, "ahorro_total":430108.712966667, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":250000.0, "cuota":16845.0, "saldo":243460.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.0262, "fecha_inicio":"2023-11-29", "tipo_deuda":"I", "ahorro_cuota_mensual":7141.4901508604, "ahorro_total":257093.6454309744, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":10, "monto_otorgado":50000.0, "cuota":1409.0, "saldo":49702.0, "tasa_externa":0.233, "tasa_kubo":0.2, "numero_pagos_otorgado":60.0, "numero_pagos_restante":57.0, "frecuencia_externa":"M", "avance":0.006, "fecha_inicio":"2024-01-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-6.274874508095081, "ahorro_total":-376.49247048570487, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":47900.0, "cuota":1297.0, "saldo":43646.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0888, "fecha_inicio":"2023-11-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-4552.832742675132, "ahorro_total":-40975.49468407619, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":145000.0, "cuota":7250.0, "saldo":142838.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":156.0, "numero_pagos_restante":68.0, "frecuencia_externa":"Z", "avance":0.0149, "fecha_inicio":"2016-12-17", "tipo_deuda":"R", "ahorro_cuota_mensual":4341.812274605973, "ahorro_total":677322.7148385317, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":4, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-08-12", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":19600.0, "cuota":19318.0, "saldo":19318.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0144, "fecha_inicio":"2022-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":38635.99999999996, "ahorro_total":-38635.99999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":15951.0, "cuota":1472.0, "saldo":13451.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.1567, "fecha_inicio":"2024-01-11", "tipo_deuda":"I", "ahorro_cuota_mensual":-30.151445812489783, "ahorro_total":-361.8173497498774, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":165000.0, "cuota":5472.0, "saldo":118676.0, "tasa_externa":0.2203, "tasa_kubo":0.2, "numero_pagos_otorgado":44.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.2808, "fecha_inicio":"2023-03-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-130.50569265885042, "ahorro_total":-5742.2504769894185, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":94200.0, "cuota":4710.0, "saldo":93693.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0054, "fecha_inicio":"2011-11-11", "tipo_deuda":"R", "ahorro_cuota_mensual":98402.99999999981, "ahorro_total":-98402.99999999981, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":70600.0, "cuota":5514.0, "saldo":67080.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0499, "fecha_inicio":"2023-02-02", "tipo_deuda":"R", "ahorro_cuota_mensual":72593.99999999987, "ahorro_total":-72593.99999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":246900.0, "cuota":6962.0, "saldo":189052.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":48.0, "numero_pagos_restante":32.0, "frecuencia_externa":"M", "avance":0.2343, "fecha_inicio":"2022-12-23", "tipo_deuda":"I", "ahorro_cuota_mensual":-978.5874505077318, "ahorro_total":-46972.197624371125, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4426818, "monto_maximo_cliente": 209516.0, "cuota_externa_total": 30873.0, "capacidad_maxima_pago": 10191.0, "bursolnum": 7438215, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1282.6757280888382, "monto_max": 209516.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 23.0, "plazo_min": 4, "tasa": 0.6722, "kubo_score": "D4", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":32, "monto_otorgado":2000.0, "cuota":256.0, "saldo":458.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.771, "fecha_inicio":"2022-05-08", "tipo_deuda":"I", "ahorro_cuota_mensual":10.89105110209212, "ahorro_total":130.69261322510545, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":33, "monto_otorgado":5000.0, "cuota":1123.0, "saldo":5015.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.003, "fecha_inicio":"2023-02-27", "tipo_deuda":"I", "ahorro_cuota_mensual":90.22491464645645, "ahorro_total":541.3494878787387, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":34, "monto_otorgado":6000.0, "cuota":2288.0, "saldo":4130.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3117, "fecha_inicio":"2023-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":22.63186720740441, "ahorro_total":67.89560162221323, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":35, "monto_otorgado":4700.0, "cuota":586.0, "saldo":2811.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4019, "fecha_inicio":"2022-08-30", "tipo_deuda":"I", "ahorro_cuota_mensual":9.993970089916502, "ahorro_total":119.92764107899802, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":36, "monto_otorgado":5000.0, "cuota":1055.0, "saldo":2762.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4476, "fecha_inicio":"2022-11-29", "tipo_deuda":"I", "ahorro_cuota_mensual":22.224914646456455, "ahorro_total":133.34948787873873, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":37, "monto_otorgado":880.0, "cuota":132.0, "saldo":240.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7273, "fecha_inicio":"2022-08-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-0.19771269255036827, "ahorro_total":-1.7794142329533145, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":19, "monto_otorgado":100000.0, "cuota":7066.0, "saldo":79961.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":36.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.2004, "fecha_inicio":"2022-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-183.61210904599739, "ahorro_total":-6610.035925655906, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-01-26", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":17, "monto_otorgado":20000.0, "cuota":2471.0, "saldo":12203.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3899, "fecha_inicio":"2023-08-17", "tipo_deuda":"I", "ahorro_cuota_mensual":19.91051102092115, "ahorro_total":238.9261322510538, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":22, "monto_otorgado":837.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-03-31", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":23, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"1991-10-11", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":25, "monto_otorgado":1527.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-10-15", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":21, "monto_otorgado":15100.0, "cuota":1794.0, "saldo":15087.0, "tasa_externa":0.7213, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0009, "fecha_inicio":"2021-07-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-56.57256417920462, "ahorro_total":-678.8707701504554, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":2, "monto_otorgado":5000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-01-27", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":20, "monto_otorgado":5000.0, "cuota":851.0, "saldo":5504.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.1008, "fecha_inicio":"2013-01-18", "tipo_deuda":"R", "ahorro_cuota_mensual":6355.000000000006, "ahorro_total":-6355.000000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":9200.0, "cuota":460.0, "saldo":9078.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0133, "fecha_inicio":"2022-09-04", "tipo_deuda":"R", "ahorro_cuota_mensual":9538.000000000011, "ahorro_total":-9538.000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":38000.0, "cuota":2378.0, "saldo":37678.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0085, "fecha_inicio":"2024-01-03", "tipo_deuda":"R", "ahorro_cuota_mensual":40056.000000000044, "ahorro_total":-40056.000000000044, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":2000.0, "cuota":200.0, "saldo":1694.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.153, "fecha_inicio":"2024-02-09", "tipo_deuda":"R", "ahorro_cuota_mensual":1894.000000000002, "ahorro_total":-1894.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":48651.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":49.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.027, "fecha_inicio":"2020-03-20", "tipo_deuda":"R", "ahorro_cuota_mensual":-812.8336795635632, "ahorro_total":-39828.8502986146, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":27000.0, "cuota":1350.0, "saldo":26541.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":65.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.017, "fecha_inicio":"2018-11-15", "tipo_deuda":"R", "ahorro_cuota_mensual":-403.91405623964283, "ahorro_total":-26254.413655576784, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":5600.0, "cuota":1278.0, "saldo":4837.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1362, "fecha_inicio":"2024-02-02", "tipo_deuda":"I", "ahorro_cuota_mensual":121.29190440403113, "ahorro_total":727.7514264241868, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":2400.0, "cuota":532.0, "saldo":935.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6104, "fecha_inicio":"2023-11-03", "tipo_deuda":"I", "ahorro_cuota_mensual":36.26795903029904, "ahorro_total":217.60775418179423, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":4000.0, "cuota":1627.0, "saldo":1476.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.631, "fecha_inicio":"2023-12-28", "tipo_deuda":"I", "ahorro_cuota_mensual":116.75457813826961, "ahorro_total":350.2637344148088, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":100.0, "cuota":14.0, "saldo":13.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.87, "fecha_inicio":"2023-03-30", "tipo_deuda":"I", "ahorro_cuota_mensual":1.7445525551046064, "ahorro_total":20.934630661255277, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":4000.0, "cuota":674.0, "saldo":2180.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.455, "fecha_inicio":"2023-09-28", "tipo_deuda":"I", "ahorro_cuota_mensual":73.10130594295288, "ahorro_total":657.9117534865759, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":4000.0, "cuota":532.0, "saldo":1372.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.657, "fecha_inicio":"2023-05-30", "tipo_deuda":"I", "ahorro_cuota_mensual":41.78210220418424, "ahorro_total":501.3852264502109, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":4500.0, "cuota":600.0, "saldo":1987.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5584, "fecha_inicio":"2023-06-29", "tipo_deuda":"I", "ahorro_cuota_mensual":48.50486497970735, "ahorro_total":582.0583797564882, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":5000.0, "cuota":695.0, "saldo":1221.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7558, "fecha_inicio":"2023-05-04", "tipo_deuda":"I", "ahorro_cuota_mensual":82.22762775523029, "ahorro_total":986.7315330627634, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":15, "monto_otorgado":6990.0, "cuota":1430.0, "saldo":7022.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":9.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":-0.0046, "fecha_inicio":"2024-02-28", "tipo_deuda":"I", "ahorro_cuota_mensual":379.92953213530996, "ahorro_total":3419.36578921779, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":5100.0, "cuota":810.0, "saldo":1444.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7169, "fecha_inicio":"2023-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":43.85416507726495, "ahorro_total":394.68748569538457, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4446822, "monto_maximo_cliente": 366903.0, "cuota_externa_total": 48039.0, "capacidad_maxima_pago": 102792.0, "bursolnum": 7438247, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5497.726574423007, "monto_max": 366903.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 31.0, "plazo_min": 4, "tasa": 0.3813, "kubo_score": "A5", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2010-07-13", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":15, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2020-11-17", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":14, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2014-12-13", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":125700.0, "cuota":8079.0, "saldo":72253.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":24.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.4252, "fecha_inicio":"2023-01-20", "tipo_deuda":"I", "ahorro_cuota_mensual":97.70931224619198, "ahorro_total":2345.0234939086076, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":150000.0, "cuota":6770.0, "saldo":149889.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":48.0, "numero_pagos_restante":45.0, "frecuencia_externa":"M", "avance":0.0007, "fecha_inicio":"2024-01-23", "tipo_deuda":"I", "ahorro_cuota_mensual":60.4231189711918, "ahorro_total":2900.3097106172063, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":9, "monto_otorgado":1499999.0, "cuota":14669.0, "saldo":1310570.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":195.0, "numero_pagos_restante":155.0, "frecuencia_externa":"M", "avance":0.1263, "fecha_inicio":"2020-12-09", "tipo_deuda":"M", "ahorro_cuota_mensual":-33678.89411252966, "ahorro_total":-6567384.351943284, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":13, "monto_otorgado":13000.0, "cuota":650.0, "saldo":7878.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.394, "fecha_inicio":"2016-11-29", "tipo_deuda":"R", "ahorro_cuota_mensual":8528.000000000018, "ahorro_total":-8528.000000000018, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":12, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-11-21", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":80000.0, "cuota":3796.0, "saldo":57211.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":43.0, "numero_pagos_restante":12.0, "frecuencia_externa":"S", "avance":0.2849, "fecha_inicio":"2023-07-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-1574.9732919526668, "ahorro_total":-34649.412422958674, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":80000.0, "cuota":5156.0, "saldo":78201.0, "tasa_externa":0.3847, "tasa_kubo":0.3813, "numero_pagos_otorgado":43.0, "numero_pagos_restante":16.0, "frecuencia_externa":"S", "avance":0.0225, "fecha_inicio":"2023-10-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-214.97329195266684, "ahorro_total":-4729.4124229586705, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":40600.0, "cuota":276.0, "saldo":34118.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1597, "fecha_inicio":"2006-10-09", "tipo_deuda":"R", "ahorro_cuota_mensual":34394.00000000008, "ahorro_total":-34394.00000000008, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":54000.0, "cuota":2700.0, "saldo":39848.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2621, "fecha_inicio":"2008-11-27", "tipo_deuda":"R", "ahorro_cuota_mensual":42548.00000000009, "ahorro_total":-42548.00000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":20590.0, "cuota":872.0, "saldo":11441.0, "tasa_externa":0.4105, "tasa_kubo":0.3813, "numero_pagos_otorgado":48.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.4443, "fecha_inicio":"2021-09-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-49.00125320255438, "ahorro_total":-2352.0601537226103, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":60600.0, "cuota":3030.0, "saldo":55843.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0785, "fecha_inicio":"2021-04-05", "tipo_deuda":"R", "ahorro_cuota_mensual":58873.000000000124, "ahorro_total":-58873.000000000124, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":48400.0, "cuota":3404.0, "saldo":48626.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0047, "fecha_inicio":"2022-08-18", "tipo_deuda":"R", "ahorro_cuota_mensual":52030.0000000001, "ahorro_total":-52030.0000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4475229, "monto_maximo_cliente": 155752.0, "cuota_externa_total": 16746.0, "capacidad_maxima_pago": 68111.0, "bursolnum": 7438276, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3485.367365228652, "monto_max": 155752.0, "cuota_min": 269.2747621622814, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.8317, "kubo_score": "E3", "comision": 0.0466, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":30000.0, "cuota":2976.0, "saldo":29435.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":22.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.0188, "fecha_inicio":"2024-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":672.8035626298793, "ahorro_total":14801.678377857344, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":80000.0, "cuota":5532.0, "saldo":73993.0, "tasa_externa":0.4748, "tasa_kubo":0.5292, "numero_pagos_otorgado":43.0, "numero_pagos_restante":10.0, "frecuencia_externa":"S", "avance":0.0751, "fecha_inicio":"2023-04-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-609.8571663203211, "ahorro_total":-13416.857659047064, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":34000.0, "cuota":2449.0, "saldo":33249.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0221, "fecha_inicio":"2023-11-30", "tipo_deuda":"R", "ahorro_cuota_mensual":35698.000000000015, "ahorro_total":-35698.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":55000.0, "cuota":3992.0, "saldo":51790.0, "tasa_externa":0.5386, "tasa_kubo":0.5292, "numero_pagos_otorgado":43.0, "numero_pagos_restante":12.0, "frecuencia_externa":"S", "avance":0.0584, "fecha_inicio":"2023-06-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-230.5268018452207, "ahorro_total":-5071.589640594855, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":23900.0, "cuota":1195.0, "saldo":14300.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4017, "fecha_inicio":"2022-12-07", "tipo_deuda":"R", "ahorro_cuota_mensual":15495.000000000005, "ahorro_total":-15495.000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":46500.0, "cuota":2325.0, "saldo":34703.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2537, "fecha_inicio":"2023-09-18", "tipo_deuda":"R", "ahorro_cuota_mensual":37028.00000000001, "ahorro_total":-37028.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":21400.0, "cuota":1070.0, "saldo":18500.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1355, "fecha_inicio":"2021-09-06", "tipo_deuda":"R", "ahorro_cuota_mensual":19570.000000000007, "ahorro_total":-19570.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4488665, "monto_maximo_cliente": 182243.0, "cuota_externa_total": 8651.0, "capacidad_maxima_pago": 72949.0, "bursolnum": 7438302, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3436.688563478484, "monto_max": 182243.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.7007, "kubo_score": "D5", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "CIA Q' OTORGA", "registro":9, "monto_otorgado":47632.0, "cuota":0.0, "saldo":9474.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.8011, "fecha_inicio":"2022-07-11", "tipo_deuda":"O", "ahorro_cuota_mensual":9474.000000000013, "ahorro_total":-9474.000000000013, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":24600.0, "cuota":1911.0, "saldo":21062.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.1438, "fecha_inicio":"2022-10-04", "tipo_deuda":"I", "ahorro_cuota_mensual":127.59542117468459, "ahorro_total":4593.435162288645, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":13, "monto_otorgado":2483.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-11-27", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":51600.0, "cuota":4004.0, "saldo":46777.0, "tasa_externa":0.9338, "tasa_kubo":0.6722, "numero_pagos_otorgado":120.0, "numero_pagos_restante":45.0, "frecuencia_externa":"S", "avance":0.0935, "fecha_inicio":"2023-01-09", "tipo_deuda":"I", "ahorro_cuota_mensual":572.5413973464492, "ahorro_total":34352.483840786954, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":27100.0, "cuota":2104.0, "saldo":24766.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0861, "fecha_inicio":"2023-02-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-1665.3725222857188, "ahorro_total":-16653.72522285719, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":22601.0, "cuota":3000.0, "saldo":20132.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1092, "fecha_inicio":"2020-02-24", "tipo_deuda":"R", "ahorro_cuota_mensual":23132.000000000022, "ahorro_total":-23132.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":2, "monto_otorgado":15000.0, "cuota":-1.0, "saldo":6122.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5919, "fecha_inicio":"2023-11-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":15000.0, "cuota":1603.0, "saldo":17136.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.1424, "fecha_inicio":"2022-11-09", "tipo_deuda":"R", "ahorro_cuota_mensual":18739.000000000022, "ahorro_total":-18739.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":18000.0, "cuota":1587.0, "saldo":15876.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.118, "fecha_inicio":"2022-10-28", "tipo_deuda":"R", "ahorro_cuota_mensual":17463.000000000022, "ahorro_total":-17463.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":4, "monto_otorgado":14916.0, "cuota":-1.0, "saldo":5578.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.626, "fecha_inicio":"2024-02-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":3, "monto_otorgado":14933.0, "cuota":-1.0, "saldo":3969.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7342, "fecha_inicio":"2024-01-02", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":14000.0, "cuota":700.0, "saldo":13729.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0194, "fecha_inicio":"2022-07-07", "tipo_deuda":"R", "ahorro_cuota_mensual":14429.000000000016, "ahorro_total":-14429.000000000016, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":13000.0, "cuota":1270.0, "saldo":11527.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1133, "fecha_inicio":"2021-10-29", "tipo_deuda":"R", "ahorro_cuota_mensual":12797.000000000015, "ahorro_total":-12797.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4503596, "monto_maximo_cliente": 199076.0, "cuota_externa_total": 19650.0, "capacidad_maxima_pago": 149214.0, "bursolnum": 7438310, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 10485.061141968403, "monto_max": 199076.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.6722, "kubo_score": "D4", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":6000.0, "cuota":300.0, "saldo":3551.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4082, "fecha_inicio":"2022-03-18", "tipo_deuda":"R", "ahorro_cuota_mensual":3851.000000000004, "ahorro_total":-3851.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":8000.0, "cuota":988.0, "saldo":4776.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.403, "fecha_inicio":"2023-08-29", "tipo_deuda":"I", "ahorro_cuota_mensual":7.564204408368482, "ahorro_total":90.77045290042179, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":13, "monto_otorgado":14500.0, "cuota":725.0, "saldo":2213.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8474, "fecha_inicio":"2017-01-27", "tipo_deuda":"R", "ahorro_cuota_mensual":2938.0000000000023, "ahorro_total":-2938.0000000000023, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":8000.0, "cuota":400.0, "saldo":6032.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.246, "fecha_inicio":"2022-04-28", "tipo_deuda":"R", "ahorro_cuota_mensual":6432.000000000007, "ahorro_total":-6432.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":9600.0, "cuota":480.0, "saldo":1854.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8069, "fecha_inicio":"2023-12-28", "tipo_deuda":"R", "ahorro_cuota_mensual":2334.000000000002, "ahorro_total":-2334.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":6000.0, "cuota":362.0, "saldo":3612.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.398, "fecha_inicio":"2022-01-16", "tipo_deuda":"R", "ahorro_cuota_mensual":3974.0000000000045, "ahorro_total":-3974.0000000000045, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":4, "monto_otorgado":150.0, "cuota":351.0, "saldo":1404.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-8.36, "fecha_inicio":"2024-02-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":3, "monto_otorgado":4549.0, "cuota":80.0, "saldo":160.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9648, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":20000.0, "cuota":3770.0, "saldo":13375.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":21.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.3313, "fecha_inicio":"2023-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":2584.9980210088447, "ahorro_total":54284.958441185736, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":20000.0, "cuota":2700.0, "saldo":13375.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3313, "fecha_inicio":"2023-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":16075.000000000015, "ahorro_total":-16075.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":153500.0, "cuota":13063.0, "saldo":152144.0, "tasa_externa":1.0131, "tasa_kubo":0.6722, "numero_pagos_otorgado":48.0, "numero_pagos_restante":43.0, "frecuencia_externa":"M", "avance":0.0088, "fecha_inicio":"2023-11-28", "tipo_deuda":"I", "ahorro_cuota_mensual":2577.938858031597, "ahorro_total":123741.06518551667, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4557872, "monto_maximo_cliente": 303779.0, "cuota_externa_total": 42544.0, "capacidad_maxima_pago": 173956.0, "bursolnum": 7438398, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7308.096433568694, "monto_max": 303779.0, "cuota_min": 200.2991210698785, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0428, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":25000.0, "cuota":26566.0, "saldo":25928.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0371, "fecha_inicio":"2024-02-13", "tipo_deuda":"I", "ahorro_cuota_mensual":691.8916666666955, "ahorro_total":691.8916666666955, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":47000.0, "cuota":3020.0, "saldo":37831.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":36.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.1951, "fecha_inicio":"2022-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":704.8318992146183, "ahorro_total":25373.948371726256, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":38500.0, "cuota":1483.0, "saldo":36659.0, "tasa_externa":0.402, "tasa_kubo":0.3617, "numero_pagos_otorgado":60.0, "numero_pagos_restante":47.0, "frecuencia_externa":"M", "avance":0.0478, "fecha_inicio":"2023-03-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-59.30323223806454, "ahorro_total":-3558.1939342838723, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":18400.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-05-16", "tipo_deuda":"I", "ahorro_cuota_mensual":-19043.343733333313, "ahorro_total":-19043.343733333313, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":26000.0, "cuota":0.0, "saldo":141.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9946, "fecha_inicio":"2024-01-26", "tipo_deuda":"R", "ahorro_cuota_mensual":140.99999999999966, "ahorro_total":-140.99999999999966, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":54000.0, "cuota":2942.0, "saldo":18460.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6581, "fecha_inicio":"2023-05-08", "tipo_deuda":"R", "ahorro_cuota_mensual":21401.999999999956, "ahorro_total":-21401.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":10000.0, "cuota":500.0, "saldo":1069.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8931, "fecha_inicio":"2019-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":1568.9999999999975, "ahorro_total":-1568.9999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":20800.0, "cuota":1382.0, "saldo":10966.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4728, "fecha_inicio":"2017-07-04", "tipo_deuda":"R", "ahorro_cuota_mensual":12347.999999999976, "ahorro_total":-12347.999999999976, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":27000.0, "cuota":1350.0, "saldo":10685.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6043, "fecha_inicio":"2022-12-09", "tipo_deuda":"R", "ahorro_cuota_mensual":12034.999999999975, "ahorro_total":-12034.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":6000.0, "cuota":544.0, "saldo":846.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.859, "fecha_inicio":"2017-12-20", "tipo_deuda":"R", "ahorro_cuota_mensual":1389.9999999999982, "ahorro_total":-1389.9999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":69000.0, "cuota":3239.0, "saldo":29945.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.566, "fecha_inicio":"2022-02-11", "tipo_deuda":"R", "ahorro_cuota_mensual":33183.999999999935, "ahorro_total":-33183.999999999935, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":12600.0, "cuota":910.0, "saldo":529.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.958, "fecha_inicio":"2018-03-29", "tipo_deuda":"R", "ahorro_cuota_mensual":1438.9999999999986, "ahorro_total":-1438.9999999999986, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":181500.0, "cuota":7826.0, "saldo":158779.0, "tasa_externa":0.4228, "tasa_kubo":0.3617, "numero_pagos_otorgado":48.0, "numero_pagos_restante":37.0, "frecuencia_externa":"M", "avance":0.1252, "fecha_inicio":"2023-05-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-29.198571371619437, "ahorro_total":-1401.531425837733, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":18900.0, "cuota":500.0, "saldo":1106.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9415, "fecha_inicio":"2023-12-11", "tipo_deuda":"R", "ahorro_cuota_mensual":1605.9999999999975, "ahorro_total":-1605.9999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":13520.0, "cuota":676.0, "saldo":5132.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6204, "fecha_inicio":"2017-07-04", "tipo_deuda":"R", "ahorro_cuota_mensual":5807.999999999988, "ahorro_total":-5807.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4604014, "monto_maximo_cliente": 57512.0, "cuota_externa_total": 4017.0, "capacidad_maxima_pago": 47082.0, "bursolnum": 7438490, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1064.501838899779, "monto_max": 57512.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.4428, "kubo_score": "B2", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "kubo_scores": ['K1'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2009-09-03", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":15000.0, "cuota":988.0, "saldo":7987.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.4675, "fecha_inicio":"2022-12-27", "tipo_deuda":"I", "ahorro_cuota_mensual":200.9101998771721, "ahorro_total":4821.84479705213, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":10000.0, "cuota":4200.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-08-11", "tipo_deuda":"R", "ahorro_cuota_mensual":4200.0, "ahorro_total":-4200.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":33099.0, "cuota":1520.0, "saldo":9476.0, "tasa_externa":0.3793, "tasa_kubo":0.2, "numero_pagos_otorgado":37.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7137, "fecha_inicio":"2021-09-28", "tipo_deuda":"I", "ahorro_cuota_mensual":259.3859848546108, "ahorro_total":9597.2814396206, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":15000.0, "cuota":1139.0, "saldo":13986.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0676, "fecha_inicio":"2021-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":15124.999999999975, "ahorro_total":-15124.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":25000.0, "cuota":1250.0, "saldo":10427.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5829, "fecha_inicio":"2023-05-30", "tipo_deuda":"R", "ahorro_cuota_mensual":11676.99999999998, "ahorro_total":-11676.99999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":8300.0, "cuota":168.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-11-15", "tipo_deuda":"R", "ahorro_cuota_mensual":168.0, "ahorro_total":-168.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4637424, "monto_maximo_cliente": 564367.0, "cuota_externa_total": 36780.0, "capacidad_maxima_pago": 129279.0, "bursolnum": 7438550, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7398.095591338296, "monto_max": 564367.0, "cuota_min": 269.2747621622814, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5486, "kubo_score": "C3", "comision": 0.0466, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "HIPOTECARIA", "registro":10, "monto_otorgado":1154637.0, "cuota":12780.0, "saldo":1059797.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":360.0, "numero_pagos_restante":340.0, "frecuencia_externa":"M", "avance":0.0821, "fecha_inicio":"2022-08-15", "tipo_deuda":"M", "ahorro_cuota_mensual":-41434.976190888476, "ahorro_total":-14916591.428719852, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":69000.0, "cuota":4961.0, "saldo":32464.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":23.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5295, "fecha_inicio":"2022-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-210.32397012088313, "ahorro_total":-4837.451312780312, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":2, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-03-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":4495.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"1989-02-01", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":26300.0, "cuota":1315.0, "saldo":18364.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3017, "fecha_inicio":"2010-08-01", "tipo_deuda":"R", "ahorro_cuota_mensual":19679.000000000004, "ahorro_total":-19679.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":137000.0, "cuota":8000.0, "saldo":132300.0, "tasa_externa":0.6526, "tasa_kubo":0.5292, "numero_pagos_otorgado":48.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.0343, "fecha_inicio":"2023-10-30", "tipo_deuda":"I", "ahorro_cuota_mensual":288.35722441554935, "ahorro_total":13841.146771946369, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":220000.0, "cuota":11000.0, "saldo":143233.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3489, "fecha_inicio":"2010-04-06", "tipo_deuda":"R", "ahorro_cuota_mensual":154233.00000000003, "ahorro_total":-154233.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":350000.0, "cuota":25000.0, "saldo":205516.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4128, "fecha_inicio":"2010-12-30", "tipo_deuda":"R", "ahorro_cuota_mensual":230516.00000000006, "ahorro_total":-230516.00000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":63100.0, "cuota":8000.0, "saldo":60254.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0451, "fecha_inicio":"2018-05-02", "tipo_deuda":"R", "ahorro_cuota_mensual":68254.00000000003, "ahorro_total":-68254.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4639545, "monto_maximo_cliente": 190808.0, "cuota_externa_total": 29907.0, "capacidad_maxima_pago": 5493.0, "bursolnum": 7438554, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1671.3667353325393, "monto_max": 190808.0, "cuota_min": 278.44180193239873, "monto_min": 5000, "plazo_max": 17.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":113, "monto_otorgado":352.0, "cuota":41.0, "saldo":304.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1364, "fecha_inicio":"2023-01-11", "tipo_deuda":"I", "ahorro_cuota_mensual":0.5642884240374713, "ahorro_total":6.771461088449655, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":10000.0, "cuota":1339.0, "saldo":1323.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8677, "fecha_inicio":"2023-03-01", "tipo_deuda":"I", "ahorro_cuota_mensual":190.25819386470084, "ahorro_total":2283.09832637641, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":26, "monto_otorgado":8000.0, "cuota":1398.0, "saldo":7476.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0655, "fecha_inicio":"2023-06-20", "tipo_deuda":"R", "ahorro_cuota_mensual":8873.999999999993, "ahorro_total":-8873.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "GUBERNAMENTALES", "registro":27, "monto_otorgado":49545.0, "cuota":2064.0, "saldo":22755.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":21.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.5407, "fecha_inicio":"2023-05-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-1910.0771484740003, "ahorro_total":-40111.62011795401, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "GUBERNAMENTALES", "registro":28, "monto_otorgado":51357.0, "cuota":1712.0, "saldo":31839.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":30.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.38, "fecha_inicio":"2023-05-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-1751.8976345788856, "ahorro_total":-52556.929037366564, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":29, "monto_otorgado":3000.0, "cuota":393.0, "saldo":2562.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.146, "fecha_inicio":"2023-03-08", "tipo_deuda":"R", "ahorro_cuota_mensual":2954.9999999999977, "ahorro_total":-2954.9999999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":31, "monto_otorgado":3000.0, "cuota":261.0, "saldo":2685.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.105, "fecha_inicio":"2022-04-05", "tipo_deuda":"R", "ahorro_cuota_mensual":2945.999999999998, "ahorro_total":-2945.999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":32, "monto_otorgado":18400.0, "cuota":2202.0, "saldo":17285.0, "tasa_externa":0.7374, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0606, "fecha_inicio":"2022-03-17", "tipo_deuda":"I", "ahorro_cuota_mensual":88.31507671104964, "ahorro_total":1059.7809205325957, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":112, "monto_otorgado":336.0, "cuota":69.0, "saldo":289.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1399, "fecha_inicio":"2023-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":2.1220147861450016, "ahorro_total":12.73208871687001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":114, "monto_otorgado":1000.0, "cuota":131.0, "saldo":756.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.244, "fecha_inicio":"2022-11-06", "tipo_deuda":"I", "ahorro_cuota_mensual":16.125819386470084, "ahorro_total":193.509832637641, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":21, "monto_otorgado":220.0, "cuota":35.0, "saldo":193.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1227, "fecha_inicio":"2023-12-10", "tipo_deuda":"I", "ahorro_cuota_mensual":3.6048604706568774, "ahorro_total":32.44374423591189, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":116, "monto_otorgado":1500.0, "cuota":197.0, "saldo":1293.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.138, "fecha_inicio":"2023-01-17", "tipo_deuda":"I", "ahorro_cuota_mensual":24.688729079705126, "ahorro_total":296.2647489564615, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":117, "monto_otorgado":1500.0, "cuota":208.0, "saldo":1274.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1507, "fecha_inicio":"2022-11-26", "tipo_deuda":"I", "ahorro_cuota_mensual":35.688729079705126, "ahorro_total":428.2647489564615, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":118, "monto_otorgado":500.0, "cuota":67.0, "saldo":376.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.248, "fecha_inicio":"2022-11-11", "tipo_deuda":"I", "ahorro_cuota_mensual":9.562909693235042, "ahorro_total":114.7549163188205, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":119, "monto_otorgado":4000.0, "cuota":525.0, "saldo":2963.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2592, "fecha_inicio":"2022-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":65.50327754588034, "ahorro_total":786.039330550564, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":120, "monto_otorgado":1500.0, "cuota":188.0, "saldo":985.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3433, "fecha_inicio":"2022-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":15.688729079705126, "ahorro_total":188.26474895646152, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":121, "monto_otorgado":1000.0, "cuota":133.0, "saldo":749.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.251, "fecha_inicio":"2022-11-13", "tipo_deuda":"I", "ahorro_cuota_mensual":18.125819386470084, "ahorro_total":217.509832637641, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":30, "monto_otorgado":41500.0, "cuota":2453.0, "saldo":33737.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":36.0, "numero_pagos_restante":20.0, "frecuencia_externa":"M", "avance":0.1871, "fecha_inicio":"2022-12-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-159.1595404102054, "ahorro_total":-5729.743454767395, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":33, "monto_otorgado":1651.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-06-14", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":34, "monto_otorgado":2938.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-08-19", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":115, "monto_otorgado":1500.0, "cuota":204.0, "saldo":1340.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1067, "fecha_inicio":"2023-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":31.688729079705126, "ahorro_total":380.2647489564615, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":24, "monto_otorgado":400.0, "cuota":56.0, "saldo":362.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.095, "fecha_inicio":"2023-11-03", "tipo_deuda":"I", "ahorro_cuota_mensual":10.050327754588032, "ahorro_total":120.60393305505639, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":500.0, "cuota":80.0, "saldo":536.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":-0.072, "fecha_inicio":"2024-02-11", "tipo_deuda":"I", "ahorro_cuota_mensual":22.562909693235042, "ahorro_total":270.7549163188205, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":2500.0, "cuota":397.0, "saldo":392.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8432, "fecha_inicio":"2023-06-08", "tipo_deuda":"I", "ahorro_cuota_mensual":40.2370508029191, "ahorro_total":362.1334572262719, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":23, "monto_otorgado":405.0, "cuota":87.0, "saldo":308.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2395, "fecha_inicio":"2023-12-07", "tipo_deuda":"I", "ahorro_cuota_mensual":6.388142822585493, "ahorro_total":38.32885693551296, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":4000.0, "cuota":11525.0, "saldo":11525.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.8812, "fecha_inicio":"2024-03-05", "tipo_deuda":"I", "ahorro_cuota_mensual":7312.178666666667, "ahorro_total":7312.178666666667, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":653.0, "cuota":144.0, "saldo":507.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2236, "fecha_inicio":"2023-11-28", "tipo_deuda":"I", "ahorro_cuota_mensual":14.025820402835393, "ahorro_total":84.15492241701236, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":219.0, "cuota":31.0, "saldo":165.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2466, "fecha_inicio":"2023-09-13", "tipo_deuda":"I", "ahorro_cuota_mensual":5.842554445636949, "ahorro_total":70.11065334764339, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":300.0, "cuota":48.0, "saldo":310.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":-0.0333, "fecha_inicio":"2024-01-11", "tipo_deuda":"I", "ahorro_cuota_mensual":13.537745815941022, "ahorro_total":162.45294979129227, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":300.0, "cuota":47.0, "saldo":300.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-01-19", "tipo_deuda":"I", "ahorro_cuota_mensual":12.537745815941022, "ahorro_total":150.45294979129227, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":803.0, "cuota":131.0, "saldo":807.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":9.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":-0.005, "fecha_inicio":"2024-02-27", "tipo_deuda":"I", "ahorro_cuota_mensual":16.407740717897624, "ahorro_total":147.66966646107863, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":2272.0, "cuota":363.0, "saldo":2017.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1122, "fecha_inicio":"2023-12-05", "tipo_deuda":"I", "ahorro_cuota_mensual":38.77383176969289, "ahorro_total":348.964485927236, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":2271.0, "cuota":329.0, "saldo":2053.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.096, "fecha_inicio":"2023-11-08", "tipo_deuda":"I", "ahorro_cuota_mensual":68.12073582667352, "ahorro_total":817.4488299200823, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":749.0, "cuota":167.0, "saldo":165.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7797, "fecha_inicio":"2023-09-13", "tipo_deuda":"I", "ahorro_cuota_mensual":17.917824627448255, "ahorro_total":107.50694776468953, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":2000.0, "cuota":322.0, "saldo":2169.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":-0.0845, "fecha_inicio":"2024-02-08", "tipo_deuda":"I", "ahorro_cuota_mensual":92.25163877294017, "ahorro_total":1107.019665275282, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":4400.0, "cuota":719.0, "saldo":4640.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":-0.0545, "fecha_inicio":"2024-01-05", "tipo_deuda":"I", "ahorro_cuota_mensual":213.55360530046835, "ahorro_total":2562.64326360562, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":6000.0, "cuota":797.0, "saldo":3931.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3448, "fecha_inicio":"2023-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":107.7549163188205, "ahorro_total":1293.058995825846, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":400.0, "cuota":53.0, "saldo":315.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2125, "fecha_inicio":"2023-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":7.050327754588032, "ahorro_total":84.60393305505639, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":15, "monto_otorgado":800.0, "cuota":128.0, "saldo":782.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.0225, "fecha_inicio":"2023-12-13", "tipo_deuda":"I", "ahorro_cuota_mensual":36.100655509176065, "ahorro_total":433.2078661101128, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":150.0, "cuota":23.0, "saldo":135.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.1, "fecha_inicio":"2023-11-20", "tipo_deuda":"I", "ahorro_cuota_mensual":5.768872907970511, "ahorro_total":69.22647489564613, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":350.0, "cuota":53.0, "saldo":357.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":-0.02, "fecha_inicio":"2024-02-24", "tipo_deuda":"I", "ahorro_cuota_mensual":12.794036785264531, "ahorro_total":153.52844142317437, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":19, "monto_otorgado":1500.0, "cuota":209.0, "saldo":1129.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2473, "fecha_inicio":"2023-09-06", "tipo_deuda":"I", "ahorro_cuota_mensual":36.688729079705126, "ahorro_total":440.2647489564615, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":20, "monto_otorgado":1903.0, "cuota":231.0, "saldo":443.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7672, "fecha_inicio":"2023-04-05", "tipo_deuda":"I", "ahorro_cuota_mensual":12.394434292452559, "ahorro_total":148.7332115094307, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":2500.0, "cuota":347.0, "saldo":2229.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.1084, "fecha_inicio":"2023-11-08", "tipo_deuda":"I", "ahorro_cuota_mensual":59.81454846617521, "ahorro_total":717.7745815941025, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4714725, "monto_maximo_cliente": 193638.0, "cuota_externa_total": 12063.0, "capacidad_maxima_pago": 32537.0, "bursolnum": 7438657, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3215.995620247574, "monto_max": 193638.0, "cuota_min": 269.2747621622814, "monto_min": 5000, "plazo_max": 14.0, "plazo_min": 4, "tasa": 0.5292, "kubo_score": "C1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":25000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2024-02-11", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":25000.0, "cuota":1674.0, "saldo":17368.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":27.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.3053, "fecha_inicio":"2023-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-54.26137069856122, "ahorro_total":-1465.057008861153, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":8000.0, "cuota":198.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-09-25", "tipo_deuda":"R", "ahorro_cuota_mensual":198.0, "ahorro_total":-198.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":1200.0, "cuota":106.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-04-23", "tipo_deuda":"R", "ahorro_cuota_mensual":106.0, "ahorro_total":-106.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":86300.0, "cuota":5324.0, "saldo":66618.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.2281, "fecha_inicio":"2022-10-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-5915.072859642982, "ahorro_total":-59150.72859642982, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":30000.0, "cuota":1099.0, "saldo":3735.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8755, "fecha_inicio":"2020-10-02", "tipo_deuda":"R", "ahorro_cuota_mensual":4834.000000000002, "ahorro_total":-4834.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":51800.0, "cuota":662.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-05-28", "tipo_deuda":"R", "ahorro_cuota_mensual":662.0, "ahorro_total":-662.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":72003.0, "cuota":1260.0, "saldo":57421.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":120.0, "numero_pagos_restante":42.0, "frecuencia_externa":"S", "avance":0.2025, "fecha_inicio":"2022-10-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-2617.718139994149, "ahorro_total":-157063.08839964896, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":31600.0, "cuota":3805.0, "saldo":15426.0, "tasa_externa":0.7511, "tasa_kubo":0.5292, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5118, "fecha_inicio":"2022-05-07", "tipo_deuda":"I", "ahorro_cuota_mensual":216.4347266402201, "ahorro_total":2597.2167196826413, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4721997, "monto_maximo_cliente": 707489.0, "cuota_externa_total": 37068.0, "capacidad_maxima_pago": 545470.0, "bursolnum": 7438667, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 18782.26383703736, "monto_max": 707489.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0423, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":55000.0, "cuota":5052.0, "saldo":9580.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":17.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8258, "fecha_inicio":"2023-01-06", "tipo_deuda":"I", "ahorro_cuota_mensual":798.3028579834163, "ahorro_total":13571.148585718078, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":7500.0, "cuota":888.0, "saldo":4585.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3887, "fecha_inicio":"2023-08-02", "tipo_deuda":"I", "ahorro_cuota_mensual":124.34413642980121, "ahorro_total":1492.1296371576145, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":12000.0, "cuota":1133.0, "saldo":9726.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":17.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.1895, "fecha_inicio":"2023-09-20", "tipo_deuda":"I", "ahorro_cuota_mensual":204.92062356001804, "ahorro_total":3483.650600520307, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":30000.0, "cuota":2200.0, "saldo":28365.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":30.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.0545, "fecha_inicio":"2023-10-30", "tipo_deuda":"I", "ahorro_cuota_mensual":624.4188030116782, "ahorro_total":18732.564090350344, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":14, "monto_otorgado":492800.0, "cuota":19473.0, "saldo":308535.0, "tasa_externa":0.364, "tasa_kubo":0.3337, "numero_pagos_otorgado":48.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.3739, "fecha_inicio":"2022-01-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-851.3735649083137, "ahorro_total":-40865.93111559906, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":36964.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"1999-06-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":3100.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-01-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":3000.0, "cuota":219.0, "saldo":2070.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.31, "fecha_inicio":"2022-03-11", "tipo_deuda":"R", "ahorro_cuota_mensual":2288.9999999999945, "ahorro_total":-2288.9999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":118080.0, "cuota":5904.0, "saldo":117555.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0044, "fecha_inicio":"2001-11-15", "tipo_deuda":"R", "ahorro_cuota_mensual":123458.99999999971, "ahorro_total":-123458.99999999971, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":92000.0, "cuota":4600.0, "saldo":91992.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0001, "fecha_inicio":"2017-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":96591.99999999977, "ahorro_total":-96591.99999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":3100.0, "cuota":562.0, "saldo":3072.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.009, "fecha_inicio":"2023-05-19", "tipo_deuda":"R", "ahorro_cuota_mensual":-2609.0955519999925, "ahorro_total":-2609.0955519999925, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4733672, "monto_maximo_cliente": 265972.0, "cuota_externa_total": 15636.0, "capacidad_maxima_pago": 111927.0, "bursolnum": 7438676, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4571.230944555158, "monto_max": 265972.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0433, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":20, "monto_otorgado":651.0, "cuota":86.0, "saldo":684.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":-0.0507, "fecha_inicio":"2024-02-10", "tipo_deuda":"I", "ahorro_cuota_mensual":17.892815794507726, "ahorro_total":214.7137895340927, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":4200.0, "cuota":568.0, "saldo":4496.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":-0.0705, "fecha_inicio":"2024-02-03", "tipo_deuda":"I", "ahorro_cuota_mensual":128.59881157746918, "ahorro_total":1543.1857389296301, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":10.0, "cuota":10.0, "saldo":10.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-02-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-0.36859000000000464, "ahorro_total":-0.36859000000000464, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":19, "monto_otorgado":1000.0, "cuota":1049.0, "saldo":1032.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.032, "fecha_inicio":"2024-02-17", "tipo_deuda":"I", "ahorro_cuota_mensual":12.140999999999394, "ahorro_total":12.140999999999394, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":21, "monto_otorgado":10.0, "cuota":10.0, "saldo":10.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-02-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-0.36859000000000464, "ahorro_total":-0.36859000000000464, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":1300.0, "cuota":281.0, "saldo":985.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2423, "fecha_inicio":"2023-12-10", "tipo_deuda":"I", "ahorro_cuota_mensual":35.539498899172145, "ahorro_total":213.23699339503287, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":23, "monto_otorgado":10.0, "cuota":11.0, "saldo":10.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-02-06", "tipo_deuda":"I", "ahorro_cuota_mensual":0.6314099999999954, "ahorro_total":0.6314099999999954, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":24, "monto_otorgado":2543.0, "cuota":398.0, "saldo":2411.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0519, "fecha_inicio":"2024-01-19", "tipo_deuda":"I", "ahorro_cuota_mensual":60.86222004609618, "ahorro_total":547.7599804148656, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":900.0, "cuota":200.0, "saldo":978.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0867, "fecha_inicio":"2024-01-28", "tipo_deuda":"I", "ahorro_cuota_mensual":30.065806930196118, "ahorro_total":180.3948415811767, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":26, "monto_otorgado":35800.0, "cuota":2113.0, "saldo":29440.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":36.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.1777, "fecha_inicio":"2023-01-18", "tipo_deuda":"I", "ahorro_cuota_mensual":301.17321678134317, "ahorro_total":10842.235804128355, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":27, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2015-05-01", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":10.0, "cuota":10.0, "saldo":10.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-02-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-0.36859000000000464, "ahorro_total":-0.36859000000000464, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":15, "monto_otorgado":1200.0, "cuota":446.0, "saldo":439.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6342, "fecha_inicio":"2023-12-25", "tipo_deuda":"I", "ahorro_cuota_mensual":16.157105249563358, "ahorro_total":48.471315748690074, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":7000.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2017-08-19", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-3.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":252.0, "cuota":84.0, "saldo":231.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.0833, "fecha_inicio":"2024-02-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-6.267007897591682, "ahorro_total":-18.801023692775047, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":14, "monto_otorgado":360.0, "cuota":80.0, "saldo":360.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.0, "fecha_inicio":"2024-03-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-18.44331079988143, "ahorro_total":-73.77324319952572, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":81620.0, "cuota":2120.0, "saldo":71920.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":154.0, "numero_pagos_restante":33.0, "frecuencia_externa":"W", "avance":0.1188, "fecha_inicio":"2023-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":-1905.8792424638523, "ahorro_total":-72423.41121362639, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":53600.0, "cuota":2144.0, "saldo":51992.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":100.0, "numero_pagos_restante":24.0, "frecuencia_externa":"W", "avance":0.03, "fecha_inicio":"2024-03-05", "tipo_deuda":"I", "ahorro_cuota_mensual":-1174.0810483728333, "ahorro_total":-29352.026209320833, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":108000.0, "cuota":5274.0, "saldo":101040.0, "tasa_externa":0.512, "tasa_kubo":0.3813, "numero_pagos_otorgado":48.0, "numero_pagos_restante":40.0, "frecuencia_externa":"M", "avance":0.0644, "fecha_inicio":"2023-08-21", "tipo_deuda":"I", "ahorro_cuota_mensual":443.1046456592585, "ahorro_total":21269.022991644408, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":22600.0, "cuota":1057.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-01-20", "tipo_deuda":"R", "ahorro_cuota_mensual":1057.0, "ahorro_total":-1057.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":6144.0, "cuota":192.0, "saldo":5712.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":128.0, "numero_pagos_restante":29.0, "frecuencia_externa":"W", "avance":0.0703, "fecha_inicio":"2024-01-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-138.1329728550038, "ahorro_total":-4420.255131360122, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":832.0, "cuota":104.0, "saldo":676.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":32.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.1875, "fecha_inicio":"2024-01-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-17.9774241787279, "ahorro_total":-143.8193934298232, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":378.0, "cuota":84.0, "saldo":294.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.2222, "fecha_inicio":"2024-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-19.365476339875485, "ahorro_total":-77.46190535950194, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":252.0, "cuota":84.0, "saldo":168.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.3333, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-6.267007897591682, "ahorro_total":-18.801023692775047, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":11, "monto_otorgado":936.0, "cuota":104.0, "saldo":832.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.1111, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-20.090036192235146, "ahorro_total":-180.81032573011632, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":360.0, "cuota":80.0, "saldo":300.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.1667, "fecha_inicio":"2024-02-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-18.44331079988143, "ahorro_total":-73.77324319952572, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":1404.0, "cuota":104.0, "saldo":1274.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":54.0, "numero_pagos_restante":11.0, "frecuencia_externa":"W", "avance":0.0926, "fecha_inicio":"2024-01-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-26.173834506572348, "ahorro_total":-366.43368309201287, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4754385, "monto_maximo_cliente": 284480.0, "cuota_externa_total": 42641.0, "capacidad_maxima_pago": 75453.0, "bursolnum": 7438701, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5293.744643303981, "monto_max": 284480.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.6722, "kubo_score": "D4", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":1397.0, "cuota":533.0, "saldo":1441.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0315, "fecha_inicio":"2024-02-17", "tipo_deuda":"I", "ahorro_cuota_mensual":15.398065054909807, "ahorro_total":46.19419516472942, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVS. GRALES.", "registro":20, "monto_otorgado":30000.0, "cuota":2442.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-10-02", "tipo_deuda":"R", "ahorro_cuota_mensual":2442.0, "ahorro_total":-2442.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":19, "monto_otorgado":195499.0, "cuota":5940.0, "saldo":104445.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":48.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.4658, "fecha_inicio":"2021-10-17", "tipo_deuda":"I", "ahorro_cuota_mensual":-5668.527423363692, "ahorro_total":-272089.3163214572, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":17, "monto_otorgado":72000.0, "cuota":5143.0, "saldo":68476.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.0489, "fecha_inicio":"2023-07-21", "tipo_deuda":"I", "ahorro_cuota_mensual":520.6179927202402, "ahorro_total":18742.247737928647, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":30000.0, "cuota":2848.0, "saldo":27052.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":18.0, "numero_pagos_restante":12.0, "frecuencia_externa":"M", "avance":0.0983, "fecha_inicio":"2023-10-05", "tipo_deuda":"I", "ahorro_cuota_mensual":184.6780423439127, "ahorro_total":3324.2047621904285, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":42100.0, "cuota":3084.0, "saldo":41842.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":36.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":0.0061, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":381.1905207433624, "ahorro_total":13722.858746761047, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":91724.0, "cuota":4632.0, "saldo":56306.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":24.0, "numero_pagos_restante":13.0, "frecuencia_externa":"M", "avance":0.3861, "fecha_inicio":"2023-05-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-2328.4723794211413, "ahorro_total":-55883.33710610739, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":20000.0, "cuota":4153.0, "saldo":18900.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.055, "fecha_inicio":"2023-02-07", "tipo_deuda":"R", "ahorro_cuota_mensual":23053.000000000004, "ahorro_total":-23053.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":13000.0, "cuota":11671.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-04-05", "tipo_deuda":"R", "ahorro_cuota_mensual":11671.0, "ahorro_total":-11671.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":80000.0, "cuota":5896.0, "saldo":77621.0, "tasa_externa":0.559, "tasa_kubo":0.5668, "numero_pagos_otorgado":43.0, "numero_pagos_restante":13.0, "frecuencia_externa":"S", "avance":0.0297, "fecha_inicio":"2023-07-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-449.85407781089634, "ahorro_total":-9896.78971183972, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":99500.0, "cuota":3817.0, "saldo":28680.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7118, "fecha_inicio":"2019-03-20", "tipo_deuda":"R", "ahorro_cuota_mensual":32497.000000000007, "ahorro_total":-32497.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":25000.0, "cuota":995.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-06-26", "tipo_deuda":"R", "ahorro_cuota_mensual":995.0, "ahorro_total":-995.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":15000.0, "cuota":3695.0, "saldo":12487.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1675, "fecha_inicio":"2024-01-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-931.5535874440529, "ahorro_total":-2794.660762332159, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":5, "monto_otorgado":10992.0, "cuota":550.0, "saldo":2112.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8079, "fecha_inicio":"2024-01-03", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":4, "monto_otorgado":10935.0, "cuota":547.0, "saldo":808.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9261, "fecha_inicio":"2023-12-05", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":3, "monto_otorgado":10918.0, "cuota":186.0, "saldo":372.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9659, "fecha_inicio":"2023-11-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":35000.0, "cuota":3316.0, "saldo":31118.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1109, "fecha_inicio":"2017-11-05", "tipo_deuda":"R", "ahorro_cuota_mensual":34434.00000000001, "ahorro_total":-34434.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":10, "monto_otorgado":66256.0, "cuota":2283.0, "saldo":16882.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7452, "fecha_inicio":"2022-05-17", "tipo_deuda":"O", "ahorro_cuota_mensual":19165.000000000004, "ahorro_total":-19165.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4759224, "monto_maximo_cliente": 362108.0, "cuota_externa_total": 46240.0, "capacidad_maxima_pago": 133998.0, "bursolnum": 7438706, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5293.744643303981, "monto_max": 362108.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.8317, "kubo_score": "E3", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":20, "monto_otorgado":12000.0, "cuota":1820.0, "saldo":13420.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.1183, "fecha_inicio":"2022-07-22", "tipo_deuda":"R", "ahorro_cuota_mensual":15240.000000000004, "ahorro_total":-15240.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":21, "monto_otorgado":37000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-03-31", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":14000.0, "cuota":1150.0, "saldo":13894.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0076, "fecha_inicio":"2024-02-22", "tipo_deuda":"R", "ahorro_cuota_mensual":15044.000000000004, "ahorro_total":-15044.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":103, "monto_otorgado":1000.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2009-06-09", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":227499.0, "cuota":12292.0, "saldo":70331.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":4.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6909, "fecha_inicio":"2022-09-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-52580.87840508674, "ahorro_total":-210323.51362034696, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":17, "monto_otorgado":40000.0, "cuota":5349.0, "saldo":33182.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.1704, "fecha_inicio":"2023-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":713.231542342347, "ahorro_total":8558.778508108164, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":19, "monto_otorgado":116448.0, "cuota":4175.0, "saldo":62666.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":36.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.4619, "fecha_inicio":"2022-09-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-3300.9324997737986, "ahorro_total":-118833.56999185676, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "GOBIERNO", "registro":24, "monto_otorgado":1.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2011-08-15", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":4000.0, "cuota":200.0, "saldo":2090.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4775, "fecha_inicio":"2023-08-29", "tipo_deuda":"R", "ahorro_cuota_mensual":2290.0000000000005, "ahorro_total":-2290.0000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":12500.0, "cuota":2354.0, "saldo":12367.0, "tasa_externa":2.2908, "tasa_kubo":0.5668, "numero_pagos_otorgado":96.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0106, "fecha_inicio":"2010-08-18", "tipo_deuda":"I", "ahorro_cuota_mensual":1611.762992178752, "ahorro_total":77364.6236245801, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":200.0, "cuota":400.0, "saldo":200.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0, "fecha_inicio":"2024-02-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":500.0, "cuota":49.0, "saldo":492.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.016, "fecha_inicio":"2023-11-28", "tipo_deuda":"R", "ahorro_cuota_mensual":541.0000000000001, "ahorro_total":-541.0000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":700.0, "cuota":49.0, "saldo":492.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":2.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2971, "fecha_inicio":"2023-11-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-217.3974570838647, "ahorro_total":-434.7949141677294, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":54500.0, "cuota":3970.0, "saldo":54025.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0087, "fecha_inicio":"2018-04-04", "tipo_deuda":"R", "ahorro_cuota_mensual":57995.000000000015, "ahorro_total":-57995.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":49000.0, "cuota":2450.0, "saldo":36538.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2543, "fecha_inicio":"2024-01-31", "tipo_deuda":"R", "ahorro_cuota_mensual":38988.00000000001, "ahorro_total":-38988.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":14, "monto_otorgado":2500.0, "cuota":1964.0, "saldo":982.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.6072, "fecha_inicio":"2024-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":610.3543847364599, "ahorro_total":1220.7087694729198, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":80000.0, "cuota":5896.0, "saldo":77621.0, "tasa_externa":0.559, "tasa_kubo":0.5668, "numero_pagos_otorgado":43.0, "numero_pagos_restante":13.0, "frecuencia_externa":"S", "avance":0.0297, "fecha_inicio":"2023-07-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-449.85407781089634, "ahorro_total":-9896.78971183972, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":20000.0, "cuota":3769.0, "saldo":12371.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3814, "fecha_inicio":"2022-03-30", "tipo_deuda":"R", "ahorro_cuota_mensual":16140.000000000004, "ahorro_total":-16140.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":3014.0, "cuota":6028.0, "saldo":3014.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0, "fecha_inicio":"2024-02-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":27200.0, "cuota":1851.0, "saldo":26624.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0212, "fecha_inicio":"2022-12-05", "tipo_deuda":"R", "ahorro_cuota_mensual":28475.000000000007, "ahorro_total":-28475.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4993943, "monto_maximo_cliente": 89634.0, "cuota_externa_total": 36790.0, "capacidad_maxima_pago": 48210.0, "bursolnum": 7440021, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3896.61946138083, "monto_max": 89634.0, "cuota_min": 278.44180193239873, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":80000.0, "cuota":7498.0, "saldo":67730.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":50.0, "numero_pagos_restante":13.0, "frecuencia_externa":"S", "avance":0.1534, "fecha_inicio":"2023-04-28", "tipo_deuda":"I", "ahorro_cuota_mensual":1638.088708674848, "ahorro_total":40952.2177168712, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":24200.0, "cuota":24868.0, "saldo":24868.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0276, "fecha_inicio":"2024-03-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-619.5690666666669, "ahorro_total":-619.5690666666669, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":60000.0, "cuota":4424.0, "saldo":57672.0, "tasa_externa":0.5596, "tasa_kubo":0.5504, "numero_pagos_otorgado":43.0, "numero_pagos_restante":11.0, "frecuencia_externa":"S", "avance":0.0388, "fecha_inicio":"2023-06-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-268.3670633251395, "ahorro_total":-5904.075393153069, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":7911.0, "cuota":176.0, "saldo":5434.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3131, "fecha_inicio":"2019-03-05", "tipo_deuda":"R", "ahorro_cuota_mensual":5609.999999999995, "ahorro_total":-5609.999999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 4995215, "monto_maximo_cliente": 190093.0, "cuota_externa_total": 15631.0, "capacidad_maxima_pago": 79369.0, "bursolnum": 7440023, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4105.224591686707, "monto_max": 190093.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0433, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":20000.0, "cuota":1828.0, "saldo":13039.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":18.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.348, "fecha_inicio":"2023-05-05", "tipo_deuda":"I", "ahorro_cuota_mensual":288.20113194663145, "ahorro_total":5187.620375039366, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":11, "monto_otorgado":1600.0, "cuota":105.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-10-02", "tipo_deuda":"R", "ahorro_cuota_mensual":105.0, "ahorro_total":-105.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":25000.0, "cuota":5305.0, "saldo":18168.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2733, "fecha_inicio":"2021-03-08", "tipo_deuda":"R", "ahorro_cuota_mensual":23473.00000000004, "ahorro_total":-23473.00000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":19500.0, "cuota":1275.0, "saldo":18152.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0691, "fecha_inicio":"2022-01-28", "tipo_deuda":"R", "ahorro_cuota_mensual":19427.000000000036, "ahorro_total":-19427.000000000036, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":29000.0, "cuota":1450.0, "saldo":25936.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1057, "fecha_inicio":"2022-04-20", "tipo_deuda":"R", "ahorro_cuota_mensual":27386.00000000006, "ahorro_total":-27386.00000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":32500.0, "cuota":1500.0, "saldo":23114.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2888, "fecha_inicio":"2022-04-03", "tipo_deuda":"R", "ahorro_cuota_mensual":24614.000000000047, "ahorro_total":-24614.000000000047, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":1049.0, "cuota":400.0, "saldo":753.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2822, "fecha_inicio":"2024-01-08", "tipo_deuda":"I", "ahorro_cuota_mensual":24.245669505660032, "ahorro_total":72.7370085169801, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":1184.0, "cuota":428.0, "saldo":416.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6486, "fecha_inicio":"2024-01-04", "tipo_deuda":"I", "ahorro_cuota_mensual":3.888343846235898, "ahorro_total":11.665031538707694, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":30200.0, "cuota":1510.0, "saldo":18391.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.391, "fecha_inicio":"2021-04-13", "tipo_deuda":"R", "ahorro_cuota_mensual":19901.00000000004, "ahorro_total":-19901.00000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":80000.0, "cuota":4737.0, "saldo":55330.0, "tasa_externa":0.3682, "tasa_kubo":0.3813, "numero_pagos_otorgado":24.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.3084, "fecha_inicio":"2023-06-23", "tipo_deuda":"I", "ahorro_cuota_mensual":-342.5803899785569, "ahorro_total":-8221.929359485366, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":8000.0, "cuota":1413.0, "saldo":4099.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4876, "fecha_inicio":"2023-01-06", "tipo_deuda":"R", "ahorro_cuota_mensual":5512.000000000009, "ahorro_total":-5512.000000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5008298, "monto_maximo_cliente": 91453.0, "cuota_externa_total": 22063.0, "capacidad_maxima_pago": 77284.0, "bursolnum": 7440049, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5293.744643303981, "monto_max": 91453.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":47500.0, "cuota":7054.0, "saldo":17477.0, "tasa_externa":1.6323, "tasa_kubo":0.5668, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.6321, "fecha_inicio":"2022-09-27", "tipo_deuda":"I", "ahorro_cuota_mensual":2837.073567044529, "ahorro_total":51067.324206801524, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":15000.0, "cuota":1973.0, "saldo":5418.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6388, "fecha_inicio":"2023-05-03", "tipo_deuda":"I", "ahorro_cuota_mensual":234.58682837838, "ahorro_total":2815.04194054056, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":8000.0, "cuota":6846.0, "saldo":6846.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1442, "fecha_inicio":"2022-03-24", "tipo_deuda":"R", "ahorro_cuota_mensual":13692.000000000002, "ahorro_total":-13692.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":80000.0, "cuota":5900.0, "saldo":153574.0, "tasa_externa":0.56, "tasa_kubo":0.5668, "numero_pagos_otorgado":43.0, "numero_pagos_restante":11.0, "frecuencia_externa":"S", "avance":-0.9197, "fecha_inicio":"2023-05-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-445.85407781089634, "ahorro_total":-9808.78971183972, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":7500.0, "cuota":375.0, "saldo":4607.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3857, "fecha_inicio":"2023-02-27", "tipo_deuda":"R", "ahorro_cuota_mensual":4982.000000000001, "ahorro_total":-4982.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5013364, "monto_maximo_cliente": 110010.0, "cuota_externa_total": 11831.0, "capacidad_maxima_pago": 19169.0, "bursolnum": 7440062, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 791.7037356954075, "monto_max": 110010.0, "cuota_min": 141.5274874508095, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.821, "kubo_score": "E2", "comision": 0.0384, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2], "comisiones": [0.03845], "kubo_scores": ['K1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":24, "monto_otorgado":30000.0, "cuota":2514.0, "saldo":13713.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":36.0, "numero_pagos_restante":25.0, "frecuencia_externa":"M", "avance":0.5429, "fecha_inicio":"2023-05-05", "tipo_deuda":"I", "ahorro_cuota_mensual":1349.5788181032478, "ahorro_total":48584.83745171692, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":23, "monto_otorgado":16000.0, "cuota":1958.0, "saldo":16237.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0148, "fecha_inicio":"2023-12-08", "tipo_deuda":"R", "ahorro_cuota_mensual":18194.99999999997, "ahorro_total":-18194.99999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":2000.0, "cuota":100.0, "saldo":913.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5435, "fecha_inicio":"2024-02-02", "tipo_deuda":"R", "ahorro_cuota_mensual":1012.9999999999983, "ahorro_total":-1012.9999999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":21, "monto_otorgado":17000.0, "cuota":1008.0, "saldo":20626.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.2133, "fecha_inicio":"2020-05-27", "tipo_deuda":"R", "ahorro_cuota_mensual":21633.99999999996, "ahorro_total":-21633.99999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":20, "monto_otorgado":20000.0, "cuota":1275.0, "saldo":3618.0, "tasa_externa":0.4531, "tasa_kubo":0.2, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8191, "fecha_inicio":"2022-05-16", "tipo_deuda":"I", "ahorro_cuota_mensual":225.54693316956286, "ahorro_total":5413.126396069509, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":19, "monto_otorgado":35000.0, "cuota":1851.0, "saldo":22160.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3669, "fecha_inicio":"2018-11-17", "tipo_deuda":"R", "ahorro_cuota_mensual":24010.999999999956, "ahorro_total":-24010.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":12180.0, "cuota":47.0, "saldo":452.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9629, "fecha_inicio":"2024-03-15", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":16, "monto_otorgado":12085.0, "cuota":604.0, "saldo":2411.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8005, "fecha_inicio":"2024-03-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":18, "monto_otorgado":12166.0, "cuota":32.0, "saldo":302.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9752, "fecha_inicio":"2024-03-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":14, "monto_otorgado":12164.0, "cuota":608.0, "saldo":666.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9452, "fecha_inicio":"2024-02-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":13, "monto_otorgado":12164.0, "cuota":608.0, "saldo":1746.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8565, "fecha_inicio":"2024-02-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":12180.0, "cuota":1344.0, "saldo":10752.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1172, "fecha_inicio":"2024-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":12197.0, "cuota":610.0, "saldo":1032.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9154, "fecha_inicio":"2023-12-01", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":12187.0, "cuota":126.0, "saldo":336.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9724, "fecha_inicio":"2023-11-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":11960.0, "cuota":60.0, "saldo":60.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.995, "fecha_inicio":"2023-11-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":12152.0, "cuota":-1.0, "saldo":60.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9951, "fecha_inicio":"2023-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":12000.0, "cuota":2540.0, "saldo":11987.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":10.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.0011, "fecha_inicio":"2024-01-11", "tipo_deuda":"R", "ahorro_cuota_mensual":1210.1793777297753, "ahorro_total":12101.793777297753, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":15, "monto_otorgado":12140.0, "cuota":30.0, "saldo":270.0, "tasa_externa":-1.0, "tasa_kubo":0.2, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9778, "fecha_inicio":"2024-03-02", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5064760, "monto_maximo_cliente": 610082.0, "cuota_externa_total": 47336.0, "capacidad_maxima_pago": 304356.0, "bursolnum": 7440144, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 37105.98229655993, "monto_max": 610082.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 12.0, "plazo_min": 4, "tasa": 0.6509, "kubo_score": "D3", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":11, "monto_otorgado":1540.0, "cuota":40.0, "saldo":1020.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":25.0, "frecuencia_externa":"W", "avance":0.3377, "fecha_inicio":"2023-03-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-67.47201758629838, "ahorro_total":-2563.9366682793384, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":25000.0, "cuota":2023.0, "saldo":19490.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":24.0, "numero_pagos_restante":13.0, "frecuencia_externa":"M", "avance":0.2204, "fecha_inicio":"2023-05-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-23.049553950689415, "ahorro_total":-553.189294816546, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":17, "monto_otorgado":80000.0, "cuota":18000.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-12-13", "tipo_deuda":"R", "ahorro_cuota_mensual":18000.0, "ahorro_total":-18000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":66100.0, "cuota":26468.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-03-14", "tipo_deuda":"R", "ahorro_cuota_mensual":26468.0, "ahorro_total":-26468.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":24000.0, "cuota":1825.0, "saldo":23055.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0394, "fecha_inicio":"2023-11-23", "tipo_deuda":"R", "ahorro_cuota_mensual":24880.00000000003, "ahorro_total":-24880.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":18, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":954.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-06-26", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":24332.0, "cuota":632.0, "saldo":16116.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":25.0, "frecuencia_externa":"W", "avance":0.3377, "fecha_inicio":"2023-03-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-1066.0578778635142, "ahorro_total":-40510.199358813545, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":100000.0, "cuota":5000.0, "saldo":80058.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1994, "fecha_inicio":"2024-01-30", "tipo_deuda":"R", "ahorro_cuota_mensual":85058.00000000009, "ahorro_total":-85058.00000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":21098.0, "cuota":548.0, "saldo":18632.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":33.0, "frecuencia_externa":"W", "avance":0.1169, "fecha_inicio":"2023-11-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-924.3666409322877, "ahorro_total":-35125.932355426936, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":88000.0, "cuota":12000.0, "saldo":81501.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0739, "fecha_inicio":"2017-02-20", "tipo_deuda":"R", "ahorro_cuota_mensual":93501.0000000001, "ahorro_total":-93501.0000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":306170.0, "cuota":38084.0, "saldo":187021.0, "tasa_externa":0.8241, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3892, "fecha_inicio":"2023-09-19", "tipo_deuda":"I", "ahorro_cuota_mensual":978.0177034400695, "ahorro_total":11736.212441280833, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":56056.0, "cuota":1456.0, "saldo":39312.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":26.0, "frecuencia_externa":"W", "avance":0.2987, "fecha_inicio":"2023-05-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-2455.981440141261, "ahorro_total":-93327.29472536792, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":3080.0, "cuota":80.0, "saldo":2720.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":33.0, "frecuencia_externa":"W", "avance":0.1169, "fecha_inicio":"2023-11-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-134.94403517259676, "ahorro_total":-5127.873336558677, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":8192.0, "cuota":256.0, "saldo":6464.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":128.0, "numero_pagos_restante":25.0, "frecuencia_externa":"W", "avance":0.2109, "fecha_inicio":"2023-09-11", "tipo_deuda":"I", "ahorro_cuota_mensual":-344.6786330014219, "ahorro_total":-11029.7162560455, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":3080.0, "cuota":80.0, "saldo":2160.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":26.0, "frecuencia_externa":"W", "avance":0.2987, "fecha_inicio":"2023-05-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-134.94403517259676, "ahorro_total":-5127.873336558677, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":1920.0, "cuota":60.0, "saldo":1515.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":128.0, "numero_pagos_restante":25.0, "frecuencia_externa":"W", "avance":0.2109, "fecha_inicio":"2023-09-11", "tipo_deuda":"I", "ahorro_cuota_mensual":-80.78405460970825, "ahorro_total":-2585.089747510664, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5153135, "monto_maximo_cliente": 415807.0, "cuota_externa_total": 28202.0, "capacidad_maxima_pago": 73562.0, "bursolnum": 7440287, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2613.4866898297028, "monto_max": 415807.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5668, "kubo_score": "C5", "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":1921.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-06-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":13, "monto_otorgado":1921.0, "cuota":548.0, "saldo":548.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7147, "fecha_inicio":"2019-11-23", "tipo_deuda":"O", "ahorro_cuota_mensual":1095.9999999999986, "ahorro_total":-1095.9999999999986, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":41900.0, "cuota":3075.0, "saldo":33912.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":25.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1906, "fecha_inicio":"2023-06-28", "tipo_deuda":"I", "ahorro_cuota_mensual":717.6071618955334, "ahorro_total":17940.179047388334, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":203600.0, "cuota":6059.0, "saldo":79519.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.6094, "fecha_inicio":"2021-06-14", "tipo_deuda":"I", "ahorro_cuota_mensual":-1728.853783698978, "ahorro_total":-82984.98161755095, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":1506.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-07-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":1921.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-07-02", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":14, "monto_otorgado":1200.0, "cuota":299.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-07-09", "tipo_deuda":"R", "ahorro_cuota_mensual":299.0, "ahorro_total":-299.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":35000.0, "cuota":8663.0, "saldo":6861.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.804, "fecha_inicio":"2023-11-27", "tipo_deuda":"R", "ahorro_cuota_mensual":15523.999999999982, "ahorro_total":-15523.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":2000.0, "cuota":100.0, "saldo":319.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8405, "fecha_inicio":"2024-01-12", "tipo_deuda":"R", "ahorro_cuota_mensual":418.99999999999915, "ahorro_total":-418.99999999999915, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":12179.0, "cuota":1141.0, "saldo":3248.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7333, "fecha_inicio":"2023-06-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-69.19051618456706, "ahorro_total":-830.2861942148047, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":74764.0, "cuota":3143.0, "saldo":50368.0, "tasa_externa":0.4054, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.3263, "fecha_inicio":"2022-04-29", "tipo_deuda":"I", "ahorro_cuota_mensual":283.220529054664, "ahorro_total":13594.585394623871, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":214000.0, "cuota":6000.0, "saldo":184947.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1358, "fecha_inicio":"2017-10-09", "tipo_deuda":"R", "ahorro_cuota_mensual":190946.9999999995, "ahorro_total":-190946.9999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":7500.0, "cuota":400.0, "saldo":400.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":15.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.9467, "fecha_inicio":"2023-10-07", "tipo_deuda":"R", "ahorro_cuota_mensual":366.9356323232766, "ahorro_total":5504.034484849149, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":150432.0, "cuota":7522.0, "saldo":136337.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0937, "fecha_inicio":"2021-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":143858.99999999962, "ahorro_total":-143858.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5156228, "monto_maximo_cliente": 2640384.0, "cuota_externa_total": 47862.0, "capacidad_maxima_pago": 261667.0, "bursolnum": 7440291, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7203.655497228462, "monto_max": 2640384.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0433, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "OTRAS FINANCIERA", "registro":11, "monto_otorgado":950000.0, "cuota":0.0, "saldo":950000.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":950000.0000000021, "ahorro_total":-950000.0000000021, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":1000.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-11-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":811.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-01-08", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":80000.0, "cuota":10511.0, "saldo":34979.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5628, "fecha_inicio":"2023-06-30", "tipo_deuda":"I", "ahorro_cuota_mensual":2141.453553856556, "ahorro_total":25697.442646278672, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":811.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-05-21", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":26000.0, "cuota":1390.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-12-05", "tipo_deuda":"R", "ahorro_cuota_mensual":1390.0, "ahorro_total":-1390.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":159778.0, "cuota":7851.0, "saldo":123366.0, "tasa_externa":0.4233, "tasa_kubo":0.3813, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.2279, "fecha_inicio":"2022-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-235.3145186902393, "ahorro_total":-8471.322672848615, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "OTRAS FINANCIERA", "registro":10, "monto_otorgado":1200000.0, "cuota":0.0, "saldo":1032568.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.1395, "fecha_inicio":"2023-07-31", "tipo_deuda":"I", "ahorro_cuota_mensual":1200000.0000000026, "ahorro_total":-1200000.0000000026, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":48000.0, "cuota":2400.0, "saldo":26801.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4416, "fecha_inicio":"2021-05-21", "tipo_deuda":"R", "ahorro_cuota_mensual":29201.00000000006, "ahorro_total":-29201.00000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":108300.0, "cuota":15693.0, "saldo":61312.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4339, "fecha_inicio":"2023-07-04", "tipo_deuda":"I", "ahorro_cuota_mensual":4362.726498533313, "ahorro_total":52352.71798239976, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":243000.0, "cuota":12150.0, "saldo":195505.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1955, "fecha_inicio":"2023-03-02", "tipo_deuda":"R", "ahorro_cuota_mensual":207655.00000000044, "ahorro_total":-207655.00000000044, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5217560, "monto_maximo_cliente": 65518.0, "cuota_externa_total": 8567.0, "capacidad_maxima_pago": 36823.0, "bursolnum": 7440352, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1419.900523217919, "monto_max": 65518.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.5668, "kubo_score": "C5", "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":7161.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2001-06-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVS. GRALES.", "registro":9, "monto_otorgado":67500.0, "cuota":1457.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-05-18", "tipo_deuda":"R", "ahorro_cuota_mensual":1457.0, "ahorro_total":-1457.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":21100.0, "cuota":1582.0, "saldo":17622.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1648, "fecha_inicio":"2023-07-21", "tipo_deuda":"I", "ahorro_cuota_mensual":360.54916321974974, "ahorro_total":8653.179917273994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-06-15", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":11830.0, "cuota":592.0, "saldo":2528.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7863, "fecha_inicio":"2001-05-29", "tipo_deuda":"R", "ahorro_cuota_mensual":3119.999999999993, "ahorro_total":-3119.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":40000.0, "cuota":2000.0, "saldo":22686.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4328, "fecha_inicio":"2006-02-02", "tipo_deuda":"R", "ahorro_cuota_mensual":24685.999999999938, "ahorro_total":-24685.999999999938, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":18000.0, "cuota":2151.0, "saldo":1415.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9214, "fecha_inicio":"2015-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":3565.9999999999964, "ahorro_total":-3565.9999999999964, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":74360.0, "cuota":3718.0, "saldo":4416.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9406, "fecha_inicio":"2005-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":8133.999999999988, "ahorro_total":-8133.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":31342.0, "cuota":1976.0, "saldo":17724.0, "tasa_externa":0.4402, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.4345, "fecha_inicio":"2023-01-23", "tipo_deuda":"I", "ahorro_cuota_mensual":161.6534537267014, "ahorro_total":3879.6828894408336, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":7986.0, "cuota":400.0, "saldo":3131.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6079, "fecha_inicio":"2015-10-29", "tipo_deuda":"R", "ahorro_cuota_mensual":3530.9999999999914, "ahorro_total":-3530.9999999999914, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":5000.0, "cuota":697.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-08-26", "tipo_deuda":"R", "ahorro_cuota_mensual":697.0, "ahorro_total":-697.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5222923, "monto_maximo_cliente": 102873.0, "cuota_externa_total": 22029.0, "capacidad_maxima_pago": 45755.0, "bursolnum": 7440359, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4870.031302228124, "monto_max": 102873.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 18.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":3217.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-07-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":702.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-11-09", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":18000.0, "cuota":2144.0, "saldo":8281.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.5399, "fecha_inicio":"2023-07-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.4056439152259372, "ahorro_total":-16.867726982711247, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":12, "monto_otorgado":10000.0, "cuota":972.0, "saldo":12966.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.2966, "fecha_inicio":"2013-06-30", "tipo_deuda":"R", "ahorro_cuota_mensual":13938.000000000002, "ahorro_total":-13938.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":1795.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-01-21", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":10, "monto_otorgado":91591.0, "cuota":4915.0, "saldo":8774.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.9042, "fecha_inicio":"2022-02-18", "tipo_deuda":"O", "ahorro_cuota_mensual":13689.000000000002, "ahorro_total":-13689.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":1000.0, "cuota":100.0, "saldo":1068.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.068, "fecha_inicio":"2023-08-31", "tipo_deuda":"R", "ahorro_cuota_mensual":1168.0000000000002, "ahorro_total":-1168.0000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":7000.0, "cuota":1186.0, "saldo":5889.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1587, "fecha_inicio":"2023-11-27", "tipo_deuda":"R", "ahorro_cuota_mensual":7075.000000000001, "ahorro_total":-7075.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":52784.0, "cuota":5390.0, "saldo":15286.0, "tasa_externa":0.5251, "tasa_kubo":0.6193, "numero_pagos_otorgado":13.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7104, "fecha_inicio":"2023-05-19", "tipo_deuda":"I", "ahorro_cuota_mensual":-567.8082863384379, "ahorro_total":-7381.507722399693, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":9000.0, "cuota":450.0, "saldo":7018.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2202, "fecha_inicio":"2020-03-10", "tipo_deuda":"R", "ahorro_cuota_mensual":7468.000000000002, "ahorro_total":-7468.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":2000.0, "cuota":182.0, "saldo":1699.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":10.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1505, "fecha_inicio":"2023-05-04", "tipo_deuda":"R", "ahorro_cuota_mensual":-48.692768587167365, "ahorro_total":-486.92768587167365, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":33000.0, "cuota":6824.0, "saldo":12675.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6159, "fecha_inicio":"2022-07-29", "tipo_deuda":"R", "ahorro_cuota_mensual":19499.000000000004, "ahorro_total":-19499.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5245488, "monto_maximo_cliente": 58463.0, "cuota_externa_total": 9931.0, "capacidad_maxima_pago": 46069.0, "bursolnum": 7440384, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1734.2526365022495, "monto_max": 58463.0, "cuota_min": 299.79381766541826, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.5991, "kubo_score": "D1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "HIPOTECAGOBIERNO", "registro":10, "monto_otorgado":103181.0, "cuota":2716.0, "saldo":57910.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":360.0, "numero_pagos_restante":345.0, "frecuencia_externa":"M", "avance":0.4388, "fecha_inicio":"2023-01-06", "tipo_deuda":"M", "ahorro_cuota_mensual":-637.7418352911027, "ahorro_total":-229587.06070479698, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVS. GRALES.", "registro":9, "monto_otorgado":72000.0, "cuota":1111.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2015-12-02", "tipo_deuda":"R", "ahorro_cuota_mensual":1111.0, "ahorro_total":-1111.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":1449.0, "cuota":1163.0, "saldo":1163.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1974, "fecha_inicio":"2019-04-13", "tipo_deuda":"O", "ahorro_cuota_mensual":2325.999999999999, "ahorro_total":-2325.999999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1397.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-03-20", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":25000.0, "cuota":1929.0, "saldo":20708.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":24.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1717, "fecha_inicio":"2023-07-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-24.724780249763626, "ahorro_total":-593.394725994327, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":8519.0, "cuota":580.0, "saldo":7709.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0951, "fecha_inicio":"2018-12-19", "tipo_deuda":"R", "ahorro_cuota_mensual":8288.999999999993, "ahorro_total":-8288.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":26000.0, "cuota":2556.0, "saldo":15454.0, "tasa_externa":1.1535, "tasa_kubo":0.5991, "numero_pagos_otorgado":72.0, "numero_pagos_restante":14.0, "frecuencia_externa":"S", "avance":0.4056, "fecha_inicio":"2022-06-06", "tipo_deuda":"I", "ahorro_cuota_mensual":821.7473634977505, "ahorro_total":29582.905085919017, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":20000.0, "cuota":1000.0, "saldo":3049.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":15.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.8476, "fecha_inicio":"2023-01-04", "tipo_deuda":"R", "ahorro_cuota_mensual":690.3333575968736, "ahorro_total":10355.000363953104, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":19500.0, "cuota":7945.0, "saldo":5194.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7336, "fecha_inicio":"2022-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":13138.999999999995, "ahorro_total":-13138.999999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":19000.0, "cuota":950.0, "saldo":16511.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.131, "fecha_inicio":"2007-11-08", "tipo_deuda":"R", "ahorro_cuota_mensual":17460.99999999998, "ahorro_total":-17460.99999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":212603.0, "cuota":1.0, "saldo":210232.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":60.0, "numero_pagos_restante":57.0, "frecuencia_externa":"M", "avance":0.0112, "fecha_inicio":"2024-02-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-12746.413003424184, "ahorro_total":-764784.7802054511, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5262916, "monto_maximo_cliente": 61375.0, "cuota_externa_total": 12881.0, "capacidad_maxima_pago": 39719.0, "bursolnum": 7440430, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3967.3261972531327, "monto_max": 61375.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 18.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":8, "monto_otorgado":20500.0, "cuota":650.0, "saldo":1022.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9501, "fecha_inicio":"2023-07-28", "tipo_deuda":"R", "ahorro_cuota_mensual":1672.0000000000005, "ahorro_total":-1672.0000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":10000.0, "cuota":1204.0, "saldo":6092.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3908, "fecha_inicio":"2023-08-10", "tipo_deuda":"I", "ahorro_cuota_mensual":12.10797560265246, "ahorro_total":145.2957072318295, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2018-02-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":25000.0, "cuota":1250.0, "saldo":3310.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8676, "fecha_inicio":"2021-05-25", "tipo_deuda":"R", "ahorro_cuota_mensual":4560.000000000001, "ahorro_total":-4560.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":10400.0, "cuota":6067.0, "saldo":1809.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8261, "fecha_inicio":"2023-10-12", "tipo_deuda":"R", "ahorro_cuota_mensual":7876.0, "ahorro_total":-7876.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":12000.0, "cuota":-1.0, "saldo":406.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9662, "fecha_inicio":"2021-01-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":222.0, "cuota":233.0, "saldo":226.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.018, "fecha_inicio":"2024-02-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-2.290178000000253, "ahorro_total":-2.290178000000253, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":186.0, "cuota":195.0, "saldo":189.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0161, "fecha_inicio":"2024-02-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-2.1350140000002114, "ahorro_total":-2.1350140000002114, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":43000.0, "cuota":4482.0, "saldo":30365.0, "tasa_externa":0.4408, "tasa_kubo":0.6193, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2938, "fecha_inicio":"2023-10-19", "tipo_deuda":"I", "ahorro_cuota_mensual":-643.1357049085955, "ahorro_total":-7717.628458903146, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":31200.0, "cuota":3550.0, "saldo":10420.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.666, "fecha_inicio":"2023-09-05", "tipo_deuda":"R", "ahorro_cuota_mensual":13970.000000000002, "ahorro_total":-13970.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":1000.0, "cuota":388.0, "saldo":715.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.285, "fecha_inicio":"2024-01-18", "tipo_deuda":"I", "ahorro_cuota_mensual":13.983164414838257, "ahorro_total":41.94949324451477, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5359375, "monto_maximo_cliente": 103592.0, "cuota_externa_total": 12925.0, "capacidad_maxima_pago": 80598.0, "bursolnum": 6685658, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5849.050498914599, "monto_max": 103592.0, "cuota_min": 345.4415646244417, "monto_min": 5000, "plazo_max": 42.0, "plazo_min": 4, "tasa": 0.8145, "kubo_score": "E3", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":43947.0, "cuota":3308.0, "saldo":2453.0, "tasa_externa":0.8352, "tasa_kubo":0.7007, "numero_pagos_otorgado":72.0, "numero_pagos_restante":21.0, "frecuencia_externa":"S", "avance":0.9442, "fecha_inicio":"2023-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":20.706778322396076, "ahorro_total":745.4440196062587, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":36900.0, "cuota":3416.0, "saldo":36656.0, "tasa_externa":0.9457, "tasa_kubo":0.7007, "numero_pagos_otorgado":48.0, "numero_pagos_restante":14.0, "frecuencia_externa":"S", "avance":0.0066, "fecha_inicio":"2023-06-20", "tipo_deuda":"I", "ahorro_cuota_mensual":262.44367221045013, "ahorro_total":6298.648133050803, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":15400.0, "cuota":2000.0, "saldo":15232.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0109, "fecha_inicio":"2022-01-03", "tipo_deuda":"R", "ahorro_cuota_mensual":17231.999999999993, "ahorro_total":-17231.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":3000.0, "cuota":225.0, "saldo":2244.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.252, "fecha_inicio":"2021-10-17", "tipo_deuda":"R", "ahorro_cuota_mensual":2468.9999999999986, "ahorro_total":-2468.9999999999986, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":4800.0, "cuota":1400.0, "saldo":5269.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0977, "fecha_inicio":"2021-10-18", "tipo_deuda":"R", "ahorro_cuota_mensual":6668.999999999997, "ahorro_total":-6668.999999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":10000.0, "cuota":2088.0, "saldo":7734.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.2266, "fecha_inicio":"2023-05-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-3425.554561629422, "ahorro_total":-6851.109123258844, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":20000.0, "cuota":1636.0, "saldo":19226.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0387, "fecha_inicio":"2023-04-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-9391.109123258844, "ahorro_total":-18782.21824651769, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":7000.0, "cuota":852.0, "saldo":5792.0, "tasa_externa":-1.0, "tasa_kubo":0.7007, "numero_pagos_otorgado":7.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1726, "fecha_inicio":"2023-02-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-1204.0367417742682, "ahorro_total":-4816.146967097073, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5431910, "monto_maximo_cliente": 724826.0, "cuota_externa_total": 58595.0, "capacidad_maxima_pago": 644641.33, "bursolnum": 7161237, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 26393.811192044283, "monto_max": 724826.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.5991, "kubo_score": "D1", "comision": 0.046, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":6, "monto_otorgado":875.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-05-26", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":100000.0, "cuota":8991.0, "saldo":93575.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":18.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.0643, "fecha_inicio":"2023-09-27", "tipo_deuda":"I", "ahorro_cuota_mensual":663.835437085585, "ahorro_total":11949.03786754053, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":150000.0, "cuota":7500.0, "saldo":10051.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.933, "fecha_inicio":"2021-05-04", "tipo_deuda":"R", "ahorro_cuota_mensual":17551.000000000022, "ahorro_total":-17551.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":92000.0, "cuota":4492.0, "saldo":822.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9911, "fecha_inicio":"2019-02-15", "tipo_deuda":"R", "ahorro_cuota_mensual":5314.000000000002, "ahorro_total":-5314.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":115000.0, "cuota":13390.0, "saldo":84077.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2689, "fecha_inicio":"2018-04-24", "tipo_deuda":"R", "ahorro_cuota_mensual":97467.00000000017, "ahorro_total":-97467.00000000017, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":598500.0, "cuota":27980.0, "saldo":540786.0, "tasa_externa":0.3818, "tasa_kubo":0.4818, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.0964, "fecha_inicio":"2023-07-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-6613.010307011056, "ahorro_total":-238068.37105239803, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":94500.0, "cuota":4725.0, "saldo":31376.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.668, "fecha_inicio":"2019-10-09", "tipo_deuda":"R", "ahorro_cuota_mensual":36101.000000000065, "ahorro_total":-36101.000000000065, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5446124, "monto_maximo_cliente": 96883.0, "cuota_externa_total": 12986.0, "capacidad_maxima_pago": 97014.0, "bursolnum": 7308539, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5328.199323222455, "monto_max": 96883.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":18200.0, "cuota":910.0, "saldo":16883.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0724, "fecha_inicio":"2022-09-07", "tipo_deuda":"R", "ahorro_cuota_mensual":17793.000000000022, "ahorro_total":-17793.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":80000.0, "cuota":5900.0, "saldo":77486.0, "tasa_externa":0.8923, "tasa_kubo":0.6722, "numero_pagos_otorgado":144.0, "numero_pagos_restante":61.0, "frecuencia_externa":"S", "avance":0.0314, "fecha_inicio":"2023-05-05", "tipo_deuda":"I", "ahorro_cuota_mensual":645.1603508888957, "ahorro_total":46451.54526400049, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":50000.0, "cuota":6354.0, "saldo":43476.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1305, "fecha_inicio":"2023-10-03", "tipo_deuda":"I", "ahorro_cuota_mensual":226.27627755230333, "ahorro_total":2715.31533062764, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
-  </si>
-  <si>
-    <t>{"Prospecto": 5544014, "monto_maximo_cliente": 20776.0, "cuota_externa_total": 8008.0, "capacidad_maxima_pago": 23226.0, "bursolnum": 7439720, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1647.3817702448512, "monto_max": 20776.0, "cuota_min": 370.5085944866793, "monto_min": 5000, "plazo_max": 23.0, "plazo_min": 4, "tasa": 0.821, "kubo_score": "E2", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914, 0.2622, 0.2306, 0.2], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417, 0.03845, 0.03845, 0.03845], "kubo_scores": ['E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2', 'K3', 'K2', 'K1'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":906.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-06-08", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":2880.0, "cuota":144.0, "saldo":2676.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0708, "fecha_inicio":"2023-01-31", "tipo_deuda":"R", "ahorro_cuota_mensual":2820.0, "ahorro_total":-2820.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":18100.0, "cuota":2166.0, "saldo":17009.0, "tasa_externa":0.7373, "tasa_kubo":0.7554, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.0603, "fecha_inicio":"2024-01-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-149.6663517107122, "ahorro_total":-1795.9962205285465, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":10000.0, "cuota":1070.0, "saldo":9723.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":18.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.0277, "fecha_inicio":"2024-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":54.08549508704277, "ahorro_total":973.5389115667699, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":30000.0, "cuota":2577.0, "saldo":29756.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":36.0, "numero_pagos_restante":32.0, "frecuencia_externa":"M", "avance":0.0081, "fecha_inicio":"2023-12-29", "tipo_deuda":"I", "ahorro_cuota_mensual":198.21587934326863, "ahorro_total":7135.7716563576705, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":6, "monto_otorgado":305797.0, "cuota":2092.0, "saldo":206484.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":360.0, "numero_pagos_restante":324.0, "frecuencia_externa":"M", "avance":0.3248, "fecha_inicio":"2021-05-01", "tipo_deuda":"M", "ahorro_cuota_mensual":-12985.874648144287, "ahorro_total":-4674914.8733319435, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 24059, "monto_maximo_cliente": 962287.0, "cuota_externa_total": 41450.0, "capacidad_maxima_pago": 524380.0, "bursolnum": 6149272, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 19056.680029461608, "monto_max": 962287.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6265, "kubo_score": "D3", "comision": -0.01, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": -1, "comisiones": -1, "kubo_scores": -1, "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":90000.0, "cuota":6131.0, "saldo":36957.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5894, "fecha_inicio":"2007-09-19", "tipo_deuda":"R", "ahorro_cuota_mensual":43087.999999999905, "ahorro_total":-43087.999999999905, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":2, "monto_otorgado":259758.0, "cuota":0.0, "saldo":316127.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":-0.217, "fecha_inicio":"2021-03-19", "tipo_deuda":"O", "ahorro_cuota_mensual":316126.9999999992, "ahorro_total":-316126.9999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":3, "monto_otorgado":25000.0, "cuota":13291.0, "saldo":6666.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7334, "fecha_inicio":"2022-04-23", "tipo_deuda":"R", "ahorro_cuota_mensual":19956.99999999998, "ahorro_total":-19956.99999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":500000.0, "cuota":20063.0, "saldo":410362.0, "tasa_externa":0.3741, "tasa_kubo":0.3337, "numero_pagos_otorgado":48.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.1793, "fecha_inicio":"2022-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-558.320581278731, "ahorro_total":-26799.387901379087, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":188100.0, "cuota":116.0, "saldo":83383.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5567, "fecha_inicio":"2020-02-11", "tipo_deuda":"R", "ahorro_cuota_mensual":83498.9999999998, "ahorro_total":-83498.9999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":418000.0, "cuota":1.0, "saldo":11913.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9715, "fecha_inicio":"2023-03-09", "tipo_deuda":"R", "ahorro_cuota_mensual":11913.999999999969, "ahorro_total":-11913.999999999969, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":21000.0, "cuota":1050.0, "saldo":7241.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6552, "fecha_inicio":"2013-12-23", "tipo_deuda":"R", "ahorro_cuota_mensual":8290.999999999982, "ahorro_total":-8290.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":200000.0, "cuota":15001.0, "saldo":31618.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":25.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8419, "fecha_inicio":"2021-04-20", "tipo_deuda":"I", "ahorro_cuota_mensual":3224.5802279166437, "ahorro_total":80614.50569791609, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":380000.0, "cuota":39530.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":900.0, "numero_pagos_restante":802.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-02-12", "tipo_deuda":"R", "ahorro_cuota_mensual":39530.0, "ahorro_total":35577000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>Tasas, scores y comisiones viene con -1</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 189189, "monto_maximo_cliente": 528488.0, "cuota_externa_total": 32607.0, "capacidad_maxima_pago": 220250.0, "bursolnum": 7438900, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 12456.883028022743, "monto_max": 528488.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 50.0, "plazo_min": 4, "tasa": 0.5991, "kubo_score": "D1", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":78000.0, "cuota":4897.0, "saldo":59756.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.2339, "fecha_inicio":"2022-10-27", "tipo_deuda":"I", "ahorro_cuota_mensual":388.6377544747493, "ahorro_total":13990.959161090974, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":1921.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-02-10", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":4, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-10-18", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":15000.0, "cuota":8126.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2015-09-19", "tipo_deuda":"R", "ahorro_cuota_mensual":8126.0, "ahorro_total":-8126.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":80000.0, "cuota":4428.0, "saldo":79840.0, "tasa_externa":0.6591, "tasa_kubo":0.4818, "numero_pagos_otorgado":144.0, "numero_pagos_restante":67.0, "frecuencia_externa":"S", "avance":0.002, "fecha_inicio":"2023-12-04", "tipo_deuda":"I", "ahorro_cuota_mensual":556.0318719877932, "ahorro_total":40034.29478312111, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":50.0, "cuota":53.0, "saldo":51.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.02, "fecha_inicio":"2024-02-17", "tipo_deuda":"I", "ahorro_cuota_mensual":0.6712999999998885, "ahorro_total":0.6712999999998885, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":80000.0, "cuota":4456.0, "saldo":73348.0, "tasa_externa":0.2063, "tasa_kubo":0.4818, "numero_pagos_otorgado":43.0, "numero_pagos_restante":17.0, "frecuencia_externa":"S", "avance":0.0831, "fecha_inicio":"2023-12-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-1433.2382484712107, "ahorro_total":-31531.241466366635, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":80000.0, "cuota":4456.0, "saldo":73348.0, "tasa_externa":0.2063, "tasa_kubo":0.4818, "numero_pagos_otorgado":43.0, "numero_pagos_restante":17.0, "frecuencia_externa":"S", "avance":0.0831, "fecha_inicio":"2023-12-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-1433.2382484712107, "ahorro_total":-31531.241466366635, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":80000.0, "cuota":4428.0, "saldo":79188.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":43.0, "numero_pagos_restante":19.0, "frecuencia_externa":"S", "avance":0.0101, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-1461.2382484712107, "ahorro_total":-32147.241466366635, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":80000.0, "cuota":4428.0, "saldo":79188.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":43.0, "numero_pagos_restante":19.0, "frecuencia_externa":"S", "avance":0.0101, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-1461.2382484712107, "ahorro_total":-32147.241466366635, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":80000.0, "cuota":4428.0, "saldo":79188.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":43.0, "numero_pagos_restante":19.0, "frecuencia_externa":"S", "avance":0.0101, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-1461.2382484712107, "ahorro_total":-32147.241466366635, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":82620.0, "cuota":4131.0, "saldo":46157.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4413, "fecha_inicio":"2019-09-19", "tipo_deuda":"R", "ahorro_cuota_mensual":50288.000000000095, "ahorro_total":-50288.000000000095, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":22000.0, "cuota":5000.0, "saldo":2281.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8963, "fecha_inicio":"2017-04-20", "tipo_deuda":"R", "ahorro_cuota_mensual":7281.000000000005, "ahorro_total":-7281.000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>No incluir tasa del modelo en tasas asistidas</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 230009, "monto_maximo_cliente": 135880.0, "cuota_externa_total": 32967.0, "capacidad_maxima_pago": 7501.330000000002, "bursolnum": 7438906, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1280.5016886011238, "monto_max": 135880.0, "cuota_min": 277.6602976125524, "monto_min": 5000, "plazo_max": 19.0, "plazo_min": 4, "tasa": 0.5492, "kubo_score": "C4", "comision": -0.01, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": -1, "comisiones": -1, "kubo_scores": -1, "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":45370.0, "cuota":3031.0, "saldo":36745.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":36.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.1901, "fecha_inicio":"2022-10-05", "tipo_deuda":"I", "ahorro_cuota_mensual":181.47654680003643, "ahorro_total":6533.1556848013115, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":12, "monto_otorgado":10000.0, "cuota":1071.0, "saldo":1071.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.8929, "fecha_inicio":"2023-10-31", "tipo_deuda":"O", "ahorro_cuota_mensual":2141.9999999999973, "ahorro_total":-2141.9999999999973, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":1921.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-06-24", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":31, "monto_otorgado":24000.0, "cuota":-1.0, "saldo":17889.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2546, "fecha_inicio":"2021-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":19, "monto_otorgado":1300.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-12-10", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":18, "monto_otorgado":14500.0, "cuota":789.0, "saldo":14198.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0208, "fecha_inicio":"2021-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":8000.0, "cuota":1027.0, "saldo":7847.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0191, "fecha_inicio":"2021-09-21", "tipo_deuda":"R", "ahorro_cuota_mensual":8873.999999999982, "ahorro_total":-8873.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":16, "monto_otorgado":15100.0, "cuota":1806.0, "saldo":13206.0, "tasa_externa":0.7361, "tasa_kubo":0.5486, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1254, "fecha_inicio":"2021-10-12", "tipo_deuda":"I", "ahorro_cuota_mensual":73.08630607675173, "ahorro_total":877.0356729210207, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":15, "monto_otorgado":30000.0, "cuota":3311.0, "saldo":30069.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0023, "fecha_inicio":"2022-07-25", "tipo_deuda":"R", "ahorro_cuota_mensual":33379.99999999993, "ahorro_total":-33379.99999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":11900.0, "cuota":660.0, "saldo":7377.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3801, "fecha_inicio":"2021-12-11", "tipo_deuda":"R", "ahorro_cuota_mensual":8036.999999999984, "ahorro_total":-8036.999999999984, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":4299.0, "cuota":674.0, "saldo":1272.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7041, "fecha_inicio":"2023-07-27", "tipo_deuda":"I", "ahorro_cuota_mensual":60.98221920146398, "ahorro_total":548.8399728131758, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":2528.0, "cuota":520.0, "saldo":2212.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.125, "fecha_inicio":"2024-01-25", "tipo_deuda":"I", "ahorro_cuota_mensual":17.101150384815128, "ahorro_total":102.60690230889077, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":1735.0, "cuota":1903.0, "saldo":1875.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0807, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":75.99063666667007, "ahorro_total":75.99063666667007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":10000.0, "cuota":2660.0, "saldo":2660.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.734, "fecha_inicio":"2023-05-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-7870.313333333312, "ahorro_total":-7870.313333333312, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":10000.0, "cuota":2165.0, "saldo":3239.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6761, "fecha_inicio":"2022-04-04", "tipo_deuda":"R", "ahorro_cuota_mensual":5403.999999999993, "ahorro_total":-5403.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":2200.0, "cuota":110.0, "saldo":507.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7695, "fecha_inicio":"2023-08-20", "tipo_deuda":"R", "ahorro_cuota_mensual":9.14172596720779, "ahorro_total":54.85035580324674, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":5100.0, "cuota":795.0, "saldo":6445.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.2637, "fecha_inicio":"2021-08-14", "tipo_deuda":"R", "ahorro_cuota_mensual":7239.999999999985, "ahorro_total":-7239.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":19800.0, "cuota":14647.0, "saldo":14647.0, "tasa_externa":-1.0, "tasa_kubo":0.5486, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2603, "fecha_inicio":"2021-05-24", "tipo_deuda":"R", "ahorro_cuota_mensual":29293.999999999964, "ahorro_total":-29293.999999999964, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 301784, "monto_maximo_cliente": 619161.0, "cuota_externa_total": 74716.0, "capacidad_maxima_pago": 470623.0, "bursolnum": 7438918, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 12891.679674578185, "monto_max": 619161.0, "cuota_min": 148.2848081136287, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":169900.0, "cuota":4015.0, "saldo":82194.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":60.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.5162, "fecha_inicio":"2021-03-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-1023.7177797011045, "ahorro_total":-61423.06678206627, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":9, "monto_otorgado":674577.0, "cuota":15783.0, "saldo":642060.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":48.0, "numero_pagos_restante":39.0, "frecuencia_externa":"M", "avance":0.0482, "fecha_inicio":"2023-08-05", "tipo_deuda":"I", "ahorro_cuota_mensual":-6780.126084424803, "ahorro_total":-325446.0520523905, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":100000.0, "cuota":9134.0, "saldo":77867.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":18.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.2213, "fecha_inicio":"2023-08-25", "tipo_deuda":"I", "ahorro_cuota_mensual":2389.2748448470875, "ahorro_total":43006.94720724758, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":171263.0, "cuota":2055.0, "saldo":118095.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":110.0, "numero_pagos_restante":68.0, "frecuencia_externa":"M", "avance":0.3104, "fecha_inicio":"2020-10-21", "tipo_deuda":"M", "ahorro_cuota_mensual":-731.7801647404772, "ahorro_total":-80495.8181214525, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":19, "monto_otorgado":10000.0, "cuota":548.0, "saldo":548.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.9452, "fecha_inicio":"2010-01-27", "tipo_deuda":"O", "ahorro_cuota_mensual":1095.9999999999977, "ahorro_total":-1095.9999999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":17, "monto_otorgado":1100.0, "cuota":249.0, "saldo":249.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7736, "fecha_inicio":"2020-09-11", "tipo_deuda":"O", "ahorro_cuota_mensual":497.999999999999, "ahorro_total":-497.999999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":18, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2010-02-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":20, "monto_otorgado":10000.0, "cuota":866.0, "saldo":866.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.9134, "fecha_inicio":"2010-01-15", "tipo_deuda":"O", "ahorro_cuota_mensual":1731.9999999999964, "ahorro_total":-1731.9999999999964, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":8000.0, "cuota":11525.0, "saldo":11525.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.4406, "fecha_inicio":"2024-02-23", "tipo_deuda":"I", "ahorro_cuota_mensual":3354.866666666704, "ahorro_total":3354.866666666704, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":16, "monto_otorgado":522372.0, "cuota":6620.0, "saldo":360204.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":110.0, "numero_pagos_restante":68.0, "frecuencia_externa":"M", "avance":0.3104, "fecha_inicio":"2020-10-21", "tipo_deuda":"M", "ahorro_cuota_mensual":-1880.0157708639563, "ahorro_total":-206801.73479503518, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":24, "monto_otorgado":11500.0, "cuota":1194.0, "saldo":11039.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0401, "fecha_inicio":"2024-01-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-10079.762733333282, "ahorro_total":-10079.762733333282, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":7000.0, "cuota":350.0, "saldo":814.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8837, "fecha_inicio":"2021-07-08", "tipo_deuda":"R", "ahorro_cuota_mensual":1163.9999999999966, "ahorro_total":-1163.9999999999966, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":450.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-12-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":23, "monto_otorgado":6500.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-11-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":151670.0, "cuota":0.0, "saldo":48373.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.6811, "fecha_inicio":"2018-08-27", "tipo_deuda":"O", "ahorro_cuota_mensual":48372.999999999796, "ahorro_total":-48372.999999999796, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":176537.0, "cuota":5403.0, "saldo":144020.0, "tasa_externa":0.2789, "tasa_kubo":0.22, "numero_pagos_otorgado":61.0, "numero_pagos_restante":39.0, "frecuencia_externa":"M", "avance":0.1842, "fecha_inicio":"2022-07-04", "tipo_deuda":"I", "ahorro_cuota_mensual":210.11154108965457, "ahorro_total":12816.804006468928, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":6000.0, "cuota":5181.0, "saldo":1724.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7127, "fecha_inicio":"2023-08-16", "tipo_deuda":"R", "ahorro_cuota_mensual":6904.999999999993, "ahorro_total":-6904.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":450.0, "cuota":415.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-12-18", "tipo_deuda":"R", "ahorro_cuota_mensual":415.0, "ahorro_total":-415.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":254509.0, "cuota":7819.0, "saldo":210620.0, "tasa_externa":0.2769, "tasa_kubo":0.22, "numero_pagos_otorgado":60.0, "numero_pagos_restante":39.0, "frecuencia_externa":"M", "avance":0.1724, "fecha_inicio":"2022-08-09", "tipo_deuda":"I", "ahorro_cuota_mensual":271.03635436169407, "ahorro_total":16262.181261701644, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":6000.0, "cuota":423.0, "saldo":4224.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.296, "fecha_inicio":"2020-11-10", "tipo_deuda":"R", "ahorro_cuota_mensual":4646.999999999983, "ahorro_total":-4646.999999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":41900.0, "cuota":2384.0, "saldo":31312.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2527, "fecha_inicio":"2020-11-02", "tipo_deuda":"R", "ahorro_cuota_mensual":33695.99999999987, "ahorro_total":-33695.99999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":100000.0, "cuota":6310.0, "saldo":77387.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2261, "fecha_inicio":"2021-08-23", "tipo_deuda":"R", "ahorro_cuota_mensual":83696.99999999967, "ahorro_total":-83696.99999999967, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":6500.0, "cuota":325.0, "saldo":5242.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1935, "fecha_inicio":"2024-01-08", "tipo_deuda":"R", "ahorro_cuota_mensual":5566.999999999977, "ahorro_total":-5566.999999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 820117, "monto_maximo_cliente": 667576.0, "cuota_externa_total": 87443.0, "capacidad_maxima_pago": 112557.0, "bursolnum": 7438981, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5328.82868046942, "monto_max": 667576.0, "cuota_min": 227.39637225020516, "monto_min": 5000, "plazo_max": 24.0, "plazo_min": 4, "tasa": 0.4295, "kubo_score": "B1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":24, "monto_otorgado":41000.0, "cuota":2587.0, "saldo":34444.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1599, "fecha_inicio":"2023-05-04", "tipo_deuda":"R", "ahorro_cuota_mensual":37030.99999999998, "ahorro_total":-37030.99999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":23, "monto_otorgado":19522.0, "cuota":3217.0, "saldo":9053.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":7.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5363, "fecha_inicio":"2023-10-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-53.82695757631336, "ahorro_total":-376.78870303419353, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":22, "monto_otorgado":55617.0, "cuota":3980.0, "saldo":48884.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":21.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1211, "fecha_inicio":"2023-10-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-40.01721536074774, "ahorro_total":-840.3615225757026, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":787641.0, "cuota":9310.0, "saldo":557181.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":120.0, "numero_pagos_restante":43.0, "frecuencia_externa":"S", "avance":0.2926, "fecha_inicio":"2022-11-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-26511.34120710477, "ahorro_total":-1590680.4724262862, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":632433.0, "cuota":8848.0, "saldo":544965.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":120.0, "numero_pagos_restante":43.0, "frecuencia_externa":"S", "avance":0.1383, "fecha_inicio":"2022-12-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-19914.5939782628, "ahorro_total":-1194875.638695768, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":29, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"1950-01-01", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "GOBIERNO", "registro":30, "monto_otorgado":1.0, "cuota":-1.0, "saldo":1.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0, "fecha_inicio":"2014-10-01", "tipo_deuda":"R", "ahorro_cuota_mensual":-5.551115123125783e-16, "ahorro_total":5.551115123125783e-16, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MIC CREDITO PERS", "registro":21, "monto_otorgado":281000.0, "cuota":25168.0, "saldo":390182.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":36.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":-0.3885, "fecha_inicio":"2023-10-31", "tipo_deuda":"I", "ahorro_cuota_mensual":9992.822329783108, "ahorro_total":359741.6038721919, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":135796.0, "cuota":1758.0, "saldo":117416.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":120.0, "numero_pagos_restante":46.0, "frecuencia_externa":"S", "avance":0.1354, "fecha_inicio":"2023-02-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-4417.903553217772, "ahorro_total":-265074.21319306636, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":19, "monto_otorgado":15480.0, "cuota":1215.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-07-21", "tipo_deuda":"R", "ahorro_cuota_mensual":1215.0, "ahorro_total":-1215.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":18, "monto_otorgado":107100.0, "cuota":11000.0, "saldo":91427.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1463, "fecha_inicio":"2023-03-13", "tipo_deuda":"R", "ahorro_cuota_mensual":102426.99999999994, "ahorro_total":-102426.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":10000.0, "cuota":9045.0, "saldo":9045.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0955, "fecha_inicio":"2023-06-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-1370.1833333333343, "ahorro_total":-1370.1833333333343, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":16, "monto_otorgado":123830.0, "cuota":11859.0, "saldo":49227.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6025, "fecha_inicio":"2015-01-02", "tipo_deuda":"R", "ahorro_cuota_mensual":61085.99999999997, "ahorro_total":-61085.99999999997, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":15, "monto_otorgado":80000.0, "cuota":5956.0, "saldo":76845.0, "tasa_externa":0.5727, "tasa_kubo":0.4295, "numero_pagos_otorgado":43.0, "numero_pagos_restante":10.0, "frecuencia_externa":"S", "avance":0.0394, "fecha_inicio":"2023-05-05", "tipo_deuda":"I", "ahorro_cuota_mensual":339.4593671993298, "ahorro_total":7468.106078385255, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":14, "monto_otorgado":107200.0, "cuota":5715.0, "saldo":84126.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2152, "fecha_inicio":"2021-06-28", "tipo_deuda":"R", "ahorro_cuota_mensual":89840.99999999994, "ahorro_total":-89840.99999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":71600.0, "cuota":146.0, "saldo":13409.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8127, "fecha_inicio":"2020-11-26", "tipo_deuda":"R", "ahorro_cuota_mensual":13554.999999999993, "ahorro_total":-13554.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":12, "monto_otorgado":109991.0, "cuota":0.0, "saldo":23942.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7823, "fecha_inicio":"2022-09-30", "tipo_deuda":"O", "ahorro_cuota_mensual":23941.999999999985, "ahorro_total":-23941.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":20, "monto_otorgado":9270.0, "cuota":340.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4295, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-04-26", "tipo_deuda":"R", "ahorro_cuota_mensual":340.0, "ahorro_total":-340.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 985053, "monto_maximo_cliente": 134184.0, "cuota_externa_total": 18240.0, "capacidad_maxima_pago": 83520.0, "bursolnum": 6636993, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5293.744643303981, "monto_max": 134184.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.6755, "kubo_score": "D5", "comision": -0.01, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": -1, "comisiones": -1, "kubo_scores": -1, "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-03-01", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":19000.0, "cuota":1796.0, "saldo":16658.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1233, "fecha_inicio":"2023-03-21", "tipo_deuda":"I", "ahorro_cuota_mensual":109.2294268178116, "ahorro_total":1966.1296827206088, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-01-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":70000.0, "cuota":6788.0, "saldo":44302.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.3671, "fecha_inicio":"2022-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":65, "monto_otorgado":500.0, "cuota":518.0, "saldo":518.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.036, "fecha_inicio":"2023-04-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-9.395333333333383, "ahorro_total":-9.395333333333383, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":64, "monto_otorgado":100.0, "cuota":104.0, "saldo":104.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.04, "fecha_inicio":"2023-04-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.479066666666668, "ahorro_total":-1.479066666666668, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":61, "monto_otorgado":417.0, "cuota":155.0, "saldo":306.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2662, "fecha_inicio":"2023-03-22", "tipo_deuda":"I", "ahorro_cuota_mensual":0.4974897121670381, "ahorro_total":1.4924691365011142, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":62, "monto_otorgado":512.0, "cuota":188.0, "saldo":371.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2754, "fecha_inicio":"2023-03-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.7009239025670695, "ahorro_total":-5.1027717077012085, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":17000.0, "cuota":1616.0, "saldo":14155.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1674, "fecha_inicio":"2023-05-29", "tipo_deuda":"R", "ahorro_cuota_mensual":15771.000000000004, "ahorro_total":-15771.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":60400.0, "cuota":3020.0, "saldo":35020.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4202, "fecha_inicio":"2019-12-17", "tipo_deuda":"R", "ahorro_cuota_mensual":38040.00000000001, "ahorro_total":-38040.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":80000.0, "cuota":5900.0, "saldo":79434.0, "tasa_externa":0.56, "tasa_kubo":0.5668, "numero_pagos_otorgado":43.0, "numero_pagos_restante":11.0, "frecuencia_externa":"S", "avance":0.0071, "fecha_inicio":"2023-06-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-445.85407781089634, "ahorro_total":-9808.78971183972, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":19700.0, "cuota":985.0, "saldo":3181.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8385, "fecha_inicio":"2022-12-29", "tipo_deuda":"R", "ahorro_cuota_mensual":4166.000000000001, "ahorro_total":-4166.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":63, "monto_otorgado":299.0, "cuota":60.0, "saldo":292.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0234, "fecha_inicio":"2023-03-30", "tipo_deuda":"I", "ahorro_cuota_mensual":0.18620403727186385, "ahorro_total":1.1172242236311831, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 1360950, "monto_maximo_cliente": 70378.0, "cuota_externa_total": 33180.0, "capacidad_maxima_pago": 17920.0, "bursolnum": 7439045, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2842.5496999139004, "monto_max": 70378.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 15.0, "plazo_min": 4, "tasa": 0.4818, "kubo_score": "B5", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-01-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":53000.0, "cuota":3724.0, "saldo":22085.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5833, "fecha_inicio":"2022-09-19", "tipo_deuda":"I", "ahorro_cuota_mensual":10.032892732850996, "ahorro_total":240.7894255884239, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":36000.0, "cuota":2628.0, "saldo":25338.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":24.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.2962, "fecha_inicio":"2023-03-09", "tipo_deuda":"I", "ahorro_cuota_mensual":105.30536110155936, "ahorro_total":2527.3286664374245, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":871.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-01-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":871.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-01-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-09-19", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":12863.0, "cuota":4248.0, "saldo":2872.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":13.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.7767, "fecha_inicio":"2023-12-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-445.11245256584425, "ahorro_total":-1335.3373576975328, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":30200.0, "cuota":3374.0, "saldo":13928.0, "tasa_externa":0.5872, "tasa_kubo":0.4818, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5388, "fecha_inicio":"2021-07-26", "tipo_deuda":"I", "ahorro_cuota_mensual":32.19289597740044, "ahorro_total":386.3147517288053, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-11-24", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":24100.0, "cuota":1640.0, "saldo":23315.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0326, "fecha_inicio":"2022-05-12", "tipo_deuda":"R", "ahorro_cuota_mensual":24955.00000000005, "ahorro_total":-24955.00000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":4000.0, "cuota":17566.0, "saldo":17566.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-3.3915, "fecha_inicio":"2023-10-31", "tipo_deuda":"I", "ahorro_cuota_mensual":13379.70399999999, "ahorro_total":13379.70399999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 1585349, "monto_maximo_cliente": 209409.0, "cuota_externa_total": 21707.0, "capacidad_maxima_pago": 57635.0, "bursolnum": 7439082, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1829.905006232347, "monto_max": 209409.0, "cuota_min": 160.05380240065423, "monto_min": 5000, "plazo_max": 58.0, "plazo_min": 4, "tasa": 0.4428, "kubo_score": "B2", "comision": 0.0444, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":31, "monto_otorgado":100.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-07-13", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":9, "monto_otorgado":730.0, "cuota":730.0, "saldo":730.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2005-07-20", "tipo_deuda":"O", "ahorro_cuota_mensual":1459.999999999999, "ahorro_total":-1459.999999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":22300.0, "cuota":1821.0, "saldo":11086.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5029, "fecha_inicio":"2023-03-07", "tipo_deuda":"I", "ahorro_cuota_mensual":273.59265972456296, "ahorro_total":4924.667875042133, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":67700.0, "cuota":5570.0, "saldo":45023.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":18.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.335, "fecha_inicio":"2023-06-13", "tipo_deuda":"I", "ahorro_cuota_mensual":872.2656082221038, "ahorro_total":15700.780947997868, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":7000.0, "cuota":838.0, "saldo":5448.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2217, "fecha_inicio":"2022-10-01", "tipo_deuda":"I", "ahorro_cuota_mensual":157.51411605653118, "ahorro_total":1890.1693926783742, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":14700.0, "cuota":1756.0, "saldo":12505.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1493, "fecha_inicio":"2022-11-02", "tipo_deuda":"I", "ahorro_cuota_mensual":326.97964371871535, "ahorro_total":3923.755724624584, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-03-09", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":6000.0, "cuota":1055.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-12-05", "tipo_deuda":"R", "ahorro_cuota_mensual":1055.0, "ahorro_total":-1055.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":30000.0, "cuota":4540.0, "saldo":21572.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2809, "fecha_inicio":"2023-12-24", "tipo_deuda":"I", "ahorro_cuota_mensual":784.5627748471352, "ahorro_total":7061.064973624217, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":56300.0, "cuota":2332.0, "saldo":49172.0, "tasa_externa":0.3893, "tasa_kubo":0.2538, "numero_pagos_otorgado":47.0, "numero_pagos_restante":36.0, "frecuencia_externa":"M", "avance":0.1266, "fecha_inicio":"2023-06-01", "tipo_deuda":"I", "ahorro_cuota_mensual":300.48611287105814, "ahorro_total":14122.847304939733, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":11500.0, "cuota":812.0, "saldo":2921.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.746, "fecha_inicio":"2019-07-16", "tipo_deuda":"I", "ahorro_cuota_mensual":-498.8137396729992, "ahorro_total":-4988.137396729991, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":95000.0, "cuota":4750.0, "saldo":89707.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0557, "fecha_inicio":"2022-04-20", "tipo_deuda":"R", "ahorro_cuota_mensual":94456.9999999999, "ahorro_total":-94456.9999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":16700.0, "cuota":1125.0, "saldo":202.0, "tasa_externa":-1.0, "tasa_kubo":0.2538, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9879, "fecha_inicio":"2018-02-21", "tipo_deuda":"R", "ahorro_cuota_mensual":1326.9999999999998, "ahorro_total":-1326.9999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 1669798, "monto_maximo_cliente": 149281.0, "cuota_externa_total": 22802.0, "capacidad_maxima_pago": 49020.0, "bursolnum": 6320398, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1866.531573393356, "monto_max": 149281.0, "cuota_min": 130.08822700780902, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.165, "kubo_score": "A1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.165], "comisiones": [0], "kubo_scores": ['A1'], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":20, "monto_otorgado":394.0, "cuota":80.0, "saldo":314.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.203, "fecha_inicio":"2023-03-11", "tipo_deuda":"I", "ahorro_cuota_mensual":10.61915848402279, "ahorro_total":63.71495090413674, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "HIPOTECAGOBIERNO", "registro":27, "monto_otorgado":1129549.0, "cuota":11548.0, "saldo":1140349.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":360.0, "numero_pagos_restante":334.0, "frecuencia_externa":"M", "avance":-0.0096, "fecha_inicio":"2022-02-14", "tipo_deuda":"M", "ahorro_cuota_mensual":-6701.832391336702, "ahorro_total":-2412659.660881213, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":39914.0, "cuota":2304.0, "saldo":37601.0, "tasa_externa":0.4359, "tasa_kubo":0.165, "numero_pagos_otorgado":104.0, "numero_pagos_restante":13.0, "frecuencia_externa":"W", "avance":0.0579, "fecha_inicio":"2023-03-25", "tipo_deuda":"I", "ahorro_cuota_mensual":416.55557235886386, "ahorro_total":10830.44488133046, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":26, "monto_otorgado":400.0, "cuota":81.0, "saldo":397.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0075, "fecha_inicio":"2023-04-16", "tipo_deuda":"I", "ahorro_cuota_mensual":10.56259744570842, "ahorro_total":63.37558467425052, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":25, "monto_otorgado":6000.0, "cuota":1234.0, "saldo":6022.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0037, "fecha_inicio":"2023-04-11", "tipo_deuda":"I", "ahorro_cuota_mensual":177.4389616856265, "ahorro_total":1064.633770113759, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":24, "monto_otorgado":392.0, "cuota":147.0, "saldo":291.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2577, "fecha_inicio":"2023-04-06", "tipo_deuda":"I", "ahorro_cuota_mensual":12.143081178895471, "ahorro_total":36.429243536686414, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":23, "monto_otorgado":549.0, "cuota":209.0, "saldo":412.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2495, "fecha_inicio":"2023-03-31", "tipo_deuda":"I", "ahorro_cuota_mensual":20.13150910003472, "ahorro_total":60.39452730010416, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":22, "monto_otorgado":286.0, "cuota":109.0, "saldo":216.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2448, "fecha_inicio":"2023-03-27", "tipo_deuda":"I", "ahorro_cuota_mensual":10.609492900928842, "ahorro_total":31.828478702786526, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":21, "monto_otorgado":1125.0, "cuota":416.0, "saldo":416.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6302, "fecha_inicio":"2023-03-13", "tipo_deuda":"I", "ahorro_cuota_mensual":28.974403893513795, "ahorro_total":86.92321168054139, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":18, "monto_otorgado":300.0, "cuota":112.0, "saldo":112.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6267, "fecha_inicio":"2023-03-10", "tipo_deuda":"I", "ahorro_cuota_mensual":8.79317437160367, "ahorro_total":26.379523114811008, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":17950.0, "cuota":2955.0, "saldo":14235.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.207, "fecha_inicio":"2020-05-11", "tipo_deuda":"R", "ahorro_cuota_mensual":17190.00000000007, "ahorro_total":-17190.00000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":16, "monto_otorgado":344.0, "cuota":71.0, "saldo":277.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1948, "fecha_inicio":"2023-03-05", "tipo_deuda":"I", "ahorro_cuota_mensual":10.423833803309243, "ahorro_total":62.54300281985546, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":47600.0, "cuota":2380.0, "saldo":33691.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2922, "fecha_inicio":"2021-03-08", "tipo_deuda":"R", "ahorro_cuota_mensual":36071.00000000016, "ahorro_total":-36071.00000000016, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":388.0, "cuota":79.0, "saldo":310.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.201, "fecha_inicio":"2023-03-09", "tipo_deuda":"I", "ahorro_cuota_mensual":10.675719522337175, "ahorro_total":64.05431713402305, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":15000.0, "cuota":750.0, "saldo":6143.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5905, "fecha_inicio":"2022-12-09", "tipo_deuda":"R", "ahorro_cuota_mensual":6893.00000000003, "ahorro_total":-6893.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":50822.0, "cuota":2405.0, "saldo":45008.0, "tasa_externa":0.3918, "tasa_kubo":0.165, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.1144, "fecha_inicio":"2022-10-17", "tipo_deuda":"I", "ahorro_cuota_mensual":538.468426606644, "ahorro_total":19384.863357839185, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":29400.0, "cuota":1470.0, "saldo":16303.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4455, "fecha_inicio":"2021-09-23", "tipo_deuda":"R", "ahorro_cuota_mensual":17773.00000000008, "ahorro_total":-17773.00000000008, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":17950.0, "cuota":-1.0, "saldo":14235.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.207, "fecha_inicio":"2020-05-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":299.0, "cuota":47.0, "saldo":47.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8428, "fecha_inicio":"2022-09-04", "tipo_deuda":"I", "ahorro_cuota_mensual":11.072423867181918, "ahorro_total":99.65181480463727, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":3000.0, "cuota":401.0, "saldo":1952.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3493, "fecha_inicio":"2022-09-28", "tipo_deuda":"I", "ahorro_cuota_mensual":124.32977798344541, "ahorro_total":1491.957335801345, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":375.0, "cuota":78.0, "saldo":78.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.792, "fecha_inicio":"2022-12-19", "tipo_deuda":"I", "ahorro_cuota_mensual":11.964935105351657, "ahorro_total":71.78961063210994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 1764064, "monto_maximo_cliente": 365624.0, "cuota_externa_total": 52270.0, "capacidad_maxima_pago": 63301.0, "bursolnum": 7439111, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1892.072695856917, "monto_max": 365624.0, "cuota_min": 130.08822700780902, "monto_min": 5000, "plazo_max": 37.0, "plazo_min": 4, "tasa": 0.165, "kubo_score": "A1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.165], "comisiones": [0], "kubo_scores": ['A1'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":13, "monto_otorgado":100000.0, "cuota":8572.0, "saldo":63537.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":24.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.3646, "fecha_inicio":"2022-12-06", "tipo_deuda":"I", "ahorro_cuota_mensual":3524.3337414679263, "ahorro_total":84584.00979523023, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":49169.0, "cuota":2334.0, "saldo":33288.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":32.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.323, "fecha_inicio":"2022-12-09", "tipo_deuda":"I", "ahorro_cuota_mensual":360.1716700839577, "ahorro_total":11525.493442686646, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2005-06-18", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-05-14", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-11-15", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":3, "monto_otorgado":417995.0, "cuota":13068.0, "saldo":313638.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":36.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.2497, "fecha_inicio":"2023-04-16", "tipo_deuda":"I", "ahorro_cuota_mensual":-2283.6363980275437, "ahorro_total":-82210.91032899157, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":17, "monto_otorgado":41800.0, "cuota":2090.0, "saldo":43716.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0458, "fecha_inicio":"2016-03-11", "tipo_deuda":"R", "ahorro_cuota_mensual":45806.00000000021, "ahorro_total":-45806.00000000021, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":801020.0, "cuota":16577.0, "saldo":779049.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":72.0, "numero_pagos_restante":67.0, "frecuencia_externa":"M", "avance":0.0274, "fecha_inicio":"2023-12-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-2212.484525087337, "ahorro_total":-159298.88580628825, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":52571.0, "cuota":2395.0, "saldo":30301.0, "tasa_externa":0.3606, "tasa_kubo":0.165, "numero_pagos_otorgado":36.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.4236, "fecha_inicio":"2022-06-20", "tipo_deuda":"I", "ahorro_cuota_mensual":464.23317962964643, "ahorro_total":16712.394466667272, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":12800.0, "cuota":823.0, "saldo":10120.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2094, "fecha_inicio":"2020-09-23", "tipo_deuda":"R", "ahorro_cuota_mensual":10943.00000000005, "ahorro_total":-10943.00000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":109800.0, "cuota":905.0, "saldo":104474.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0485, "fecha_inicio":"2018-12-11", "tipo_deuda":"R", "ahorro_cuota_mensual":105379.0000000005, "ahorro_total":-105379.0000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":5, "monto_otorgado":30202.0, "cuota":0.0, "saldo":4150.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.8626, "fecha_inicio":"2016-04-06", "tipo_deuda":"O", "ahorro_cuota_mensual":4150.00000000002, "ahorro_total":-4150.00000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":76000.0, "cuota":5796.0, "saldo":63719.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1616, "fecha_inicio":"2022-06-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-2486.528497391646, "ahorro_total":-24865.28497391646, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":2, "monto_otorgado":51000.0, "cuota":4500.0, "saldo":35510.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3037, "fecha_inicio":"2018-02-02", "tipo_deuda":"R", "ahorro_cuota_mensual":40010.000000000175, "ahorro_total":-40010.000000000175, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":40000.0, "cuota":2000.0, "saldo":7788.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8053, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":9788.000000000036, "ahorro_total":-9788.000000000036, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":16, "monto_otorgado":36900.0, "cuota":1904.0, "saldo":31295.0, "tasa_externa":-1.0, "tasa_kubo":0.165, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1519, "fecha_inicio":"2019-06-13", "tipo_deuda":"R", "ahorro_cuota_mensual":33199.000000000146, "ahorro_total":-33199.000000000146, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 1823294, "monto_maximo_cliente": 486133.0, "cuota_externa_total": 27020.0, "capacidad_maxima_pago": 417980.0, "bursolnum": 7439123, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 14506.941526394074, "monto_max": 486133.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":9, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2016-01-14", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1493.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-01-20", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":128100.0, "cuota":7315.0, "saldo":76840.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.4002, "fecha_inicio":"2022-04-05", "tipo_deuda":"I", "ahorro_cuota_mensual":1606.7586620762522, "ahorro_total":57843.31183474508, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":59000.0, "cuota":2950.0, "saldo":25046.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5755, "fecha_inicio":"2015-01-05", "tipo_deuda":"R", "ahorro_cuota_mensual":27995.99999999993, "ahorro_total":-27995.99999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":131100.0, "cuota":1000.0, "saldo":24391.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.814, "fecha_inicio":"2018-03-26", "tipo_deuda":"R", "ahorro_cuota_mensual":25390.999999999935, "ahorro_total":-25390.999999999935, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":415000.0, "cuota":15286.0, "saldo":375484.0, "tasa_externa":0.3185, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":39.0, "frecuencia_externa":"M", "avance":0.0952, "fecha_inicio":"2023-07-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-588.0634589149104, "ahorro_total":-28227.046027915698, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":30000.0, "cuota":400.0, "saldo":990.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.967, "fecha_inicio":"2013-07-01", "tipo_deuda":"R", "ahorro_cuota_mensual":1389.9999999999973, "ahorro_total":-1389.9999999999973, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":15100.0, "cuota":522.0, "saldo":96.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9936, "fecha_inicio":"2021-12-21", "tipo_deuda":"R", "ahorro_cuota_mensual":617.9999999999998, "ahorro_total":-617.9999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":28792.0, "cuota":1769.0, "saldo":20610.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2842, "fecha_inicio":"2016-04-05", "tipo_deuda":"R", "ahorro_cuota_mensual":22378.999999999945, "ahorro_total":-22378.999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 2352204, "monto_maximo_cliente": 867997.0, "cuota_externa_total": 24592.0, "capacidad_maxima_pago": 586213.0, "bursolnum": 7439208, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 14953.948852997342, "monto_max": 867997.0, "cuota_min": 148.2848081136287, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.2914, "kubo_score": "A2", "comision": 0.0417, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.2914], "comisiones": [0.0417], "kubo_scores": ['A2'], "deudas_buro": [ {"entidad": "CIA Q' OTORGA", "registro":8, "monto_otorgado":356776.0, "cuota":0.0, "saldo":169286.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.5255, "fecha_inicio":"2013-08-03", "tipo_deuda":"O", "ahorro_cuota_mensual":169285.9999999993, "ahorro_total":-169285.9999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":42675.0, "cuota":1878.0, "saldo":20079.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":38.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.5295, "fecha_inicio":"2022-01-26", "tipo_deuda":"I", "ahorro_cuota_mensual":229.4534837769495, "ahorro_total":8719.23238352408, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":50200.0, "cuota":2943.0, "saldo":18390.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6337, "fecha_inicio":"2022-09-29", "tipo_deuda":"I", "ahorro_cuota_mensual":250.63456150123966, "ahorro_total":6015.229476029752, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":9, "monto_otorgado":12000.0, "cuota":2500.0, "saldo":10830.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0975, "fecha_inicio":"2017-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":13329.999999999955, "ahorro_total":-13329.999999999955, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":39000.0, "cuota":2540.0, "saldo":28885.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2594, "fecha_inicio":"2005-09-01", "tipo_deuda":"R", "ahorro_cuota_mensual":31424.99999999988, "ahorro_total":-31424.99999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":28, "monto_otorgado":9999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2006-10-07", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":5, "monto_otorgado":35000.0, "cuota":2471.0, "saldo":30995.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1144, "fecha_inicio":"2006-09-14", "tipo_deuda":"R", "ahorro_cuota_mensual":33465.99999999987, "ahorro_total":-33465.99999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":9000.0, "cuota":450.0, "saldo":5746.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3616, "fecha_inicio":"2005-07-24", "tipo_deuda":"R", "ahorro_cuota_mensual":6195.999999999975, "ahorro_total":-6195.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":5000.0, "cuota":253.0, "saldo":2501.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4998, "fecha_inicio":"2012-04-09", "tipo_deuda":"R", "ahorro_cuota_mensual":2753.9999999999895, "ahorro_total":-2753.9999999999895, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":2, "monto_otorgado":213238.0, "cuota":0.0, "saldo":60363.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7169, "fecha_inicio":"2012-12-07", "tipo_deuda":"O", "ahorro_cuota_mensual":60362.999999999745, "ahorro_total":-60362.999999999745, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":12000.0, "cuota":-1.0, "saldo":9391.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2174, "fecha_inicio":"2017-11-06", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":550000.0, "cuota":14085.0, "saldo":540423.0, "tasa_externa":0.2313, "tasa_kubo":0.22, "numero_pagos_otorgado":72.0, "numero_pagos_restante":69.0, "frecuencia_externa":"M", "avance":0.0174, "fecha_inicio":"2024-01-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-906.4253813884698, "ahorro_total":-65262.62745996982, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 2371630, "monto_maximo_cliente": 139935.0, "cuota_externa_total": 27210.0, "capacidad_maxima_pago": 59999.0, "bursolnum": 7439210, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2164.828653666244, "monto_max": 139935.0, "cuota_min": 170.12097245160408, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.4818, "kubo_score": "B5", "comision": 0.046, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "FONDOS Y FIDEIC", "registro":16, "monto_otorgado":235954.0, "cuota":11798.0, "saldo":51714.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":40.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.7808, "fecha_inicio":"2015-08-26", "tipo_deuda":"R", "ahorro_cuota_mensual":9659.4198476293, "ahorro_total":386376.79390517203, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":13, "monto_otorgado":1298.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-04-12", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":21000.0, "cuota":1222.0, "saldo":13279.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":36.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.3677, "fecha_inicio":"2022-07-27", "tipo_deuda":"I", "ahorro_cuota_mensual":299.31004486451513, "ahorro_total":10775.161615122544, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":49000.0, "cuota":3445.0, "saldo":27469.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":24.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.4394, "fecha_inicio":"2022-12-16", "tipo_deuda":"I", "ahorro_cuota_mensual":636.9976107745451, "ahorro_total":15287.942658589083, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":1800.0, "cuota":1575.0, "saldo":1575.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.125, "fecha_inicio":"2023-03-20", "tipo_deuda":"O", "ahorro_cuota_mensual":3149.999999999996, "ahorro_total":-3149.999999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":22, "monto_otorgado":20000.0, "cuota":1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2013-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "OTRAS FINANCIERA", "registro":18, "monto_otorgado":0.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-1.0, "fecha_inicio":"2020-02-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":100000.0, "cuota":5391.0, "saldo":5391.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9461, "fecha_inicio":"2022-08-03", "tipo_deuda":"O", "ahorro_cuota_mensual":5023.766402053347, "ahorro_total":95451.56163901358, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":26, "monto_otorgado":4700.0, "cuota":1709.0, "saldo":3124.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3353, "fecha_inicio":"2023-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":56.21467074270049, "ahorro_total":168.64401222810147, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":14, "monto_otorgado":3000.0, "cuota":364.0, "saldo":2830.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0567, "fecha_inicio":"2022-02-14", "tipo_deuda":"R", "ahorro_cuota_mensual":3193.9999999999927, "ahorro_total":-3193.9999999999927, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":779.0, "cuota":290.0, "saldo":516.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3376, "fecha_inicio":"2024-02-18", "tipo_deuda":"I", "ahorro_cuota_mensual":16.059623086928468, "ahorro_total":48.178869260785405, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":797.0, "cuota":301.0, "saldo":536.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3275, "fecha_inicio":"2024-02-11", "tipo_deuda":"I", "ahorro_cuota_mensual":20.729806932326028, "ahorro_total":62.189420796978084, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":3000.0, "cuota":1236.0, "saldo":1099.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6337, "fecha_inicio":"2024-01-06", "tipo_deuda":"I", "ahorro_cuota_mensual":181.03064089959594, "ahorro_total":543.0919226987878, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":3000.0, "cuota":755.0, "saldo":2278.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2407, "fecha_inicio":"2023-12-24", "tipo_deuda":"I", "ahorro_cuota_mensual":206.26162374403384, "ahorro_total":1237.569742464203, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":57000.0, "cuota":2667.0, "saldo":42813.0, "tasa_externa":0.3825, "tasa_kubo":0.2818, "numero_pagos_otorgado":36.0, "numero_pagos_restante":23.0, "frecuencia_externa":"M", "avance":0.2489, "fecha_inicio":"2023-04-04", "tipo_deuda":"I", "ahorro_cuota_mensual":162.555836060827, "ahorro_total":5852.010098189772, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":45500.0, "cuota":3240.0, "saldo":44206.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0284, "fecha_inicio":"2019-07-03", "tipo_deuda":"R", "ahorro_cuota_mensual":47445.99999999989, "ahorro_total":-47445.99999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":15, "monto_otorgado":18232.0, "cuota":1.0, "saldo":1.0, "tasa_externa":-1.0, "tasa_kubo":0.2818, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9999, "fecha_inicio":"2021-08-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-800.0706315252457, "ahorro_total":-28802.542734908846, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 2417292, "monto_maximo_cliente": 180701.0, "cuota_externa_total": 25756.0, "capacidad_maxima_pago": 98866.0, "bursolnum": 7439212, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2560.7719869453163, "monto_max": 180701.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":66376.0, "cuota":3504.0, "saldo":49592.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":45.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.2529, "fecha_inicio":"2022-03-03", "tipo_deuda":"I", "ahorro_cuota_mensual":883.5556335192136, "ahorro_total":39760.003508364614, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":20000.0, "cuota":398.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-02-22", "tipo_deuda":"O", "ahorro_cuota_mensual":398.0, "ahorro_total":-398.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":275295.0, "cuota":7607.0, "saldo":270472.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":44.0, "frecuencia_externa":"M", "avance":0.0175, "fecha_inicio":"2023-12-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-2923.2416865589894, "ahorro_total":-140315.6009548315, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-04-02", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":84000.0, "cuota":5399.0, "saldo":75288.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1037, "fecha_inicio":"2023-01-19", "tipo_deuda":"R", "ahorro_cuota_mensual":80686.9999999998, "ahorro_total":-80686.9999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":4000.0, "cuota":5762.0, "saldo":5762.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.4405, "fecha_inicio":"2024-03-02", "tipo_deuda":"I", "ahorro_cuota_mensual":1649.3253333333432, "ahorro_total":1649.3253333333432, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":66272.0, "cuota":3085.0, "saldo":19180.0, "tasa_externa":0.3782, "tasa_kubo":0.2914, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7106, "fecha_inicio":"2021-09-27", "tipo_deuda":"I", "ahorro_cuota_mensual":131.86518386508487, "ahorro_total":4747.146619143055, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":38000.0, "cuota":1900.0, "saldo":35141.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0752, "fecha_inicio":"2019-09-12", "tipo_deuda":"R", "ahorro_cuota_mensual":37040.999999999905, "ahorro_total":-37040.999999999905, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-1.0, "fecha_inicio":"2024-02-01", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 2433653, "monto_maximo_cliente": 21803.0, "cuota_externa_total": 3187.0, "capacidad_maxima_pago": 19013.0, "bursolnum": 7439215, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 894.9272142949885, "monto_max": 21803.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 23.0, "plazo_min": 4, "tasa": 0.5668, "kubo_score": "C5", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":12000.0, "cuota":1419.0, "saldo":8251.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3124, "fecha_inicio":"2023-09-08", "tipo_deuda":"I", "ahorro_cuota_mensual":226.59617421670055, "ahorro_total":2719.1540906004066, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2020-07-23", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":7500.0, "cuota":375.0, "saldo":4538.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3949, "fecha_inicio":"2021-03-29", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":11000.0, "cuota":550.0, "saldo":2147.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8048, "fecha_inicio":"2024-01-30", "tipo_deuda":"R", "ahorro_cuota_mensual":2696.999999999994, "ahorro_total":-2696.999999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":15000.0, "cuota":1426.0, "saldo":1426.0, "tasa_externa":0.2539, "tasa_kubo":0.2914, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9049, "fecha_inicio":"2023-03-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-64.5047822291242, "ahorro_total":-774.0573867494904, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":4000.0, "cuota":50.0, "saldo":118.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9705, "fecha_inicio":"2023-10-07", "tipo_deuda":"R", "ahorro_cuota_mensual":167.99999999999966, "ahorro_total":-167.99999999999966, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 2696976, "monto_maximo_cliente": 284982.0, "cuota_externa_total": 29232.0, "capacidad_maxima_pago": 29868.0, "bursolnum": 7439250, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1169.5751965916932, "monto_max": 284982.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 22.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":40000.0, "cuota":3209.0, "saldo":39670.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":24.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.0082, "fecha_inicio":"2024-01-23", "tipo_deuda":"I", "ahorro_cuota_mensual":25.795009600895355, "ahorro_total":619.0802304214885, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":10000.0, "cuota":539.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-08-21", "tipo_deuda":"R", "ahorro_cuota_mensual":539.0, "ahorro_total":-539.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":19500.0, "cuota":2764.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-01-23", "tipo_deuda":"R", "ahorro_cuota_mensual":2764.0, "ahorro_total":-2764.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":14100.0, "cuota":1687.0, "saldo":11368.0, "tasa_externa":0.7368, "tasa_kubo":0.6193, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1938, "fecha_inicio":"2021-08-20", "tipo_deuda":"I", "ahorro_cuota_mensual":6.432245599739872, "ahorro_total":77.18694719687846, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":16000.0, "cuota":800.0, "saldo":8600.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4625, "fecha_inicio":"2022-03-09", "tipo_deuda":"R", "ahorro_cuota_mensual":9400.000000000002, "ahorro_total":-9400.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":17200.0, "cuota":1786.0, "saldo":1786.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8962, "fecha_inicio":"2023-05-15", "tipo_deuda":"R", "ahorro_cuota_mensual":3572.0, "ahorro_total":-3572.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":23819.0, "cuota":1509.0, "saldo":9068.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6193, "fecha_inicio":"2023-03-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-688.6219230784272, "ahorro_total":-12395.19461541169, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":15000.0, "cuota":2055.0, "saldo":13840.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0773, "fecha_inicio":"2023-07-13", "tipo_deuda":"R", "ahorro_cuota_mensual":15895.000000000002, "ahorro_total":-15895.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":180000.0, "cuota":17380.0, "saldo":150265.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.1652, "fecha_inicio":"2023-06-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":39740.0, "cuota":1987.0, "saldo":30677.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2281, "fecha_inicio":"2021-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":32664.000000000007, "ahorro_total":-32664.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":2, "monto_otorgado":8600.0, "cuota":-1.0, "saldo":11718.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.3626, "fecha_inicio":"2024-01-19", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":2800.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-11-01", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":7000.0, "cuota":350.0, "saldo":442.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9369, "fecha_inicio":"2021-01-26", "tipo_deuda":"R", "ahorro_cuota_mensual":792.0000000000001, "ahorro_total":-792.0000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 2769844, "monto_maximo_cliente": 97559.0, "cuota_externa_total": 6547.0, "capacidad_maxima_pago": 76494.0, "bursolnum": 7439258, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1973.2120964962958, "monto_max": 97559.0, "cuota_min": 168.08525285014431, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.6722, "kubo_score": "D4", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":11, "monto_otorgado":3000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-08-08", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":13, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2015-07-02", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":17400.0, "cuota":1706.0, "saldo":3135.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8198, "fecha_inicio":"2022-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":475.9081412845642, "ahorro_total":8566.346543122156, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-12-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":528.0, "cuota":202.0, "saldo":551.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0436, "fecha_inicio":"2024-02-08", "tipo_deuda":"I", "ahorro_cuota_mensual":16.519299735855043, "ahorro_total":49.55789920756513, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":1163.0, "cuota":432.0, "saldo":418.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6406, "fecha_inicio":"2023-12-23", "tipo_deuda":"I", "ahorro_cuota_mensual":23.450654531817122, "ahorro_total":70.35196359545137, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":32346.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-10-05", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":12500.0, "cuota":1.0, "saldo":5891.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5287, "fecha_inicio":"2023-04-11", "tipo_deuda":"R", "ahorro_cuota_mensual":5891.999999999965, "ahorro_total":-5891.999999999965, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":35500.0, "cuota":1775.0, "saldo":19879.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.44, "fecha_inicio":"2017-10-21", "tipo_deuda":"R", "ahorro_cuota_mensual":21653.999999999884, "ahorro_total":-21653.999999999884, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":16500.0, "cuota":825.0, "saldo":14557.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1178, "fecha_inicio":"2021-10-14", "tipo_deuda":"R", "ahorro_cuota_mensual":15381.999999999916, "ahorro_total":-15381.999999999916, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":53041.0, "cuota":2474.0, "saldo":48879.0, "tasa_externa":0.3919, "tasa_kubo":0.2762, "numero_pagos_otorgado":37.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":0.0785, "fecha_inicio":"2023-09-26", "tipo_deuda":"I", "ahorro_cuota_mensual":200.05559187150402, "ahorro_total":7402.056899245648, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":2500.0, "cuota":554.0, "saldo":2281.0, "tasa_externa":-1.0, "tasa_kubo":0.2762, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0876, "fecha_inicio":"2024-01-09", "tipo_deuda":"I", "ahorro_cuota_mensual":97.5422184780009, "ahorro_total":585.2533108680054, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 2776466, "monto_maximo_cliente": 125700.0, "cuota_externa_total": 12413.0, "capacidad_maxima_pago": 73180.0, "bursolnum": 7439259, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1968.2821328186785, "monto_max": 125700.0, "cuota_min": 149.243287010584, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5668, "kubo_score": "C5", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "HIPOTECAGOBIERNO", "registro":10, "monto_otorgado":376362.0, "cuota":3755.0, "saldo":296059.0, "tasa_externa":-1.0, "tasa_kubo":0.2228, "numero_pagos_otorgado":360.0, "numero_pagos_restante":280.0, "frecuencia_externa":"M", "avance":0.2134, "fecha_inicio":"2017-08-30", "tipo_deuda":"M", "ahorro_cuota_mensual":-2624.2947133265343, "ahorro_total":-944746.0967975523, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":35000.0, "cuota":2270.0, "saldo":35094.0, "tasa_externa":-1.0, "tasa_kubo":0.2228, "numero_pagos_otorgado":36.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":-0.0027, "fecha_inicio":"2024-01-22", "tipo_deuda":"I", "ahorro_cuota_mensual":862.7202953408669, "ahorro_total":31057.930632271207, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":4000.0, "cuota":200.0, "saldo":1480.0, "tasa_externa":-1.0, "tasa_kubo":0.2228, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.63, "fecha_inicio":"2019-02-19", "tipo_deuda":"R", "ahorro_cuota_mensual":1680.0000000000011, "ahorro_total":-1680.0000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":1300.0, "cuota":157.0, "saldo":797.0, "tasa_externa":-1.0, "tasa_kubo":0.2228, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3869, "fecha_inicio":"2023-08-12", "tipo_deuda":"I", "ahorro_cuota_mensual":32.90897484653736, "ahorro_total":394.90769815844834, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":18500.0, "cuota":925.0, "saldo":12510.0, "tasa_externa":-1.0, "tasa_kubo":0.2228, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3238, "fecha_inicio":"2022-05-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":15700.0, "cuota":2010.0, "saldo":1531.0, "tasa_externa":-1.0, "tasa_kubo":0.2228, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9025, "fecha_inicio":"2023-12-27", "tipo_deuda":"R", "ahorro_cuota_mensual":3541.000000000001, "ahorro_total":-3541.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":13200.0, "cuota":660.0, "saldo":5189.0, "tasa_externa":-1.0, "tasa_kubo":0.2228, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6069, "fecha_inicio":"2022-03-07", "tipo_deuda":"R", "ahorro_cuota_mensual":5849.000000000004, "ahorro_total":-5849.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":65394.0, "cuota":2469.0, "saldo":55756.0, "tasa_externa":0.3903, "tasa_kubo":0.2228, "numero_pagos_otorgado":60.0, "numero_pagos_restante":39.0, "frecuencia_externa":"M", "avance":0.1474, "fecha_inicio":"2022-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":517.0768978459739, "ahorro_total":31024.613870758436, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":35970.0, "cuota":910.0, "saldo":34093.0, "tasa_externa":-1.0, "tasa_kubo":0.2228, "numero_pagos_otorgado":144.0, "numero_pagos_restante":59.0, "frecuencia_externa":"S", "avance":0.0522, "fecha_inicio":"2023-03-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-77.6597511168626, "ahorro_total":-5591.502080414107, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":2326.0, "cuota":282.0, "saldo":1624.0, "tasa_externa":-1.0, "tasa_kubo":0.2228, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3018, "fecha_inicio":"2023-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":59.972519610035334, "ahorro_total":719.670235320424, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 2871236, "monto_maximo_cliente": 346145.0, "cuota_externa_total": 34673.0, "capacidad_maxima_pago": 47657.0, "bursolnum": 7439278, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2090.5199217582876, "monto_max": 346145.0, "cuota_min": 167.14383956263904, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5486, "kubo_score": "C3", "comision": 0.0476, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":13, "monto_otorgado":5800.0, "cuota":370.0, "saldo":2256.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.611, "fecha_inicio":"2022-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":2625.999999999998, "ahorro_total":-2625.999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "HIPOTECARIA", "registro":47, "monto_otorgado":296539.0, "cuota":2219.0, "saldo":183061.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":360.0, "numero_pagos_restante":52.0, "frecuencia_externa":"M", "avance":0.3827, "fecha_inicio":"1998-08-18", "tipo_deuda":"M", "ahorro_cuota_mensual":-2622.998861384078, "ahorro_total":-944279.590098268, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":18, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":947.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-11-20", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":17, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":869.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-06-08", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":16, "monto_otorgado":73000.0, "cuota":3894.0, "saldo":3894.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9467, "fecha_inicio":"2021-03-24", "tipo_deuda":"I", "ahorro_cuota_mensual":725.1522429168913, "ahorro_total":26105.480745008084, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":78000.0, "cuota":4420.0, "saldo":74251.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":48.0, "numero_pagos_restante":38.0, "frecuencia_externa":"M", "avance":0.0481, "fecha_inicio":"2023-06-30", "tipo_deuda":"I", "ahorro_cuota_mensual":1532.1594857922182, "ahorro_total":73543.65531802647, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":14, "monto_otorgado":12958.0, "cuota":12709.0, "saldo":12709.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.0192, "fecha_inicio":"2024-02-22", "tipo_deuda":"O", "ahorro_cuota_mensual":25417.99999999999, "ahorro_total":-25417.99999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":1075.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-09-23", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":12, "monto_otorgado":5500.0, "cuota":400.0, "saldo":1835.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6664, "fecha_inicio":"2022-09-27", "tipo_deuda":"R", "ahorro_cuota_mensual":2234.999999999998, "ahorro_total":-2234.999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":19, "monto_otorgado":46000.0, "cuota":61.0, "saldo":231.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.995, "fecha_inicio":"2018-12-15", "tipo_deuda":"R", "ahorro_cuota_mensual":291.9999999999998, "ahorro_total":-291.9999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":62100.0, "cuota":2591.0, "saldo":47872.0, "tasa_externa":0.4003, "tasa_kubo":0.2736, "numero_pagos_otorgado":48.0, "numero_pagos_restante":29.0, "frecuencia_externa":"M", "avance":0.2291, "fecha_inicio":"2022-09-12", "tipo_deuda":"I", "ahorro_cuota_mensual":291.8346675345738, "ahorro_total":14008.064041659542, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":13000.0, "cuota":14.0, "saldo":7392.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4314, "fecha_inicio":"2019-10-11", "tipo_deuda":"R", "ahorro_cuota_mensual":7405.999999999994, "ahorro_total":-7405.999999999994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":43648.0, "cuota":1364.0, "saldo":27280.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":128.0, "numero_pagos_restante":20.0, "frecuencia_externa":"W", "avance":0.375, "fecha_inicio":"2023-04-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-674.6005391158128, "ahorro_total":-21587.21725170601, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":133364.0, "cuota":3464.0, "saldo":91519.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":154.0, "numero_pagos_restante":26.0, "frecuencia_externa":"W", "avance":0.3138, "fecha_inicio":"2023-04-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-2142.2928472012145, "ahorro_total":-81407.12819364615, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":3080.0, "cuota":80.0, "saldo":2120.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":154.0, "numero_pagos_restante":26.0, "frecuencia_externa":"W", "avance":0.3117, "fecha_inicio":"2023-04-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-49.475585385709365, "ahorro_total":-1880.072244656956, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":15900.0, "cuota":795.0, "saldo":11123.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3004, "fecha_inicio":"2021-06-17", "tipo_deuda":"R", "ahorro_cuota_mensual":11917.999999999989, "ahorro_total":-11917.999999999989, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":57596.0, "cuota":1496.0, "saldo":56100.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":154.0, "numero_pagos_restante":36.0, "frecuencia_externa":"W", "avance":0.026, "fecha_inicio":"2024-02-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-925.1934467127649, "ahorro_total":-35157.350975085064, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":50600.0, "cuota":2530.0, "saldo":3416.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9325, "fecha_inicio":"2022-09-12", "tipo_deuda":"R", "ahorro_cuota_mensual":5945.999999999996, "ahorro_total":-5945.999999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":3080.0, "cuota":80.0, "saldo":3000.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":154.0, "numero_pagos_restante":36.0, "frecuencia_externa":"W", "avance":0.026, "fecha_inicio":"2024-02-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-49.475585385709365, "ahorro_total":-1880.072244656956, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":17024.0, "cuota":532.0, "saldo":11438.0, "tasa_externa":-1.0, "tasa_kubo":0.2736, "numero_pagos_otorgado":128.0, "numero_pagos_restante":21.0, "frecuencia_externa":"W", "avance":0.3281, "fecha_inicio":"2023-06-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-263.1139932621792, "ahorro_total":-8419.647784389734, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3002968, "monto_maximo_cliente": 85285.0, "cuota_externa_total": 7616.0, "capacidad_maxima_pago": 48952.0, "bursolnum": 7439315, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1836.5609341023332, "monto_max": 85285.0, "cuota_min": 159.69948534503877, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.5668, "kubo_score": "C5", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":2, "monto_otorgado":15000.0, "cuota":1195.0, "saldo":14741.0, "tasa_externa":-1.0, "tasa_kubo":0.2528, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0173, "fecha_inicio":"2018-12-14", "tipo_deuda":"R", "ahorro_cuota_mensual":15936.000000000056, "ahorro_total":-15936.000000000056, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":21000.0, "cuota":1788.0, "saldo":18976.0, "tasa_externa":-1.0, "tasa_kubo":0.2528, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0964, "fecha_inicio":"2010-12-16", "tipo_deuda":"R", "ahorro_cuota_mensual":20764.000000000073, "ahorro_total":-20764.000000000073, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":51568.0, "cuota":2337.0, "saldo":23798.0, "tasa_externa":0.3687, "tasa_kubo":0.2528, "numero_pagos_otorgado":37.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.5385, "fecha_inicio":"2022-02-01", "tipo_deuda":"I", "ahorro_cuota_mensual":203.6302277400564, "ahorro_total":7534.318426382087, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVICIOS", "registro":1, "monto_otorgado":844.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2528, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-08-30", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":39000.0, "cuota":2296.0, "saldo":4308.0, "tasa_externa":-1.0, "tasa_kubo":0.2528, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8895, "fecha_inicio":"2021-04-26", "tipo_deuda":"I", "ahorro_cuota_mensual":654.7784723083482, "ahorro_total":23572.025003100534, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3052806, "monto_maximo_cliente": 205933.0, "cuota_externa_total": 27981.0, "capacidad_maxima_pago": 80257.0, "bursolnum": 7439333, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4238.020125483156, "monto_max": 205933.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 44.0, "plazo_min": 4, "tasa": 0.4818, "kubo_score": "B5", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":9, "monto_otorgado":17628.0, "cuota":3093.0, "saldo":17317.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0176, "fecha_inicio":"2020-03-17", "tipo_deuda":"R", "ahorro_cuota_mensual":20410.000000000036, "ahorro_total":-20410.000000000036, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":180000.0, "cuota":13090.0, "saldo":117229.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":24.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.3487, "fecha_inicio":"2023-02-20", "tipo_deuda":"I", "ahorro_cuota_mensual":476.52680550779587, "ahorro_total":11436.6433321871, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":19500.0, "cuota":1245.0, "saldo":4334.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7777, "fecha_inicio":"2012-03-10", "tipo_deuda":"R", "ahorro_cuota_mensual":5579.000000000009, "ahorro_total":-5579.000000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":78717.0, "cuota":4740.0, "saldo":7088.0, "tasa_externa":0.6091, "tasa_kubo":0.4818, "numero_pagos_otorgado":72.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.91, "fecha_inicio":"2021-05-13", "tipo_deuda":"I", "ahorro_cuota_mensual":190.195501525498, "ahorro_total":6847.038054917928, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":40000.0, "cuota":3307.0, "saldo":39597.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0101, "fecha_inicio":"2022-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":42904.00000000009, "ahorro_total":-42904.00000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":21000.0, "cuota":2506.0, "saldo":10739.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4886, "fecha_inicio":"2011-08-03", "tipo_deuda":"R", "ahorro_cuota_mensual":13245.000000000022, "ahorro_total":-13245.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":61000.0, "cuota":3000.0, "saldo":55229.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0946, "fecha_inicio":"2018-04-17", "tipo_deuda":"R", "ahorro_cuota_mensual":58229.00000000012, "ahorro_total":-58229.00000000012, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3190170, "monto_maximo_cliente": 341101.0, "cuota_externa_total": 34548.0, "capacidad_maxima_pago": 137552.0, "bursolnum": 7439387, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7745.528415344514, "monto_max": 341101.0, "cuota_min": 269.2747621622814, "monto_min": 5000, "plazo_max": 52.0, "plazo_min": 4, "tasa": 0.5292, "kubo_score": "C1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":1048.0, "cuota":214.0, "saldo":407.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6116, "fecha_inicio":"2023-10-13", "tipo_deuda":"I", "ahorro_cuota_mensual":6.761753202789862, "ahorro_total":40.57051921673917, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":26, "monto_otorgado":63000.0, "cuota":3322.0, "saldo":12002.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8095, "fecha_inicio":"2021-06-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-542.0784543044992, "ahorro_total":-19514.824354961973, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":49, "monto_otorgado":5500.0, "cuota":1160.0, "saldo":2194.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6011, "fecha_inicio":"2022-10-04", "tipo_deuda":"I", "ahorro_cuota_mensual":72.39469715204609, "ahorro_total":434.36818291227655, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":32, "monto_otorgado":25000.0, "cuota":2460.0, "saldo":7024.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.719, "fecha_inicio":"2023-03-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-379.05480487324303, "ahorro_total":-4548.657658478916, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":27, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2018-06-29", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":28, "monto_otorgado":10000.0, "cuota":500.0, "saldo":6711.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3289, "fecha_inicio":"2022-06-13", "tipo_deuda":"R", "ahorro_cuota_mensual":7211.000000000003, "ahorro_total":-7211.000000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":25, "monto_otorgado":12700.0, "cuota":748.0, "saldo":7992.0, "tasa_externa":0.6918, "tasa_kubo":0.5292, "numero_pagos_otorgado":120.0, "numero_pagos_restante":27.0, "frecuencia_externa":"S", "avance":0.3707, "fecha_inicio":"2021-08-06", "tipo_deuda":"I", "ahorro_cuota_mensual":64.04210410780524, "ahorro_total":3842.5262464683146, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":24, "monto_otorgado":127400.0, "cuota":7512.0, "saldo":97201.0, "tasa_externa":0.6927, "tasa_kubo":0.5292, "numero_pagos_otorgado":120.0, "numero_pagos_restante":36.0, "frecuencia_externa":"S", "avance":0.237, "fecha_inicio":"2022-04-28", "tipo_deuda":"I", "ahorro_cuota_mensual":650.8790601050705, "ahorro_total":39052.743606304226, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":23, "monto_otorgado":15000.0, "cuota":7771.0, "saldo":7771.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4819, "fecha_inicio":"2022-04-07", "tipo_deuda":"R", "ahorro_cuota_mensual":15542.000000000004, "ahorro_total":-15542.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":21, "monto_otorgado":76300.0, "cuota":3815.0, "saldo":32496.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5741, "fecha_inicio":"2023-10-05", "tipo_deuda":"R", "ahorro_cuota_mensual":36311.000000000015, "ahorro_total":-36311.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":20, "monto_otorgado":1115.0, "cuota":226.0, "saldo":221.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8018, "fecha_inicio":"2023-09-17", "tipo_deuda":"I", "ahorro_cuota_mensual":5.512743149914826, "ahorro_total":33.076458899488955, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":19, "monto_otorgado":1376.0, "cuota":275.0, "saldo":269.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8045, "fecha_inicio":"2023-09-24", "tipo_deuda":"I", "ahorro_cuota_mensual":2.900927869311886, "ahorro_total":17.405567215871315, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":2448.0, "cuota":354.0, "saldo":1541.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3705, "fecha_inicio":"2023-10-25", "tipo_deuda":"I", "ahorro_cuota_mensual":7.81552043079472, "ahorro_total":70.33968387715248, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":3000.0, "cuota":296.0, "saldo":348.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":23.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.884, "fecha_inicio":"2022-05-11", "tipo_deuda":"R", "ahorro_cuota_mensual":269.91853997678163, "ahorro_total":6208.126419465978, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":759.0, "cuota":161.0, "saldo":437.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4242, "fecha_inicio":"2023-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":10.910468206982358, "ahorro_total":65.46280924189415, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":873.0, "cuota":184.0, "saldo":643.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2635, "fecha_inicio":"2023-12-20", "tipo_deuda":"I", "ahorro_cuota_mensual":11.367376475224773, "ahorro_total":68.20425885134864, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":735.0, "cuota":145.0, "saldo":737.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0027, "fecha_inicio":"2024-02-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-0.3436177442265773, "ahorro_total":-2.061706465359464, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":910.0, "cuota":359.0, "saldo":976.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0725, "fecha_inicio":"2024-02-01", "tipo_deuda":"I", "ahorro_cuota_mensual":24.11612930799936, "ahorro_total":72.34838792399808, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":362.0, "cuota":143.0, "saldo":268.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2597, "fecha_inicio":"2024-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":9.78246023021515, "ahorro_total":29.34738069064545, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":825.0, "cuota":325.0, "saldo":883.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0703, "fecha_inicio":"2024-02-02", "tipo_deuda":"I", "ahorro_cuota_mensual":21.39649085615332, "ahorro_total":64.18947256845996, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":227.0, "cuota":89.0, "saldo":168.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2599, "fecha_inicio":"2024-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":5.463034453753707, "ahorro_total":16.38910336126112, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":961.0, "cuota":381.0, "saldo":715.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.256, "fecha_inicio":"2024-01-01", "tipo_deuda":"I", "ahorro_cuota_mensual":27.347912379107015, "ahorro_total":82.04373713732105, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":337.0, "cuota":127.0, "saldo":345.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0237, "fecha_inicio":"2024-02-20", "tipo_deuda":"I", "ahorro_cuota_mensual":2.982566567907469, "ahorro_total":8.947699703722407, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":10000.0, "cuota":540.0, "saldo":18528.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":43.0, "numero_pagos_restante":11.0, "frecuencia_externa":"S", "avance":-0.8528, "fecha_inicio":"2023-05-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-227.73214579004014, "ahorro_total":-5010.107207380883, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":30000.0, "cuota":1660.0, "saldo":57336.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":43.0, "numero_pagos_restante":13.0, "frecuencia_externa":"S", "avance":-0.9112, "fecha_inicio":"2023-08-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-643.1964373701207, "ahorro_total":-14150.321622142656, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":70000.0, "cuota":3876.0, "saldo":138580.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":43.0, "numero_pagos_restante":19.0, "frecuencia_externa":"S", "avance":-0.9797, "fecha_inicio":"2024-02-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-1498.1250205302822, "ahorro_total":-32958.75045166621, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":1199.0, "cuota":255.0, "saldo":693.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.422, "fecha_inicio":"2023-11-16", "tipo_deuda":"I", "ahorro_cuota_mensual":17.902043979146043, "ahorro_total":107.41226387487626, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3332202, "monto_maximo_cliente": 325284.0, "cuota_externa_total": 28182.0, "capacidad_maxima_pago": 219949.0, "bursolnum": 7439443, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7932.571742423747, "monto_max": 325284.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":50000.0, "cuota":3094.0, "saldo":46214.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.0757, "fecha_inicio":"2023-07-26", "tipo_deuda":"I", "ahorro_cuota_mensual":726.011675047012, "ahorro_total":26136.42030169243, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":91000.0, "cuota":5815.0, "saldo":85364.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":33.0, "numero_pagos_restante":23.0, "frecuencia_externa":"M", "avance":0.0619, "fecha_inicio":"2023-07-03", "tipo_deuda":"I", "ahorro_cuota_mensual":1293.7409739580107, "ahorro_total":42693.452140614354, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2005-10-13", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":40000.0, "cuota":2543.0, "saldo":38950.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":36.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.0262, "fecha_inicio":"2023-11-27", "tipo_deuda":"I", "ahorro_cuota_mensual":648.6093400376094, "ahorro_total":23349.93624135394, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":62046.0, "cuota":3636.0, "saldo":46892.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":71.0, "numero_pagos_restante":27.0, "frecuencia_externa":"S", "avance":0.2442, "fecha_inicio":"2023-08-01", "tipo_deuda":"I", "ahorro_cuota_mensual":697.515927799338, "ahorro_total":25110.573400776168, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":41364.0, "cuota":2424.0, "saldo":33009.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":71.0, "numero_pagos_restante":29.0, "frecuencia_externa":"S", "avance":0.202, "fecha_inicio":"2023-09-12", "tipo_deuda":"I", "ahorro_cuota_mensual":465.01061853289207, "ahorro_total":16740.382267184115, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":52210.0, "cuota":2610.0, "saldo":17874.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6577, "fecha_inicio":"2012-01-25", "tipo_deuda":"R", "ahorro_cuota_mensual":20483.999999999953, "ahorro_total":-20483.999999999953, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":204000.0, "cuota":8641.0, "saldo":192245.0, "tasa_externa":0.4106, "tasa_kubo":0.3337, "numero_pagos_otorgado":48.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.0576, "fecha_inicio":"2023-10-12", "tipo_deuda":"I", "ahorro_cuota_mensual":227.5012028382771, "ahorro_total":10920.0577362373, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3334267, "monto_maximo_cliente": 238332.0, "cuota_externa_total": 16380.0, "capacidad_maxima_pago": 57628.0, "bursolnum": 7439444, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1503.586666356246, "monto_max": 238332.0, "cuota_min": 168.0490006105383, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.5391, "kubo_score": "C2", "comision": 0.0471, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":1318.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-04-29", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":10, "monto_otorgado":875.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-04-29", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":70000.0, "cuota":3772.0, "saldo":20039.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7137, "fecha_inicio":"2021-08-13", "tipo_deuda":"I", "ahorro_cuota_mensual":722.1192507701217, "ahorro_total":25996.29302772438, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":3, "monto_otorgado":136635.0, "cuota":4427.0, "saldo":94057.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":48.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.3116, "fecha_inicio":"2022-07-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-655.1091538355686, "ahorro_total":-31445.23938410729, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":1, "monto_otorgado":12990.0, "cuota":650.0, "saldo":9351.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":312.0, "numero_pagos_restante":218.0, "frecuencia_externa":"Z", "avance":0.2801, "fecha_inicio":"2016-06-14", "tipo_deuda":"R", "ahorro_cuota_mensual":400.35758425954003, "ahorro_total":124911.5662889765, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":12, "monto_otorgado":90995.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"S", "avance":1.0, "fecha_inicio":"2018-09-18", "tipo_deuda":"I", "ahorro_cuota_mensual":90994.99999999962, "ahorro_total":-90994.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":40000.0, "cuota":2006.0, "saldo":36491.0, "tasa_externa":0.4406, "tasa_kubo":0.2761, "numero_pagos_otorgado":36.0, "numero_pagos_restante":29.0, "frecuencia_externa":"M", "avance":0.0877, "fecha_inicio":"2023-09-29", "tipo_deuda":"I", "ahorro_cuota_mensual":263.2110004400695, "ahorro_total":9475.5960158425, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":11673.0, "cuota":1000.0, "saldo":6369.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4544, "fecha_inicio":"2010-04-26", "tipo_deuda":"R", "ahorro_cuota_mensual":7368.999999999974, "ahorro_total":-7368.999999999974, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":104500.0, "cuota":5225.0, "saldo":21645.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7929, "fecha_inicio":"2012-01-01", "tipo_deuda":"R", "ahorro_cuota_mensual":26869.99999999991, "ahorro_total":-26869.99999999991, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":77400.0, "cuota":968.0, "saldo":2236.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9711, "fecha_inicio":"2023-07-31", "tipo_deuda":"R", "ahorro_cuota_mensual":3203.999999999991, "ahorro_total":-3203.999999999991, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":84000.0, "cuota":4200.0, "saldo":22087.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7371, "fecha_inicio":"2012-08-01", "tipo_deuda":"R", "ahorro_cuota_mensual":26286.99999999991, "ahorro_total":-26286.99999999991, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":55000.0, "cuota":1907.0, "saldo":19481.0, "tasa_externa":-1.0, "tasa_kubo":0.2761, "numero_pagos_otorgado":36.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.6458, "fecha_inicio":"2022-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-489.33487439490455, "ahorro_total":-17616.055478216564, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3590341, "monto_maximo_cliente": 369159.0, "cuota_externa_total": 24466.0, "capacidad_maxima_pago": 95534.0, "bursolnum": 6203346, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 6310.318696733804, "monto_max": 369159.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 38.0, "plazo_min": 4, "tasa": 0.5951, "kubo_score": "D2", "comision": -0.01, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": -1, "comisiones": -1, "kubo_scores": -1, "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":1816.0, "cuota":908.0, "saldo":1135.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":8.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.375, "fecha_inicio":"2023-03-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-75.28817492743553, "ahorro_total":-150.57634985487107, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":761.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-08-09", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":21011.0, "cuota":1352.0, "saldo":20237.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":36.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.0368, "fecha_inicio":"2022-08-31", "tipo_deuda":"I", "ahorro_cuota_mensual":3.099050625624386, "ahorro_total":111.5658225224779, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "MICROFINANCIERA", "registro":104, "monto_otorgado":11000.0, "cuota":620.0, "saldo":311.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.9717, "fecha_inicio":"2018-10-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-654.8363258558547, "ahorro_total":-7858.035910270257, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":19500.0, "cuota":975.0, "saldo":19436.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0033, "fecha_inicio":"2023-01-13", "tipo_deuda":"R", "ahorro_cuota_mensual":20411.000000000007, "ahorro_total":-20411.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":55000.0, "cuota":4185.0, "saldo":55513.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":24.0, "numero_pagos_restante":12.0, "frecuencia_externa":"M", "avance":-0.0093, "fecha_inicio":"2023-04-24", "tipo_deuda":"I", "ahorro_cuota_mensual":11.327015086970277, "ahorro_total":271.84836208728666, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":19900.0, "cuota":995.0, "saldo":19246.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0329, "fecha_inicio":"2019-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":20241.000000000004, "ahorro_total":-20241.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":70000.0, "cuota":8748.0, "saldo":39263.0, "tasa_externa":1.4207, "tasa_kubo":0.5668, "numero_pagos_otorgado":48.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.4391, "fecha_inicio":"2022-03-08", "tipo_deuda":"I", "ahorro_cuota_mensual":3436.0525646561437, "ahorro_total":82465.26155174745, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":196497.0, "cuota":4093.0, "saldo":151466.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":37.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.2292, "fecha_inicio":"2022-05-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-8410.522715927074, "ahorro_total":-311189.3404893018, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":30000.0, "cuota":2212.0, "saldo":30399.0, "tasa_externa":0.8921, "tasa_kubo":0.5668, "numero_pagos_otorgado":144.0, "numero_pagos_restante":59.0, "frecuencia_externa":"S", "avance":-0.0133, "fecha_inicio":"2023-03-28", "tipo_deuda":"I", "ahorro_cuota_mensual":532.1983858143121, "ahorro_total":38318.28377863047, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":21164.0, "cuota":1628.0, "saldo":10435.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":52.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.5069, "fecha_inicio":"2022-11-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-690.4767827836872, "ahorro_total":-8976.198176187934, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3636540, "monto_maximo_cliente": 86445.0, "cuota_externa_total": 8027.0, "capacidad_maxima_pago": 31573.0, "bursolnum": 7439538, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3124.003761660951, "monto_max": 86445.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 16.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":909.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-09-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":39000.0, "cuota":2452.0, "saldo":18740.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":36.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.5195, "fecha_inicio":"2021-12-23", "tipo_deuda":"I", "ahorro_cuota_mensual":-211.13048186121387, "ahorro_total":-7600.697347003699, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":7000.0, "cuota":416.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-12-12", "tipo_deuda":"R", "ahorro_cuota_mensual":416.0, "ahorro_total":-416.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":31600.0, "cuota":3749.0, "saldo":27454.0, "tasa_externa":0.7181, "tasa_kubo":0.6193, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1312, "fecha_inicio":"2022-05-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-17.378797095618665, "ahorro_total":-208.54556514742399, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":18200.0, "cuota":910.0, "saldo":10884.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.402, "fecha_inicio":"2020-12-24", "tipo_deuda":"R", "ahorro_cuota_mensual":11794.000000000002, "ahorro_total":-11794.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":3000.0, "cuota":1232.0, "saldo":3728.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.2427, "fecha_inicio":"2021-12-08", "tipo_deuda":"R", "ahorro_cuota_mensual":4960.000000000001, "ahorro_total":-4960.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":43100.0, "cuota":1200.0, "saldo":40233.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0665, "fecha_inicio":"2021-08-27", "tipo_deuda":"R", "ahorro_cuota_mensual":41433.00000000001, "ahorro_total":-41433.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":4000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-07-04", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":4800.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-05-18", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3651682, "monto_maximo_cliente": 104739.0, "cuota_externa_total": 17674.0, "capacidad_maxima_pago": 47326.0, "bursolnum": 7439543, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1196.3159082397874, "monto_max": 104739.0, "cuota_min": 148.2848081136287, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5292, "kubo_score": "C1", "comision": 0.0466, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":17, "monto_otorgado":148333.0, "cuota":4252.0, "saldo":78550.0, "tasa_externa":0.2415, "tasa_kubo":0.22, "numero_pagos_otorgado":60.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4704, "fecha_inicio":"2011-09-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-147.10608838377811, "ahorro_total":-8826.365303026687, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":18, "monto_otorgado":120253.0, "cuota":3247.0, "saldo":80979.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":48.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3266, "fecha_inicio":"2013-06-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-775.1999875927222, "ahorro_total":-37209.599404450666, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":741.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-04-16", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":15000.0, "cuota":1007.0, "saldo":8460.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":27.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.436, "fecha_inicio":"2022-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":271.0342970202413, "ahorro_total":7317.926019546515, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":44700.0, "cuota":3504.0, "saldo":26222.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.4134, "fecha_inicio":"2021-11-16", "tipo_deuda":"I", "ahorro_cuota_mensual":-19561.465476433867, "ahorro_total":-39122.93095286773, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":20000.0, "cuota":1644.0, "saldo":9437.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":5.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.5282, "fecha_inicio":"2021-06-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-8676.118781402178, "ahorro_total":-17352.237562804356, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":24700.0, "cuota":988.0, "saldo":1642.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":100.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.9335, "fecha_inicio":"2022-06-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-296.03578540133003, "ahorro_total":-7400.894635033251, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":40000.0, "cuota":1068.0, "saldo":21158.0, "tasa_externa":0.2065, "tasa_kubo":0.22, "numero_pagos_otorgado":60.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.471, "fecha_inicio":"2021-04-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-118.27846490902971, "ahorro_total":-7096.7078945417825, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":24000.0, "cuota":1200.0, "saldo":7793.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6753, "fecha_inicio":"2012-05-01", "tipo_deuda":"R", "ahorro_cuota_mensual":8992.999999999967, "ahorro_total":-8992.999999999967, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":2000.0, "cuota":80.0, "saldo":140.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":100.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.93, "fecha_inicio":"2022-06-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-23.97050893937896, "ahorro_total":-599.262723484474, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":30000.0, "cuota":1472.0, "saldo":23551.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":24.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.215, "fecha_inicio":"2023-09-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-136.9833297801356, "ahorro_total":-3287.599914723254, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":246.0, "cuota":12.0, "saldo":3.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":82.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.9878, "fecha_inicio":"2022-06-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-3.22907878315441, "ahorro_total":-64.5815756630882, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3787395, "monto_maximo_cliente": 96578.0, "cuota_externa_total": 26867.0, "capacidad_maxima_pago": 60460.0, "bursolnum": 7439593, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2836.744033099388, "monto_max": 96578.0, "cuota_min": 200.2991210698785, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.4818, "kubo_score": "B5", "comision": 0.046, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "HIPOTECAGOBIERNO", "registro":10, "monto_otorgado":974491.0, "cuota":9055.0, "saldo":986134.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":360.0, "numero_pagos_restante":354.0, "frecuencia_externa":"M", "avance":-0.0119, "fecha_inicio":"2023-10-26", "tipo_deuda":"M", "ahorro_cuota_mensual":-25424.663911575328, "ahorro_total":-9152879.008167118, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":1125.0, "cuota":716.0, "saldo":716.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3636, "fecha_inicio":"2018-07-17", "tipo_deuda":"O", "ahorro_cuota_mensual":1431.9999999999982, "ahorro_total":-1431.9999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":706.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-06-06", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1061.0, "cuota":786.0, "saldo":786.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2592, "fecha_inicio":"2021-06-19", "tipo_deuda":"O", "ahorro_cuota_mensual":1571.9999999999982, "ahorro_total":-1571.9999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":60000.0, "cuota":3186.0, "saldo":43275.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.2788, "fecha_inicio":"2022-10-28", "tipo_deuda":"I", "ahorro_cuota_mensual":230.4662543165341, "ahorro_total":8296.785155395228, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":65000.0, "cuota":3376.0, "saldo":37761.0, "tasa_externa":0.4747, "tasa_kubo":0.3617, "numero_pagos_otorgado":72.0, "numero_pagos_restante":26.0, "frecuencia_externa":"S", "avance":0.4191, "fecha_inicio":"2023-06-16", "tipo_deuda":"I", "ahorro_cuota_mensual":174.17177550957877, "ahorro_total":6270.183918344836, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":32, "monto_otorgado":999.0, "cuota":999.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-03-10", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":25000.0, "cuota":676.0, "saldo":11957.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":43.0, "numero_pagos_restante":17.0, "frecuencia_externa":"S", "avance":0.5217, "fecha_inicio":"2023-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-971.726599369646, "ahorro_total":-21377.985186132213, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":24900.0, "cuota":350.0, "saldo":1138.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9543, "fecha_inicio":"2017-06-06", "tipo_deuda":"R", "ahorro_cuota_mensual":1487.9999999999975, "ahorro_total":-1487.9999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":24000.0, "cuota":1200.0, "saldo":5440.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7733, "fecha_inicio":"2018-09-28", "tipo_deuda":"R", "ahorro_cuota_mensual":6639.999999999987, "ahorro_total":-6639.999999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "AUTOMOTRIZ", "registro":5, "monto_otorgado":555820.0, "cuota":7456.0, "saldo":427425.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":60.0, "numero_pagos_restante":43.0, "frecuencia_externa":"M", "avance":0.231, "fecha_inicio":"2022-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-14810.051494611977, "ahorro_total":-888603.0896767186, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3901833, "monto_maximo_cliente": 17200.0, "cuota_externa_total": 4349.0, "capacidad_maxima_pago": 24851.0, "bursolnum": 7439635, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1536.5203379078412, "monto_max": 17200.0, "cuota_min": 244.39480798426723, "monto_min": 5000, "plazo_max": 16.0, "plazo_min": 4, "tasa": 0.4706, "kubo_score": "B4", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":2524.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-07-24", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":4, "monto_otorgado":811.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-05-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":933.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-10-08", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":17200.0, "cuota":2057.0, "saldo":9911.0, "tasa_externa":0.7359, "tasa_kubo":0.4706, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4238, "fecha_inicio":"2023-08-19", "tipo_deuda":"I", "ahorro_cuota_mensual":165.4361637582299, "ahorro_total":1985.2339650987587, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":19500.0, "cuota":285.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-05-03", "tipo_deuda":"R", "ahorro_cuota_mensual":285.0, "ahorro_total":-285.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":40000.0, "cuota":2292.0, "saldo":31436.0, "tasa_externa":-1.0, "tasa_kubo":0.4706, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.2141, "fecha_inicio":"2022-11-04", "tipo_deuda":"I", "ahorro_cuota_mensual":12.909881874620169, "ahorro_total":464.7557474863261, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 3965394, "monto_maximo_cliente": 64186.0, "cuota_externa_total": 7548.0, "capacidad_maxima_pago": 37144.0, "bursolnum": 7439652, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1087.8815832369983, "monto_max": 64186.0, "cuota_min": 149.00338370164636, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.5391, "kubo_score": "C2", "comision": 0.0471, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":1850.0, "cuota":1896.0, "saldo":1896.0, "tasa_externa":-1.0, "tasa_kubo":0.2221, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0249, "fecha_inicio":"2024-03-25", "tipo_deuda":"I", "ahorro_cuota_mensual":6.281116666673597, "ahorro_total":6.281116666673597, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":39000.0, "cuota":1950.0, "saldo":18446.0, "tasa_externa":-1.0, "tasa_kubo":0.2221, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.527, "fecha_inicio":"2021-03-17", "tipo_deuda":"R", "ahorro_cuota_mensual":20395.999999999978, "ahorro_total":-20395.999999999978, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":32000.0, "cuota":1589.0, "saldo":22789.0, "tasa_externa":0.4322, "tasa_kubo":0.2221, "numero_pagos_otorgado":36.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.2878, "fecha_inicio":"2023-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":303.72649868452686, "ahorro_total":10934.153952642966, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":22100.0, "cuota":1105.0, "saldo":11654.0, "tasa_externa":-1.0, "tasa_kubo":0.2221, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4727, "fecha_inicio":"2021-07-19", "tipo_deuda":"R", "ahorro_cuota_mensual":12758.999999999985, "ahorro_total":-12758.999999999985, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":3000.0, "cuota":150.0, "saldo":236.0, "tasa_externa":-1.0, "tasa_kubo":0.2221, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9213, "fecha_inicio":"2019-06-14", "tipo_deuda":"R", "ahorro_cuota_mensual":385.99999999999966, "ahorro_total":-385.99999999999966, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":20000.0, "cuota":2293.0, "saldo":16403.0, "tasa_externa":-1.0, "tasa_kubo":0.2221, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.1798, "fecha_inicio":"2023-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":384.6971209848448, "ahorro_total":4616.365451818137, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2221, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-01-06", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4100476, "monto_maximo_cliente": 453540.0, "cuota_externa_total": 32891.0, "capacidad_maxima_pago": 85385.0, "bursolnum": 7439697, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5225.90843441975, "monto_max": 453540.0, "cuota_min": 370.5085944866793, "monto_min": 5000, "plazo_max": 21.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":7, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"1991-07-06", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":52600.0, "cuota":5540.0, "saldo":38823.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":18.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.2619, "fecha_inicio":"2023-06-14", "tipo_deuda":"I", "ahorro_cuota_mensual":196.28970415784534, "ahorro_total":3533.214674841216, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "OTRAS FINANCIERA", "registro":10, "monto_otorgado":42000.0, "cuota":-1.0, "saldo":40611.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0331, "fecha_inicio":"2024-01-25", "tipo_deuda":"R", "ahorro_cuota_mensual":40610.00000000001, "ahorro_total":-40610.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":80000.0, "cuota":8168.0, "saldo":77105.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":15.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.0362, "fecha_inicio":"2023-11-28", "tipo_deuda":"O", "ahorro_cuota_mensual":-460.0154006330904, "ahorro_total":-6900.231009496356, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "OTRAS FINANCIERA", "registro":9, "monto_otorgado":60000.0, "cuota":-1.0, "saldo":33819.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4364, "fecha_inicio":"2023-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":33818.0, "ahorro_total":-33818.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":55276.0, "cuota":5800.0, "saldo":26016.0, "tasa_externa":0.5792, "tasa_kubo":0.7554, "numero_pagos_otorgado":13.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5293, "fecha_inicio":"2023-07-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-927.5612441832855, "ahorro_total":-12058.29617438271, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":100000.0, "cuota":5000.0, "saldo":14740.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8526, "fecha_inicio":"2023-08-24", "tipo_deuda":"R", "ahorro_cuota_mensual":19740.0, "ahorro_total":-19740.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":285200.0, "cuota":14260.0, "saldo":204522.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2829, "fecha_inicio":"2021-09-14", "tipo_deuda":"R", "ahorro_cuota_mensual":218782.00000000003, "ahorro_total":-218782.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":31300.0, "cuota":1565.0, "saldo":11795.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6232, "fecha_inicio":"2022-06-13", "tipo_deuda":"R", "ahorro_cuota_mensual":13360.000000000002, "ahorro_total":-13360.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":16500.0, "cuota":825.0, "saldo":15672.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0502, "fecha_inicio":"2022-01-21", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4161166, "monto_maximo_cliente": 191829.0, "cuota_externa_total": 12031.0, "capacidad_maxima_pago": 70552.0, "bursolnum": 7437950, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2702.237228177656, "monto_max": 191829.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5486, "kubo_score": "C3", "comision": 0.0476, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":30000.0, "cuota":1885.0, "saldo":20583.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":36.0, "numero_pagos_restante":13.0, "frecuencia_externa":"M", "avance":0.3139, "fecha_inicio":"2022-06-09", "tipo_deuda":"I", "ahorro_cuota_mensual":464.2070050282073, "ahorro_total":16711.452181015462, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":12, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2009-11-03", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":10000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2019-01-06", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":16, "monto_otorgado":24339.0, "cuota":4793.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2009-12-03", "tipo_deuda":"R", "ahorro_cuota_mensual":4793.0, "ahorro_total":-4793.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":16000.0, "cuota":1620.0, "saldo":17517.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0948, "fecha_inicio":"2022-05-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":3000.0, "cuota":445.0, "saldo":3325.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.1083, "fecha_inicio":"2023-02-09", "tipo_deuda":"R", "ahorro_cuota_mensual":3769.999999999992, "ahorro_total":-3769.999999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":39577.0, "cuota":2688.0, "saldo":38175.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":96.0, "numero_pagos_restante":38.0, "frecuencia_externa":"S", "avance":0.0354, "fecha_inicio":"2023-07-06", "tipo_deuda":"I", "ahorro_cuota_mensual":1055.7399907094634, "ahorro_total":50675.51955405425, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":70900.0, "cuota":3340.0, "saldo":56696.0, "tasa_externa":0.4856, "tasa_kubo":0.3337, "numero_pagos_otorgado":48.0, "numero_pagos_restante":30.0, "frecuencia_externa":"M", "avance":0.2003, "fecha_inicio":"2022-10-27", "tipo_deuda":"I", "ahorro_cuota_mensual":415.89674157467607, "ahorro_total":19963.04359558445, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":2560.0, "cuota":80.0, "saldo":920.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":128.0, "numero_pagos_restante":12.0, "frecuencia_externa":"W", "avance":0.6406, "fecha_inicio":"2022-08-22", "tipo_deuda":"I", "ahorro_cuota_mensual":-49.44727545633333, "ahorro_total":-1582.3128146026665, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":1280.0, "cuota":40.0, "saldo":1270.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":128.0, "numero_pagos_restante":31.0, "frecuencia_externa":"W", "avance":0.0078, "fecha_inicio":"2024-03-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-24.723637728166665, "ahorro_total":-791.1564073013333, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":12416.0, "cuota":388.0, "saldo":12319.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":128.0, "numero_pagos_restante":31.0, "frecuencia_externa":"W", "avance":0.0078, "fecha_inicio":"2024-03-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-239.81928596321666, "ahorro_total":-7674.217150822933, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":17500.0, "cuota":875.0, "saldo":17099.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0229, "fecha_inicio":"2024-02-06", "tipo_deuda":"R", "ahorro_cuota_mensual":17973.999999999956, "ahorro_total":-17973.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":16500.0, "cuota":825.0, "saldo":12226.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.259, "fecha_inicio":"2022-08-31", "tipo_deuda":"R", "ahorro_cuota_mensual":13050.999999999969, "ahorro_total":-13050.999999999969, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":10310.0, "cuota":899.0, "saldo":8792.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1472, "fecha_inicio":"2009-05-25", "tipo_deuda":"R", "ahorro_cuota_mensual":9690.999999999978, "ahorro_total":-9690.999999999978, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":7000.0, "cuota":583.0, "saldo":6137.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1233, "fecha_inicio":"2008-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":6719.9999999999845, "ahorro_total":-6719.9999999999845, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4177829, "monto_maximo_cliente": 55510.0, "cuota_externa_total": 18053.0, "capacidad_maxima_pago": 31947.0, "bursolnum": 7437953, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 849.5676230122074, "monto_max": 55510.0, "cuota_min": 148.2848081136287, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":26, "monto_otorgado":693.0, "cuota":257.0, "saldo":715.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0317, "fecha_inicio":"2023-02-09", "tipo_deuda":"I", "ahorro_cuota_mensual":16.10588560859003, "ahorro_total":48.31765682577009, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":31600.0, "cuota":2446.0, "saldo":29239.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":36.0, "numero_pagos_restante":23.0, "frecuencia_externa":"M", "avance":0.0747, "fecha_inicio":"2023-03-14", "tipo_deuda":"I", "ahorro_cuota_mensual":1180.8825116185506, "ahorro_total":42511.77041826782, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":15000.0, "cuota":1930.0, "saldo":12949.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1367, "fecha_inicio":"2023-11-07", "tipo_deuda":"I", "ahorro_cuota_mensual":500.5491382197181, "ahorro_total":6006.589658636617, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":50000.0, "cuota":5117.0, "saldo":49370.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":18.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.0126, "fecha_inicio":"2024-01-22", "tipo_deuda":"I", "ahorro_cuota_mensual":1744.6374224235437, "ahorro_total":31403.47360362379, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":28, "monto_otorgado":1293.0, "cuota":476.0, "saldo":1304.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0085, "fecha_inicio":"2023-02-24", "tipo_deuda":"I", "ahorro_cuota_mensual":26.539552802174455, "ahorro_total":79.61865840652337, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":27, "monto_otorgado":1050.0, "cuota":389.0, "saldo":1084.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0324, "fecha_inicio":"2023-02-09", "tipo_deuda":"I", "ahorro_cuota_mensual":24.008917588772704, "ahorro_total":72.02675276631811, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":22300.0, "cuota":1222.0, "saldo":17425.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2186, "fecha_inicio":"2022-07-15", "tipo_deuda":"R", "ahorro_cuota_mensual":18646.999999999927, "ahorro_total":-18646.999999999927, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":2076.0, "cuota":802.0, "saldo":2152.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0366, "fecha_inicio":"2024-02-15", "tipo_deuda":"I", "ahorro_cuota_mensual":80.36048848980215, "ahorro_total":241.08146546940645, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":1099.0, "cuota":433.0, "saldo":801.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2712, "fecha_inicio":"2024-01-09", "tipo_deuda":"I", "ahorro_cuota_mensual":50.97600040958213, "ahorro_total":152.92800122874638, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":9000.0, "cuota":1544.0, "saldo":6309.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.299, "fecha_inicio":"2021-11-11", "tipo_deuda":"R", "ahorro_cuota_mensual":7852.999999999974, "ahorro_total":-7852.999999999974, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":419.0, "cuota":164.0, "saldo":303.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2768, "fecha_inicio":"2024-01-12", "tipo_deuda":"I", "ahorro_cuota_mensual":18.351177590186467, "ahorro_total":55.0535327705594, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":1132.0, "cuota":447.0, "saldo":829.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2677, "fecha_inicio":"2024-01-07", "tipo_deuda":"I", "ahorro_cuota_mensual":53.504852105229304, "ahorro_total":160.5145563156879, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":4014.0, "cuota":1570.0, "saldo":2913.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2743, "fecha_inicio":"2024-01-11", "tipo_deuda":"I", "ahorro_cuota_mensual":174.69123352507972, "ahorro_total":524.0737005752392, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":20000.0, "cuota":1256.0, "saldo":18985.0, "tasa_externa":0.3521, "tasa_kubo":0.22, "numero_pagos_otorgado":43.0, "numero_pagos_restante":15.0, "frecuencia_externa":"S", "avance":0.0507, "fecha_inicio":"2023-10-02", "tipo_deuda":"I", "ahorro_cuota_mensual":108.25858199916343, "ahorro_total":2381.6888039815954, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4268611, "monto_maximo_cliente": 325496.0, "cuota_externa_total": 17804.0, "capacidad_maxima_pago": 141736.0, "bursolnum": 7438040, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4373.426876745378, "monto_max": 325496.0, "cuota_min": 161.3323702779843, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":17, "monto_otorgado":100.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2574, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":70000.0, "cuota":4509.0, "saldo":50084.0, "tasa_externa":-1.0, "tasa_kubo":0.2574, "numero_pagos_otorgado":36.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.2845, "fecha_inicio":"2022-07-15", "tipo_deuda":"I", "ahorro_cuota_mensual":1542.8160201096484, "ahorro_total":55541.376723947345, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":7, "monto_otorgado":42500.0, "cuota":2860.0, "saldo":40917.0, "tasa_externa":-1.0, "tasa_kubo":0.2574, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0372, "fecha_inicio":"2017-09-22", "tipo_deuda":"R", "ahorro_cuota_mensual":43776.99999999987, "ahorro_total":-43776.99999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":86040.0, "cuota":2346.0, "saldo":80891.0, "tasa_externa":0.3146, "tasa_kubo":0.2574, "numero_pagos_otorgado":116.0, "numero_pagos_restante":84.0, "frecuencia_externa":"M", "avance":0.0598, "fecha_inicio":"2021-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":73.8516504672798, "ahorro_total":8566.791454204456, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":48500.0, "cuota":2533.0, "saldo":37819.0, "tasa_externa":0.4757, "tasa_kubo":0.2574, "numero_pagos_otorgado":36.0, "numero_pagos_restante":22.0, "frecuencia_externa":"M", "avance":0.2202, "fecha_inicio":"2023-02-27", "tipo_deuda":"I", "ahorro_cuota_mensual":477.858242504542, "ahorro_total":17202.896730163513, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":89900.0, "cuota":1500.0, "saldo":40105.0, "tasa_externa":-1.0, "tasa_kubo":0.2574, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5539, "fecha_inicio":"2020-07-21", "tipo_deuda":"R", "ahorro_cuota_mensual":41604.99999999987, "ahorro_total":-41604.99999999987, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":102000.0, "cuota":5556.0, "saldo":105693.0, "tasa_externa":-1.0, "tasa_kubo":0.2574, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0362, "fecha_inicio":"2022-08-05", "tipo_deuda":"R", "ahorro_cuota_mensual":111248.99999999967, "ahorro_total":-111248.99999999967, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":38000.0, "cuota":2089.0, "saldo":4241.0, "tasa_externa":-1.0, "tasa_kubo":0.2574, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8884, "fecha_inicio":"2022-01-03", "tipo_deuda":"R", "ahorro_cuota_mensual":6329.999999999986, "ahorro_total":-6329.999999999986, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4302913, "monto_maximo_cliente": 199726.0, "cuota_externa_total": 23809.0, "capacidad_maxima_pago": 24898.0, "bursolnum": 7438070, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 232.67088876615762, "monto_max": 199726.0, "cuota_min": 148.2848081136287, "monto_min": 5000, "plazo_max": 51.0, "plazo_min": 4, "tasa": 0.8317, "kubo_score": "E3", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.8317, 0.821, 0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['E3', 'E2', 'E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":100000.0, "cuota":8657.0, "saldo":99114.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":36.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":0.0089, "fecha_inicio":"2024-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":4653.463644362502, "ahorro_total":167524.6911970501, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":9, "monto_otorgado":36900.0, "cuota":1072.0, "saldo":34860.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0553, "fecha_inicio":"2023-05-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-36612.73999999983, "ahorro_total":-36612.73999999983, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":1302381.0, "cuota":13825.0, "saldo":1174319.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":180.0, "numero_pagos_restante":144.0, "frecuencia_externa":"M", "avance":0.0983, "fecha_inicio":"2021-04-30", "tipo_deuda":"M", "ahorro_cuota_mensual":-11727.458707994698, "ahorro_total":-2110942.5674390458, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":2, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2014-07-26", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":12, "monto_otorgado":23000.0, "cuota":2853.0, "saldo":500.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9783, "fecha_inicio":"2017-04-18", "tipo_deuda":"R", "ahorro_cuota_mensual":3352.9999999999977, "ahorro_total":-3352.9999999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":21000.0, "cuota":2000.0, "saldo":10162.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5161, "fecha_inicio":"2019-01-26", "tipo_deuda":"R", "ahorro_cuota_mensual":12161.999999999956, "ahorro_total":-12161.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":82800.0, "cuota":85597.0, "saldo":79982.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.034, "fecha_inicio":"2018-12-27", "tipo_deuda":"R", "ahorro_cuota_mensual":165578.99999999965, "ahorro_total":-165578.99999999965, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":27000.0, "cuota":2000.0, "saldo":18517.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3142, "fecha_inicio":"2020-02-22", "tipo_deuda":"R", "ahorro_cuota_mensual":20516.999999999924, "ahorro_total":-20516.999999999924, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":30000.0, "cuota":146.0, "saldo":13651.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.545, "fecha_inicio":"2022-12-13", "tipo_deuda":"R", "ahorro_cuota_mensual":13796.999999999942, "ahorro_total":-13796.999999999942, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":7200.0, "cuota":255.0, "saldo":6559.0, "tasa_externa":0.3537, "tasa_kubo":0.22, "numero_pagos_otorgado":60.0, "numero_pagos_restante":46.0, "frecuencia_externa":"M", "avance":0.089, "fecha_inicio":"2023-02-14", "tipo_deuda":"I", "ahorro_cuota_mensual":41.46987631637464, "ahorro_total":2488.192578982478, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":135500.0, "cuota":5100.0, "saldo":69714.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4855, "fecha_inicio":"2022-04-20", "tipo_deuda":"R", "ahorro_cuota_mensual":74813.99999999971, "ahorro_total":-74813.99999999971, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4323421, "monto_maximo_cliente": 503880.0, "cuota_externa_total": 90443.0, "capacidad_maxima_pago": 203056.0, "bursolnum": 7438089, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5117.408961455153, "monto_max": 503880.0, "cuota_min": 148.2848081136287, "monto_min": 5000, "plazo_max": 55.0, "plazo_min": 4, "tasa": 0.5991, "kubo_score": "D1", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":9, "monto_otorgado":210000.0, "cuota":5419.0, "saldo":184781.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1201, "fecha_inicio":"2023-07-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-20465.017982247933, "ahorro_total":-184185.1618402314, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "OTRAS FINANCIERA", "registro":15, "monto_otorgado":317011.0, "cuota":0.0, "saldo":65449.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7935, "fecha_inicio":"2021-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":317010.99999999866, "ahorro_total":-317010.99999999866, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":14, "monto_otorgado":1138.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-10-14", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":13, "monto_otorgado":350000.0, "cuota":20217.0, "saldo":131219.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":48.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":0.6251, "fecha_inicio":"2023-01-20", "tipo_deuda":"I", "ahorro_cuota_mensual":8510.26506900075, "ahorro_total":408492.723312036, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":250000.0, "cuota":16845.0, "saldo":243460.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":36.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.0262, "fecha_inicio":"2023-11-29", "tipo_deuda":"I", "ahorro_cuota_mensual":6836.159110906254, "ahorro_total":246101.72799262515, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":10, "monto_otorgado":50000.0, "cuota":1409.0, "saldo":49702.0, "tasa_externa":0.233, "tasa_kubo":0.22, "numero_pagos_otorgado":60.0, "numero_pagos_restante":57.0, "frecuencia_externa":"M", "avance":0.006, "fecha_inicio":"2024-01-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-73.84808113628719, "ahorro_total":-4430.8848681772315, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":47900.0, "cuota":1297.0, "saldo":43646.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0888, "fecha_inicio":"2023-11-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-4607.021244522267, "ahorro_total":-41463.1912007004, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":145000.0, "cuota":7250.0, "saldo":142838.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":156.0, "numero_pagos_restante":68.0, "frecuencia_externa":"Z", "avance":0.0149, "fecha_inicio":"2016-12-17", "tipo_deuda":"R", "ahorro_cuota_mensual":4093.8866797961496, "ahorro_total":638646.3220481994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":4, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-08-12", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":19600.0, "cuota":19318.0, "saldo":19318.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0144, "fecha_inicio":"2022-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":38635.99999999992, "ahorro_total":-38635.99999999992, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":15951.0, "cuota":1472.0, "saldo":13451.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.1567, "fecha_inicio":"2024-01-11", "tipo_deuda":"I", "ahorro_cuota_mensual":-48.078046417151654, "ahorro_total":-576.9365570058199, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":165000.0, "cuota":5472.0, "saldo":118676.0, "tasa_externa":0.2203, "tasa_kubo":0.22, "numero_pagos_otorgado":44.0, "numero_pagos_restante":31.0, "frecuencia_externa":"M", "avance":0.2808, "fecha_inicio":"2023-03-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-339.19877095331594, "ahorro_total":-14924.745921945902, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":94200.0, "cuota":4710.0, "saldo":93693.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0054, "fecha_inicio":"2011-11-11", "tipo_deuda":"R", "ahorro_cuota_mensual":98402.9999999996, "ahorro_total":-98402.9999999996, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":70600.0, "cuota":5514.0, "saldo":67080.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0499, "fecha_inicio":"2023-02-02", "tipo_deuda":"R", "ahorro_cuota_mensual":72593.99999999972, "ahorro_total":-72593.99999999972, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":246900.0, "cuota":6962.0, "saldo":189052.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":48.0, "numero_pagos_restante":32.0, "frecuencia_externa":"M", "avance":0.2343, "fecha_inicio":"2022-12-23", "tipo_deuda":"I", "ahorro_cuota_mensual":-1296.265298467757, "ahorro_total":-62220.73432645234, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4426818, "monto_maximo_cliente": 209516.0, "cuota_externa_total": 30873.0, "capacidad_maxima_pago": 10191.0, "bursolnum": 7438215, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1282.6757280888382, "monto_max": 209516.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 23.0, "plazo_min": 4, "tasa": 0.6722, "kubo_score": "D4", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":32, "monto_otorgado":2000.0, "cuota":256.0, "saldo":458.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.771, "fecha_inicio":"2022-05-08", "tipo_deuda":"I", "ahorro_cuota_mensual":10.89105110209212, "ahorro_total":130.69261322510545, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":33, "monto_otorgado":5000.0, "cuota":1123.0, "saldo":5015.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.003, "fecha_inicio":"2023-02-27", "tipo_deuda":"I", "ahorro_cuota_mensual":90.22491464645645, "ahorro_total":541.3494878787387, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":34, "monto_otorgado":6000.0, "cuota":2288.0, "saldo":4130.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3117, "fecha_inicio":"2023-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":22.63186720740441, "ahorro_total":67.89560162221323, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":35, "monto_otorgado":4700.0, "cuota":586.0, "saldo":2811.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4019, "fecha_inicio":"2022-08-30", "tipo_deuda":"I", "ahorro_cuota_mensual":9.993970089916502, "ahorro_total":119.92764107899802, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":36, "monto_otorgado":5000.0, "cuota":1055.0, "saldo":2762.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4476, "fecha_inicio":"2022-11-29", "tipo_deuda":"I", "ahorro_cuota_mensual":22.224914646456455, "ahorro_total":133.34948787873873, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":37, "monto_otorgado":880.0, "cuota":132.0, "saldo":240.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7273, "fecha_inicio":"2022-08-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-0.19771269255036827, "ahorro_total":-1.7794142329533145, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":19, "monto_otorgado":100000.0, "cuota":7066.0, "saldo":79961.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":36.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.2004, "fecha_inicio":"2022-09-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-183.61210904599739, "ahorro_total":-6610.035925655906, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":1571.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-01-26", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":17, "monto_otorgado":20000.0, "cuota":2471.0, "saldo":12203.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3899, "fecha_inicio":"2023-08-17", "tipo_deuda":"I", "ahorro_cuota_mensual":19.91051102092115, "ahorro_total":238.9261322510538, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":22, "monto_otorgado":837.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-03-31", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":23, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"1991-10-11", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":25, "monto_otorgado":1527.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-10-15", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":21, "monto_otorgado":15100.0, "cuota":1794.0, "saldo":15087.0, "tasa_externa":0.7213, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0009, "fecha_inicio":"2021-07-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-56.57256417920462, "ahorro_total":-678.8707701504554, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":2, "monto_otorgado":5000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-01-27", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":20, "monto_otorgado":5000.0, "cuota":851.0, "saldo":5504.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.1008, "fecha_inicio":"2013-01-18", "tipo_deuda":"R", "ahorro_cuota_mensual":6355.000000000006, "ahorro_total":-6355.000000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":4000.0, "cuota":674.0, "saldo":2180.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.455, "fecha_inicio":"2023-09-28", "tipo_deuda":"I", "ahorro_cuota_mensual":73.10130594295288, "ahorro_total":657.9117534865759, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":38000.0, "cuota":2378.0, "saldo":37678.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0085, "fecha_inicio":"2024-01-03", "tipo_deuda":"R", "ahorro_cuota_mensual":40056.000000000044, "ahorro_total":-40056.000000000044, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":2000.0, "cuota":200.0, "saldo":1694.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.153, "fecha_inicio":"2024-02-09", "tipo_deuda":"R", "ahorro_cuota_mensual":1894.000000000002, "ahorro_total":-1894.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":50000.0, "cuota":2500.0, "saldo":48651.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":49.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.027, "fecha_inicio":"2020-03-20", "tipo_deuda":"R", "ahorro_cuota_mensual":-812.8336795635632, "ahorro_total":-39828.8502986146, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":27000.0, "cuota":1350.0, "saldo":26541.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":65.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.017, "fecha_inicio":"2018-11-15", "tipo_deuda":"R", "ahorro_cuota_mensual":-403.91405623964283, "ahorro_total":-26254.413655576784, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":5600.0, "cuota":1278.0, "saldo":4837.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1362, "fecha_inicio":"2024-02-02", "tipo_deuda":"I", "ahorro_cuota_mensual":121.29190440403113, "ahorro_total":727.7514264241868, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":2400.0, "cuota":532.0, "saldo":935.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6104, "fecha_inicio":"2023-11-03", "tipo_deuda":"I", "ahorro_cuota_mensual":36.26795903029904, "ahorro_total":217.60775418179423, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":4000.0, "cuota":1627.0, "saldo":1476.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.631, "fecha_inicio":"2023-12-28", "tipo_deuda":"I", "ahorro_cuota_mensual":116.75457813826961, "ahorro_total":350.2637344148088, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":100.0, "cuota":14.0, "saldo":13.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.87, "fecha_inicio":"2023-03-30", "tipo_deuda":"I", "ahorro_cuota_mensual":1.7445525551046064, "ahorro_total":20.934630661255277, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":4000.0, "cuota":532.0, "saldo":1372.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.657, "fecha_inicio":"2023-05-30", "tipo_deuda":"I", "ahorro_cuota_mensual":41.78210220418424, "ahorro_total":501.3852264502109, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":4500.0, "cuota":600.0, "saldo":1987.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5584, "fecha_inicio":"2023-06-29", "tipo_deuda":"I", "ahorro_cuota_mensual":48.50486497970735, "ahorro_total":582.0583797564882, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":5000.0, "cuota":695.0, "saldo":1221.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7558, "fecha_inicio":"2023-05-04", "tipo_deuda":"I", "ahorro_cuota_mensual":82.22762775523029, "ahorro_total":986.7315330627634, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":15, "monto_otorgado":6990.0, "cuota":1430.0, "saldo":7022.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":9.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":-0.0046, "fecha_inicio":"2024-02-28", "tipo_deuda":"I", "ahorro_cuota_mensual":379.92953213530996, "ahorro_total":3419.36578921779, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":5100.0, "cuota":810.0, "saldo":1444.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7169, "fecha_inicio":"2023-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":43.85416507726495, "ahorro_total":394.68748569538457, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":9200.0, "cuota":460.0, "saldo":9078.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0133, "fecha_inicio":"2022-09-04", "tipo_deuda":"R", "ahorro_cuota_mensual":9538.000000000011, "ahorro_total":-9538.000000000011, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4446822, "monto_maximo_cliente": 366903.0, "cuota_externa_total": 48039.0, "capacidad_maxima_pago": 102792.0, "bursolnum": 7438247, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5497.726574423007, "monto_max": 366903.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 31.0, "plazo_min": 4, "tasa": 0.3813, "kubo_score": "A5", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0428, 0.0423, 0.0417], "kubo_scores": ['A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":15, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2020-11-17", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2010-07-13", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":14, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2014-12-13", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":12, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-11-21", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":125700.0, "cuota":8079.0, "saldo":72253.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":24.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.4252, "fecha_inicio":"2023-01-20", "tipo_deuda":"I", "ahorro_cuota_mensual":97.70931224619198, "ahorro_total":2345.0234939086076, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":10, "monto_otorgado":150000.0, "cuota":6770.0, "saldo":149889.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":48.0, "numero_pagos_restante":45.0, "frecuencia_externa":"M", "avance":0.0007, "fecha_inicio":"2024-01-23", "tipo_deuda":"I", "ahorro_cuota_mensual":60.4231189711918, "ahorro_total":2900.3097106172063, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":9, "monto_otorgado":1499999.0, "cuota":14669.0, "saldo":1310570.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":195.0, "numero_pagos_restante":154.0, "frecuencia_externa":"M", "avance":0.1263, "fecha_inicio":"2020-12-09", "tipo_deuda":"M", "ahorro_cuota_mensual":-33678.89411252966, "ahorro_total":-6567384.351943284, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":20590.0, "cuota":872.0, "saldo":11441.0, "tasa_externa":0.4105, "tasa_kubo":0.3813, "numero_pagos_otorgado":48.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.4443, "fecha_inicio":"2021-09-06", "tipo_deuda":"I", "ahorro_cuota_mensual":-49.00125320255438, "ahorro_total":-2352.0601537226103, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":80000.0, "cuota":3796.0, "saldo":57211.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":43.0, "numero_pagos_restante":12.0, "frecuencia_externa":"S", "avance":0.2849, "fecha_inicio":"2023-07-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-1574.9732919526668, "ahorro_total":-34649.412422958674, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":80000.0, "cuota":5156.0, "saldo":78201.0, "tasa_externa":0.3847, "tasa_kubo":0.3813, "numero_pagos_otorgado":43.0, "numero_pagos_restante":16.0, "frecuencia_externa":"S", "avance":0.0225, "fecha_inicio":"2023-10-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-214.97329195266684, "ahorro_total":-4729.4124229586705, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":40600.0, "cuota":276.0, "saldo":34118.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1597, "fecha_inicio":"2006-10-09", "tipo_deuda":"R", "ahorro_cuota_mensual":34394.00000000008, "ahorro_total":-34394.00000000008, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":54000.0, "cuota":2700.0, "saldo":39848.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2621, "fecha_inicio":"2008-11-27", "tipo_deuda":"R", "ahorro_cuota_mensual":42548.00000000009, "ahorro_total":-42548.00000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":60600.0, "cuota":3030.0, "saldo":55843.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0785, "fecha_inicio":"2021-04-05", "tipo_deuda":"R", "ahorro_cuota_mensual":58873.000000000124, "ahorro_total":-58873.000000000124, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":48400.0, "cuota":3404.0, "saldo":48626.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0047, "fecha_inicio":"2022-08-18", "tipo_deuda":"R", "ahorro_cuota_mensual":52030.0000000001, "ahorro_total":-52030.0000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":13000.0, "cuota":650.0, "saldo":7878.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.394, "fecha_inicio":"2016-11-29", "tipo_deuda":"R", "ahorro_cuota_mensual":8528.000000000018, "ahorro_total":-8528.000000000018, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4475229, "monto_maximo_cliente": 155752.0, "cuota_externa_total": 16746.0, "capacidad_maxima_pago": 68111.0, "bursolnum": 7438276, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3485.367365228652, "monto_max": 155752.0, "cuota_min": 269.2747621622814, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.8317, "kubo_score": "E3", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.8317, 0.821, 0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['E3', 'E2', 'E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":30000.0, "cuota":2976.0, "saldo":29435.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":22.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.0188, "fecha_inicio":"2024-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":672.8035626298793, "ahorro_total":14801.678377857344, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":4, "monto_otorgado":80000.0, "cuota":5532.0, "saldo":73993.0, "tasa_externa":0.4748, "tasa_kubo":0.5292, "numero_pagos_otorgado":43.0, "numero_pagos_restante":9.0, "frecuencia_externa":"S", "avance":0.0751, "fecha_inicio":"2023-04-04", "tipo_deuda":"I", "ahorro_cuota_mensual":-609.8571663203211, "ahorro_total":-13416.857659047064, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":34000.0, "cuota":2449.0, "saldo":33249.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0221, "fecha_inicio":"2023-11-30", "tipo_deuda":"R", "ahorro_cuota_mensual":35698.000000000015, "ahorro_total":-35698.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":55000.0, "cuota":3992.0, "saldo":51790.0, "tasa_externa":0.5386, "tasa_kubo":0.5292, "numero_pagos_otorgado":43.0, "numero_pagos_restante":12.0, "frecuencia_externa":"S", "avance":0.0584, "fecha_inicio":"2023-06-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-230.5268018452207, "ahorro_total":-5071.589640594855, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":23900.0, "cuota":1195.0, "saldo":14300.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4017, "fecha_inicio":"2022-12-07", "tipo_deuda":"R", "ahorro_cuota_mensual":15495.000000000005, "ahorro_total":-15495.000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":46500.0, "cuota":2325.0, "saldo":34703.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2537, "fecha_inicio":"2023-09-18", "tipo_deuda":"R", "ahorro_cuota_mensual":37028.00000000001, "ahorro_total":-37028.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":21400.0, "cuota":1070.0, "saldo":18500.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1355, "fecha_inicio":"2021-09-06", "tipo_deuda":"R", "ahorro_cuota_mensual":19570.000000000007, "ahorro_total":-19570.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4488665, "monto_maximo_cliente": 182243.0, "cuota_externa_total": 8651.0, "capacidad_maxima_pago": 72949.0, "bursolnum": 7438302, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3436.688563478484, "monto_max": 182243.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.7007, "kubo_score": "D5", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":8, "monto_otorgado":22601.0, "cuota":3000.0, "saldo":20132.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1092, "fecha_inicio":"2020-02-24", "tipo_deuda":"R", "ahorro_cuota_mensual":23132.000000000022, "ahorro_total":-23132.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":13, "monto_otorgado":2483.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-11-27", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":12, "monto_otorgado":24600.0, "cuota":1911.0, "saldo":21062.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":36.0, "numero_pagos_restante":17.0, "frecuencia_externa":"M", "avance":0.1438, "fecha_inicio":"2022-10-04", "tipo_deuda":"I", "ahorro_cuota_mensual":127.59542117468459, "ahorro_total":4593.435162288645, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":10, "monto_otorgado":27100.0, "cuota":2104.0, "saldo":24766.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0861, "fecha_inicio":"2023-02-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-1665.3725222857188, "ahorro_total":-16653.72522285719, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":9, "monto_otorgado":47632.0, "cuota":0.0, "saldo":9474.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.8011, "fecha_inicio":"2022-07-11", "tipo_deuda":"O", "ahorro_cuota_mensual":9474.000000000013, "ahorro_total":-9474.000000000013, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":13000.0, "cuota":1270.0, "saldo":11527.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1133, "fecha_inicio":"2021-10-29", "tipo_deuda":"R", "ahorro_cuota_mensual":12797.000000000015, "ahorro_total":-12797.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":51600.0, "cuota":4004.0, "saldo":46777.0, "tasa_externa":0.9338, "tasa_kubo":0.6722, "numero_pagos_otorgado":120.0, "numero_pagos_restante":44.0, "frecuencia_externa":"S", "avance":0.0935, "fecha_inicio":"2023-01-09", "tipo_deuda":"I", "ahorro_cuota_mensual":572.5413973464492, "ahorro_total":34352.483840786954, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":18000.0, "cuota":1587.0, "saldo":15876.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.118, "fecha_inicio":"2022-10-28", "tipo_deuda":"R", "ahorro_cuota_mensual":17463.000000000022, "ahorro_total":-17463.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":4, "monto_otorgado":14916.0, "cuota":-1.0, "saldo":5578.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.626, "fecha_inicio":"2024-02-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":3, "monto_otorgado":14933.0, "cuota":-1.0, "saldo":3969.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7342, "fecha_inicio":"2024-01-02", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":15000.0, "cuota":1603.0, "saldo":17136.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.1424, "fecha_inicio":"2022-11-09", "tipo_deuda":"R", "ahorro_cuota_mensual":18739.000000000022, "ahorro_total":-18739.000000000022, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":2, "monto_otorgado":15000.0, "cuota":-1.0, "saldo":6122.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5919, "fecha_inicio":"2023-11-17", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":14000.0, "cuota":700.0, "saldo":13729.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0194, "fecha_inicio":"2022-07-07", "tipo_deuda":"R", "ahorro_cuota_mensual":14429.000000000016, "ahorro_total":-14429.000000000016, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4503596, "monto_maximo_cliente": 199076.0, "cuota_externa_total": 19650.0, "capacidad_maxima_pago": 149214.0, "bursolnum": 7438310, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 10485.061141968403, "monto_max": 199076.0, "cuota_min": 332.5056785517006, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.6722, "kubo_score": "D4", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":8000.0, "cuota":988.0, "saldo":4776.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.403, "fecha_inicio":"2023-08-29", "tipo_deuda":"I", "ahorro_cuota_mensual":7.564204408368482, "ahorro_total":90.77045290042179, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":13, "monto_otorgado":14500.0, "cuota":725.0, "saldo":2213.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8474, "fecha_inicio":"2017-01-27", "tipo_deuda":"R", "ahorro_cuota_mensual":2938.0000000000023, "ahorro_total":-2938.0000000000023, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":8000.0, "cuota":400.0, "saldo":6032.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.246, "fecha_inicio":"2022-04-28", "tipo_deuda":"R", "ahorro_cuota_mensual":6432.000000000007, "ahorro_total":-6432.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":6000.0, "cuota":300.0, "saldo":3551.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4082, "fecha_inicio":"2022-03-18", "tipo_deuda":"R", "ahorro_cuota_mensual":3851.000000000004, "ahorro_total":-3851.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":6000.0, "cuota":362.0, "saldo":3612.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.398, "fecha_inicio":"2022-01-16", "tipo_deuda":"R", "ahorro_cuota_mensual":3974.0000000000045, "ahorro_total":-3974.0000000000045, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":9600.0, "cuota":480.0, "saldo":1854.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8069, "fecha_inicio":"2023-12-28", "tipo_deuda":"R", "ahorro_cuota_mensual":2334.000000000002, "ahorro_total":-2334.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":153500.0, "cuota":13063.0, "saldo":152144.0, "tasa_externa":1.0131, "tasa_kubo":0.6722, "numero_pagos_otorgado":48.0, "numero_pagos_restante":43.0, "frecuencia_externa":"M", "avance":0.0088, "fecha_inicio":"2023-11-28", "tipo_deuda":"I", "ahorro_cuota_mensual":2577.938858031597, "ahorro_total":123741.06518551667, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":4, "monto_otorgado":150.0, "cuota":351.0, "saldo":1404.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-8.36, "fecha_inicio":"2024-02-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":3, "monto_otorgado":4549.0, "cuota":80.0, "saldo":160.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9648, "fecha_inicio":"2023-11-18", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":20000.0, "cuota":3770.0, "saldo":13375.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":21.0, "numero_pagos_restante":13.0, "frecuencia_externa":"M", "avance":0.3313, "fecha_inicio":"2023-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":2584.9980210088447, "ahorro_total":54284.958441185736, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":20000.0, "cuota":2700.0, "saldo":13375.0, "tasa_externa":-1.0, "tasa_kubo":0.6722, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3313, "fecha_inicio":"2023-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":16075.000000000015, "ahorro_total":-16075.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4557872, "monto_maximo_cliente": 303779.0, "cuota_externa_total": 42544.0, "capacidad_maxima_pago": 173956.0, "bursolnum": 7438398, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7308.096433568694, "monto_max": 303779.0, "cuota_min": 200.2991210698785, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":47000.0, "cuota":3020.0, "saldo":37831.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":36.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.1951, "fecha_inicio":"2022-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":704.8318992146183, "ahorro_total":25373.948371726256, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":11, "monto_otorgado":38500.0, "cuota":1483.0, "saldo":36659.0, "tasa_externa":0.402, "tasa_kubo":0.3617, "numero_pagos_otorgado":60.0, "numero_pagos_restante":47.0, "frecuencia_externa":"M", "avance":0.0478, "fecha_inicio":"2023-03-15", "tipo_deuda":"I", "ahorro_cuota_mensual":-59.30323223806454, "ahorro_total":-3558.1939342838723, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":15, "monto_otorgado":18400.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2022-05-16", "tipo_deuda":"I", "ahorro_cuota_mensual":-19043.343733333313, "ahorro_total":-19043.343733333313, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":13, "monto_otorgado":26000.0, "cuota":0.0, "saldo":141.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9946, "fecha_inicio":"2024-01-26", "tipo_deuda":"R", "ahorro_cuota_mensual":140.99999999999966, "ahorro_total":-140.99999999999966, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":25000.0, "cuota":26566.0, "saldo":25928.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0371, "fecha_inicio":"2024-02-13", "tipo_deuda":"I", "ahorro_cuota_mensual":691.8916666666955, "ahorro_total":691.8916666666955, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":10, "monto_otorgado":54000.0, "cuota":2942.0, "saldo":18460.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6581, "fecha_inicio":"2023-05-08", "tipo_deuda":"R", "ahorro_cuota_mensual":21401.999999999956, "ahorro_total":-21401.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":9, "monto_otorgado":10000.0, "cuota":500.0, "saldo":1069.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8931, "fecha_inicio":"2019-11-14", "tipo_deuda":"R", "ahorro_cuota_mensual":1568.9999999999975, "ahorro_total":-1568.9999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":18900.0, "cuota":500.0, "saldo":1106.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9415, "fecha_inicio":"2023-12-11", "tipo_deuda":"R", "ahorro_cuota_mensual":1605.9999999999975, "ahorro_total":-1605.9999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":20800.0, "cuota":1382.0, "saldo":10966.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4728, "fecha_inicio":"2017-07-04", "tipo_deuda":"R", "ahorro_cuota_mensual":12347.999999999976, "ahorro_total":-12347.999999999976, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":27000.0, "cuota":1350.0, "saldo":10685.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6043, "fecha_inicio":"2022-12-09", "tipo_deuda":"R", "ahorro_cuota_mensual":12034.999999999975, "ahorro_total":-12034.999999999975, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":6000.0, "cuota":544.0, "saldo":846.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.859, "fecha_inicio":"2017-12-20", "tipo_deuda":"R", "ahorro_cuota_mensual":1389.9999999999982, "ahorro_total":-1389.9999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":69000.0, "cuota":3239.0, "saldo":29945.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.566, "fecha_inicio":"2022-02-11", "tipo_deuda":"R", "ahorro_cuota_mensual":33183.999999999935, "ahorro_total":-33183.999999999935, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":12600.0, "cuota":910.0, "saldo":529.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.958, "fecha_inicio":"2018-03-29", "tipo_deuda":"R", "ahorro_cuota_mensual":1438.9999999999986, "ahorro_total":-1438.9999999999986, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":181500.0, "cuota":7826.0, "saldo":158779.0, "tasa_externa":0.4228, "tasa_kubo":0.3617, "numero_pagos_otorgado":48.0, "numero_pagos_restante":37.0, "frecuencia_externa":"M", "avance":0.1252, "fecha_inicio":"2023-05-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-29.198571371619437, "ahorro_total":-1401.531425837733, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":13520.0, "cuota":676.0, "saldo":5132.0, "tasa_externa":-1.0, "tasa_kubo":0.3617, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6204, "fecha_inicio":"2017-07-04", "tipo_deuda":"R", "ahorro_cuota_mensual":5807.999999999988, "ahorro_total":-5807.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4604014, "monto_maximo_cliente": 57512.0, "cuota_externa_total": 4017.0, "capacidad_maxima_pago": 47082.0, "bursolnum": 7438490, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1107.0891985175547, "monto_max": 57512.0, "cuota_min": 148.2848081136287, "monto_min": 5000, "plazo_max": 48.0, "plazo_min": 4, "tasa": 0.4428, "kubo_score": "B2", "comision": 0.0444, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2009-09-03", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":15000.0, "cuota":988.0, "saldo":7987.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":24.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.4675, "fecha_inicio":"2022-12-27", "tipo_deuda":"I", "ahorro_cuota_mensual":183.5083351099322, "ahorro_total":4404.200042638373, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":10000.0, "cuota":4200.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2017-08-11", "tipo_deuda":"R", "ahorro_cuota_mensual":4200.0, "ahorro_total":-4200.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":33099.0, "cuota":1520.0, "saldo":9476.0, "tasa_externa":0.3793, "tasa_kubo":0.22, "numero_pagos_otorgado":37.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7137, "fecha_inicio":"2021-09-28", "tipo_deuda":"I", "ahorro_cuota_mensual":218.78308529516198, "ahorro_total":8094.974155920993, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":15000.0, "cuota":1139.0, "saldo":13986.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0676, "fecha_inicio":"2021-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":15124.999999999942, "ahorro_total":-15124.999999999942, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":25000.0, "cuota":1250.0, "saldo":10427.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5829, "fecha_inicio":"2023-05-30", "tipo_deuda":"R", "ahorro_cuota_mensual":11676.999999999956, "ahorro_total":-11676.999999999956, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":8300.0, "cuota":168.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-11-15", "tipo_deuda":"R", "ahorro_cuota_mensual":168.0, "ahorro_total":-168.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4637424, "monto_maximo_cliente": 564367.0, "cuota_externa_total": 36780.0, "capacidad_maxima_pago": 129279.0, "bursolnum": 7438550, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7398.095591338296, "monto_max": 564367.0, "cuota_min": 269.2747621622814, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5486, "kubo_score": "C3", "comision": 0.0476, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":69000.0, "cuota":4961.0, "saldo":32464.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":23.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5295, "fecha_inicio":"2022-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-210.32397012088313, "ahorro_total":-4837.451312780312, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":1, "monto_otorgado":350000.0, "cuota":25000.0, "saldo":205516.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4128, "fecha_inicio":"2010-12-30", "tipo_deuda":"R", "ahorro_cuota_mensual":230516.00000000006, "ahorro_total":-230516.00000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":26300.0, "cuota":1315.0, "saldo":18364.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3017, "fecha_inicio":"2010-08-01", "tipo_deuda":"R", "ahorro_cuota_mensual":19679.000000000004, "ahorro_total":-19679.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":220000.0, "cuota":11000.0, "saldo":143233.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3489, "fecha_inicio":"2010-04-06", "tipo_deuda":"R", "ahorro_cuota_mensual":154233.00000000003, "ahorro_total":-154233.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":137000.0, "cuota":8000.0, "saldo":132300.0, "tasa_externa":0.6526, "tasa_kubo":0.5292, "numero_pagos_otorgado":48.0, "numero_pagos_restante":42.0, "frecuencia_externa":"M", "avance":0.0343, "fecha_inicio":"2023-10-30", "tipo_deuda":"I", "ahorro_cuota_mensual":288.35722441554935, "ahorro_total":13841.146771946369, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":63100.0, "cuota":8000.0, "saldo":60254.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0451, "fecha_inicio":"2018-05-02", "tipo_deuda":"R", "ahorro_cuota_mensual":68254.00000000003, "ahorro_total":-68254.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":4495.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"1989-02-01", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":2, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2013-03-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECARIA", "registro":10, "monto_otorgado":1154637.0, "cuota":12780.0, "saldo":1059797.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":360.0, "numero_pagos_restante":340.0, "frecuencia_externa":"M", "avance":0.0821, "fecha_inicio":"2022-08-15", "tipo_deuda":"M", "ahorro_cuota_mensual":-41434.976190888476, "ahorro_total":-14916591.428719852, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4639545, "monto_maximo_cliente": 190808.0, "cuota_externa_total": 29907.0, "capacidad_maxima_pago": 5493.0, "bursolnum": 7438554, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1671.3667353325393, "monto_max": 190808.0, "cuota_min": 278.44180193239873, "monto_min": 5000, "plazo_max": 17.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":32, "monto_otorgado":18400.0, "cuota":2202.0, "saldo":17285.0, "tasa_externa":0.7374, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0606, "fecha_inicio":"2022-03-17", "tipo_deuda":"I", "ahorro_cuota_mensual":88.31507671104964, "ahorro_total":1059.7809205325957, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":31, "monto_otorgado":3000.0, "cuota":261.0, "saldo":2685.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.105, "fecha_inicio":"2022-04-05", "tipo_deuda":"R", "ahorro_cuota_mensual":2945.999999999998, "ahorro_total":-2945.999999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":29, "monto_otorgado":3000.0, "cuota":393.0, "saldo":2562.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.146, "fecha_inicio":"2023-03-08", "tipo_deuda":"R", "ahorro_cuota_mensual":2954.9999999999977, "ahorro_total":-2954.9999999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":24, "monto_otorgado":400.0, "cuota":56.0, "saldo":362.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.095, "fecha_inicio":"2023-11-03", "tipo_deuda":"I", "ahorro_cuota_mensual":10.050327754588032, "ahorro_total":120.60393305505639, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "GUBERNAMENTALES", "registro":27, "monto_otorgado":49545.0, "cuota":2064.0, "saldo":22755.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":21.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.5407, "fecha_inicio":"2023-05-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-1910.0771484740003, "ahorro_total":-40111.62011795401, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":26, "monto_otorgado":8000.0, "cuota":1398.0, "saldo":7476.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0655, "fecha_inicio":"2023-06-20", "tipo_deuda":"R", "ahorro_cuota_mensual":8873.999999999993, "ahorro_total":-8873.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":10000.0, "cuota":1339.0, "saldo":1323.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8677, "fecha_inicio":"2023-03-01", "tipo_deuda":"I", "ahorro_cuota_mensual":190.25819386470084, "ahorro_total":2283.09832637641, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":112, "monto_otorgado":336.0, "cuota":69.0, "saldo":289.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1399, "fecha_inicio":"2023-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":2.1220147861450016, "ahorro_total":12.73208871687001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "GUBERNAMENTALES", "registro":28, "monto_otorgado":51357.0, "cuota":1712.0, "saldo":31839.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":30.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.38, "fecha_inicio":"2023-05-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-1751.8976345788856, "ahorro_total":-52556.929037366564, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":113, "monto_otorgado":352.0, "cuota":41.0, "saldo":304.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1364, "fecha_inicio":"2023-01-11", "tipo_deuda":"I", "ahorro_cuota_mensual":0.5642884240374713, "ahorro_total":6.771461088449655, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":34, "monto_otorgado":2938.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-08-19", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":115, "monto_otorgado":1500.0, "cuota":204.0, "saldo":1340.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1067, "fecha_inicio":"2023-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":31.688729079705126, "ahorro_total":380.2647489564615, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":116, "monto_otorgado":1500.0, "cuota":197.0, "saldo":1293.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.138, "fecha_inicio":"2023-01-17", "tipo_deuda":"I", "ahorro_cuota_mensual":24.688729079705126, "ahorro_total":296.2647489564615, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":117, "monto_otorgado":1500.0, "cuota":208.0, "saldo":1274.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1507, "fecha_inicio":"2022-11-26", "tipo_deuda":"I", "ahorro_cuota_mensual":35.688729079705126, "ahorro_total":428.2647489564615, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":118, "monto_otorgado":500.0, "cuota":67.0, "saldo":376.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.248, "fecha_inicio":"2022-11-11", "tipo_deuda":"I", "ahorro_cuota_mensual":9.562909693235042, "ahorro_total":114.7549163188205, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":119, "monto_otorgado":4000.0, "cuota":525.0, "saldo":2963.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2592, "fecha_inicio":"2022-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":65.50327754588034, "ahorro_total":786.039330550564, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":120, "monto_otorgado":1500.0, "cuota":188.0, "saldo":985.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3433, "fecha_inicio":"2022-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":15.688729079705126, "ahorro_total":188.26474895646152, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":121, "monto_otorgado":1000.0, "cuota":133.0, "saldo":749.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.251, "fecha_inicio":"2022-11-13", "tipo_deuda":"I", "ahorro_cuota_mensual":18.125819386470084, "ahorro_total":217.509832637641, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":30, "monto_otorgado":41500.0, "cuota":2453.0, "saldo":33737.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":36.0, "numero_pagos_restante":19.0, "frecuencia_externa":"M", "avance":0.1871, "fecha_inicio":"2022-12-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-159.1595404102054, "ahorro_total":-5729.743454767395, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":33, "monto_otorgado":1651.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-06-14", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":114, "monto_otorgado":1000.0, "cuota":131.0, "saldo":756.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.244, "fecha_inicio":"2022-11-06", "tipo_deuda":"I", "ahorro_cuota_mensual":16.125819386470084, "ahorro_total":193.509832637641, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":23, "monto_otorgado":405.0, "cuota":87.0, "saldo":308.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2395, "fecha_inicio":"2023-12-07", "tipo_deuda":"I", "ahorro_cuota_mensual":6.388142822585493, "ahorro_total":38.32885693551296, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":300.0, "cuota":47.0, "saldo":300.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-01-19", "tipo_deuda":"I", "ahorro_cuota_mensual":12.537745815941022, "ahorro_total":150.45294979129227, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":21, "monto_otorgado":220.0, "cuota":35.0, "saldo":193.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1227, "fecha_inicio":"2023-12-10", "tipo_deuda":"I", "ahorro_cuota_mensual":3.6048604706568774, "ahorro_total":32.44374423591189, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":4000.0, "cuota":11525.0, "saldo":11525.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.8812, "fecha_inicio":"2024-03-05", "tipo_deuda":"I", "ahorro_cuota_mensual":7312.178666666667, "ahorro_total":7312.178666666667, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":653.0, "cuota":144.0, "saldo":507.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2236, "fecha_inicio":"2023-11-28", "tipo_deuda":"I", "ahorro_cuota_mensual":14.025820402835393, "ahorro_total":84.15492241701236, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":2500.0, "cuota":397.0, "saldo":392.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8432, "fecha_inicio":"2023-06-08", "tipo_deuda":"I", "ahorro_cuota_mensual":40.2370508029191, "ahorro_total":362.1334572262719, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":300.0, "cuota":48.0, "saldo":310.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":-0.0333, "fecha_inicio":"2024-01-11", "tipo_deuda":"I", "ahorro_cuota_mensual":13.537745815941022, "ahorro_total":162.45294979129227, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":803.0, "cuota":131.0, "saldo":807.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":9.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":-0.005, "fecha_inicio":"2024-02-27", "tipo_deuda":"I", "ahorro_cuota_mensual":16.407740717897624, "ahorro_total":147.66966646107863, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":2272.0, "cuota":363.0, "saldo":2017.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1122, "fecha_inicio":"2023-12-05", "tipo_deuda":"I", "ahorro_cuota_mensual":38.77383176969289, "ahorro_total":348.964485927236, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":2271.0, "cuota":329.0, "saldo":2053.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.096, "fecha_inicio":"2023-11-08", "tipo_deuda":"I", "ahorro_cuota_mensual":68.12073582667352, "ahorro_total":817.4488299200823, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":2000.0, "cuota":322.0, "saldo":2169.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":-0.0845, "fecha_inicio":"2024-02-08", "tipo_deuda":"I", "ahorro_cuota_mensual":92.25163877294017, "ahorro_total":1107.019665275282, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":749.0, "cuota":167.0, "saldo":165.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7797, "fecha_inicio":"2023-09-13", "tipo_deuda":"I", "ahorro_cuota_mensual":17.917824627448255, "ahorro_total":107.50694776468953, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":219.0, "cuota":31.0, "saldo":165.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2466, "fecha_inicio":"2023-09-13", "tipo_deuda":"I", "ahorro_cuota_mensual":5.842554445636949, "ahorro_total":70.11065334764339, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":4400.0, "cuota":719.0, "saldo":4640.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":-0.0545, "fecha_inicio":"2024-01-05", "tipo_deuda":"I", "ahorro_cuota_mensual":213.55360530046835, "ahorro_total":2562.64326360562, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":13, "monto_otorgado":6000.0, "cuota":797.0, "saldo":3931.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3448, "fecha_inicio":"2023-08-04", "tipo_deuda":"I", "ahorro_cuota_mensual":107.7549163188205, "ahorro_total":1293.058995825846, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":400.0, "cuota":53.0, "saldo":315.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2125, "fecha_inicio":"2023-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":7.050327754588032, "ahorro_total":84.60393305505639, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":15, "monto_otorgado":800.0, "cuota":128.0, "saldo":782.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.0225, "fecha_inicio":"2023-12-13", "tipo_deuda":"I", "ahorro_cuota_mensual":36.100655509176065, "ahorro_total":433.2078661101128, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":150.0, "cuota":23.0, "saldo":135.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.1, "fecha_inicio":"2023-11-20", "tipo_deuda":"I", "ahorro_cuota_mensual":5.768872907970511, "ahorro_total":69.22647489564613, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":500.0, "cuota":80.0, "saldo":536.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":-0.072, "fecha_inicio":"2024-02-11", "tipo_deuda":"I", "ahorro_cuota_mensual":22.562909693235042, "ahorro_total":270.7549163188205, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":350.0, "cuota":53.0, "saldo":357.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":-0.02, "fecha_inicio":"2024-02-24", "tipo_deuda":"I", "ahorro_cuota_mensual":12.794036785264531, "ahorro_total":153.52844142317437, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":19, "monto_otorgado":1500.0, "cuota":209.0, "saldo":1129.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2473, "fecha_inicio":"2023-09-06", "tipo_deuda":"I", "ahorro_cuota_mensual":36.688729079705126, "ahorro_total":440.2647489564615, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":20, "monto_otorgado":1903.0, "cuota":231.0, "saldo":443.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7672, "fecha_inicio":"2023-04-05", "tipo_deuda":"I", "ahorro_cuota_mensual":12.394434292452559, "ahorro_total":148.7332115094307, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":2500.0, "cuota":347.0, "saldo":2229.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1084, "fecha_inicio":"2023-11-08", "tipo_deuda":"I", "ahorro_cuota_mensual":59.81454846617521, "ahorro_total":717.7745815941025, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4714725, "monto_maximo_cliente": 193638.0, "cuota_externa_total": 12063.0, "capacidad_maxima_pago": 32537.0, "bursolnum": 7438657, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3215.995620247574, "monto_max": 193638.0, "cuota_min": 269.2747621622814, "monto_min": 5000, "plazo_max": 14.0, "plazo_min": 4, "tasa": 0.5292, "kubo_score": "C1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":25000.0, "cuota":1674.0, "saldo":17368.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":27.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.3053, "fecha_inicio":"2023-01-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-54.26137069856122, "ahorro_total":-1465.057008861153, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":8000.0, "cuota":198.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-09-25", "tipo_deuda":"R", "ahorro_cuota_mensual":198.0, "ahorro_total":-198.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":25000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2024-02-11", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":1200.0, "cuota":106.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-04-23", "tipo_deuda":"R", "ahorro_cuota_mensual":106.0, "ahorro_total":-106.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":86300.0, "cuota":5324.0, "saldo":66618.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":19.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.2281, "fecha_inicio":"2022-10-03", "tipo_deuda":"I", "ahorro_cuota_mensual":-5915.072859642982, "ahorro_total":-59150.72859642982, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":30000.0, "cuota":1099.0, "saldo":3735.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8755, "fecha_inicio":"2020-10-02", "tipo_deuda":"R", "ahorro_cuota_mensual":4834.000000000002, "ahorro_total":-4834.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":51800.0, "cuota":662.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-05-28", "tipo_deuda":"R", "ahorro_cuota_mensual":662.0, "ahorro_total":-662.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":72003.0, "cuota":1260.0, "saldo":57421.0, "tasa_externa":-1.0, "tasa_kubo":0.5292, "numero_pagos_otorgado":120.0, "numero_pagos_restante":41.0, "frecuencia_externa":"S", "avance":0.2025, "fecha_inicio":"2022-10-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-2617.718139994149, "ahorro_total":-157063.08839964896, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":31600.0, "cuota":3805.0, "saldo":15426.0, "tasa_externa":0.7511, "tasa_kubo":0.5292, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5118, "fecha_inicio":"2022-05-07", "tipo_deuda":"I", "ahorro_cuota_mensual":216.4347266402201, "ahorro_total":2597.2167196826413, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4721997, "monto_maximo_cliente": 707489.0, "cuota_externa_total": 37068.0, "capacidad_maxima_pago": 545470.0, "bursolnum": 7438667, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 18782.26383703736, "monto_max": 707489.0, "cuota_min": 189.49186879271792, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":30000.0, "cuota":2200.0, "saldo":28365.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":30.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.0545, "fecha_inicio":"2023-10-30", "tipo_deuda":"I", "ahorro_cuota_mensual":624.4188030116782, "ahorro_total":18732.564090350344, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":7500.0, "cuota":888.0, "saldo":4585.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3887, "fecha_inicio":"2023-08-02", "tipo_deuda":"I", "ahorro_cuota_mensual":124.34413642980121, "ahorro_total":1492.1296371576145, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":12000.0, "cuota":1133.0, "saldo":9726.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":17.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":0.1895, "fecha_inicio":"2023-09-20", "tipo_deuda":"I", "ahorro_cuota_mensual":204.92062356001804, "ahorro_total":3483.650600520307, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":9, "monto_otorgado":55000.0, "cuota":5052.0, "saldo":9580.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":17.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8258, "fecha_inicio":"2023-01-06", "tipo_deuda":"I", "ahorro_cuota_mensual":798.3028579834163, "ahorro_total":13571.148585718078, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":14, "monto_otorgado":492800.0, "cuota":19473.0, "saldo":308535.0, "tasa_externa":0.364, "tasa_kubo":0.3337, "numero_pagos_otorgado":48.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.3739, "fecha_inicio":"2022-01-27", "tipo_deuda":"I", "ahorro_cuota_mensual":-851.3735649083137, "ahorro_total":-40865.93111559906, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":3000.0, "cuota":219.0, "saldo":2070.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.31, "fecha_inicio":"2022-03-11", "tipo_deuda":"R", "ahorro_cuota_mensual":2288.9999999999945, "ahorro_total":-2288.9999999999945, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":3100.0, "cuota":562.0, "saldo":3072.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.009, "fecha_inicio":"2023-05-19", "tipo_deuda":"R", "ahorro_cuota_mensual":-2609.0955519999925, "ahorro_total":-2609.0955519999925, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":3100.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2023-01-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":3, "monto_otorgado":118080.0, "cuota":5904.0, "saldo":117555.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0044, "fecha_inicio":"2001-11-15", "tipo_deuda":"R", "ahorro_cuota_mensual":123458.99999999971, "ahorro_total":-123458.99999999971, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":92000.0, "cuota":4600.0, "saldo":91992.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0001, "fecha_inicio":"2017-12-22", "tipo_deuda":"R", "ahorro_cuota_mensual":96591.99999999977, "ahorro_total":-96591.99999999977, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":36964.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3337, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"1999-06-10", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4733672, "monto_maximo_cliente": 265972.0, "cuota_externa_total": 15636.0, "capacidad_maxima_pago": 111927.0, "bursolnum": 7438676, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4571.230944555158, "monto_max": 265972.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5504, "kubo_score": "C4", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":1300.0, "cuota":281.0, "saldo":985.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2423, "fecha_inicio":"2023-12-10", "tipo_deuda":"I", "ahorro_cuota_mensual":35.539498899172145, "ahorro_total":213.23699339503287, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":17, "monto_otorgado":4200.0, "cuota":568.0, "saldo":4496.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":-0.0705, "fecha_inicio":"2024-02-03", "tipo_deuda":"I", "ahorro_cuota_mensual":128.59881157746918, "ahorro_total":1543.1857389296301, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":10.0, "cuota":10.0, "saldo":10.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-02-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-0.36859000000000464, "ahorro_total":-0.36859000000000464, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":19, "monto_otorgado":1000.0, "cuota":1049.0, "saldo":1032.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.032, "fecha_inicio":"2024-02-17", "tipo_deuda":"I", "ahorro_cuota_mensual":12.140999999999394, "ahorro_total":12.140999999999394, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":20, "monto_otorgado":651.0, "cuota":86.0, "saldo":684.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":10.0, "frecuencia_externa":"M", "avance":-0.0507, "fecha_inicio":"2024-02-10", "tipo_deuda":"I", "ahorro_cuota_mensual":17.892815794507726, "ahorro_total":214.7137895340927, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":23, "monto_otorgado":10.0, "cuota":11.0, "saldo":10.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-02-06", "tipo_deuda":"I", "ahorro_cuota_mensual":0.6314099999999954, "ahorro_total":0.6314099999999954, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":10.0, "cuota":10.0, "saldo":10.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-02-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-0.36859000000000464, "ahorro_total":-0.36859000000000464, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":15, "monto_otorgado":1200.0, "cuota":446.0, "saldo":439.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6342, "fecha_inicio":"2023-12-25", "tipo_deuda":"I", "ahorro_cuota_mensual":16.157105249563358, "ahorro_total":48.471315748690074, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":24, "monto_otorgado":2543.0, "cuota":398.0, "saldo":2411.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":9.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0519, "fecha_inicio":"2024-01-19", "tipo_deuda":"I", "ahorro_cuota_mensual":60.86222004609618, "ahorro_total":547.7599804148656, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":26, "monto_otorgado":35800.0, "cuota":2113.0, "saldo":29440.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":36.0, "numero_pagos_restante":21.0, "frecuencia_externa":"M", "avance":0.1777, "fecha_inicio":"2023-01-18", "tipo_deuda":"I", "ahorro_cuota_mensual":301.17321678134317, "ahorro_total":10842.235804128355, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVICIOS", "registro":27, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"B", "avance":-1.0, "fecha_inicio":"2015-05-01", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":21, "monto_otorgado":10.0, "cuota":10.0, "saldo":10.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-02-10", "tipo_deuda":"I", "ahorro_cuota_mensual":-0.36859000000000464, "ahorro_total":-0.36859000000000464, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":14, "monto_otorgado":360.0, "cuota":80.0, "saldo":360.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.0, "fecha_inicio":"2024-03-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-18.44331079988143, "ahorro_total":-73.77324319952572, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":25, "monto_otorgado":900.0, "cuota":200.0, "saldo":978.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":6.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0867, "fecha_inicio":"2024-01-28", "tipo_deuda":"I", "ahorro_cuota_mensual":30.065806930196118, "ahorro_total":180.3948415811767, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":360.0, "cuota":80.0, "saldo":300.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.1667, "fecha_inicio":"2024-02-07", "tipo_deuda":"I", "ahorro_cuota_mensual":-18.44331079988143, "ahorro_total":-73.77324319952572, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":11, "monto_otorgado":936.0, "cuota":104.0, "saldo":832.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.1111, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-20.090036192235146, "ahorro_total":-180.81032573011632, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":252.0, "cuota":84.0, "saldo":168.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.3333, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-6.267007897591682, "ahorro_total":-18.801023692775047, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":378.0, "cuota":84.0, "saldo":294.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.2222, "fecha_inicio":"2024-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":-19.365476339875485, "ahorro_total":-77.46190535950194, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":832.0, "cuota":104.0, "saldo":676.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":32.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.1875, "fecha_inicio":"2024-01-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-17.9774241787279, "ahorro_total":-143.8193934298232, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":1404.0, "cuota":104.0, "saldo":1274.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":54.0, "numero_pagos_restante":11.0, "frecuencia_externa":"W", "avance":0.0926, "fecha_inicio":"2024-01-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-26.173834506572348, "ahorro_total":-366.43368309201287, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":22600.0, "cuota":1057.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-01-20", "tipo_deuda":"R", "ahorro_cuota_mensual":1057.0, "ahorro_total":-1057.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":5, "monto_otorgado":108000.0, "cuota":5274.0, "saldo":101040.0, "tasa_externa":0.512, "tasa_kubo":0.3813, "numero_pagos_otorgado":48.0, "numero_pagos_restante":40.0, "frecuencia_externa":"M", "avance":0.0644, "fecha_inicio":"2023-08-21", "tipo_deuda":"I", "ahorro_cuota_mensual":443.1046456592585, "ahorro_total":21269.022991644408, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":53600.0, "cuota":2144.0, "saldo":51992.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":100.0, "numero_pagos_restante":23.0, "frecuencia_externa":"W", "avance":0.03, "fecha_inicio":"2024-03-05", "tipo_deuda":"I", "ahorro_cuota_mensual":-1174.0810483728333, "ahorro_total":-29352.026209320833, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":3, "monto_otorgado":6144.0, "cuota":192.0, "saldo":5712.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":128.0, "numero_pagos_restante":29.0, "frecuencia_externa":"W", "avance":0.0703, "fecha_inicio":"2024-01-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-138.1329728550038, "ahorro_total":-4420.255131360122, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":13, "monto_otorgado":252.0, "cuota":84.0, "saldo":231.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"W", "avance":0.0833, "fecha_inicio":"2024-02-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-6.267007897591682, "ahorro_total":-18.801023692775047, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":2, "monto_otorgado":81620.0, "cuota":2120.0, "saldo":71920.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":154.0, "numero_pagos_restante":33.0, "frecuencia_externa":"W", "avance":0.1188, "fecha_inicio":"2023-11-17", "tipo_deuda":"I", "ahorro_cuota_mensual":-1905.8792424638523, "ahorro_total":-72423.41121362639, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":7000.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2017-08-19", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-3.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4754385, "monto_maximo_cliente": 284480.0, "cuota_externa_total": 42641.0, "capacidad_maxima_pago": 75453.0, "bursolnum": 7438701, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5293.744643303981, "monto_max": 284480.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.6722, "kubo_score": "D4", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":12, "monto_otorgado":1397.0, "cuota":533.0, "saldo":1441.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0315, "fecha_inicio":"2024-02-17", "tipo_deuda":"I", "ahorro_cuota_mensual":15.398065054909807, "ahorro_total":46.19419516472942, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":16, "monto_otorgado":20000.0, "cuota":4153.0, "saldo":18900.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.055, "fecha_inicio":"2023-02-07", "tipo_deuda":"R", "ahorro_cuota_mensual":23053.000000000004, "ahorro_total":-23053.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":91724.0, "cuota":4632.0, "saldo":56306.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":24.0, "numero_pagos_restante":12.0, "frecuencia_externa":"M", "avance":0.3861, "fecha_inicio":"2023-05-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-2328.4723794211413, "ahorro_total":-55883.33710610739, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "SERVS. GRALES.", "registro":20, "monto_otorgado":30000.0, "cuota":2442.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-10-02", "tipo_deuda":"R", "ahorro_cuota_mensual":2442.0, "ahorro_total":-2442.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":30000.0, "cuota":2848.0, "saldo":27052.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":18.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.0983, "fecha_inicio":"2023-10-05", "tipo_deuda":"I", "ahorro_cuota_mensual":184.6780423439127, "ahorro_total":3324.2047621904285, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":17, "monto_otorgado":72000.0, "cuota":5143.0, "saldo":68476.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.0489, "fecha_inicio":"2023-07-21", "tipo_deuda":"I", "ahorro_cuota_mensual":520.6179927202402, "ahorro_total":18742.247737928647, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "AUTOMOTRIZ", "registro":19, "monto_otorgado":195499.0, "cuota":5940.0, "saldo":104445.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":48.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.4658, "fecha_inicio":"2021-10-17", "tipo_deuda":"I", "ahorro_cuota_mensual":-5668.527423363692, "ahorro_total":-272089.3163214572, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":14, "monto_otorgado":42100.0, "cuota":3084.0, "saldo":41842.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":36.0, "numero_pagos_restante":33.0, "frecuencia_externa":"M", "avance":0.0061, "fecha_inicio":"2024-01-29", "tipo_deuda":"I", "ahorro_cuota_mensual":381.1905207433624, "ahorro_total":13722.858746761047, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":11, "monto_otorgado":13000.0, "cuota":11671.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2023-04-05", "tipo_deuda":"R", "ahorro_cuota_mensual":11671.0, "ahorro_total":-11671.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":9, "monto_otorgado":99500.0, "cuota":3817.0, "saldo":28680.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7118, "fecha_inicio":"2019-03-20", "tipo_deuda":"R", "ahorro_cuota_mensual":32497.000000000007, "ahorro_total":-32497.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":8, "monto_otorgado":80000.0, "cuota":5896.0, "saldo":77621.0, "tasa_externa":0.559, "tasa_kubo":0.5668, "numero_pagos_otorgado":43.0, "numero_pagos_restante":13.0, "frecuencia_externa":"S", "avance":0.0297, "fecha_inicio":"2023-07-18", "tipo_deuda":"I", "ahorro_cuota_mensual":-449.85407781089634, "ahorro_total":-9896.78971183972, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":25000.0, "cuota":995.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2020-06-26", "tipo_deuda":"R", "ahorro_cuota_mensual":995.0, "ahorro_total":-995.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":15000.0, "cuota":3695.0, "saldo":12487.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1675, "fecha_inicio":"2024-01-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-931.5535874440529, "ahorro_total":-2794.660762332159, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":5, "monto_otorgado":10992.0, "cuota":550.0, "saldo":2112.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8079, "fecha_inicio":"2024-01-03", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":4, "monto_otorgado":10935.0, "cuota":547.0, "saldo":808.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9261, "fecha_inicio":"2023-12-05", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":3, "monto_otorgado":10918.0, "cuota":186.0, "saldo":372.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9659, "fecha_inicio":"2023-11-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":1, "monto_otorgado":35000.0, "cuota":3316.0, "saldo":31118.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1109, "fecha_inicio":"2017-11-05", "tipo_deuda":"R", "ahorro_cuota_mensual":34434.00000000001, "ahorro_total":-34434.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "CIA Q' OTORGA", "registro":10, "monto_otorgado":66256.0, "cuota":2283.0, "saldo":16882.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7452, "fecha_inicio":"2022-05-17", "tipo_deuda":"O", "ahorro_cuota_mensual":19165.000000000004, "ahorro_total":-19165.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4759224, "monto_maximo_cliente": 362108.0, "cuota_externa_total": 46240.0, "capacidad_maxima_pago": 133998.0, "bursolnum": 7438706, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5293.744643303981, "monto_max": 362108.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.8317, "kubo_score": "E3", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.8317, 0.821, 0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['E3', 'E2', 'E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":20, "monto_otorgado":12000.0, "cuota":1820.0, "saldo":13420.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.1183, "fecha_inicio":"2022-07-22", "tipo_deuda":"R", "ahorro_cuota_mensual":15240.000000000004, "ahorro_total":-15240.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":21, "monto_otorgado":37000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-03-31", "tipo_deuda":"R", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":14000.0, "cuota":1150.0, "saldo":13894.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0076, "fecha_inicio":"2024-02-22", "tipo_deuda":"R", "ahorro_cuota_mensual":15044.000000000004, "ahorro_total":-15044.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "GOBIERNO", "registro":24, "monto_otorgado":1.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2011-08-15", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":103, "monto_otorgado":1000.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2009-06-09", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":8, "monto_otorgado":227499.0, "cuota":12292.0, "saldo":70331.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":4.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6909, "fecha_inicio":"2022-09-12", "tipo_deuda":"I", "ahorro_cuota_mensual":-52580.87840508674, "ahorro_total":-210323.51362034696, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":17, "monto_otorgado":40000.0, "cuota":5349.0, "saldo":33182.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":12.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.1704, "fecha_inicio":"2023-11-30", "tipo_deuda":"I", "ahorro_cuota_mensual":713.231542342347, "ahorro_total":8558.778508108164, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":19, "monto_otorgado":116448.0, "cuota":4175.0, "saldo":62666.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":36.0, "numero_pagos_restante":16.0, "frecuencia_externa":"M", "avance":0.4619, "fecha_inicio":"2022-09-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-3300.9324997737986, "ahorro_total":-118833.56999185676, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":12500.0, "cuota":2354.0, "saldo":12367.0, "tasa_externa":2.2908, "tasa_kubo":0.5668, "numero_pagos_otorgado":96.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0106, "fecha_inicio":"2010-08-18", "tipo_deuda":"I", "ahorro_cuota_mensual":1611.762992178752, "ahorro_total":77364.6236245801, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":18, "monto_otorgado":4000.0, "cuota":200.0, "saldo":2090.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4775, "fecha_inicio":"2023-08-29", "tipo_deuda":"R", "ahorro_cuota_mensual":2290.0000000000005, "ahorro_total":-2290.0000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":54500.0, "cuota":3970.0, "saldo":54025.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0087, "fecha_inicio":"2018-04-04", "tipo_deuda":"R", "ahorro_cuota_mensual":57995.000000000015, "ahorro_total":-57995.000000000015, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":200.0, "cuota":400.0, "saldo":200.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0, "fecha_inicio":"2024-02-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":3014.0, "cuota":6028.0, "saldo":3014.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.0, "fecha_inicio":"2024-02-28", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":20000.0, "cuota":3769.0, "saldo":12371.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3814, "fecha_inicio":"2022-03-30", "tipo_deuda":"R", "ahorro_cuota_mensual":16140.000000000004, "ahorro_total":-16140.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":80000.0, "cuota":5896.0, "saldo":77621.0, "tasa_externa":0.559, "tasa_kubo":0.5668, "numero_pagos_otorgado":43.0, "numero_pagos_restante":13.0, "frecuencia_externa":"S", "avance":0.0297, "fecha_inicio":"2023-07-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-449.85407781089634, "ahorro_total":-9896.78971183972, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":27200.0, "cuota":1851.0, "saldo":26624.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0212, "fecha_inicio":"2022-12-05", "tipo_deuda":"R", "ahorro_cuota_mensual":28475.000000000007, "ahorro_total":-28475.000000000007, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":49000.0, "cuota":2450.0, "saldo":36538.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2543, "fecha_inicio":"2024-01-31", "tipo_deuda":"R", "ahorro_cuota_mensual":38988.00000000001, "ahorro_total":-38988.00000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":14, "monto_otorgado":2500.0, "cuota":1964.0, "saldo":982.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.6072, "fecha_inicio":"2024-01-31", "tipo_deuda":"I", "ahorro_cuota_mensual":610.3543847364599, "ahorro_total":1220.7087694729198, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":700.0, "cuota":49.0, "saldo":492.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":2.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2971, "fecha_inicio":"2023-11-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-217.3974570838647, "ahorro_total":-434.7949141677294, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":500.0, "cuota":49.0, "saldo":492.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.016, "fecha_inicio":"2023-11-28", "tipo_deuda":"R", "ahorro_cuota_mensual":541.0000000000001, "ahorro_total":-541.0000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 4993943, "monto_maximo_cliente": 89634.0, "cuota_externa_total": 36790.0, "capacidad_maxima_pago": 48210.0, "bursolnum": 7440021, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3896.61946138083, "monto_max": 89634.0, "cuota_min": 278.44180193239873, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":24200.0, "cuota":24868.0, "saldo":24868.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0276, "fecha_inicio":"2024-03-25", "tipo_deuda":"I", "ahorro_cuota_mensual":-619.5690666666669, "ahorro_total":-619.5690666666669, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":60000.0, "cuota":4424.0, "saldo":57672.0, "tasa_externa":0.5596, "tasa_kubo":0.5504, "numero_pagos_otorgado":43.0, "numero_pagos_restante":11.0, "frecuencia_externa":"S", "avance":0.0388, "fecha_inicio":"2023-06-01", "tipo_deuda":"I", "ahorro_cuota_mensual":-268.3670633251395, "ahorro_total":-5904.075393153069, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":7911.0, "cuota":176.0, "saldo":5434.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3131, "fecha_inicio":"2019-03-05", "tipo_deuda":"R", "ahorro_cuota_mensual":5609.999999999995, "ahorro_total":-5609.999999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":80000.0, "cuota":7498.0, "saldo":67730.0, "tasa_externa":-1.0, "tasa_kubo":0.5504, "numero_pagos_otorgado":50.0, "numero_pagos_restante":13.0, "frecuencia_externa":"S", "avance":0.1534, "fecha_inicio":"2023-04-28", "tipo_deuda":"I", "ahorro_cuota_mensual":1638.088708674848, "ahorro_total":40952.2177168712, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5008298, "monto_maximo_cliente": 91453.0, "cuota_externa_total": 22063.0, "capacidad_maxima_pago": 77284.0, "bursolnum": 7440049, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5293.744643303981, "monto_max": 91453.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":15000.0, "cuota":1973.0, "saldo":5418.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.6388, "fecha_inicio":"2023-05-03", "tipo_deuda":"I", "ahorro_cuota_mensual":234.58682837838, "ahorro_total":2815.04194054056, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":1, "monto_otorgado":47500.0, "cuota":7054.0, "saldo":17477.0, "tasa_externa":1.6323, "tasa_kubo":0.5668, "numero_pagos_otorgado":36.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.6321, "fecha_inicio":"2022-09-27", "tipo_deuda":"I", "ahorro_cuota_mensual":2837.073567044529, "ahorro_total":51067.324206801524, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":80000.0, "cuota":5900.0, "saldo":153574.0, "tasa_externa":0.56, "tasa_kubo":0.5668, "numero_pagos_otorgado":43.0, "numero_pagos_restante":10.0, "frecuencia_externa":"S", "avance":-0.9197, "fecha_inicio":"2023-05-08", "tipo_deuda":"I", "ahorro_cuota_mensual":-445.85407781089634, "ahorro_total":-9808.78971183972, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":7500.0, "cuota":375.0, "saldo":4607.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3857, "fecha_inicio":"2023-02-27", "tipo_deuda":"R", "ahorro_cuota_mensual":4982.000000000001, "ahorro_total":-4982.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":8000.0, "cuota":6846.0, "saldo":6846.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1442, "fecha_inicio":"2022-03-24", "tipo_deuda":"R", "ahorro_cuota_mensual":13692.000000000002, "ahorro_total":-13692.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5013364, "monto_maximo_cliente": 110010.0, "cuota_externa_total": 11831.0, "capacidad_maxima_pago": 19169.0, "bursolnum": 7440062, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 816.0229586942755, "monto_max": 110010.0, "cuota_min": 148.2848081136287, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.821, "kubo_score": "E2", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.821, 0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['E2', 'E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "MICROFINANCIERA", "registro":17, "monto_otorgado":12180.0, "cuota":47.0, "saldo":452.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9629, "fecha_inicio":"2024-03-15", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":23, "monto_otorgado":16000.0, "cuota":1958.0, "saldo":16237.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.0148, "fecha_inicio":"2023-12-08", "tipo_deuda":"R", "ahorro_cuota_mensual":18194.999999999935, "ahorro_total":-18194.999999999935, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":22, "monto_otorgado":2000.0, "cuota":100.0, "saldo":913.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.5435, "fecha_inicio":"2024-02-02", "tipo_deuda":"R", "ahorro_cuota_mensual":1012.9999999999962, "ahorro_total":-1012.9999999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":21, "monto_otorgado":17000.0, "cuota":1008.0, "saldo":20626.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.2133, "fecha_inicio":"2020-05-27", "tipo_deuda":"R", "ahorro_cuota_mensual":21633.999999999913, "ahorro_total":-21633.999999999913, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":24, "monto_otorgado":30000.0, "cuota":2514.0, "saldo":13713.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":36.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.5429, "fecha_inicio":"2023-05-05", "tipo_deuda":"I", "ahorro_cuota_mensual":1312.9390933087504, "ahorro_total":47265.80735911502, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":20, "monto_otorgado":20000.0, "cuota":1275.0, "saldo":3618.0, "tasa_externa":0.4531, "tasa_kubo":0.22, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8191, "fecha_inicio":"2022-05-16", "tipo_deuda":"I", "ahorro_cuota_mensual":202.34444681324294, "ahorro_total":4856.2667235178305, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":19, "monto_otorgado":35000.0, "cuota":1851.0, "saldo":22160.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3669, "fecha_inicio":"2018-11-17", "tipo_deuda":"R", "ahorro_cuota_mensual":24010.99999999991, "ahorro_total":-24010.99999999991, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":18, "monto_otorgado":12166.0, "cuota":32.0, "saldo":302.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9752, "fecha_inicio":"2024-03-30", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":16, "monto_otorgado":12085.0, "cuota":604.0, "saldo":2411.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8005, "fecha_inicio":"2024-03-14", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":10, "monto_otorgado":12187.0, "cuota":126.0, "saldo":336.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9724, "fecha_inicio":"2023-11-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":14, "monto_otorgado":12164.0, "cuota":608.0, "saldo":666.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9452, "fecha_inicio":"2024-02-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":13, "monto_otorgado":12164.0, "cuota":608.0, "saldo":1746.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.8565, "fecha_inicio":"2024-02-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":12, "monto_otorgado":12180.0, "cuota":1344.0, "saldo":10752.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1172, "fecha_inicio":"2024-02-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":11, "monto_otorgado":12197.0, "cuota":610.0, "saldo":1032.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9154, "fecha_inicio":"2023-12-01", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":9, "monto_otorgado":11960.0, "cuota":60.0, "saldo":60.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.995, "fecha_inicio":"2023-11-16", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":8, "monto_otorgado":12152.0, "cuota":-1.0, "saldo":60.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9951, "fecha_inicio":"2023-11-12", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":12000.0, "cuota":2540.0, "saldo":11987.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":10.0, "numero_pagos_restante":7.0, "frecuencia_externa":"M", "avance":0.0011, "fecha_inicio":"2024-01-11", "tipo_deuda":"R", "ahorro_cuota_mensual":1196.6696142256196, "ahorro_total":11966.696142256196, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "MICROFINANCIERA", "registro":15, "monto_otorgado":12140.0, "cuota":30.0, "saldo":270.0, "tasa_externa":-1.0, "tasa_kubo":0.22, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9778, "fecha_inicio":"2024-03-02", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5064760, "monto_maximo_cliente": 610082.0, "cuota_externa_total": 47336.0, "capacidad_maxima_pago": 304356.0, "bursolnum": 7440144, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 37105.98229655993, "monto_max": 610082.0, "cuota_min": 322.9006720425269, "monto_min": 5000, "plazo_max": 12.0, "plazo_min": 4, "tasa": 0.6509, "kubo_score": "D3", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "TIENDA COMERCIAL", "registro":11, "monto_otorgado":1540.0, "cuota":40.0, "saldo":1020.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":25.0, "frecuencia_externa":"W", "avance":0.3377, "fecha_inicio":"2023-03-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-67.47201758629838, "ahorro_total":-2563.9366682793384, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":15, "monto_otorgado":25000.0, "cuota":2023.0, "saldo":19490.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":24.0, "numero_pagos_restante":13.0, "frecuencia_externa":"M", "avance":0.2204, "fecha_inicio":"2023-05-29", "tipo_deuda":"I", "ahorro_cuota_mensual":-23.049553950689415, "ahorro_total":-553.189294816546, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":17, "monto_otorgado":80000.0, "cuota":18000.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-12-13", "tipo_deuda":"R", "ahorro_cuota_mensual":18000.0, "ahorro_total":-18000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":18, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":954.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-06-26", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":16, "monto_otorgado":66100.0, "cuota":26468.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-03-14", "tipo_deuda":"R", "ahorro_cuota_mensual":26468.0, "ahorro_total":-26468.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":14, "monto_otorgado":24000.0, "cuota":1825.0, "saldo":23055.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0394, "fecha_inicio":"2023-11-23", "tipo_deuda":"R", "ahorro_cuota_mensual":24880.00000000003, "ahorro_total":-24880.00000000003, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":100000.0, "cuota":5000.0, "saldo":80058.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1994, "fecha_inicio":"2024-01-30", "tipo_deuda":"R", "ahorro_cuota_mensual":85058.00000000009, "ahorro_total":-85058.00000000009, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":24332.0, "cuota":632.0, "saldo":16116.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":25.0, "frecuencia_externa":"W", "avance":0.3377, "fecha_inicio":"2023-03-20", "tipo_deuda":"I", "ahorro_cuota_mensual":-1066.0578778635142, "ahorro_total":-40510.199358813545, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":56056.0, "cuota":1456.0, "saldo":39312.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":26.0, "frecuencia_externa":"W", "avance":0.2987, "fecha_inicio":"2023-05-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-2455.981440141261, "ahorro_total":-93327.29472536792, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":21098.0, "cuota":548.0, "saldo":18632.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":33.0, "frecuencia_externa":"W", "avance":0.1169, "fecha_inicio":"2023-11-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-924.3666409322877, "ahorro_total":-35125.932355426936, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":7, "monto_otorgado":1920.0, "cuota":60.0, "saldo":1515.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":128.0, "numero_pagos_restante":25.0, "frecuencia_externa":"W", "avance":0.2109, "fecha_inicio":"2023-09-11", "tipo_deuda":"I", "ahorro_cuota_mensual":-80.78405460970825, "ahorro_total":-2585.089747510664, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":8192.0, "cuota":256.0, "saldo":6464.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":128.0, "numero_pagos_restante":25.0, "frecuencia_externa":"W", "avance":0.2109, "fecha_inicio":"2023-09-11", "tipo_deuda":"I", "ahorro_cuota_mensual":-344.6786330014219, "ahorro_total":-11029.7162560455, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":5, "monto_otorgado":3080.0, "cuota":80.0, "saldo":2160.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":26.0, "frecuencia_externa":"W", "avance":0.2987, "fecha_inicio":"2023-05-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-134.94403517259676, "ahorro_total":-5127.873336558677, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":306170.0, "cuota":38084.0, "saldo":187021.0, "tasa_externa":0.8241, "tasa_kubo":0.6509, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3892, "fecha_inicio":"2023-09-19", "tipo_deuda":"I", "ahorro_cuota_mensual":978.0177034400695, "ahorro_total":11736.212441280833, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":88000.0, "cuota":12000.0, "saldo":81501.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0739, "fecha_inicio":"2017-02-20", "tipo_deuda":"R", "ahorro_cuota_mensual":93501.0000000001, "ahorro_total":-93501.0000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":9, "monto_otorgado":3080.0, "cuota":80.0, "saldo":2720.0, "tasa_externa":-1.0, "tasa_kubo":0.6509, "numero_pagos_otorgado":154.0, "numero_pagos_restante":33.0, "frecuencia_externa":"W", "avance":0.1169, "fecha_inicio":"2023-11-13", "tipo_deuda":"I", "ahorro_cuota_mensual":-134.94403517259676, "ahorro_total":-5127.873336558677, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5153135, "monto_maximo_cliente": 415807.0, "cuota_externa_total": 28202.0, "capacidad_maxima_pago": 73562.0, "bursolnum": 7440287, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 2613.4866898297028, "monto_max": 415807.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 59.0, "plazo_min": 4, "tasa": 0.5668, "kubo_score": "C5", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":13, "monto_otorgado":1921.0, "cuota":548.0, "saldo":548.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.7147, "fecha_inicio":"2019-11-23", "tipo_deuda":"O", "ahorro_cuota_mensual":1095.9999999999986, "ahorro_total":-1095.9999999999986, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":11, "monto_otorgado":41900.0, "cuota":3075.0, "saldo":33912.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":25.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1906, "fecha_inicio":"2023-06-28", "tipo_deuda":"I", "ahorro_cuota_mensual":717.6071618955334, "ahorro_total":17940.179047388334, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":8, "monto_otorgado":203600.0, "cuota":6059.0, "saldo":79519.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":14.0, "frecuencia_externa":"M", "avance":0.6094, "fecha_inicio":"2021-06-14", "tipo_deuda":"I", "ahorro_cuota_mensual":-1728.853783698978, "ahorro_total":-82984.98161755095, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":1506.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-07-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":3, "monto_otorgado":1921.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2018-07-02", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":1, "monto_otorgado":1921.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-06-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":14, "monto_otorgado":1200.0, "cuota":299.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2018-07-09", "tipo_deuda":"R", "ahorro_cuota_mensual":299.0, "ahorro_total":-299.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":10, "monto_otorgado":35000.0, "cuota":8663.0, "saldo":6861.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.804, "fecha_inicio":"2023-11-27", "tipo_deuda":"R", "ahorro_cuota_mensual":15523.999999999982, "ahorro_total":-15523.999999999982, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":2000.0, "cuota":100.0, "saldo":319.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8405, "fecha_inicio":"2024-01-12", "tipo_deuda":"R", "ahorro_cuota_mensual":418.99999999999915, "ahorro_total":-418.99999999999915, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":12179.0, "cuota":1141.0, "saldo":3248.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7333, "fecha_inicio":"2023-06-09", "tipo_deuda":"I", "ahorro_cuota_mensual":-69.19051618456706, "ahorro_total":-830.2861942148047, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":6, "monto_otorgado":74764.0, "cuota":3143.0, "saldo":50368.0, "tasa_externa":0.4054, "tasa_kubo":0.2914, "numero_pagos_otorgado":48.0, "numero_pagos_restante":24.0, "frecuencia_externa":"M", "avance":0.3263, "fecha_inicio":"2022-04-29", "tipo_deuda":"I", "ahorro_cuota_mensual":283.220529054664, "ahorro_total":13594.585394623871, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":214000.0, "cuota":6000.0, "saldo":184947.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1358, "fecha_inicio":"2017-10-09", "tipo_deuda":"R", "ahorro_cuota_mensual":190946.9999999995, "ahorro_total":-190946.9999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":2, "monto_otorgado":7500.0, "cuota":400.0, "saldo":400.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":15.0, "numero_pagos_restante":8.0, "frecuencia_externa":"M", "avance":0.9467, "fecha_inicio":"2023-10-07", "tipo_deuda":"R", "ahorro_cuota_mensual":366.9356323232766, "ahorro_total":5504.034484849149, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":12, "monto_otorgado":150432.0, "cuota":7522.0, "saldo":136337.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0937, "fecha_inicio":"2021-06-16", "tipo_deuda":"R", "ahorro_cuota_mensual":143858.99999999962, "ahorro_total":-143858.99999999962, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5156228, "monto_maximo_cliente": 2640384.0, "cuota_externa_total": 47862.0, "capacidad_maxima_pago": 261667.0, "bursolnum": 7440291, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 7203.655497228462, "monto_max": 2640384.0, "cuota_min": 208.00254263563033, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.7554, "kubo_score": "E1", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":80000.0, "cuota":10511.0, "saldo":34979.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.5628, "fecha_inicio":"2023-06-30", "tipo_deuda":"I", "ahorro_cuota_mensual":2141.453553856556, "ahorro_total":25697.442646278672, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":811.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2021-05-21", "tipo_deuda":"O", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":1000.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2015-11-11", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":6, "monto_otorgado":811.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-01-08", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "OTRAS FINANCIERA", "registro":11, "monto_otorgado":950000.0, "cuota":0.0, "saldo":950000.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.0, "fecha_inicio":"2024-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":950000.0000000021, "ahorro_total":-950000.0000000021, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":159778.0, "cuota":7851.0, "saldo":123366.0, "tasa_externa":0.4233, "tasa_kubo":0.3813, "numero_pagos_otorgado":36.0, "numero_pagos_restante":18.0, "frecuencia_externa":"M", "avance":0.2279, "fecha_inicio":"2022-10-24", "tipo_deuda":"I", "ahorro_cuota_mensual":-235.3145186902393, "ahorro_total":-8471.322672848615, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":26000.0, "cuota":1390.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2019-12-05", "tipo_deuda":"R", "ahorro_cuota_mensual":1390.0, "ahorro_total":-1390.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":108300.0, "cuota":15693.0, "saldo":61312.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.4339, "fecha_inicio":"2023-07-04", "tipo_deuda":"I", "ahorro_cuota_mensual":4362.726498533313, "ahorro_total":52352.71798239976, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":243000.0, "cuota":12150.0, "saldo":195505.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1955, "fecha_inicio":"2023-03-02", "tipo_deuda":"R", "ahorro_cuota_mensual":207655.00000000044, "ahorro_total":-207655.00000000044, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":48000.0, "cuota":2400.0, "saldo":26801.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4416, "fecha_inicio":"2021-05-21", "tipo_deuda":"R", "ahorro_cuota_mensual":29201.00000000006, "ahorro_total":-29201.00000000006, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "OTRAS FINANCIERA", "registro":10, "monto_otorgado":1200000.0, "cuota":0.0, "saldo":1032568.0, "tasa_externa":-1.0, "tasa_kubo":0.3813, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.1395, "fecha_inicio":"2023-07-31", "tipo_deuda":"I", "ahorro_cuota_mensual":1200000.0000000026, "ahorro_total":-1200000.0000000026, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5217560, "monto_maximo_cliente": 65518.0, "cuota_externa_total": 8567.0, "capacidad_maxima_pago": 36823.0, "bursolnum": 7440352, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1419.900523217919, "monto_max": 65518.0, "cuota_min": 173.6361078775173, "monto_min": 5000, "plazo_max": 35.0, "plazo_min": 4, "tasa": 0.5668, "kubo_score": "C5", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "SERVS. GRALES.", "registro":9, "monto_otorgado":67500.0, "cuota":1457.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-05-18", "tipo_deuda":"R", "ahorro_cuota_mensual":1457.0, "ahorro_total":-1457.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":8, "monto_otorgado":21100.0, "cuota":1582.0, "saldo":17622.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1648, "fecha_inicio":"2023-07-21", "tipo_deuda":"I", "ahorro_cuota_mensual":360.54916321974974, "ahorro_total":8653.179917273994, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":20000.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2012-06-15", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":12, "monto_otorgado":7161.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2001-06-28", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":10, "monto_otorgado":11830.0, "cuota":592.0, "saldo":2528.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7863, "fecha_inicio":"2001-05-29", "tipo_deuda":"R", "ahorro_cuota_mensual":3119.999999999993, "ahorro_total":-3119.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":7, "monto_otorgado":40000.0, "cuota":2000.0, "saldo":22686.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4328, "fecha_inicio":"2006-02-02", "tipo_deuda":"R", "ahorro_cuota_mensual":24685.999999999938, "ahorro_total":-24685.999999999938, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":4, "monto_otorgado":74360.0, "cuota":3718.0, "saldo":4416.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9406, "fecha_inicio":"2005-09-08", "tipo_deuda":"R", "ahorro_cuota_mensual":8133.999999999988, "ahorro_total":-8133.999999999988, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":31342.0, "cuota":1976.0, "saldo":17724.0, "tasa_externa":0.4402, "tasa_kubo":0.2914, "numero_pagos_otorgado":24.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.4345, "fecha_inicio":"2023-01-23", "tipo_deuda":"I", "ahorro_cuota_mensual":161.6534537267014, "ahorro_total":3879.6828894408336, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":7986.0, "cuota":400.0, "saldo":3131.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6079, "fecha_inicio":"2015-10-29", "tipo_deuda":"R", "ahorro_cuota_mensual":3530.9999999999914, "ahorro_total":-3530.9999999999914, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":5000.0, "cuota":697.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2016-08-26", "tipo_deuda":"R", "ahorro_cuota_mensual":697.0, "ahorro_total":-697.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "TIENDA COMERCIAL", "registro":6, "monto_otorgado":18000.0, "cuota":2151.0, "saldo":1415.0, "tasa_externa":-1.0, "tasa_kubo":0.2914, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9214, "fecha_inicio":"2015-10-24", "tipo_deuda":"R", "ahorro_cuota_mensual":3565.9999999999964, "ahorro_total":-3565.9999999999964, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5222923, "monto_maximo_cliente": 102873.0, "cuota_externa_total": 22029.0, "capacidad_maxima_pago": 45755.0, "bursolnum": 7440359, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 4870.031302228124, "monto_max": 102873.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 18.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":12, "monto_otorgado":10000.0, "cuota":972.0, "saldo":12966.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.2966, "fecha_inicio":"2013-06-30", "tipo_deuda":"R", "ahorro_cuota_mensual":13938.000000000002, "ahorro_total":-13938.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":9, "monto_otorgado":3217.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-07-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":702.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-11-09", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":6, "monto_otorgado":18000.0, "cuota":2144.0, "saldo":8281.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":24.0, "numero_pagos_restante":6.0, "frecuencia_externa":"S", "avance":0.5399, "fecha_inicio":"2023-07-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-1.4056439152259372, "ahorro_total":-16.867726982711247, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":1795.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2022-01-21", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "CIA Q' OTORGA", "registro":10, "monto_otorgado":91591.0, "cuota":4915.0, "saldo":8774.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":0.9042, "fecha_inicio":"2022-02-18", "tipo_deuda":"O", "ahorro_cuota_mensual":13689.000000000002, "ahorro_total":-13689.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":7000.0, "cuota":1186.0, "saldo":5889.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1587, "fecha_inicio":"2023-11-27", "tipo_deuda":"R", "ahorro_cuota_mensual":7075.000000000001, "ahorro_total":-7075.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":1000.0, "cuota":100.0, "saldo":1068.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":-0.068, "fecha_inicio":"2023-08-31", "tipo_deuda":"R", "ahorro_cuota_mensual":1168.0000000000002, "ahorro_total":-1168.0000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":2000.0, "cuota":182.0, "saldo":1699.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":10.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.1505, "fecha_inicio":"2023-05-04", "tipo_deuda":"R", "ahorro_cuota_mensual":-48.692768587167365, "ahorro_total":-486.92768587167365, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "TIENDA COMERCIAL", "registro":8, "monto_otorgado":33000.0, "cuota":6824.0, "saldo":12675.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.6159, "fecha_inicio":"2022-07-29", "tipo_deuda":"R", "ahorro_cuota_mensual":19499.000000000004, "ahorro_total":-19499.000000000004, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":52784.0, "cuota":5390.0, "saldo":15286.0, "tasa_externa":0.5251, "tasa_kubo":0.6193, "numero_pagos_otorgado":13.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.7104, "fecha_inicio":"2023-05-19", "tipo_deuda":"I", "ahorro_cuota_mensual":-567.8082863384379, "ahorro_total":-7381.507722399693, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":9000.0, "cuota":450.0, "saldo":7018.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.2202, "fecha_inicio":"2020-03-10", "tipo_deuda":"R", "ahorro_cuota_mensual":7468.000000000002, "ahorro_total":-7468.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5245488, "monto_maximo_cliente": 58463.0, "cuota_externa_total": 9931.0, "capacidad_maxima_pago": 46069.0, "bursolnum": 7440384, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1734.2526365022495, "monto_max": 58463.0, "cuota_min": 299.79381766541826, "monto_min": 5000, "plazo_max": 36.0, "plazo_min": 4, "tasa": 0.5991, "kubo_score": "D1", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "HIPOTECAGOBIERNO", "registro":10, "monto_otorgado":103181.0, "cuota":2716.0, "saldo":57910.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":360.0, "numero_pagos_restante":344.0, "frecuencia_externa":"M", "avance":0.4388, "fecha_inicio":"2023-01-06", "tipo_deuda":"M", "ahorro_cuota_mensual":-637.7418352911027, "ahorro_total":-229587.06070479698, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "SERVS. GRALES.", "registro":9, "monto_otorgado":72000.0, "cuota":1111.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2015-12-02", "tipo_deuda":"R", "ahorro_cuota_mensual":1111.0, "ahorro_total":-1111.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":8, "monto_otorgado":1449.0, "cuota":1163.0, "saldo":1163.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.1974, "fecha_inicio":"2019-04-13", "tipo_deuda":"O", "ahorro_cuota_mensual":2325.999999999999, "ahorro_total":-2325.999999999999, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "COMUNICACIONES", "registro":7, "monto_otorgado":1397.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2020-03-20", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":5, "monto_otorgado":25000.0, "cuota":1929.0, "saldo":20708.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":24.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.1717, "fecha_inicio":"2023-07-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-24.724780249763626, "ahorro_total":-593.394725994327, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":6, "monto_otorgado":26000.0, "cuota":2556.0, "saldo":15454.0, "tasa_externa":1.1535, "tasa_kubo":0.5991, "numero_pagos_otorgado":72.0, "numero_pagos_restante":13.0, "frecuencia_externa":"S", "avance":0.4056, "fecha_inicio":"2022-06-06", "tipo_deuda":"I", "ahorro_cuota_mensual":821.7473634977505, "ahorro_total":29582.905085919017, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":20000.0, "cuota":1000.0, "saldo":3049.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":15.0, "numero_pagos_restante":6.0, "frecuencia_externa":"Z", "avance":0.8476, "fecha_inicio":"2023-01-04", "tipo_deuda":"R", "ahorro_cuota_mensual":690.3333575968736, "ahorro_total":10355.000363953104, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":19500.0, "cuota":7945.0, "saldo":5194.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7336, "fecha_inicio":"2022-08-02", "tipo_deuda":"R", "ahorro_cuota_mensual":13138.999999999995, "ahorro_total":-13138.999999999995, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":19000.0, "cuota":950.0, "saldo":16511.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.131, "fecha_inicio":"2007-11-08", "tipo_deuda":"R", "ahorro_cuota_mensual":17460.99999999998, "ahorro_total":-17460.99999999998, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":11, "monto_otorgado":8519.0, "cuota":580.0, "saldo":7709.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0951, "fecha_inicio":"2018-12-19", "tipo_deuda":"R", "ahorro_cuota_mensual":8288.999999999993, "ahorro_total":-8288.999999999993, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":212603.0, "cuota":1.0, "saldo":210232.0, "tasa_externa":-1.0, "tasa_kubo":0.5991, "numero_pagos_otorgado":60.0, "numero_pagos_restante":57.0, "frecuencia_externa":"M", "avance":0.0112, "fecha_inicio":"2024-02-02", "tipo_deuda":"I", "ahorro_cuota_mensual":-12746.413003424184, "ahorro_total":-764784.7802054511, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5262916, "monto_maximo_cliente": 61375.0, "cuota_externa_total": 12881.0, "capacidad_maxima_pago": 39719.0, "bursolnum": 7440430, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 3967.3261972531327, "monto_max": 61375.0, "cuota_min": 308.7596227438041, "monto_min": 5000, "plazo_max": 18.0, "plazo_min": 4, "tasa": 0.6193, "kubo_score": "D2", "comision": 0.0, "proba": 0, "segmento": 26, "tipo_flujo": "Autogestivo", "comprobante_tasa": 0, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":8, "monto_otorgado":20500.0, "cuota":650.0, "saldo":1022.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9501, "fecha_inicio":"2023-07-28", "tipo_deuda":"R", "ahorro_cuota_mensual":1672.0000000000005, "ahorro_total":-1672.0000000000005, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "COMUNICACIONES", "registro":11, "monto_otorgado":0.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":18.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-1.0, "fecha_inicio":"2018-02-04", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":7, "monto_otorgado":10000.0, "cuota":1204.0, "saldo":6092.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.3908, "fecha_inicio":"2023-08-10", "tipo_deuda":"I", "ahorro_cuota_mensual":12.10797560265246, "ahorro_total":145.2957072318295, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":10, "monto_otorgado":12000.0, "cuota":-1.0, "saldo":406.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":0.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.9662, "fecha_inicio":"2021-01-22", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":9, "monto_otorgado":25000.0, "cuota":1250.0, "saldo":3310.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8676, "fecha_inicio":"2021-05-25", "tipo_deuda":"R", "ahorro_cuota_mensual":4560.000000000001, "ahorro_total":-4560.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":6, "monto_otorgado":10400.0, "cuota":6067.0, "saldo":1809.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.8261, "fecha_inicio":"2023-10-12", "tipo_deuda":"R", "ahorro_cuota_mensual":7876.0, "ahorro_total":-7876.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":4, "monto_otorgado":222.0, "cuota":233.0, "saldo":226.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.018, "fecha_inicio":"2024-02-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-2.290178000000253, "ahorro_total":-2.290178000000253, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":3, "monto_otorgado":186.0, "cuota":195.0, "saldo":189.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":1.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":-0.0161, "fecha_inicio":"2024-02-21", "tipo_deuda":"I", "ahorro_cuota_mensual":-2.1350140000002114, "ahorro_total":-2.1350140000002114, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":43000.0, "cuota":4482.0, "saldo":30365.0, "tasa_externa":0.4408, "tasa_kubo":0.6193, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2938, "fecha_inicio":"2023-10-19", "tipo_deuda":"I", "ahorro_cuota_mensual":-643.1357049085955, "ahorro_total":-7717.628458903146, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":31200.0, "cuota":3550.0, "saldo":10420.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.666, "fecha_inicio":"2023-09-05", "tipo_deuda":"R", "ahorro_cuota_mensual":13970.000000000002, "ahorro_total":-13970.000000000002, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "FINANCIERA", "registro":5, "monto_otorgado":1000.0, "cuota":388.0, "saldo":715.0, "tasa_externa":-1.0, "tasa_kubo":0.6193, "numero_pagos_otorgado":3.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.285, "fecha_inicio":"2024-01-18", "tipo_deuda":"I", "ahorro_cuota_mensual":13.983164414838257, "ahorro_total":41.94949324451477, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5431910, "monto_maximo_cliente": 800245.0, "cuota_externa_total": 62823.0, "capacidad_maxima_pago": 640413.33, "bursolnum": 7445351, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 26393.811192044283, "monto_max": 800245.0, "cuota_min": 249.09435350839087, "monto_min": 5000, "plazo_max": 47.0, "plazo_min": 4, "tasa": 0.5991, "kubo_score": "D1", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "SERVICIOS", "registro":6, "monto_otorgado":1370.0, "cuota":0.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":1.0, "fecha_inicio":"2021-05-26", "tipo_deuda":"O", "ahorro_cuota_mensual":0.0, "ahorro_total":-0.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":7, "monto_otorgado":150000.0, "cuota":7500.0, "saldo":7961.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.9469, "fecha_inicio":"2021-05-04", "tipo_deuda":"R", "ahorro_cuota_mensual":15461.000000000016, "ahorro_total":-15461.000000000016, "estatus_tasa":"No calculable", "tipo_revolvencia":"Transactor", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":5, "monto_otorgado":94500.0, "cuota":4725.0, "saldo":50392.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.4668, "fecha_inicio":"2019-10-09", "tipo_deuda":"R", "ahorro_cuota_mensual":55117.0000000001, "ahorro_total":-55117.0000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":100000.0, "cuota":8991.0, "saldo":81638.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":18.0, "numero_pagos_restante":11.0, "frecuencia_externa":"M", "avance":0.1836, "fecha_inicio":"2023-09-27", "tipo_deuda":"I", "ahorro_cuota_mensual":663.835437085585, "ahorro_total":11949.03786754053, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "BANCO", "registro":2, "monto_otorgado":92000.0, "cuota":6897.0, "saldo":63392.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.311, "fecha_inicio":"2019-02-15", "tipo_deuda":"R", "ahorro_cuota_mensual":70289.00000000013, "ahorro_total":-70289.00000000013, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":1, "monto_otorgado":115000.0, "cuota":14520.0, "saldo":80000.0, "tasa_externa":-1.0, "tasa_kubo":0.4818, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.3043, "fecha_inicio":"2018-04-24", "tipo_deuda":"R", "ahorro_cuota_mensual":94520.00000000017, "ahorro_total":-94520.00000000017, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":4, "monto_otorgado":598500.0, "cuota":27881.0, "saldo":515623.0, "tasa_externa":0.3788, "tasa_kubo":0.4818, "numero_pagos_otorgado":36.0, "numero_pagos_restante":27.0, "frecuencia_externa":"M", "avance":0.1385, "fecha_inicio":"2023-07-31", "tipo_deuda":"I", "ahorro_cuota_mensual":-6712.010307011056, "ahorro_total":-241632.37105239803, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5446124, "monto_maximo_cliente": 84012.0, "cuota_externa_total": 13379.0, "capacidad_maxima_pago": 96621.0, "bursolnum": 7445370, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 5293.744643303981, "monto_max": 84012.0, "cuota_min": 285.5882600985808, "monto_min": 5000, "plazo_max": 33.0, "plazo_min": 4, "tasa": 0.7007, "kubo_score": "D5", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Pre-aprobado", "comprobante_tasa": 1, "comprobante_ingresos": 0, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "BANCO", "registro":1, "monto_otorgado":18200.0, "cuota":1125.0, "saldo":4012.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.7796, "fecha_inicio":"2022-09-07", "tipo_deuda":"R", "ahorro_cuota_mensual":5137.000000000001, "ahorro_total":-5137.000000000001, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":2, "monto_otorgado":80000.0, "cuota":5900.0, "saldo":153574.0, "tasa_externa":0.56, "tasa_kubo":0.5668, "numero_pagos_otorgado":43.0, "numero_pagos_restante":10.0, "frecuencia_externa":"S", "avance":-0.9197, "fecha_inicio":"2023-05-05", "tipo_deuda":"I", "ahorro_cuota_mensual":-445.85407781089634, "ahorro_total":-9808.78971183972, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":3, "monto_otorgado":50000.0, "cuota":6354.0, "saldo":39776.0, "tasa_externa":-1.0, "tasa_kubo":0.5668, "numero_pagos_otorgado":12.0, "numero_pagos_restante":6.0, "frecuencia_externa":"M", "avance":0.2045, "fecha_inicio":"2023-10-03", "tipo_deuda":"I", "ahorro_cuota_mensual":559.2894279279335, "ahorro_total":6711.473135135202, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
+  </si>
+  <si>
+    <t>{"Prospecto": 5544014, "monto_maximo_cliente": 20776.0, "cuota_externa_total": 8008.0, "capacidad_maxima_pago": 23226.0, "bursolnum": 7439720, "Oferta Automatico": [{"loan_type": "CON", "sub_loan_type": "CONSOLIDACION_FLEXIBLE" , "cuota_max": 1647.3817702448512, "monto_max": 20776.0, "cuota_min": 370.5085944866793, "monto_min": 5000, "plazo_max": 23.0, "plazo_min": 4, "tasa": 0.821, "kubo_score": "E2", "comision": 0.0481, "proba": 0, "segmento": 26, "tipo_flujo": "Tradicional", "comprobante_tasa": 1, "comprobante_ingresos": 1, "frecuencia": ["M", "S", "K", "W"] , "tasa_asistida": [0.821, 0.7554, 0.7007, 0.6722, 0.6509, 0.6193, 0.5991, 0.5668, 0.5504, 0.5486, 0.5391, 0.5292, 0.4818, 0.4706, 0.4582, 0.4428, 0.4295, 0.3813, 0.3617, 0.3337, 0.2914], "comisiones": [0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0481, 0.0476, 0.0471, 0.0466, 0.046, 0.0455, 0.0449, 0.0444, 0.0439, 0.0433, 0.0428, 0.0423, 0.0417], "kubo_scores": ['E2', 'E1', 'D5', 'D4', 'D3', 'D2', 'D1', 'C5', 'C4', 'C3', 'C2', 'C1', 'B5', 'B4', 'B3', 'B2', 'B1', 'A5', 'A4', 'A3', 'A2'], "deudas_buro": [ {"entidad": "COMUNICACIONES", "registro":5, "monto_otorgado":999.0, "cuota":-1.0, "saldo":0.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":1000.0, "numero_pagos_restante":905.0, "frecuencia_externa":"M", "avance":1.0, "fecha_inicio":"2016-06-08", "tipo_deuda":"R", "ahorro_cuota_mensual":-1.0, "ahorro_total":-1000.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "FINANCIERA", "registro":1, "monto_otorgado":2880.0, "cuota":144.0, "saldo":2676.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":-1.0, "numero_pagos_restante":-1.0, "frecuencia_externa":"Z", "avance":0.0708, "fecha_inicio":"2023-01-31", "tipo_deuda":"R", "ahorro_cuota_mensual":2820.0, "ahorro_total":-2820.0, "estatus_tasa":"No calculable", "tipo_revolvencia":"Light Revolver", "deuda_consolidable":1}, {"entidad": "BANCO", "registro":3, "monto_otorgado":18100.0, "cuota":2166.0, "saldo":17009.0, "tasa_externa":0.7373, "tasa_kubo":0.7554, "numero_pagos_otorgado":12.0, "numero_pagos_restante":9.0, "frecuencia_externa":"M", "avance":0.0603, "fecha_inicio":"2024-01-26", "tipo_deuda":"I", "ahorro_cuota_mensual":-149.6663517107122, "ahorro_total":-1795.9962205285465, "estatus_tasa":"Calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":1}, {"entidad": "KUBO FINANCIERO", "registro":2, "monto_otorgado":10000.0, "cuota":1070.0, "saldo":9723.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":18.0, "numero_pagos_restante":15.0, "frecuencia_externa":"M", "avance":0.0277, "fecha_inicio":"2024-01-30", "tipo_deuda":"I", "ahorro_cuota_mensual":54.08549508704277, "ahorro_total":973.5389115667699, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "KUBO FINANCIERO", "registro":4, "monto_otorgado":30000.0, "cuota":2577.0, "saldo":29756.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":36.0, "numero_pagos_restante":32.0, "frecuencia_externa":"M", "avance":0.0081, "fecha_inicio":"2023-12-29", "tipo_deuda":"I", "ahorro_cuota_mensual":198.21587934326863, "ahorro_total":7135.7716563576705, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}, {"entidad": "HIPOTECAGOBIERNO", "registro":6, "monto_otorgado":305797.0, "cuota":2092.0, "saldo":206484.0, "tasa_externa":-1.0, "tasa_kubo":0.7554, "numero_pagos_otorgado":360.0, "numero_pagos_restante":324.0, "frecuencia_externa":"M", "avance":0.3248, "fecha_inicio":"2021-05-01", "tipo_deuda":"M", "ahorro_cuota_mensual":-12985.874648144287, "ahorro_total":-4674914.8733319435, "estatus_tasa":"No calculable", "tipo_revolvencia":"High Revolver", "deuda_consolidable":0}]}]}</t>
   </si>
 </sst>
 </file>
@@ -611,551 +611,608 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="82.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="52.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3">
         <v>24059</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3">
         <v>189189</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3">
         <v>230009</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3">
         <v>301784</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3">
-        <v>653012</v>
+        <v>820117</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="3">
+        <v>985053</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="3">
+        <v>1360950</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3">
-        <v>820117</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="3">
-        <v>985053</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3">
-        <v>1360950</v>
+        <v>1585349</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3">
-        <v>1585349</v>
+        <v>1669798</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3">
-        <v>1669798</v>
+        <v>1764064</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3">
-        <v>1764064</v>
+        <v>1823294</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3">
-        <v>1823294</v>
+        <v>2352204</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+        <v>16</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3">
-        <v>2352204</v>
+        <v>2371630</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3">
-        <v>2371630</v>
+        <v>2417292</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3">
-        <v>2417292</v>
+        <v>2433653</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3">
-        <v>2433653</v>
+        <v>2696976</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C17" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3">
-        <v>2696976</v>
+        <v>2769844</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C18" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="3">
-        <v>2769844</v>
+        <v>2776466</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+        <v>22</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="3">
-        <v>2776466</v>
+        <v>2871236</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+        <v>23</v>
+      </c>
+      <c r="C20" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="3">
-        <v>2871236</v>
+        <v>3002968</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+        <v>24</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="3">
-        <v>3002968</v>
+        <v>3052806</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+        <v>25</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="3">
-        <v>3052806</v>
+        <v>3190170</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+        <v>26</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="3">
-        <v>3190170</v>
+        <v>3332202</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+        <v>27</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="3">
-        <v>3332202</v>
+        <v>3334267</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C25" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="3">
-        <v>3334267</v>
+        <v>3590341</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>26</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C26" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="3">
-        <v>3590341</v>
+        <v>3636540</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C27" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="3">
-        <v>3636540</v>
+        <v>3651682</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C28" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="3">
-        <v>3651682</v>
+        <v>3787395</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C29" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="3">
-        <v>3787395</v>
+        <v>3901833</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C30" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="3">
-        <v>3901833</v>
+        <v>3965394</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C31" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="3">
-        <v>3965394</v>
+        <v>4100476</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C32" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="3">
-        <v>4100476</v>
+        <v>4161166</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>33</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C33" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="3">
-        <v>4161166</v>
+        <v>4177829</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>34</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C34" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="3">
-        <v>4177829</v>
+        <v>4268611</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C35" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="3">
-        <v>4268611</v>
+        <v>4302913</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>36</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C36" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="3">
-        <v>4302913</v>
+        <v>4323421</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>37</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C37" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="3">
-        <v>4323421</v>
+        <v>4426818</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C38" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="3">
-        <v>4426818</v>
+        <v>4446822</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C39" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="3">
-        <v>4446822</v>
+        <v>4475229</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C40" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="3">
-        <v>4475229</v>
+        <v>4488665</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C41" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
       <c r="A42" s="3">
-        <v>4488665</v>
+        <v>4503596</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C42" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
       <c r="A43" s="3">
-        <v>4503596</v>
+        <v>4557872</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C43" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
       <c r="A44" s="3">
-        <v>4557872</v>
+        <v>4604014</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C44" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
       <c r="A45" s="3">
-        <v>4604014</v>
+        <v>4637424</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C45" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
       <c r="A46" s="3">
-        <v>4637424</v>
+        <v>4639545</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>46</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C46" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
       <c r="A47" s="3">
-        <v>4639545</v>
+        <v>4714725</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C47" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
       <c r="A48" s="3">
-        <v>4714725</v>
+        <v>4721997</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>48</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C48" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
       <c r="A49" s="3">
-        <v>4721997</v>
+        <v>4733672</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C49" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
       <c r="A50" s="3">
-        <v>4733672</v>
+        <v>4754385</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C50" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
       <c r="A51" s="3">
-        <v>4754385</v>
+        <v>4759224</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>51</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C51" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
       <c r="A52" s="3">
-        <v>4759224</v>
+        <v>4993943</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C52" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
       <c r="A53" s="3">
-        <v>4993943</v>
+        <v>5008298</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C53" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
       <c r="A54" s="3">
-        <v>4995215</v>
+        <v>5013364</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C54" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
       <c r="A55" s="3">
-        <v>5008298</v>
+        <v>5064760</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>55</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C55" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
       <c r="A56" s="3">
-        <v>5013364</v>
+        <v>5153135</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C56" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
       <c r="A57" s="3">
-        <v>5064760</v>
+        <v>5156228</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>57</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C57" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
       <c r="A58" s="3">
-        <v>5153135</v>
+        <v>5217560</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C58" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
       <c r="A59" s="3">
-        <v>5156228</v>
+        <v>5222923</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>59</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C59" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
       <c r="A60" s="3">
-        <v>5217560</v>
+        <v>5245488</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C60" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
       <c r="A61" s="3">
-        <v>5222923</v>
+        <v>5262916</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>61</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C61" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
       <c r="A62" s="3">
-        <v>5245488</v>
+        <v>5431910</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C62" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
       <c r="A63" s="3">
-        <v>5262916</v>
+        <v>5446124</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C63" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
       <c r="A64" s="3">
-        <v>5359375</v>
+        <v>5544014</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
-      <c r="A65" s="3">
-        <v>5431910</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
-      <c r="A66" s="3">
-        <v>5446124</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25">
-      <c r="A67" s="3">
-        <v>5544014</v>
-      </c>
-      <c r="B67" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="C64" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agrega validación para asignar tasa original en la oferta cuando la lista de tasas asistidas vienen vacias.
</commit_message>
<xml_diff>
--- a/Json_ofertas.xlsx
+++ b/Json_ofertas.xlsx
@@ -622,7 +622,7 @@
     <col min="3" max="3" style="6" width="52.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>24059</v>
       </c>
@@ -644,7 +644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>189189</v>
       </c>
@@ -655,7 +655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>230009</v>
       </c>
@@ -666,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>301784</v>
       </c>
@@ -677,7 +677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>820117</v>
       </c>
@@ -688,7 +688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>985053</v>
       </c>
@@ -699,7 +699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>1360950</v>
       </c>
@@ -710,7 +710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>1585349</v>
       </c>
@@ -719,7 +719,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>1669798</v>
       </c>
@@ -728,7 +728,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>1764064</v>
       </c>
@@ -737,7 +737,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
         <v>1823294</v>
       </c>
@@ -746,7 +746,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3">
         <v>2352204</v>
       </c>
@@ -755,7 +755,7 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3">
         <v>2371630</v>
       </c>
@@ -764,7 +764,7 @@
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3">
         <v>2417292</v>
       </c>
@@ -773,7 +773,7 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3">
         <v>2433653</v>
       </c>
@@ -782,7 +782,7 @@
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3">
         <v>2696976</v>
       </c>
@@ -791,7 +791,7 @@
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3">
         <v>2769844</v>
       </c>

</xml_diff>

<commit_message>
Se agregan cambios para calculos de comisión sobre el monto de oferta
</commit_message>
<xml_diff>
--- a/Json_ofertas.xlsx
+++ b/Json_ofertas.xlsx
@@ -68,7 +68,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -455,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>24059</v>
       </c>
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>189189</v>
       </c>
@@ -471,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>230009</v>
       </c>
@@ -479,7 +479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>301784</v>
       </c>
@@ -487,7 +487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>820117</v>
       </c>
@@ -495,7 +495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>985053</v>
       </c>
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>1360950</v>
       </c>
@@ -511,7 +511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>2117837</v>
       </c>

</xml_diff>

<commit_message>
se agrega funcionalidad para extender plazos
</commit_message>
<xml_diff>
--- a/Json_ofertas.xlsx
+++ b/Json_ofertas.xlsx
@@ -447,7 +447,7 @@
     <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3">
         <v>24059</v>
       </c>
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3">
         <v>189189</v>
       </c>
@@ -471,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3">
         <v>230009</v>
       </c>
@@ -479,7 +479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3">
         <v>301784</v>
       </c>
@@ -487,7 +487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3">
         <v>820117</v>
       </c>
@@ -495,7 +495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3">
         <v>985053</v>
       </c>
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3">
         <v>1360950</v>
       </c>
@@ -511,7 +511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3">
         <v>2117837</v>
       </c>

</xml_diff>